<commit_message>
somehow, we missed fixproppmtct
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="80" windowWidth="27480" windowHeight="15460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
     <sheet name="Transitions" sheetId="2" r:id="rId2"/>
     <sheet name="Parameters" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1176,7 +1176,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1864,10 +1864,10 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2197,37 +2197,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="25" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="31" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="8.83203125" style="2"/>
-    <col min="38" max="38" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="8.85546875" style="2"/>
+    <col min="38" max="38" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
@@ -2348,7 +2348,7 @@
         <v>lost-lt50</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="16">
+    <row r="2" spans="1:39" ht="16.5">
       <c r="A2" s="23" t="str">
         <f>Compartments!A2</f>
         <v>susreg</v>
@@ -2396,7 +2396,7 @@
       <c r="AL2" s="16"/>
       <c r="AM2" s="19"/>
     </row>
-    <row r="3" spans="1:39" ht="16">
+    <row r="3" spans="1:39" ht="16.5">
       <c r="A3" s="23" t="str">
         <f>Compartments!A3</f>
         <v>progcirc</v>
@@ -2444,7 +2444,7 @@
       <c r="AL3" s="17"/>
       <c r="AM3" s="21"/>
     </row>
-    <row r="4" spans="1:39" ht="16">
+    <row r="4" spans="1:39" ht="16.5">
       <c r="A4" s="7" t="str">
         <f>Compartments!A4</f>
         <v>undx-acute</v>
@@ -2496,7 +2496,7 @@
       <c r="AL4" s="16"/>
       <c r="AM4" s="19"/>
     </row>
-    <row r="5" spans="1:39" ht="16">
+    <row r="5" spans="1:39" ht="16.5">
       <c r="A5" s="7" t="str">
         <f>Compartments!A5</f>
         <v>undx-gt500</v>
@@ -2548,7 +2548,7 @@
       <c r="AL5" s="16"/>
       <c r="AM5" s="19"/>
     </row>
-    <row r="6" spans="1:39" ht="16">
+    <row r="6" spans="1:39" ht="16.5">
       <c r="A6" s="7" t="str">
         <f>Compartments!A6</f>
         <v>undx-gt350</v>
@@ -2600,7 +2600,7 @@
       <c r="AL6" s="16"/>
       <c r="AM6" s="19"/>
     </row>
-    <row r="7" spans="1:39" ht="16">
+    <row r="7" spans="1:39" ht="16.5">
       <c r="A7" s="7" t="str">
         <f>Compartments!A7</f>
         <v>undx-gt200</v>
@@ -2652,7 +2652,7 @@
       <c r="AL7" s="16"/>
       <c r="AM7" s="19"/>
     </row>
-    <row r="8" spans="1:39" ht="16">
+    <row r="8" spans="1:39" ht="16.5">
       <c r="A8" s="7" t="str">
         <f>Compartments!A8</f>
         <v>undx-gt50</v>
@@ -2704,7 +2704,7 @@
       <c r="AL8" s="16"/>
       <c r="AM8" s="19"/>
     </row>
-    <row r="9" spans="1:39" ht="16">
+    <row r="9" spans="1:39" ht="16.5">
       <c r="A9" s="7" t="str">
         <f>Compartments!A9</f>
         <v>undx-lt50</v>
@@ -2752,7 +2752,7 @@
       <c r="AL9" s="17"/>
       <c r="AM9" s="21"/>
     </row>
-    <row r="10" spans="1:39" ht="16">
+    <row r="10" spans="1:39" ht="16.5">
       <c r="A10" s="8" t="str">
         <f>Compartments!A10</f>
         <v>dx-acute</v>
@@ -2804,7 +2804,7 @@
       <c r="AL10" s="16"/>
       <c r="AM10" s="19"/>
     </row>
-    <row r="11" spans="1:39" ht="16">
+    <row r="11" spans="1:39" ht="16.5">
       <c r="A11" s="8" t="str">
         <f>Compartments!A11</f>
         <v>dx-gt500</v>
@@ -2856,7 +2856,7 @@
       <c r="AL11" s="16"/>
       <c r="AM11" s="19"/>
     </row>
-    <row r="12" spans="1:39" ht="16">
+    <row r="12" spans="1:39" ht="16.5">
       <c r="A12" s="8" t="str">
         <f>Compartments!A12</f>
         <v>dx-gt350</v>
@@ -2908,7 +2908,7 @@
       <c r="AL12" s="16"/>
       <c r="AM12" s="19"/>
     </row>
-    <row r="13" spans="1:39" ht="16">
+    <row r="13" spans="1:39" ht="16.5">
       <c r="A13" s="8" t="str">
         <f>Compartments!A13</f>
         <v>dx-gt200</v>
@@ -2960,7 +2960,7 @@
       <c r="AL13" s="16"/>
       <c r="AM13" s="19"/>
     </row>
-    <row r="14" spans="1:39" ht="16">
+    <row r="14" spans="1:39" ht="16.5">
       <c r="A14" s="8" t="str">
         <f>Compartments!A14</f>
         <v>dx-gt50</v>
@@ -3012,7 +3012,7 @@
       <c r="AL14" s="16"/>
       <c r="AM14" s="19"/>
     </row>
-    <row r="15" spans="1:39" ht="16">
+    <row r="15" spans="1:39" ht="16.5">
       <c r="A15" s="8" t="str">
         <f>Compartments!A15</f>
         <v>dx-lt50</v>
@@ -3060,7 +3060,7 @@
       <c r="AL15" s="17"/>
       <c r="AM15" s="21"/>
     </row>
-    <row r="16" spans="1:39" ht="16">
+    <row r="16" spans="1:39" ht="16.5">
       <c r="A16" s="9" t="str">
         <f>Compartments!A16</f>
         <v>care-acute</v>
@@ -3112,7 +3112,7 @@
       <c r="AL16" s="16"/>
       <c r="AM16" s="19"/>
     </row>
-    <row r="17" spans="1:39" ht="16">
+    <row r="17" spans="1:39" ht="16.5">
       <c r="A17" s="9" t="str">
         <f>Compartments!A17</f>
         <v>care-gt500</v>
@@ -3164,7 +3164,7 @@
       <c r="AL17" s="16"/>
       <c r="AM17" s="19"/>
     </row>
-    <row r="18" spans="1:39" ht="16">
+    <row r="18" spans="1:39" ht="16.5">
       <c r="A18" s="9" t="str">
         <f>Compartments!A18</f>
         <v>care-gt350</v>
@@ -3216,7 +3216,7 @@
       <c r="AL18" s="16"/>
       <c r="AM18" s="19"/>
     </row>
-    <row r="19" spans="1:39" ht="16">
+    <row r="19" spans="1:39" ht="16.5">
       <c r="A19" s="9" t="str">
         <f>Compartments!A19</f>
         <v>care-gt200</v>
@@ -3268,7 +3268,7 @@
       </c>
       <c r="AM19" s="19"/>
     </row>
-    <row r="20" spans="1:39" ht="16">
+    <row r="20" spans="1:39" ht="16.5">
       <c r="A20" s="9" t="str">
         <f>Compartments!A20</f>
         <v>care-gt50</v>
@@ -3320,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="16">
+    <row r="21" spans="1:39" ht="16.5">
       <c r="A21" s="9" t="str">
         <f>Compartments!A21</f>
         <v>care-lt50</v>
@@ -3368,7 +3368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="16">
+    <row r="22" spans="1:39" ht="16.5">
       <c r="A22" s="10" t="str">
         <f>Compartments!A22</f>
         <v>usvl-acute</v>
@@ -3424,7 +3424,7 @@
       <c r="AL22" s="16"/>
       <c r="AM22" s="19"/>
     </row>
-    <row r="23" spans="1:39" ht="16">
+    <row r="23" spans="1:39" ht="16.5">
       <c r="A23" s="10" t="str">
         <f>Compartments!A23</f>
         <v>usvl-gt500</v>
@@ -3480,7 +3480,7 @@
       <c r="AL23" s="16"/>
       <c r="AM23" s="19"/>
     </row>
-    <row r="24" spans="1:39" ht="16">
+    <row r="24" spans="1:39" ht="16.5">
       <c r="A24" s="10" t="str">
         <f>Compartments!A24</f>
         <v>usvl-gt350</v>
@@ -3542,7 +3542,7 @@
       <c r="AL24" s="16"/>
       <c r="AM24" s="19"/>
     </row>
-    <row r="25" spans="1:39" ht="16">
+    <row r="25" spans="1:39" ht="16.5">
       <c r="A25" s="10" t="str">
         <f>Compartments!A25</f>
         <v>usvl-gt200</v>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="AM25" s="19"/>
     </row>
-    <row r="26" spans="1:39" ht="16">
+    <row r="26" spans="1:39" ht="16.5">
       <c r="A26" s="10" t="str">
         <f>Compartments!A26</f>
         <v>usvl-gt50</v>
@@ -3666,7 +3666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="16">
+    <row r="27" spans="1:39" ht="16.5">
       <c r="A27" s="10" t="str">
         <f>Compartments!A27</f>
         <v>usvl-lt50</v>
@@ -3722,7 +3722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="16">
+    <row r="28" spans="1:39" ht="16.5">
       <c r="A28" s="4" t="str">
         <f>Compartments!A28</f>
         <v>svl-acute</v>
@@ -3778,7 +3778,7 @@
       <c r="AL28" s="16"/>
       <c r="AM28" s="19"/>
     </row>
-    <row r="29" spans="1:39" ht="16">
+    <row r="29" spans="1:39" ht="16.5">
       <c r="A29" s="4" t="str">
         <f>Compartments!A29</f>
         <v>svl-gt500</v>
@@ -3828,7 +3828,7 @@
       <c r="AL29" s="16"/>
       <c r="AM29" s="19"/>
     </row>
-    <row r="30" spans="1:39" ht="16">
+    <row r="30" spans="1:39" ht="16.5">
       <c r="A30" s="4" t="str">
         <f>Compartments!A30</f>
         <v>svl-gt350</v>
@@ -3884,7 +3884,7 @@
       <c r="AL30" s="16"/>
       <c r="AM30" s="19"/>
     </row>
-    <row r="31" spans="1:39" ht="16">
+    <row r="31" spans="1:39" ht="16.5">
       <c r="A31" s="4" t="str">
         <f>Compartments!A31</f>
         <v>svl-gt200</v>
@@ -3940,7 +3940,7 @@
       <c r="AL31" s="16"/>
       <c r="AM31" s="19"/>
     </row>
-    <row r="32" spans="1:39" ht="16">
+    <row r="32" spans="1:39" ht="16.5">
       <c r="A32" s="4" t="str">
         <f>Compartments!A32</f>
         <v>svl-gt50</v>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="AM32" s="19"/>
     </row>
-    <row r="33" spans="1:39" ht="16">
+    <row r="33" spans="1:39" ht="16.5">
       <c r="A33" s="4" t="str">
         <f>Compartments!A33</f>
         <v>svl-lt50</v>
@@ -4052,7 +4052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="16">
+    <row r="34" spans="1:39" ht="16.5">
       <c r="A34" s="5" t="str">
         <f>Compartments!A34</f>
         <v>lost-acute</v>
@@ -4104,7 +4104,7 @@
       <c r="AL34" s="16"/>
       <c r="AM34" s="19"/>
     </row>
-    <row r="35" spans="1:39" ht="16">
+    <row r="35" spans="1:39" ht="16.5">
       <c r="A35" s="5" t="str">
         <f>Compartments!A35</f>
         <v>lost-gt500</v>
@@ -4156,7 +4156,7 @@
       <c r="AL35" s="16"/>
       <c r="AM35" s="19"/>
     </row>
-    <row r="36" spans="1:39" ht="16">
+    <row r="36" spans="1:39" ht="16.5">
       <c r="A36" s="5" t="str">
         <f>Compartments!A36</f>
         <v>lost-gt350</v>
@@ -4208,7 +4208,7 @@
       <c r="AL36" s="16"/>
       <c r="AM36" s="19"/>
     </row>
-    <row r="37" spans="1:39" ht="16">
+    <row r="37" spans="1:39" ht="16.5">
       <c r="A37" s="5" t="str">
         <f>Compartments!A37</f>
         <v>lost-gt200</v>
@@ -4260,7 +4260,7 @@
       </c>
       <c r="AM37" s="19"/>
     </row>
-    <row r="38" spans="1:39" ht="16">
+    <row r="38" spans="1:39" ht="16.5">
       <c r="A38" s="5" t="str">
         <f>Compartments!A38</f>
         <v>lost-gt50</v>
@@ -4312,7 +4312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="16">
+    <row r="39" spans="1:39" ht="16.5">
       <c r="A39" s="5" t="str">
         <f>Compartments!A39</f>
         <v>lost-lt50</v>
@@ -4380,26 +4380,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="26"/>
+    <col min="1" max="1" width="55.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="25" customFormat="1">

</xml_diff>

<commit_message>
MODEL-INPUT CHANGES for vl
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="80" windowWidth="27480" windowHeight="15460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
     <sheet name="Transitions" sheetId="2" r:id="rId2"/>
     <sheet name="Parameters" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -632,9 +632,6 @@
     <t>Viral load monitoring (number/year)</t>
   </si>
   <si>
-    <t>freqvlmon</t>
-  </si>
-  <si>
     <t>Loss to follow-up rate (per year)</t>
   </si>
   <si>
@@ -1170,13 +1167,16 @@
   </si>
   <si>
     <t>partinj</t>
+  </si>
+  <si>
+    <t>numvlmon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1394,7 +1394,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1402,6 +1402,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1503,7 +1505,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="47">
     <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
     <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
     <cellStyle name="60% - Accent5" xfId="6" builtinId="48"/>
@@ -1527,6 +1529,7 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
@@ -1547,6 +1550,7 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1864,10 +1868,10 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2201,33 +2205,33 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="25" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="31" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="8.85546875" style="2"/>
-    <col min="38" max="38" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="8.83203125" style="2"/>
+    <col min="38" max="38" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
@@ -2348,7 +2352,7 @@
         <v>lost-lt50</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="16.5">
+    <row r="2" spans="1:39" ht="16">
       <c r="A2" s="23" t="str">
         <f>Compartments!A2</f>
         <v>susreg</v>
@@ -2396,7 +2400,7 @@
       <c r="AL2" s="16"/>
       <c r="AM2" s="19"/>
     </row>
-    <row r="3" spans="1:39" ht="16.5">
+    <row r="3" spans="1:39" ht="16">
       <c r="A3" s="23" t="str">
         <f>Compartments!A3</f>
         <v>progcirc</v>
@@ -2444,7 +2448,7 @@
       <c r="AL3" s="17"/>
       <c r="AM3" s="21"/>
     </row>
-    <row r="4" spans="1:39" ht="16.5">
+    <row r="4" spans="1:39" ht="16">
       <c r="A4" s="7" t="str">
         <f>Compartments!A4</f>
         <v>undx-acute</v>
@@ -2496,7 +2500,7 @@
       <c r="AL4" s="16"/>
       <c r="AM4" s="19"/>
     </row>
-    <row r="5" spans="1:39" ht="16.5">
+    <row r="5" spans="1:39" ht="16">
       <c r="A5" s="7" t="str">
         <f>Compartments!A5</f>
         <v>undx-gt500</v>
@@ -2548,7 +2552,7 @@
       <c r="AL5" s="16"/>
       <c r="AM5" s="19"/>
     </row>
-    <row r="6" spans="1:39" ht="16.5">
+    <row r="6" spans="1:39" ht="16">
       <c r="A6" s="7" t="str">
         <f>Compartments!A6</f>
         <v>undx-gt350</v>
@@ -2600,7 +2604,7 @@
       <c r="AL6" s="16"/>
       <c r="AM6" s="19"/>
     </row>
-    <row r="7" spans="1:39" ht="16.5">
+    <row r="7" spans="1:39" ht="16">
       <c r="A7" s="7" t="str">
         <f>Compartments!A7</f>
         <v>undx-gt200</v>
@@ -2652,7 +2656,7 @@
       <c r="AL7" s="16"/>
       <c r="AM7" s="19"/>
     </row>
-    <row r="8" spans="1:39" ht="16.5">
+    <row r="8" spans="1:39" ht="16">
       <c r="A8" s="7" t="str">
         <f>Compartments!A8</f>
         <v>undx-gt50</v>
@@ -2704,7 +2708,7 @@
       <c r="AL8" s="16"/>
       <c r="AM8" s="19"/>
     </row>
-    <row r="9" spans="1:39" ht="16.5">
+    <row r="9" spans="1:39" ht="16">
       <c r="A9" s="7" t="str">
         <f>Compartments!A9</f>
         <v>undx-lt50</v>
@@ -2752,7 +2756,7 @@
       <c r="AL9" s="17"/>
       <c r="AM9" s="21"/>
     </row>
-    <row r="10" spans="1:39" ht="16.5">
+    <row r="10" spans="1:39" ht="16">
       <c r="A10" s="8" t="str">
         <f>Compartments!A10</f>
         <v>dx-acute</v>
@@ -2804,7 +2808,7 @@
       <c r="AL10" s="16"/>
       <c r="AM10" s="19"/>
     </row>
-    <row r="11" spans="1:39" ht="16.5">
+    <row r="11" spans="1:39" ht="16">
       <c r="A11" s="8" t="str">
         <f>Compartments!A11</f>
         <v>dx-gt500</v>
@@ -2856,7 +2860,7 @@
       <c r="AL11" s="16"/>
       <c r="AM11" s="19"/>
     </row>
-    <row r="12" spans="1:39" ht="16.5">
+    <row r="12" spans="1:39" ht="16">
       <c r="A12" s="8" t="str">
         <f>Compartments!A12</f>
         <v>dx-gt350</v>
@@ -2908,7 +2912,7 @@
       <c r="AL12" s="16"/>
       <c r="AM12" s="19"/>
     </row>
-    <row r="13" spans="1:39" ht="16.5">
+    <row r="13" spans="1:39" ht="16">
       <c r="A13" s="8" t="str">
         <f>Compartments!A13</f>
         <v>dx-gt200</v>
@@ -2960,7 +2964,7 @@
       <c r="AL13" s="16"/>
       <c r="AM13" s="19"/>
     </row>
-    <row r="14" spans="1:39" ht="16.5">
+    <row r="14" spans="1:39" ht="16">
       <c r="A14" s="8" t="str">
         <f>Compartments!A14</f>
         <v>dx-gt50</v>
@@ -3012,7 +3016,7 @@
       <c r="AL14" s="16"/>
       <c r="AM14" s="19"/>
     </row>
-    <row r="15" spans="1:39" ht="16.5">
+    <row r="15" spans="1:39" ht="16">
       <c r="A15" s="8" t="str">
         <f>Compartments!A15</f>
         <v>dx-lt50</v>
@@ -3060,7 +3064,7 @@
       <c r="AL15" s="17"/>
       <c r="AM15" s="21"/>
     </row>
-    <row r="16" spans="1:39" ht="16.5">
+    <row r="16" spans="1:39" ht="16">
       <c r="A16" s="9" t="str">
         <f>Compartments!A16</f>
         <v>care-acute</v>
@@ -3112,7 +3116,7 @@
       <c r="AL16" s="16"/>
       <c r="AM16" s="19"/>
     </row>
-    <row r="17" spans="1:39" ht="16.5">
+    <row r="17" spans="1:39" ht="16">
       <c r="A17" s="9" t="str">
         <f>Compartments!A17</f>
         <v>care-gt500</v>
@@ -3164,7 +3168,7 @@
       <c r="AL17" s="16"/>
       <c r="AM17" s="19"/>
     </row>
-    <row r="18" spans="1:39" ht="16.5">
+    <row r="18" spans="1:39" ht="16">
       <c r="A18" s="9" t="str">
         <f>Compartments!A18</f>
         <v>care-gt350</v>
@@ -3216,7 +3220,7 @@
       <c r="AL18" s="16"/>
       <c r="AM18" s="19"/>
     </row>
-    <row r="19" spans="1:39" ht="16.5">
+    <row r="19" spans="1:39" ht="16">
       <c r="A19" s="9" t="str">
         <f>Compartments!A19</f>
         <v>care-gt200</v>
@@ -3268,7 +3272,7 @@
       </c>
       <c r="AM19" s="19"/>
     </row>
-    <row r="20" spans="1:39" ht="16.5">
+    <row r="20" spans="1:39" ht="16">
       <c r="A20" s="9" t="str">
         <f>Compartments!A20</f>
         <v>care-gt50</v>
@@ -3320,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="16.5">
+    <row r="21" spans="1:39" ht="16">
       <c r="A21" s="9" t="str">
         <f>Compartments!A21</f>
         <v>care-lt50</v>
@@ -3368,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="16.5">
+    <row r="22" spans="1:39" ht="16">
       <c r="A22" s="10" t="str">
         <f>Compartments!A22</f>
         <v>usvl-acute</v>
@@ -3424,7 +3428,7 @@
       <c r="AL22" s="16"/>
       <c r="AM22" s="19"/>
     </row>
-    <row r="23" spans="1:39" ht="16.5">
+    <row r="23" spans="1:39" ht="16">
       <c r="A23" s="10" t="str">
         <f>Compartments!A23</f>
         <v>usvl-gt500</v>
@@ -3480,7 +3484,7 @@
       <c r="AL23" s="16"/>
       <c r="AM23" s="19"/>
     </row>
-    <row r="24" spans="1:39" ht="16.5">
+    <row r="24" spans="1:39" ht="16">
       <c r="A24" s="10" t="str">
         <f>Compartments!A24</f>
         <v>usvl-gt350</v>
@@ -3542,7 +3546,7 @@
       <c r="AL24" s="16"/>
       <c r="AM24" s="19"/>
     </row>
-    <row r="25" spans="1:39" ht="16.5">
+    <row r="25" spans="1:39" ht="16">
       <c r="A25" s="10" t="str">
         <f>Compartments!A25</f>
         <v>usvl-gt200</v>
@@ -3604,7 +3608,7 @@
       </c>
       <c r="AM25" s="19"/>
     </row>
-    <row r="26" spans="1:39" ht="16.5">
+    <row r="26" spans="1:39" ht="16">
       <c r="A26" s="10" t="str">
         <f>Compartments!A26</f>
         <v>usvl-gt50</v>
@@ -3666,7 +3670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="16.5">
+    <row r="27" spans="1:39" ht="16">
       <c r="A27" s="10" t="str">
         <f>Compartments!A27</f>
         <v>usvl-lt50</v>
@@ -3722,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="16.5">
+    <row r="28" spans="1:39" ht="16">
       <c r="A28" s="4" t="str">
         <f>Compartments!A28</f>
         <v>svl-acute</v>
@@ -3778,7 +3782,7 @@
       <c r="AL28" s="16"/>
       <c r="AM28" s="19"/>
     </row>
-    <row r="29" spans="1:39" ht="16.5">
+    <row r="29" spans="1:39" ht="16">
       <c r="A29" s="4" t="str">
         <f>Compartments!A29</f>
         <v>svl-gt500</v>
@@ -3828,7 +3832,7 @@
       <c r="AL29" s="16"/>
       <c r="AM29" s="19"/>
     </row>
-    <row r="30" spans="1:39" ht="16.5">
+    <row r="30" spans="1:39" ht="16">
       <c r="A30" s="4" t="str">
         <f>Compartments!A30</f>
         <v>svl-gt350</v>
@@ -3884,7 +3888,7 @@
       <c r="AL30" s="16"/>
       <c r="AM30" s="19"/>
     </row>
-    <row r="31" spans="1:39" ht="16.5">
+    <row r="31" spans="1:39" ht="16">
       <c r="A31" s="4" t="str">
         <f>Compartments!A31</f>
         <v>svl-gt200</v>
@@ -3940,7 +3944,7 @@
       <c r="AL31" s="16"/>
       <c r="AM31" s="19"/>
     </row>
-    <row r="32" spans="1:39" ht="16.5">
+    <row r="32" spans="1:39" ht="16">
       <c r="A32" s="4" t="str">
         <f>Compartments!A32</f>
         <v>svl-gt50</v>
@@ -3996,7 +4000,7 @@
       </c>
       <c r="AM32" s="19"/>
     </row>
-    <row r="33" spans="1:39" ht="16.5">
+    <row r="33" spans="1:39" ht="16">
       <c r="A33" s="4" t="str">
         <f>Compartments!A33</f>
         <v>svl-lt50</v>
@@ -4052,7 +4056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="16.5">
+    <row r="34" spans="1:39" ht="16">
       <c r="A34" s="5" t="str">
         <f>Compartments!A34</f>
         <v>lost-acute</v>
@@ -4104,7 +4108,7 @@
       <c r="AL34" s="16"/>
       <c r="AM34" s="19"/>
     </row>
-    <row r="35" spans="1:39" ht="16.5">
+    <row r="35" spans="1:39" ht="16">
       <c r="A35" s="5" t="str">
         <f>Compartments!A35</f>
         <v>lost-gt500</v>
@@ -4156,7 +4160,7 @@
       <c r="AL35" s="16"/>
       <c r="AM35" s="19"/>
     </row>
-    <row r="36" spans="1:39" ht="16.5">
+    <row r="36" spans="1:39" ht="16">
       <c r="A36" s="5" t="str">
         <f>Compartments!A36</f>
         <v>lost-gt350</v>
@@ -4208,7 +4212,7 @@
       <c r="AL36" s="16"/>
       <c r="AM36" s="19"/>
     </row>
-    <row r="37" spans="1:39" ht="16.5">
+    <row r="37" spans="1:39" ht="16">
       <c r="A37" s="5" t="str">
         <f>Compartments!A37</f>
         <v>lost-gt200</v>
@@ -4260,7 +4264,7 @@
       </c>
       <c r="AM37" s="19"/>
     </row>
-    <row r="38" spans="1:39" ht="16.5">
+    <row r="38" spans="1:39" ht="16">
       <c r="A38" s="5" t="str">
         <f>Compartments!A38</f>
         <v>lost-gt50</v>
@@ -4312,7 +4316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="16.5">
+    <row r="39" spans="1:39" ht="16">
       <c r="A39" s="5" t="str">
         <f>Compartments!A39</f>
         <v>lost-lt50</v>
@@ -4381,25 +4385,25 @@
   <dimension ref="A1:M118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="26"/>
+    <col min="1" max="1" width="55.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="25" customFormat="1">
@@ -5681,13 +5685,13 @@
         <v>202</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>203</v>
+        <v>382</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>203</v>
+        <v>382</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F32" s="26" t="s">
         <v>131</v>
@@ -5705,7 +5709,7 @@
         <v>1</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="L32" s="26">
         <v>1</v>
@@ -5716,16 +5720,16 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="C33" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="C33" s="26" t="s">
-        <v>206</v>
-      </c>
       <c r="D33" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E33" s="26" t="s">
         <v>109</v>
@@ -5757,16 +5761,16 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B34" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="C34" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="C34" s="26" t="s">
-        <v>209</v>
-      </c>
       <c r="D34" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E34" s="26" t="s">
         <v>109</v>
@@ -5798,16 +5802,16 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>211</v>
-      </c>
       <c r="D35" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E35" s="26" t="s">
         <v>94</v>
@@ -5839,16 +5843,16 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="B36" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>213</v>
-      </c>
       <c r="D36" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E36" s="26" t="s">
         <v>94</v>
@@ -5880,16 +5884,16 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="B37" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="26" t="s">
-        <v>215</v>
-      </c>
       <c r="D37" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E37" s="26" t="s">
         <v>94</v>
@@ -5921,16 +5925,16 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="B38" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>217</v>
-      </c>
       <c r="D38" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E38" s="26" t="s">
         <v>94</v>
@@ -5962,16 +5966,16 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="B39" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>219</v>
-      </c>
       <c r="D39" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E39" s="26" t="s">
         <v>94</v>
@@ -6003,25 +6007,25 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="B40" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="26" t="s">
+      <c r="D40" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E40" s="26" t="s">
         <v>221</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>222</v>
       </c>
       <c r="F40" s="26" t="s">
         <v>131</v>
       </c>
       <c r="G40" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H40" s="26" t="s">
         <v>111</v>
@@ -6039,30 +6043,30 @@
         <v>0</v>
       </c>
       <c r="M40" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="B41" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>226</v>
-      </c>
       <c r="D41" s="26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F41" s="26" t="s">
         <v>131</v>
       </c>
       <c r="G41" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H41" s="26" t="s">
         <v>111</v>
@@ -6080,30 +6084,30 @@
         <v>0</v>
       </c>
       <c r="M41" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="B42" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>228</v>
-      </c>
       <c r="D42" s="26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F42" s="26" t="s">
         <v>131</v>
       </c>
       <c r="G42" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H42" s="26" t="s">
         <v>111</v>
@@ -6121,30 +6125,30 @@
         <v>0</v>
       </c>
       <c r="M42" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B43" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>230</v>
-      </c>
       <c r="D43" s="26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F43" s="26" t="s">
         <v>131</v>
       </c>
       <c r="G43" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H43" s="26" t="s">
         <v>111</v>
@@ -6162,30 +6166,30 @@
         <v>0</v>
       </c>
       <c r="M43" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="B44" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>232</v>
-      </c>
       <c r="D44" s="26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F44" s="26" t="s">
         <v>131</v>
       </c>
       <c r="G44" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H44" s="26" t="s">
         <v>111</v>
@@ -6203,21 +6207,21 @@
         <v>0</v>
       </c>
       <c r="M44" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="C45" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="D45" s="26" t="s">
         <v>233</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="D45" s="26" t="s">
-        <v>234</v>
       </c>
       <c r="E45" s="26" t="s">
         <v>98</v>
@@ -6249,16 +6253,16 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B46" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="C46" s="26" t="s">
-        <v>237</v>
-      </c>
       <c r="D46" s="26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E46" s="26" t="s">
         <v>94</v>
@@ -6267,10 +6271,10 @@
         <v>131</v>
       </c>
       <c r="G46" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H46" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I46" s="26" t="s">
         <v>92</v>
@@ -6285,21 +6289,21 @@
         <v>1</v>
       </c>
       <c r="M46" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C47" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="B47" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C47" s="26" t="s">
-        <v>240</v>
-      </c>
       <c r="D47" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E47" s="26" t="s">
         <v>94</v>
@@ -6308,10 +6312,10 @@
         <v>131</v>
       </c>
       <c r="G47" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H47" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I47" s="26" t="s">
         <v>92</v>
@@ -6326,21 +6330,21 @@
         <v>1</v>
       </c>
       <c r="M47" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C48" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="B48" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>242</v>
-      </c>
       <c r="D48" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E48" s="26" t="s">
         <v>94</v>
@@ -6349,10 +6353,10 @@
         <v>131</v>
       </c>
       <c r="G48" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H48" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I48" s="26" t="s">
         <v>92</v>
@@ -6367,21 +6371,21 @@
         <v>1</v>
       </c>
       <c r="M48" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C49" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="B49" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>244</v>
-      </c>
       <c r="D49" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E49" s="26" t="s">
         <v>94</v>
@@ -6390,10 +6394,10 @@
         <v>131</v>
       </c>
       <c r="G49" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H49" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I49" s="26" t="s">
         <v>92</v>
@@ -6408,21 +6412,21 @@
         <v>1</v>
       </c>
       <c r="M49" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C50" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="B50" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>246</v>
-      </c>
       <c r="D50" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E50" s="26" t="s">
         <v>94</v>
@@ -6431,10 +6435,10 @@
         <v>131</v>
       </c>
       <c r="G50" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I50" s="26" t="s">
         <v>92</v>
@@ -6449,21 +6453,21 @@
         <v>1</v>
       </c>
       <c r="M50" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C51" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="B51" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C51" s="26" t="s">
-        <v>248</v>
-      </c>
       <c r="D51" s="26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E51" s="26" t="s">
         <v>94</v>
@@ -6472,10 +6476,10 @@
         <v>131</v>
       </c>
       <c r="G51" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H51" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I51" s="26" t="s">
         <v>92</v>
@@ -6490,21 +6494,21 @@
         <v>1</v>
       </c>
       <c r="M51" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C52" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="B52" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>250</v>
-      </c>
       <c r="D52" s="26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E52" s="26" t="s">
         <v>94</v>
@@ -6513,10 +6517,10 @@
         <v>131</v>
       </c>
       <c r="G52" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H52" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I52" s="26" t="s">
         <v>92</v>
@@ -6531,21 +6535,21 @@
         <v>1</v>
       </c>
       <c r="M52" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C53" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="B53" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>252</v>
-      </c>
       <c r="D53" s="26" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E53" s="26" t="s">
         <v>102</v>
@@ -6554,10 +6558,10 @@
         <v>131</v>
       </c>
       <c r="G53" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I53" s="26" t="s">
         <v>92</v>
@@ -6572,21 +6576,21 @@
         <v>1</v>
       </c>
       <c r="M53" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C54" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="B54" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>254</v>
-      </c>
       <c r="D54" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E54" s="26" t="s">
         <v>102</v>
@@ -6595,10 +6599,10 @@
         <v>131</v>
       </c>
       <c r="G54" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I54" s="26" t="s">
         <v>92</v>
@@ -6613,21 +6617,21 @@
         <v>1</v>
       </c>
       <c r="M54" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C55" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="B55" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>256</v>
-      </c>
       <c r="D55" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E55" s="26" t="s">
         <v>102</v>
@@ -6636,10 +6640,10 @@
         <v>131</v>
       </c>
       <c r="G55" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I55" s="26" t="s">
         <v>92</v>
@@ -6654,21 +6658,21 @@
         <v>1</v>
       </c>
       <c r="M55" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="B56" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C56" s="26" t="s">
-        <v>258</v>
-      </c>
       <c r="D56" s="26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E56" s="26" t="s">
         <v>102</v>
@@ -6677,10 +6681,10 @@
         <v>131</v>
       </c>
       <c r="G56" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I56" s="26" t="s">
         <v>92</v>
@@ -6695,21 +6699,21 @@
         <v>1</v>
       </c>
       <c r="M56" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C57" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="B57" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>260</v>
-      </c>
       <c r="D57" s="26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E57" s="26" t="s">
         <v>102</v>
@@ -6718,10 +6722,10 @@
         <v>131</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I57" s="26" t="s">
         <v>92</v>
@@ -6736,21 +6740,21 @@
         <v>1</v>
       </c>
       <c r="M57" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C58" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="B58" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>262</v>
-      </c>
       <c r="D58" s="26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E58" s="26" t="s">
         <v>102</v>
@@ -6759,10 +6763,10 @@
         <v>131</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I58" s="26" t="s">
         <v>92</v>
@@ -6777,21 +6781,21 @@
         <v>1</v>
       </c>
       <c r="M58" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" s="26" t="s">
         <v>263</v>
       </c>
-      <c r="B59" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C59" s="26" t="s">
-        <v>264</v>
-      </c>
       <c r="D59" s="26" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E59" s="26" t="s">
         <v>102</v>
@@ -6800,10 +6804,10 @@
         <v>131</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I59" s="26" t="s">
         <v>92</v>
@@ -6818,21 +6822,21 @@
         <v>1</v>
       </c>
       <c r="M59" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C60" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="B60" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C60" s="26" t="s">
-        <v>266</v>
-      </c>
       <c r="D60" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E60" s="26" t="s">
         <v>198</v>
@@ -6841,10 +6845,10 @@
         <v>131</v>
       </c>
       <c r="G60" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I60" s="26" t="s">
         <v>92</v>
@@ -6859,21 +6863,21 @@
         <v>1</v>
       </c>
       <c r="M60" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C61" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="B61" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C61" s="26" t="s">
-        <v>268</v>
-      </c>
       <c r="D61" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E61" s="26" t="s">
         <v>198</v>
@@ -6882,10 +6886,10 @@
         <v>131</v>
       </c>
       <c r="G61" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H61" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I61" s="26" t="s">
         <v>92</v>
@@ -6900,21 +6904,21 @@
         <v>1</v>
       </c>
       <c r="M61" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:13">
       <c r="A62" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="B62" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C62" s="26" t="s">
         <v>269</v>
       </c>
-      <c r="B62" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C62" s="26" t="s">
-        <v>270</v>
-      </c>
       <c r="D62" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E62" s="26" t="s">
         <v>198</v>
@@ -6923,10 +6927,10 @@
         <v>131</v>
       </c>
       <c r="G62" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H62" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I62" s="26" t="s">
         <v>92</v>
@@ -6941,21 +6945,21 @@
         <v>1</v>
       </c>
       <c r="M62" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C63" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="B63" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C63" s="26" t="s">
-        <v>272</v>
-      </c>
       <c r="D63" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E63" s="26" t="s">
         <v>198</v>
@@ -6964,10 +6968,10 @@
         <v>131</v>
       </c>
       <c r="G63" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H63" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I63" s="26" t="s">
         <v>92</v>
@@ -6982,21 +6986,21 @@
         <v>1</v>
       </c>
       <c r="M63" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C64" s="26" t="s">
         <v>273</v>
       </c>
-      <c r="B64" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C64" s="26" t="s">
-        <v>274</v>
-      </c>
       <c r="D64" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E64" s="26" t="s">
         <v>198</v>
@@ -7005,10 +7009,10 @@
         <v>131</v>
       </c>
       <c r="G64" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H64" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I64" s="26" t="s">
         <v>92</v>
@@ -7023,21 +7027,21 @@
         <v>1</v>
       </c>
       <c r="M64" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="B65" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C65" s="26" t="s">
         <v>275</v>
       </c>
-      <c r="B65" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C65" s="26" t="s">
-        <v>276</v>
-      </c>
       <c r="D65" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E65" s="26" t="s">
         <v>198</v>
@@ -7046,10 +7050,10 @@
         <v>131</v>
       </c>
       <c r="G65" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H65" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I65" s="26" t="s">
         <v>92</v>
@@ -7064,21 +7068,21 @@
         <v>1</v>
       </c>
       <c r="M65" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C66" s="26" t="s">
         <v>277</v>
       </c>
-      <c r="B66" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C66" s="26" t="s">
-        <v>278</v>
-      </c>
       <c r="D66" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E66" s="26" t="s">
         <v>198</v>
@@ -7087,10 +7091,10 @@
         <v>131</v>
       </c>
       <c r="G66" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H66" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I66" s="26" t="s">
         <v>92</v>
@@ -7105,21 +7109,21 @@
         <v>1</v>
       </c>
       <c r="M66" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C67" s="26" t="s">
         <v>279</v>
       </c>
-      <c r="B67" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C67" s="26" t="s">
-        <v>280</v>
-      </c>
       <c r="D67" s="26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E67" s="26" t="s">
         <v>198</v>
@@ -7128,10 +7132,10 @@
         <v>131</v>
       </c>
       <c r="G67" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H67" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I67" s="26" t="s">
         <v>92</v>
@@ -7146,21 +7150,21 @@
         <v>1</v>
       </c>
       <c r="M67" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="B68" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C68" s="26" t="s">
         <v>281</v>
       </c>
-      <c r="B68" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C68" s="26" t="s">
-        <v>282</v>
-      </c>
       <c r="D68" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E68" s="26" t="s">
         <v>198</v>
@@ -7169,10 +7173,10 @@
         <v>131</v>
       </c>
       <c r="G68" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H68" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I68" s="26" t="s">
         <v>92</v>
@@ -7187,21 +7191,21 @@
         <v>1</v>
       </c>
       <c r="M68" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C69" s="26" t="s">
         <v>283</v>
       </c>
-      <c r="B69" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C69" s="26" t="s">
-        <v>284</v>
-      </c>
       <c r="D69" s="26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E69" s="26" t="s">
         <v>198</v>
@@ -7210,10 +7214,10 @@
         <v>131</v>
       </c>
       <c r="G69" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H69" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I69" s="26" t="s">
         <v>92</v>
@@ -7228,21 +7232,21 @@
         <v>1</v>
       </c>
       <c r="M69" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C70" s="26" t="s">
         <v>285</v>
       </c>
-      <c r="B70" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C70" s="26" t="s">
-        <v>286</v>
-      </c>
       <c r="D70" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E70" s="26" t="s">
         <v>109</v>
@@ -7251,10 +7255,10 @@
         <v>131</v>
       </c>
       <c r="G70" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H70" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I70" s="26" t="s">
         <v>92</v>
@@ -7269,21 +7273,21 @@
         <v>1</v>
       </c>
       <c r="M70" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="28" t="s">
+        <v>286</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C71" s="26" t="s">
         <v>287</v>
       </c>
-      <c r="B71" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C71" s="26" t="s">
-        <v>288</v>
-      </c>
       <c r="D71" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E71" s="26" t="s">
         <v>109</v>
@@ -7292,10 +7296,10 @@
         <v>131</v>
       </c>
       <c r="G71" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H71" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I71" s="26" t="s">
         <v>92</v>
@@ -7310,21 +7314,21 @@
         <v>1</v>
       </c>
       <c r="M71" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C72" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="B72" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C72" s="26" t="s">
-        <v>290</v>
-      </c>
       <c r="D72" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E72" s="26" t="s">
         <v>109</v>
@@ -7333,10 +7337,10 @@
         <v>131</v>
       </c>
       <c r="G72" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H72" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I72" s="26" t="s">
         <v>92</v>
@@ -7351,21 +7355,21 @@
         <v>1</v>
       </c>
       <c r="M72" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C73" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="B73" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C73" s="26" t="s">
-        <v>292</v>
-      </c>
       <c r="D73" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E73" s="26" t="s">
         <v>109</v>
@@ -7374,10 +7378,10 @@
         <v>131</v>
       </c>
       <c r="G73" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H73" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I73" s="26" t="s">
         <v>92</v>
@@ -7392,21 +7396,21 @@
         <v>1</v>
       </c>
       <c r="M73" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C74" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="B74" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C74" s="26" t="s">
-        <v>294</v>
-      </c>
       <c r="D74" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E74" s="26" t="s">
         <v>109</v>
@@ -7415,10 +7419,10 @@
         <v>131</v>
       </c>
       <c r="G74" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H74" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I74" s="26" t="s">
         <v>92</v>
@@ -7433,21 +7437,21 @@
         <v>1</v>
       </c>
       <c r="M74" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="B75" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C75" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="B75" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C75" s="26" t="s">
-        <v>296</v>
-      </c>
       <c r="D75" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E75" s="26" t="s">
         <v>109</v>
@@ -7456,10 +7460,10 @@
         <v>131</v>
       </c>
       <c r="G75" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H75" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I75" s="26" t="s">
         <v>92</v>
@@ -7474,21 +7478,21 @@
         <v>1</v>
       </c>
       <c r="M75" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C76" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="B76" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C76" s="26" t="s">
-        <v>298</v>
-      </c>
       <c r="D76" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E76" s="26" t="s">
         <v>109</v>
@@ -7497,10 +7501,10 @@
         <v>131</v>
       </c>
       <c r="G76" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H76" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I76" s="26" t="s">
         <v>92</v>
@@ -7515,21 +7519,21 @@
         <v>1</v>
       </c>
       <c r="M76" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="B77" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C77" s="26" t="s">
         <v>299</v>
       </c>
-      <c r="B77" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C77" s="26" t="s">
-        <v>300</v>
-      </c>
       <c r="D77" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E77" s="26" t="s">
         <v>109</v>
@@ -7538,10 +7542,10 @@
         <v>131</v>
       </c>
       <c r="G77" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H77" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I77" s="26" t="s">
         <v>92</v>
@@ -7556,21 +7560,21 @@
         <v>1</v>
       </c>
       <c r="M77" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="B78" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C78" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="B78" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C78" s="26" t="s">
-        <v>302</v>
-      </c>
       <c r="D78" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E78" s="26" t="s">
         <v>109</v>
@@ -7579,10 +7583,10 @@
         <v>131</v>
       </c>
       <c r="G78" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H78" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I78" s="26" t="s">
         <v>92</v>
@@ -7597,21 +7601,21 @@
         <v>1</v>
       </c>
       <c r="M78" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="B79" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C79" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="B79" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C79" s="26" t="s">
-        <v>304</v>
-      </c>
       <c r="D79" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E79" s="26" t="s">
         <v>109</v>
@@ -7620,10 +7624,10 @@
         <v>131</v>
       </c>
       <c r="G79" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H79" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I79" s="26" t="s">
         <v>92</v>
@@ -7638,21 +7642,21 @@
         <v>1</v>
       </c>
       <c r="M79" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="B80" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C80" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="B80" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C80" s="26" t="s">
-        <v>306</v>
-      </c>
       <c r="D80" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E80" s="26" t="s">
         <v>109</v>
@@ -7661,10 +7665,10 @@
         <v>131</v>
       </c>
       <c r="G80" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H80" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I80" s="26" t="s">
         <v>92</v>
@@ -7679,21 +7683,21 @@
         <v>1</v>
       </c>
       <c r="M80" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="B81" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C81" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="B81" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C81" s="26" t="s">
-        <v>308</v>
-      </c>
       <c r="D81" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E81" s="26" t="s">
         <v>109</v>
@@ -7702,10 +7706,10 @@
         <v>131</v>
       </c>
       <c r="G81" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H81" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I81" s="26" t="s">
         <v>92</v>
@@ -7720,21 +7724,21 @@
         <v>1</v>
       </c>
       <c r="M81" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="82" spans="1:13">
       <c r="A82" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="B82" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C82" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="B82" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C82" s="28" t="s">
-        <v>310</v>
-      </c>
       <c r="D82" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E82" s="26" t="s">
         <v>109</v>
@@ -7743,10 +7747,10 @@
         <v>131</v>
       </c>
       <c r="G82" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H82" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I82" s="26" t="s">
         <v>92</v>
@@ -7761,21 +7765,21 @@
         <v>1</v>
       </c>
       <c r="M82" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" spans="1:13">
       <c r="A83" s="28" t="s">
+        <v>310</v>
+      </c>
+      <c r="B83" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C83" s="28" t="s">
         <v>311</v>
       </c>
-      <c r="B83" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C83" s="28" t="s">
-        <v>312</v>
-      </c>
       <c r="D83" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E83" s="26" t="s">
         <v>109</v>
@@ -7784,10 +7788,10 @@
         <v>131</v>
       </c>
       <c r="G83" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H83" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I83" s="26" t="s">
         <v>92</v>
@@ -7802,21 +7806,21 @@
         <v>1</v>
       </c>
       <c r="M83" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="B84" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C84" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="B84" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C84" s="26" t="s">
-        <v>314</v>
-      </c>
       <c r="D84" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E84" s="26" t="s">
         <v>109</v>
@@ -7825,10 +7829,10 @@
         <v>131</v>
       </c>
       <c r="G84" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H84" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I84" s="26" t="s">
         <v>92</v>
@@ -7843,21 +7847,21 @@
         <v>1</v>
       </c>
       <c r="M84" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="B85" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C85" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="B85" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C85" s="26" t="s">
-        <v>316</v>
-      </c>
       <c r="D85" s="26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E85" s="26" t="s">
         <v>102</v>
@@ -7866,10 +7870,10 @@
         <v>131</v>
       </c>
       <c r="G85" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H85" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I85" s="26" t="s">
         <v>92</v>
@@ -7884,21 +7888,21 @@
         <v>1</v>
       </c>
       <c r="M85" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="B86" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C86" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="B86" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C86" s="26" t="s">
-        <v>318</v>
-      </c>
       <c r="D86" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E86" s="26" t="s">
         <v>102</v>
@@ -7907,10 +7911,10 @@
         <v>131</v>
       </c>
       <c r="G86" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H86" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I86" s="26" t="s">
         <v>92</v>
@@ -7925,21 +7929,21 @@
         <v>1</v>
       </c>
       <c r="M86" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="B87" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C87" s="26" t="s">
         <v>319</v>
       </c>
-      <c r="B87" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C87" s="26" t="s">
-        <v>320</v>
-      </c>
       <c r="D87" s="26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E87" s="26" t="s">
         <v>102</v>
@@ -7948,10 +7952,10 @@
         <v>131</v>
       </c>
       <c r="G87" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H87" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I87" s="26" t="s">
         <v>92</v>
@@ -7966,21 +7970,21 @@
         <v>1</v>
       </c>
       <c r="M87" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="B88" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C88" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="B88" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C88" s="26" t="s">
-        <v>322</v>
-      </c>
       <c r="D88" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E88" s="26" t="s">
         <v>94</v>
@@ -7989,10 +7993,10 @@
         <v>131</v>
       </c>
       <c r="G88" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H88" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I88" s="26" t="s">
         <v>92</v>
@@ -8007,21 +8011,21 @@
         <v>1</v>
       </c>
       <c r="M88" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="B89" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C89" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="B89" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C89" s="26" t="s">
-        <v>324</v>
-      </c>
       <c r="D89" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E89" s="26" t="s">
         <v>94</v>
@@ -8030,10 +8034,10 @@
         <v>131</v>
       </c>
       <c r="G89" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H89" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I89" s="26" t="s">
         <v>92</v>
@@ -8048,21 +8052,21 @@
         <v>1</v>
       </c>
       <c r="M89" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="90" spans="1:13">
       <c r="A90" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="B90" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C90" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="B90" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C90" s="26" t="s">
-        <v>326</v>
-      </c>
       <c r="D90" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E90" s="26" t="s">
         <v>94</v>
@@ -8071,10 +8075,10 @@
         <v>131</v>
       </c>
       <c r="G90" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H90" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I90" s="26" t="s">
         <v>92</v>
@@ -8089,21 +8093,21 @@
         <v>1</v>
       </c>
       <c r="M90" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="91" spans="1:13">
       <c r="A91" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="B91" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C91" s="26" t="s">
         <v>327</v>
       </c>
-      <c r="B91" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C91" s="26" t="s">
-        <v>328</v>
-      </c>
       <c r="D91" s="26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E91" s="26" t="s">
         <v>94</v>
@@ -8112,10 +8116,10 @@
         <v>131</v>
       </c>
       <c r="G91" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H91" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I91" s="26" t="s">
         <v>92</v>
@@ -8130,21 +8134,21 @@
         <v>1</v>
       </c>
       <c r="M91" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="B92" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C92" s="26" t="s">
         <v>329</v>
       </c>
-      <c r="B92" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C92" s="26" t="s">
-        <v>330</v>
-      </c>
       <c r="D92" s="26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E92" s="26" t="s">
         <v>94</v>
@@ -8153,10 +8157,10 @@
         <v>131</v>
       </c>
       <c r="G92" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H92" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I92" s="26" t="s">
         <v>92</v>
@@ -8171,21 +8175,21 @@
         <v>1</v>
       </c>
       <c r="M92" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="B93" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C93" s="26" t="s">
         <v>331</v>
       </c>
-      <c r="B93" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C93" s="26" t="s">
-        <v>332</v>
-      </c>
       <c r="D93" s="26" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E93" s="26" t="s">
         <v>94</v>
@@ -8194,10 +8198,10 @@
         <v>131</v>
       </c>
       <c r="G93" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H93" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I93" s="26" t="s">
         <v>92</v>
@@ -8212,21 +8216,21 @@
         <v>1</v>
       </c>
       <c r="M93" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="B94" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C94" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="B94" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C94" s="26" t="s">
-        <v>334</v>
-      </c>
       <c r="D94" s="26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E94" s="26" t="s">
         <v>94</v>
@@ -8235,10 +8239,10 @@
         <v>131</v>
       </c>
       <c r="G94" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H94" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I94" s="26" t="s">
         <v>92</v>
@@ -8253,21 +8257,21 @@
         <v>1</v>
       </c>
       <c r="M94" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="B95" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C95" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="B95" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C95" s="26" t="s">
-        <v>336</v>
-      </c>
       <c r="D95" s="26" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E95" s="26" t="s">
         <v>94</v>
@@ -8276,10 +8280,10 @@
         <v>131</v>
       </c>
       <c r="G95" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H95" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I95" s="26" t="s">
         <v>92</v>
@@ -8294,21 +8298,21 @@
         <v>1</v>
       </c>
       <c r="M95" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="B96" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C96" s="26" t="s">
         <v>337</v>
       </c>
-      <c r="B96" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C96" s="26" t="s">
-        <v>338</v>
-      </c>
       <c r="D96" s="26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E96" s="26" t="s">
         <v>94</v>
@@ -8317,7 +8321,7 @@
         <v>131</v>
       </c>
       <c r="G96" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H96" s="26" t="s">
         <v>111</v>
@@ -8340,16 +8344,16 @@
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="B97" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C97" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="B97" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C97" s="26" t="s">
-        <v>340</v>
-      </c>
       <c r="D97" s="26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E97" s="26" t="s">
         <v>94</v>
@@ -8358,7 +8362,7 @@
         <v>131</v>
       </c>
       <c r="G97" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H97" s="26" t="s">
         <v>111</v>
@@ -8381,16 +8385,16 @@
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="B98" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C98" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="B98" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C98" s="26" t="s">
-        <v>342</v>
-      </c>
       <c r="D98" s="26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E98" s="26" t="s">
         <v>94</v>
@@ -8399,7 +8403,7 @@
         <v>131</v>
       </c>
       <c r="G98" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H98" s="26" t="s">
         <v>111</v>
@@ -8422,16 +8426,16 @@
     </row>
     <row r="99" spans="1:13">
       <c r="A99" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="B99" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C99" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="B99" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C99" s="26" t="s">
-        <v>344</v>
-      </c>
       <c r="D99" s="26" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E99" s="26" t="s">
         <v>94</v>
@@ -8440,7 +8444,7 @@
         <v>131</v>
       </c>
       <c r="G99" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H99" s="26" t="s">
         <v>111</v>
@@ -8463,16 +8467,16 @@
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="B100" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C100" s="26" t="s">
         <v>345</v>
       </c>
-      <c r="B100" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C100" s="26" t="s">
-        <v>346</v>
-      </c>
       <c r="D100" s="26" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E100" s="26" t="s">
         <v>94</v>
@@ -8481,7 +8485,7 @@
         <v>131</v>
       </c>
       <c r="G100" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H100" s="26" t="s">
         <v>111</v>
@@ -8504,16 +8508,16 @@
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="B101" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C101" s="26" t="s">
         <v>347</v>
       </c>
-      <c r="B101" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C101" s="26" t="s">
-        <v>348</v>
-      </c>
       <c r="D101" s="26" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E101" s="26" t="s">
         <v>94</v>
@@ -8522,7 +8526,7 @@
         <v>131</v>
       </c>
       <c r="G101" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H101" s="26" t="s">
         <v>111</v>
@@ -8545,16 +8549,16 @@
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="B102" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C102" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="B102" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C102" s="26" t="s">
-        <v>350</v>
-      </c>
       <c r="D102" s="26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E102" s="26" t="s">
         <v>94</v>
@@ -8563,7 +8567,7 @@
         <v>131</v>
       </c>
       <c r="G102" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H102" s="26" t="s">
         <v>111</v>
@@ -8586,16 +8590,16 @@
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="B103" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="C103" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D103" s="26" t="s">
         <v>351</v>
-      </c>
-      <c r="B103" s="26" t="s">
-        <v>351</v>
-      </c>
-      <c r="C103" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D103" s="26" t="s">
-        <v>352</v>
       </c>
       <c r="E103" s="26" t="s">
         <v>92</v>
@@ -8627,16 +8631,16 @@
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="B104" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="C104" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D104" s="26" t="s">
         <v>353</v>
-      </c>
-      <c r="B104" s="26" t="s">
-        <v>353</v>
-      </c>
-      <c r="C104" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D104" s="26" t="s">
-        <v>354</v>
       </c>
       <c r="E104" s="26" t="s">
         <v>92</v>
@@ -8668,16 +8672,16 @@
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="B105" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="C105" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D105" s="26" t="s">
         <v>355</v>
-      </c>
-      <c r="B105" s="26" t="s">
-        <v>355</v>
-      </c>
-      <c r="C105" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D105" s="26" t="s">
-        <v>356</v>
       </c>
       <c r="E105" s="26" t="s">
         <v>92</v>
@@ -8709,16 +8713,16 @@
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="B106" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="C106" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D106" s="26" t="s">
         <v>357</v>
-      </c>
-      <c r="B106" s="26" t="s">
-        <v>357</v>
-      </c>
-      <c r="C106" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D106" s="26" t="s">
-        <v>358</v>
       </c>
       <c r="E106" s="26" t="s">
         <v>92</v>
@@ -8750,16 +8754,16 @@
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="B107" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="C107" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D107" s="26" t="s">
         <v>359</v>
-      </c>
-      <c r="B107" s="26" t="s">
-        <v>359</v>
-      </c>
-      <c r="C107" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D107" s="26" t="s">
-        <v>360</v>
       </c>
       <c r="E107" s="26" t="s">
         <v>92</v>
@@ -8791,16 +8795,16 @@
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="B108" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="C108" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D108" s="26" t="s">
         <v>361</v>
-      </c>
-      <c r="B108" s="26" t="s">
-        <v>361</v>
-      </c>
-      <c r="C108" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D108" s="26" t="s">
-        <v>362</v>
       </c>
       <c r="E108" s="26" t="s">
         <v>92</v>
@@ -8832,16 +8836,16 @@
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="B109" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="C109" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D109" s="26" t="s">
         <v>363</v>
-      </c>
-      <c r="B109" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="C109" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D109" s="26" t="s">
-        <v>364</v>
       </c>
       <c r="E109" s="26" t="s">
         <v>92</v>
@@ -8873,16 +8877,16 @@
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="B110" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="C110" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D110" s="26" t="s">
         <v>365</v>
-      </c>
-      <c r="B110" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="C110" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D110" s="26" t="s">
-        <v>366</v>
       </c>
       <c r="E110" s="26" t="s">
         <v>92</v>
@@ -8914,16 +8918,16 @@
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="B111" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="C111" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D111" s="26" t="s">
         <v>367</v>
-      </c>
-      <c r="B111" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="C111" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D111" s="26" t="s">
-        <v>368</v>
       </c>
       <c r="E111" s="26" t="s">
         <v>92</v>
@@ -8955,16 +8959,16 @@
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="B112" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="C112" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D112" s="26" t="s">
         <v>369</v>
-      </c>
-      <c r="B112" s="26" t="s">
-        <v>369</v>
-      </c>
-      <c r="C112" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D112" s="26" t="s">
-        <v>370</v>
       </c>
       <c r="E112" s="26" t="s">
         <v>92</v>
@@ -8996,16 +9000,16 @@
     </row>
     <row r="113" spans="1:13">
       <c r="A113" s="26" t="s">
+        <v>370</v>
+      </c>
+      <c r="B113" s="26" t="s">
+        <v>370</v>
+      </c>
+      <c r="C113" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D113" s="26" t="s">
         <v>371</v>
-      </c>
-      <c r="B113" s="26" t="s">
-        <v>371</v>
-      </c>
-      <c r="C113" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D113" s="26" t="s">
-        <v>372</v>
       </c>
       <c r="E113" s="26" t="s">
         <v>92</v>
@@ -9037,16 +9041,16 @@
     </row>
     <row r="114" spans="1:13">
       <c r="A114" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="B114" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="C114" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D114" s="26" t="s">
         <v>373</v>
-      </c>
-      <c r="B114" s="26" t="s">
-        <v>373</v>
-      </c>
-      <c r="C114" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D114" s="26" t="s">
-        <v>374</v>
       </c>
       <c r="E114" s="26" t="s">
         <v>92</v>
@@ -9078,16 +9082,16 @@
     </row>
     <row r="115" spans="1:13">
       <c r="A115" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="B115" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="C115" s="26" t="s">
         <v>375</v>
       </c>
-      <c r="B115" s="26" t="s">
+      <c r="D115" s="26" t="s">
         <v>375</v>
-      </c>
-      <c r="C115" s="26" t="s">
-        <v>376</v>
-      </c>
-      <c r="D115" s="26" t="s">
-        <v>376</v>
       </c>
       <c r="E115" s="26" t="s">
         <v>92</v>
@@ -9119,16 +9123,16 @@
     </row>
     <row r="116" spans="1:13">
       <c r="A116" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="B116" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="C116" s="26" t="s">
         <v>377</v>
       </c>
-      <c r="B116" s="26" t="s">
+      <c r="D116" s="26" t="s">
         <v>377</v>
-      </c>
-      <c r="C116" s="26" t="s">
-        <v>378</v>
-      </c>
-      <c r="D116" s="26" t="s">
-        <v>378</v>
       </c>
       <c r="E116" s="26" t="s">
         <v>92</v>
@@ -9160,16 +9164,16 @@
     </row>
     <row r="117" spans="1:13">
       <c r="A117" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="B117" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="C117" s="26" t="s">
         <v>379</v>
       </c>
-      <c r="B117" s="26" t="s">
+      <c r="D117" s="26" t="s">
         <v>379</v>
-      </c>
-      <c r="C117" s="26" t="s">
-        <v>380</v>
-      </c>
-      <c r="D117" s="26" t="s">
-        <v>380</v>
       </c>
       <c r="E117" s="26" t="s">
         <v>92</v>
@@ -9201,16 +9205,16 @@
     </row>
     <row r="118" spans="1:13">
       <c r="A118" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="B118" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="C118" s="26" t="s">
         <v>381</v>
       </c>
-      <c r="B118" s="26" t="s">
+      <c r="D118" s="26" t="s">
         <v>381</v>
-      </c>
-      <c r="C118" s="26" t="s">
-        <v>382</v>
-      </c>
-      <c r="D118" s="26" t="s">
-        <v>382</v>
       </c>
       <c r="E118" s="26" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
MODEL-INPUT CHANGES for vl again
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4385,7 +4385,7 @@
   <dimension ref="A1:M118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5703,7 +5703,7 @@
         <v>199</v>
       </c>
       <c r="I32" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" s="26">
         <v>1</v>

</xml_diff>

<commit_message>
MODEL-INPUT CHANGES for vl to transitions
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="80" windowWidth="27480" windowHeight="15460" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="80" windowWidth="27480" windowHeight="15460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -2201,8 +2201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AF27" sqref="AF27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3407,12 +3407,8 @@
       <c r="Y22" s="16"/>
       <c r="Z22" s="16"/>
       <c r="AA22" s="19"/>
-      <c r="AB22" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC22" s="3">
-        <v>1</v>
-      </c>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
       <c r="AD22" s="16"/>
       <c r="AE22" s="16"/>
       <c r="AF22" s="16"/>
@@ -3464,12 +3460,8 @@
       <c r="Z23" s="16"/>
       <c r="AA23" s="19"/>
       <c r="AB23" s="16"/>
-      <c r="AC23" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD23" s="3">
-        <v>1</v>
-      </c>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
       <c r="AE23" s="16"/>
       <c r="AF23" s="16"/>
       <c r="AG23" s="19"/>
@@ -3522,15 +3514,9 @@
       <c r="Z24" s="16"/>
       <c r="AA24" s="19"/>
       <c r="AB24" s="16"/>
-      <c r="AC24" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD24" s="3">
-        <v>1</v>
-      </c>
-      <c r="AE24" s="3">
-        <v>1</v>
-      </c>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
       <c r="AF24" s="16"/>
       <c r="AG24" s="19"/>
       <c r="AH24" s="16"/>
@@ -3585,15 +3571,9 @@
       <c r="AA25" s="19"/>
       <c r="AB25" s="16"/>
       <c r="AC25" s="16"/>
-      <c r="AD25" s="3">
-        <v>1</v>
-      </c>
-      <c r="AE25" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF25" s="3">
-        <v>1</v>
-      </c>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
       <c r="AG25" s="19"/>
       <c r="AH25" s="16"/>
       <c r="AI25" s="16"/>
@@ -3648,15 +3628,9 @@
       <c r="AB26" s="16"/>
       <c r="AC26" s="16"/>
       <c r="AD26" s="16"/>
-      <c r="AE26" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF26" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG26" s="22">
-        <v>1</v>
-      </c>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="22"/>
       <c r="AH26" s="16"/>
       <c r="AI26" s="16"/>
       <c r="AJ26" s="16"/>
@@ -3709,12 +3683,8 @@
       <c r="AC27" s="17"/>
       <c r="AD27" s="17"/>
       <c r="AE27" s="17"/>
-      <c r="AF27" s="18">
-        <v>1</v>
-      </c>
-      <c r="AG27" s="20">
-        <v>1</v>
-      </c>
+      <c r="AF27" s="18"/>
+      <c r="AG27" s="20"/>
       <c r="AH27" s="17"/>
       <c r="AI27" s="17"/>
       <c r="AJ27" s="17"/>
@@ -4384,7 +4354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
MODEL-INPUT CHANGES for vl, new parameter
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="80" windowWidth="27480" windowHeight="15460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="80" windowWidth="27480" windowHeight="15460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="385">
   <si>
     <t>Code Label</t>
   </si>
@@ -1170,6 +1170,12 @@
   </si>
   <si>
     <t>numvlmon</t>
+  </si>
+  <si>
+    <t>Number of VL tests recommended per person per year</t>
+  </si>
+  <si>
+    <t>requiredvl</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1400,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1402,6 +1408,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1505,7 +1517,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="53">
     <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
     <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
     <cellStyle name="60% - Accent5" xfId="6" builtinId="48"/>
@@ -1530,6 +1542,9 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
@@ -1551,6 +1566,9 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2201,8 +2219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AF27" sqref="AF27"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AC25" sqref="AC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4352,10 +4370,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M118"/>
+  <dimension ref="A1:M119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7207,19 +7225,19 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="28" t="s">
-        <v>284</v>
+        <v>383</v>
       </c>
       <c r="B70" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C70" s="26" t="s">
-        <v>285</v>
+        <v>384</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>285</v>
+        <v>384</v>
       </c>
       <c r="E70" s="26" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="F70" s="26" t="s">
         <v>131</v>
@@ -7248,16 +7266,16 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="28" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B71" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C71" s="26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E71" s="26" t="s">
         <v>109</v>
@@ -7288,17 +7306,17 @@
       </c>
     </row>
     <row r="72" spans="1:13">
-      <c r="A72" s="26" t="s">
-        <v>288</v>
+      <c r="A72" s="28" t="s">
+        <v>286</v>
       </c>
       <c r="B72" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C72" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E72" s="26" t="s">
         <v>109</v>
@@ -7330,16 +7348,16 @@
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="26" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B73" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E73" s="26" t="s">
         <v>109</v>
@@ -7371,16 +7389,16 @@
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B74" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E74" s="26" t="s">
         <v>109</v>
@@ -7412,16 +7430,16 @@
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="26" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B75" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C75" s="26" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D75" s="26" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E75" s="26" t="s">
         <v>109</v>
@@ -7453,16 +7471,16 @@
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="26" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B76" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D76" s="26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E76" s="26" t="s">
         <v>109</v>
@@ -7494,16 +7512,16 @@
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="26" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B77" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C77" s="26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D77" s="26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E77" s="26" t="s">
         <v>109</v>
@@ -7535,16 +7553,16 @@
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="26" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B78" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C78" s="26" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E78" s="26" t="s">
         <v>109</v>
@@ -7576,16 +7594,16 @@
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="26" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B79" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C79" s="26" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E79" s="26" t="s">
         <v>109</v>
@@ -7617,16 +7635,16 @@
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="26" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B80" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E80" s="26" t="s">
         <v>109</v>
@@ -7658,16 +7676,16 @@
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="26" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B81" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C81" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E81" s="26" t="s">
         <v>109</v>
@@ -7698,17 +7716,17 @@
       </c>
     </row>
     <row r="82" spans="1:13">
-      <c r="A82" s="28" t="s">
-        <v>308</v>
+      <c r="A82" s="26" t="s">
+        <v>306</v>
       </c>
       <c r="B82" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="C82" s="28" t="s">
-        <v>309</v>
-      </c>
-      <c r="D82" s="28" t="s">
-        <v>309</v>
+      <c r="C82" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>307</v>
       </c>
       <c r="E82" s="26" t="s">
         <v>109</v>
@@ -7740,16 +7758,16 @@
     </row>
     <row r="83" spans="1:13">
       <c r="A83" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B83" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E83" s="26" t="s">
         <v>109</v>
@@ -7780,17 +7798,17 @@
       </c>
     </row>
     <row r="84" spans="1:13">
-      <c r="A84" s="26" t="s">
-        <v>312</v>
+      <c r="A84" s="28" t="s">
+        <v>310</v>
       </c>
       <c r="B84" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="C84" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="D84" s="26" t="s">
-        <v>313</v>
+      <c r="C84" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="D84" s="28" t="s">
+        <v>311</v>
       </c>
       <c r="E84" s="26" t="s">
         <v>109</v>
@@ -7822,19 +7840,19 @@
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="26" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B85" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C85" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="F85" s="26" t="s">
         <v>131</v>
@@ -7863,16 +7881,16 @@
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="26" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B86" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C86" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D86" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E86" s="26" t="s">
         <v>102</v>
@@ -7904,16 +7922,16 @@
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="26" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B87" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C87" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E87" s="26" t="s">
         <v>102</v>
@@ -7945,19 +7963,19 @@
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="26" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B88" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C88" s="26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D88" s="26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="F88" s="26" t="s">
         <v>131</v>
@@ -7986,16 +8004,16 @@
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="26" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B89" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C89" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E89" s="26" t="s">
         <v>94</v>
@@ -8027,16 +8045,16 @@
     </row>
     <row r="90" spans="1:13">
       <c r="A90" s="26" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B90" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C90" s="26" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D90" s="26" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E90" s="26" t="s">
         <v>94</v>
@@ -8068,16 +8086,16 @@
     </row>
     <row r="91" spans="1:13">
       <c r="A91" s="26" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B91" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C91" s="26" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E91" s="26" t="s">
         <v>94</v>
@@ -8109,16 +8127,16 @@
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="26" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B92" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C92" s="26" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D92" s="26" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E92" s="26" t="s">
         <v>94</v>
@@ -8150,16 +8168,16 @@
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="26" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B93" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C93" s="26" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E93" s="26" t="s">
         <v>94</v>
@@ -8191,16 +8209,16 @@
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="26" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B94" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E94" s="26" t="s">
         <v>94</v>
@@ -8232,16 +8250,16 @@
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="26" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B95" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C95" s="26" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D95" s="26" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E95" s="26" t="s">
         <v>94</v>
@@ -8273,16 +8291,16 @@
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="26" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B96" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C96" s="26" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E96" s="26" t="s">
         <v>94</v>
@@ -8294,7 +8312,7 @@
         <v>235</v>
       </c>
       <c r="H96" s="26" t="s">
-        <v>111</v>
+        <v>237</v>
       </c>
       <c r="I96" s="26" t="s">
         <v>92</v>
@@ -8309,21 +8327,21 @@
         <v>1</v>
       </c>
       <c r="M96" s="26" t="s">
-        <v>111</v>
+        <v>237</v>
       </c>
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="26" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B97" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C97" s="26" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E97" s="26" t="s">
         <v>94</v>
@@ -8355,16 +8373,16 @@
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="26" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B98" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C98" s="26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E98" s="26" t="s">
         <v>94</v>
@@ -8396,16 +8414,16 @@
     </row>
     <row r="99" spans="1:13">
       <c r="A99" s="26" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B99" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C99" s="26" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E99" s="26" t="s">
         <v>94</v>
@@ -8437,16 +8455,16 @@
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="26" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B100" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C100" s="26" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D100" s="26" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E100" s="26" t="s">
         <v>94</v>
@@ -8478,16 +8496,16 @@
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="26" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B101" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C101" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D101" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E101" s="26" t="s">
         <v>94</v>
@@ -8519,16 +8537,16 @@
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="26" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B102" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C102" s="26" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E102" s="26" t="s">
         <v>94</v>
@@ -8560,25 +8578,25 @@
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="26" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>350</v>
+        <v>235</v>
       </c>
       <c r="C103" s="26" t="s">
-        <v>92</v>
+        <v>349</v>
       </c>
       <c r="D103" s="26" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E103" s="26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F103" s="26" t="s">
         <v>131</v>
       </c>
       <c r="G103" s="26" t="s">
-        <v>92</v>
+        <v>235</v>
       </c>
       <c r="H103" s="26" t="s">
         <v>111</v>
@@ -8601,16 +8619,16 @@
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="26" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C104" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E104" s="26" t="s">
         <v>92</v>
@@ -8642,16 +8660,16 @@
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="26" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C105" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E105" s="26" t="s">
         <v>92</v>
@@ -8683,16 +8701,16 @@
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C106" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E106" s="26" t="s">
         <v>92</v>
@@ -8724,16 +8742,16 @@
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="26" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C107" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D107" s="26" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E107" s="26" t="s">
         <v>92</v>
@@ -8765,16 +8783,16 @@
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="26" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C108" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D108" s="26" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E108" s="26" t="s">
         <v>92</v>
@@ -8806,16 +8824,16 @@
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="26" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C109" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E109" s="26" t="s">
         <v>92</v>
@@ -8847,16 +8865,16 @@
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="26" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C110" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D110" s="26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E110" s="26" t="s">
         <v>92</v>
@@ -8888,16 +8906,16 @@
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="26" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C111" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D111" s="26" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E111" s="26" t="s">
         <v>92</v>
@@ -8929,16 +8947,16 @@
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="26" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B112" s="26" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C112" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D112" s="26" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E112" s="26" t="s">
         <v>92</v>
@@ -8970,16 +8988,16 @@
     </row>
     <row r="113" spans="1:13">
       <c r="A113" s="26" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C113" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D113" s="26" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E113" s="26" t="s">
         <v>92</v>
@@ -9011,16 +9029,16 @@
     </row>
     <row r="114" spans="1:13">
       <c r="A114" s="26" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B114" s="26" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C114" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D114" s="26" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E114" s="26" t="s">
         <v>92</v>
@@ -9052,16 +9070,16 @@
     </row>
     <row r="115" spans="1:13">
       <c r="A115" s="26" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B115" s="26" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C115" s="26" t="s">
-        <v>375</v>
+        <v>92</v>
       </c>
       <c r="D115" s="26" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E115" s="26" t="s">
         <v>92</v>
@@ -9093,16 +9111,16 @@
     </row>
     <row r="116" spans="1:13">
       <c r="A116" s="26" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B116" s="26" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C116" s="26" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D116" s="26" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E116" s="26" t="s">
         <v>92</v>
@@ -9134,16 +9152,16 @@
     </row>
     <row r="117" spans="1:13">
       <c r="A117" s="26" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B117" s="26" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C117" s="26" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D117" s="26" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E117" s="26" t="s">
         <v>92</v>
@@ -9175,16 +9193,16 @@
     </row>
     <row r="118" spans="1:13">
       <c r="A118" s="26" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B118" s="26" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C118" s="26" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D118" s="26" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E118" s="26" t="s">
         <v>92</v>
@@ -9211,6 +9229,47 @@
         <v>1</v>
       </c>
       <c r="M118" s="26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13">
+      <c r="A119" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="B119" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="C119" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="D119" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="E119" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F119" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="G119" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="H119" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="I119" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J119" s="26">
+        <v>0</v>
+      </c>
+      <c r="K119" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L119" s="26">
+        <v>1</v>
+      </c>
+      <c r="M119" s="26" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MODEL-INPUT CHANGES for vl, saved
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="383">
   <si>
     <t>Code Label</t>
   </si>
@@ -1170,12 +1170,6 @@
   </si>
   <si>
     <t>numvlmon</t>
-  </si>
-  <si>
-    <t>Number of VL tests recommended per person per year</t>
-  </si>
-  <si>
-    <t>requiredvl</t>
   </si>
 </sst>
 </file>
@@ -4370,10 +4364,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M119"/>
+  <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:XFD70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7225,19 +7219,19 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="28" t="s">
-        <v>383</v>
+        <v>284</v>
       </c>
       <c r="B70" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C70" s="26" t="s">
-        <v>384</v>
+        <v>285</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>384</v>
+        <v>285</v>
       </c>
       <c r="E70" s="26" t="s">
-        <v>170</v>
+        <v>109</v>
       </c>
       <c r="F70" s="26" t="s">
         <v>131</v>
@@ -7266,16 +7260,16 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="28" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B71" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C71" s="26" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E71" s="26" t="s">
         <v>109</v>
@@ -7306,17 +7300,17 @@
       </c>
     </row>
     <row r="72" spans="1:13">
-      <c r="A72" s="28" t="s">
-        <v>286</v>
+      <c r="A72" s="26" t="s">
+        <v>288</v>
       </c>
       <c r="B72" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C72" s="26" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E72" s="26" t="s">
         <v>109</v>
@@ -7348,16 +7342,16 @@
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="26" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B73" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E73" s="26" t="s">
         <v>109</v>
@@ -7389,16 +7383,16 @@
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="26" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B74" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E74" s="26" t="s">
         <v>109</v>
@@ -7430,16 +7424,16 @@
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="26" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B75" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C75" s="26" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D75" s="26" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E75" s="26" t="s">
         <v>109</v>
@@ -7471,16 +7465,16 @@
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="26" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B76" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D76" s="26" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E76" s="26" t="s">
         <v>109</v>
@@ -7512,16 +7506,16 @@
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="26" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B77" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C77" s="26" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D77" s="26" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E77" s="26" t="s">
         <v>109</v>
@@ -7553,16 +7547,16 @@
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="26" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B78" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C78" s="26" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E78" s="26" t="s">
         <v>109</v>
@@ -7594,16 +7588,16 @@
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="26" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B79" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C79" s="26" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E79" s="26" t="s">
         <v>109</v>
@@ -7635,16 +7629,16 @@
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="26" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B80" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E80" s="26" t="s">
         <v>109</v>
@@ -7676,16 +7670,16 @@
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="26" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B81" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C81" s="26" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E81" s="26" t="s">
         <v>109</v>
@@ -7716,17 +7710,17 @@
       </c>
     </row>
     <row r="82" spans="1:13">
-      <c r="A82" s="26" t="s">
-        <v>306</v>
+      <c r="A82" s="28" t="s">
+        <v>308</v>
       </c>
       <c r="B82" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="C82" s="26" t="s">
-        <v>307</v>
-      </c>
-      <c r="D82" s="26" t="s">
-        <v>307</v>
+      <c r="C82" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="D82" s="28" t="s">
+        <v>309</v>
       </c>
       <c r="E82" s="26" t="s">
         <v>109</v>
@@ -7758,16 +7752,16 @@
     </row>
     <row r="83" spans="1:13">
       <c r="A83" s="28" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B83" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E83" s="26" t="s">
         <v>109</v>
@@ -7798,17 +7792,17 @@
       </c>
     </row>
     <row r="84" spans="1:13">
-      <c r="A84" s="28" t="s">
-        <v>310</v>
+      <c r="A84" s="26" t="s">
+        <v>312</v>
       </c>
       <c r="B84" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="C84" s="28" t="s">
-        <v>311</v>
-      </c>
-      <c r="D84" s="28" t="s">
-        <v>311</v>
+      <c r="C84" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>313</v>
       </c>
       <c r="E84" s="26" t="s">
         <v>109</v>
@@ -7840,19 +7834,19 @@
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="26" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B85" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C85" s="26" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F85" s="26" t="s">
         <v>131</v>
@@ -7881,16 +7875,16 @@
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="26" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B86" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C86" s="26" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D86" s="26" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E86" s="26" t="s">
         <v>102</v>
@@ -7922,16 +7916,16 @@
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="26" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B87" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C87" s="26" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E87" s="26" t="s">
         <v>102</v>
@@ -7963,19 +7957,19 @@
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="26" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B88" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C88" s="26" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D88" s="26" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F88" s="26" t="s">
         <v>131</v>
@@ -8004,16 +7998,16 @@
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="26" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B89" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C89" s="26" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E89" s="26" t="s">
         <v>94</v>
@@ -8045,16 +8039,16 @@
     </row>
     <row r="90" spans="1:13">
       <c r="A90" s="26" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B90" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C90" s="26" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D90" s="26" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="E90" s="26" t="s">
         <v>94</v>
@@ -8086,16 +8080,16 @@
     </row>
     <row r="91" spans="1:13">
       <c r="A91" s="26" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B91" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C91" s="26" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E91" s="26" t="s">
         <v>94</v>
@@ -8127,16 +8121,16 @@
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="26" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B92" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C92" s="26" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D92" s="26" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E92" s="26" t="s">
         <v>94</v>
@@ -8168,16 +8162,16 @@
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="26" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B93" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C93" s="26" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E93" s="26" t="s">
         <v>94</v>
@@ -8209,16 +8203,16 @@
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="26" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B94" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E94" s="26" t="s">
         <v>94</v>
@@ -8250,16 +8244,16 @@
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="26" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B95" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C95" s="26" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D95" s="26" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E95" s="26" t="s">
         <v>94</v>
@@ -8291,16 +8285,16 @@
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="26" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B96" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C96" s="26" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E96" s="26" t="s">
         <v>94</v>
@@ -8312,7 +8306,7 @@
         <v>235</v>
       </c>
       <c r="H96" s="26" t="s">
-        <v>237</v>
+        <v>111</v>
       </c>
       <c r="I96" s="26" t="s">
         <v>92</v>
@@ -8327,21 +8321,21 @@
         <v>1</v>
       </c>
       <c r="M96" s="26" t="s">
-        <v>237</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="26" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B97" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C97" s="26" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E97" s="26" t="s">
         <v>94</v>
@@ -8373,16 +8367,16 @@
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="26" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B98" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C98" s="26" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E98" s="26" t="s">
         <v>94</v>
@@ -8414,16 +8408,16 @@
     </row>
     <row r="99" spans="1:13">
       <c r="A99" s="26" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B99" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C99" s="26" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E99" s="26" t="s">
         <v>94</v>
@@ -8455,16 +8449,16 @@
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="26" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B100" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C100" s="26" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D100" s="26" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E100" s="26" t="s">
         <v>94</v>
@@ -8496,16 +8490,16 @@
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="26" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B101" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C101" s="26" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D101" s="26" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E101" s="26" t="s">
         <v>94</v>
@@ -8537,16 +8531,16 @@
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="26" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B102" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C102" s="26" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E102" s="26" t="s">
         <v>94</v>
@@ -8578,25 +8572,25 @@
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="26" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>235</v>
+        <v>350</v>
       </c>
       <c r="C103" s="26" t="s">
-        <v>349</v>
+        <v>92</v>
       </c>
       <c r="D103" s="26" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E103" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F103" s="26" t="s">
         <v>131</v>
       </c>
       <c r="G103" s="26" t="s">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="H103" s="26" t="s">
         <v>111</v>
@@ -8619,16 +8613,16 @@
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="26" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C104" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E104" s="26" t="s">
         <v>92</v>
@@ -8660,16 +8654,16 @@
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="26" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C105" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E105" s="26" t="s">
         <v>92</v>
@@ -8701,16 +8695,16 @@
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="26" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C106" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E106" s="26" t="s">
         <v>92</v>
@@ -8742,16 +8736,16 @@
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="26" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C107" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D107" s="26" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E107" s="26" t="s">
         <v>92</v>
@@ -8783,16 +8777,16 @@
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="26" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C108" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D108" s="26" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E108" s="26" t="s">
         <v>92</v>
@@ -8824,16 +8818,16 @@
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="26" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C109" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E109" s="26" t="s">
         <v>92</v>
@@ -8865,16 +8859,16 @@
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="26" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C110" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D110" s="26" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E110" s="26" t="s">
         <v>92</v>
@@ -8906,16 +8900,16 @@
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="26" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C111" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D111" s="26" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="E111" s="26" t="s">
         <v>92</v>
@@ -8947,16 +8941,16 @@
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="26" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B112" s="26" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C112" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D112" s="26" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E112" s="26" t="s">
         <v>92</v>
@@ -8988,16 +8982,16 @@
     </row>
     <row r="113" spans="1:13">
       <c r="A113" s="26" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C113" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D113" s="26" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E113" s="26" t="s">
         <v>92</v>
@@ -9029,16 +9023,16 @@
     </row>
     <row r="114" spans="1:13">
       <c r="A114" s="26" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B114" s="26" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C114" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D114" s="26" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E114" s="26" t="s">
         <v>92</v>
@@ -9070,16 +9064,16 @@
     </row>
     <row r="115" spans="1:13">
       <c r="A115" s="26" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B115" s="26" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C115" s="26" t="s">
-        <v>92</v>
+        <v>375</v>
       </c>
       <c r="D115" s="26" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E115" s="26" t="s">
         <v>92</v>
@@ -9111,16 +9105,16 @@
     </row>
     <row r="116" spans="1:13">
       <c r="A116" s="26" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B116" s="26" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C116" s="26" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D116" s="26" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E116" s="26" t="s">
         <v>92</v>
@@ -9152,16 +9146,16 @@
     </row>
     <row r="117" spans="1:13">
       <c r="A117" s="26" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B117" s="26" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C117" s="26" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D117" s="26" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E117" s="26" t="s">
         <v>92</v>
@@ -9193,16 +9187,16 @@
     </row>
     <row r="118" spans="1:13">
       <c r="A118" s="26" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B118" s="26" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C118" s="26" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D118" s="26" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E118" s="26" t="s">
         <v>92</v>
@@ -9229,47 +9223,6 @@
         <v>1</v>
       </c>
       <c r="M118" s="26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13">
-      <c r="A119" s="26" t="s">
-        <v>380</v>
-      </c>
-      <c r="B119" s="26" t="s">
-        <v>380</v>
-      </c>
-      <c r="C119" s="26" t="s">
-        <v>381</v>
-      </c>
-      <c r="D119" s="26" t="s">
-        <v>381</v>
-      </c>
-      <c r="E119" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="F119" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="G119" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="H119" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="I119" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="J119" s="26">
-        <v>0</v>
-      </c>
-      <c r="K119" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="L119" s="26">
-        <v>1</v>
-      </c>
-      <c r="M119" s="26" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
this does not seem unreasonable
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="385">
   <si>
     <t>Code Label</t>
   </si>
@@ -1170,6 +1170,12 @@
   </si>
   <si>
     <t>numvlmon</t>
+  </si>
+  <si>
+    <t>Number of VL tests recommended per person per year</t>
+  </si>
+  <si>
+    <t>requiredvl</t>
   </si>
 </sst>
 </file>
@@ -4364,10 +4370,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M118"/>
+  <dimension ref="A1:M119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:XFD70"/>
+      <selection activeCell="F70" sqref="F70:M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7219,19 +7225,19 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="28" t="s">
-        <v>284</v>
+        <v>383</v>
       </c>
       <c r="B70" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C70" s="26" t="s">
-        <v>285</v>
+        <v>384</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>285</v>
+        <v>384</v>
       </c>
       <c r="E70" s="26" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="F70" s="26" t="s">
         <v>131</v>
@@ -7260,16 +7266,16 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="28" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B71" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C71" s="26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E71" s="26" t="s">
         <v>109</v>
@@ -7300,17 +7306,17 @@
       </c>
     </row>
     <row r="72" spans="1:13">
-      <c r="A72" s="26" t="s">
-        <v>288</v>
+      <c r="A72" s="28" t="s">
+        <v>286</v>
       </c>
       <c r="B72" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C72" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E72" s="26" t="s">
         <v>109</v>
@@ -7342,16 +7348,16 @@
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="26" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B73" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E73" s="26" t="s">
         <v>109</v>
@@ -7383,16 +7389,16 @@
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B74" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E74" s="26" t="s">
         <v>109</v>
@@ -7424,16 +7430,16 @@
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="26" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B75" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C75" s="26" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D75" s="26" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E75" s="26" t="s">
         <v>109</v>
@@ -7465,16 +7471,16 @@
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="26" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B76" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D76" s="26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E76" s="26" t="s">
         <v>109</v>
@@ -7506,16 +7512,16 @@
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="26" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B77" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C77" s="26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D77" s="26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E77" s="26" t="s">
         <v>109</v>
@@ -7547,16 +7553,16 @@
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="26" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B78" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C78" s="26" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E78" s="26" t="s">
         <v>109</v>
@@ -7588,16 +7594,16 @@
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="26" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B79" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C79" s="26" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E79" s="26" t="s">
         <v>109</v>
@@ -7629,16 +7635,16 @@
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="26" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B80" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E80" s="26" t="s">
         <v>109</v>
@@ -7670,16 +7676,16 @@
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="26" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B81" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C81" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E81" s="26" t="s">
         <v>109</v>
@@ -7710,17 +7716,17 @@
       </c>
     </row>
     <row r="82" spans="1:13">
-      <c r="A82" s="28" t="s">
-        <v>308</v>
+      <c r="A82" s="26" t="s">
+        <v>306</v>
       </c>
       <c r="B82" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="C82" s="28" t="s">
-        <v>309</v>
-      </c>
-      <c r="D82" s="28" t="s">
-        <v>309</v>
+      <c r="C82" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>307</v>
       </c>
       <c r="E82" s="26" t="s">
         <v>109</v>
@@ -7752,16 +7758,16 @@
     </row>
     <row r="83" spans="1:13">
       <c r="A83" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B83" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E83" s="26" t="s">
         <v>109</v>
@@ -7792,17 +7798,17 @@
       </c>
     </row>
     <row r="84" spans="1:13">
-      <c r="A84" s="26" t="s">
-        <v>312</v>
+      <c r="A84" s="28" t="s">
+        <v>310</v>
       </c>
       <c r="B84" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="C84" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="D84" s="26" t="s">
-        <v>313</v>
+      <c r="C84" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="D84" s="28" t="s">
+        <v>311</v>
       </c>
       <c r="E84" s="26" t="s">
         <v>109</v>
@@ -7834,19 +7840,19 @@
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="26" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B85" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C85" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="F85" s="26" t="s">
         <v>131</v>
@@ -7875,16 +7881,16 @@
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="26" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B86" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C86" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D86" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E86" s="26" t="s">
         <v>102</v>
@@ -7916,16 +7922,16 @@
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="26" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B87" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C87" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E87" s="26" t="s">
         <v>102</v>
@@ -7957,19 +7963,19 @@
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="26" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B88" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C88" s="26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D88" s="26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="F88" s="26" t="s">
         <v>131</v>
@@ -7998,16 +8004,16 @@
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="26" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B89" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C89" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E89" s="26" t="s">
         <v>94</v>
@@ -8039,16 +8045,16 @@
     </row>
     <row r="90" spans="1:13">
       <c r="A90" s="26" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B90" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C90" s="26" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D90" s="26" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E90" s="26" t="s">
         <v>94</v>
@@ -8080,16 +8086,16 @@
     </row>
     <row r="91" spans="1:13">
       <c r="A91" s="26" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B91" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C91" s="26" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E91" s="26" t="s">
         <v>94</v>
@@ -8121,16 +8127,16 @@
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="26" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B92" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C92" s="26" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D92" s="26" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E92" s="26" t="s">
         <v>94</v>
@@ -8162,16 +8168,16 @@
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="26" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B93" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C93" s="26" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E93" s="26" t="s">
         <v>94</v>
@@ -8203,16 +8209,16 @@
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="26" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B94" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E94" s="26" t="s">
         <v>94</v>
@@ -8244,16 +8250,16 @@
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="26" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B95" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C95" s="26" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D95" s="26" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E95" s="26" t="s">
         <v>94</v>
@@ -8285,16 +8291,16 @@
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="26" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B96" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C96" s="26" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E96" s="26" t="s">
         <v>94</v>
@@ -8306,7 +8312,7 @@
         <v>235</v>
       </c>
       <c r="H96" s="26" t="s">
-        <v>111</v>
+        <v>237</v>
       </c>
       <c r="I96" s="26" t="s">
         <v>92</v>
@@ -8321,21 +8327,21 @@
         <v>1</v>
       </c>
       <c r="M96" s="26" t="s">
-        <v>111</v>
+        <v>237</v>
       </c>
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="26" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B97" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C97" s="26" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E97" s="26" t="s">
         <v>94</v>
@@ -8367,16 +8373,16 @@
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="26" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B98" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C98" s="26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E98" s="26" t="s">
         <v>94</v>
@@ -8408,16 +8414,16 @@
     </row>
     <row r="99" spans="1:13">
       <c r="A99" s="26" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B99" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C99" s="26" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E99" s="26" t="s">
         <v>94</v>
@@ -8449,16 +8455,16 @@
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="26" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B100" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C100" s="26" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D100" s="26" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E100" s="26" t="s">
         <v>94</v>
@@ -8490,16 +8496,16 @@
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="26" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B101" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C101" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D101" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E101" s="26" t="s">
         <v>94</v>
@@ -8531,16 +8537,16 @@
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="26" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B102" s="26" t="s">
         <v>235</v>
       </c>
       <c r="C102" s="26" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E102" s="26" t="s">
         <v>94</v>
@@ -8572,25 +8578,25 @@
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="26" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>350</v>
+        <v>235</v>
       </c>
       <c r="C103" s="26" t="s">
-        <v>92</v>
+        <v>349</v>
       </c>
       <c r="D103" s="26" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E103" s="26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F103" s="26" t="s">
         <v>131</v>
       </c>
       <c r="G103" s="26" t="s">
-        <v>92</v>
+        <v>235</v>
       </c>
       <c r="H103" s="26" t="s">
         <v>111</v>
@@ -8613,16 +8619,16 @@
     </row>
     <row r="104" spans="1:13">
       <c r="A104" s="26" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C104" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E104" s="26" t="s">
         <v>92</v>
@@ -8654,16 +8660,16 @@
     </row>
     <row r="105" spans="1:13">
       <c r="A105" s="26" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C105" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E105" s="26" t="s">
         <v>92</v>
@@ -8695,16 +8701,16 @@
     </row>
     <row r="106" spans="1:13">
       <c r="A106" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C106" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E106" s="26" t="s">
         <v>92</v>
@@ -8736,16 +8742,16 @@
     </row>
     <row r="107" spans="1:13">
       <c r="A107" s="26" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C107" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D107" s="26" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E107" s="26" t="s">
         <v>92</v>
@@ -8777,16 +8783,16 @@
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="26" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C108" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D108" s="26" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E108" s="26" t="s">
         <v>92</v>
@@ -8818,16 +8824,16 @@
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="26" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C109" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E109" s="26" t="s">
         <v>92</v>
@@ -8859,16 +8865,16 @@
     </row>
     <row r="110" spans="1:13">
       <c r="A110" s="26" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C110" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D110" s="26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E110" s="26" t="s">
         <v>92</v>
@@ -8900,16 +8906,16 @@
     </row>
     <row r="111" spans="1:13">
       <c r="A111" s="26" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C111" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D111" s="26" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E111" s="26" t="s">
         <v>92</v>
@@ -8941,16 +8947,16 @@
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="26" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B112" s="26" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C112" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D112" s="26" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E112" s="26" t="s">
         <v>92</v>
@@ -8982,16 +8988,16 @@
     </row>
     <row r="113" spans="1:13">
       <c r="A113" s="26" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C113" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D113" s="26" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E113" s="26" t="s">
         <v>92</v>
@@ -9023,16 +9029,16 @@
     </row>
     <row r="114" spans="1:13">
       <c r="A114" s="26" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B114" s="26" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C114" s="26" t="s">
         <v>92</v>
       </c>
       <c r="D114" s="26" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E114" s="26" t="s">
         <v>92</v>
@@ -9064,16 +9070,16 @@
     </row>
     <row r="115" spans="1:13">
       <c r="A115" s="26" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B115" s="26" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C115" s="26" t="s">
-        <v>375</v>
+        <v>92</v>
       </c>
       <c r="D115" s="26" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E115" s="26" t="s">
         <v>92</v>
@@ -9105,16 +9111,16 @@
     </row>
     <row r="116" spans="1:13">
       <c r="A116" s="26" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B116" s="26" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C116" s="26" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D116" s="26" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E116" s="26" t="s">
         <v>92</v>
@@ -9146,16 +9152,16 @@
     </row>
     <row r="117" spans="1:13">
       <c r="A117" s="26" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B117" s="26" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C117" s="26" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D117" s="26" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E117" s="26" t="s">
         <v>92</v>
@@ -9187,16 +9193,16 @@
     </row>
     <row r="118" spans="1:13">
       <c r="A118" s="26" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B118" s="26" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C118" s="26" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D118" s="26" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E118" s="26" t="s">
         <v>92</v>
@@ -9223,6 +9229,47 @@
         <v>1</v>
       </c>
       <c r="M118" s="26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13">
+      <c r="A119" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="B119" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="C119" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="D119" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="E119" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F119" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="G119" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="H119" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="I119" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J119" s="26">
+        <v>0</v>
+      </c>
+      <c r="K119" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L119" s="26">
+        <v>1</v>
+      </c>
+      <c r="M119" s="26" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MODEL-INPUT CHANGES, removing lost prob transitions
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="80" windowWidth="27480" windowHeight="15460" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="80" windowWidth="27480" windowHeight="15460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -2219,8 +2219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM39"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AC25" sqref="AC25"/>
+    <sheetView tabSelected="1" topLeftCell="T16" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3123,12 +3123,8 @@
       <c r="AE16" s="16"/>
       <c r="AF16" s="16"/>
       <c r="AG16" s="19"/>
-      <c r="AH16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AI16" s="3">
-        <v>1</v>
-      </c>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
       <c r="AJ16" s="16"/>
       <c r="AK16" s="16"/>
       <c r="AL16" s="16"/>
@@ -3176,12 +3172,8 @@
       <c r="AF17" s="16"/>
       <c r="AG17" s="19"/>
       <c r="AH17" s="16"/>
-      <c r="AI17" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ17" s="3">
-        <v>1</v>
-      </c>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
       <c r="AK17" s="16"/>
       <c r="AL17" s="16"/>
       <c r="AM17" s="19"/>
@@ -3229,12 +3221,8 @@
       <c r="AG18" s="19"/>
       <c r="AH18" s="16"/>
       <c r="AI18" s="16"/>
-      <c r="AJ18" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK18" s="3">
-        <v>1</v>
-      </c>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3"/>
       <c r="AL18" s="16"/>
       <c r="AM18" s="19"/>
     </row>
@@ -3282,12 +3270,8 @@
       <c r="AH19" s="16"/>
       <c r="AI19" s="16"/>
       <c r="AJ19" s="16"/>
-      <c r="AK19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL19" s="3">
-        <v>1</v>
-      </c>
+      <c r="AK19" s="3"/>
+      <c r="AL19" s="3"/>
       <c r="AM19" s="19"/>
     </row>
     <row r="20" spans="1:39" ht="16">
@@ -3335,12 +3319,8 @@
       <c r="AI20" s="16"/>
       <c r="AJ20" s="16"/>
       <c r="AK20" s="16"/>
-      <c r="AL20" s="3">
-        <v>1</v>
-      </c>
-      <c r="AM20" s="22">
-        <v>1</v>
-      </c>
+      <c r="AL20" s="3"/>
+      <c r="AM20" s="22"/>
     </row>
     <row r="21" spans="1:39" ht="16">
       <c r="A21" s="9" t="str">
@@ -3386,9 +3366,7 @@
       <c r="AJ21" s="17"/>
       <c r="AK21" s="17"/>
       <c r="AL21" s="17"/>
-      <c r="AM21" s="20">
-        <v>1</v>
-      </c>
+      <c r="AM21" s="20"/>
     </row>
     <row r="22" spans="1:39" ht="16">
       <c r="A22" s="10" t="str">
@@ -3431,12 +3409,8 @@
       <c r="AE22" s="16"/>
       <c r="AF22" s="16"/>
       <c r="AG22" s="19"/>
-      <c r="AH22" s="3">
-        <v>1</v>
-      </c>
-      <c r="AI22" s="3">
-        <v>1</v>
-      </c>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
       <c r="AJ22" s="16"/>
       <c r="AK22" s="16"/>
       <c r="AL22" s="16"/>
@@ -3484,12 +3458,8 @@
       <c r="AF23" s="16"/>
       <c r="AG23" s="19"/>
       <c r="AH23" s="16"/>
-      <c r="AI23" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ23" s="3">
-        <v>1</v>
-      </c>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
       <c r="AK23" s="16"/>
       <c r="AL23" s="16"/>
       <c r="AM23" s="19"/>
@@ -3538,15 +3508,9 @@
       <c r="AF24" s="16"/>
       <c r="AG24" s="19"/>
       <c r="AH24" s="16"/>
-      <c r="AI24" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ24" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK24" s="3">
-        <v>1</v>
-      </c>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
       <c r="AL24" s="16"/>
       <c r="AM24" s="19"/>
     </row>
@@ -3595,15 +3559,9 @@
       <c r="AG25" s="19"/>
       <c r="AH25" s="16"/>
       <c r="AI25" s="16"/>
-      <c r="AJ25" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK25" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL25" s="3">
-        <v>1</v>
-      </c>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
       <c r="AM25" s="19"/>
     </row>
     <row r="26" spans="1:39" ht="16">
@@ -3652,15 +3610,9 @@
       <c r="AH26" s="16"/>
       <c r="AI26" s="16"/>
       <c r="AJ26" s="16"/>
-      <c r="AK26" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL26" s="3">
-        <v>1</v>
-      </c>
-      <c r="AM26" s="22">
-        <v>1</v>
-      </c>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
+      <c r="AM26" s="22"/>
     </row>
     <row r="27" spans="1:39" ht="16">
       <c r="A27" s="10" t="str">
@@ -3707,12 +3659,8 @@
       <c r="AI27" s="17"/>
       <c r="AJ27" s="17"/>
       <c r="AK27" s="17"/>
-      <c r="AL27" s="18">
-        <v>1</v>
-      </c>
-      <c r="AM27" s="20">
-        <v>1</v>
-      </c>
+      <c r="AL27" s="18"/>
+      <c r="AM27" s="20"/>
     </row>
     <row r="28" spans="1:39" ht="16">
       <c r="A28" s="4" t="str">
@@ -3759,12 +3707,8 @@
       <c r="AE28" s="16"/>
       <c r="AF28" s="16"/>
       <c r="AG28" s="19"/>
-      <c r="AH28" s="3">
-        <v>1</v>
-      </c>
-      <c r="AI28" s="3">
-        <v>1</v>
-      </c>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
       <c r="AJ28" s="16"/>
       <c r="AK28" s="16"/>
       <c r="AL28" s="16"/>
@@ -3812,9 +3756,7 @@
       <c r="AF29" s="16"/>
       <c r="AG29" s="19"/>
       <c r="AH29" s="16"/>
-      <c r="AI29" s="3">
-        <v>1</v>
-      </c>
+      <c r="AI29" s="3"/>
       <c r="AJ29" s="16"/>
       <c r="AK29" s="16"/>
       <c r="AL29" s="16"/>
@@ -3866,12 +3808,8 @@
       <c r="AF30" s="16"/>
       <c r="AG30" s="19"/>
       <c r="AH30" s="16"/>
-      <c r="AI30" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ30" s="3">
-        <v>1</v>
-      </c>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
       <c r="AK30" s="16"/>
       <c r="AL30" s="16"/>
       <c r="AM30" s="19"/>
@@ -3923,12 +3861,8 @@
       <c r="AG31" s="19"/>
       <c r="AH31" s="16"/>
       <c r="AI31" s="16"/>
-      <c r="AJ31" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK31" s="3">
-        <v>1</v>
-      </c>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
       <c r="AL31" s="16"/>
       <c r="AM31" s="19"/>
     </row>
@@ -3980,12 +3914,8 @@
       <c r="AH32" s="16"/>
       <c r="AI32" s="16"/>
       <c r="AJ32" s="16"/>
-      <c r="AK32" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL32" s="3">
-        <v>1</v>
-      </c>
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="3"/>
       <c r="AM32" s="19"/>
     </row>
     <row r="33" spans="1:39" ht="16">
@@ -4037,12 +3967,8 @@
       <c r="AI33" s="17"/>
       <c r="AJ33" s="17"/>
       <c r="AK33" s="17"/>
-      <c r="AL33" s="18">
-        <v>1</v>
-      </c>
-      <c r="AM33" s="20">
-        <v>1</v>
-      </c>
+      <c r="AL33" s="18"/>
+      <c r="AM33" s="20"/>
     </row>
     <row r="34" spans="1:39" ht="16">
       <c r="A34" s="5" t="str">
@@ -4372,7 +4298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+    <sheetView topLeftCell="A66" workbookViewId="0">
       <selection activeCell="F70" sqref="F70:M70"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
not sure how spreadsheet changed, maybe removing freqvlmon
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="429">
   <si>
     <t>Code Label</t>
   </si>
@@ -8892,11 +8892,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -9436,17 +9436,17 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>169</v>
+      <c r="A19" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>171</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>102</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>111</v>
@@ -9466,16 +9466,16 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="26" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>102</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="E20" s="26" t="s">
         <v>111</v>
@@ -9495,13 +9495,13 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>173</v>
+        <v>426</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>116</v>
@@ -9509,28 +9509,28 @@
       <c r="E21" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="26">
-        <v>1</v>
-      </c>
-      <c r="H21" s="26">
-        <v>0</v>
-      </c>
-      <c r="I21" s="26">
+      <c r="G21" s="36">
+        <v>1</v>
+      </c>
+      <c r="H21" s="36">
+        <v>1</v>
+      </c>
+      <c r="I21" s="36">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="26" t="s">
-        <v>426</v>
+        <v>176</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>116</v>
@@ -9538,25 +9538,25 @@
       <c r="E22" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="G22" s="36">
-        <v>1</v>
-      </c>
-      <c r="H22" s="36">
-        <v>1</v>
-      </c>
-      <c r="I22" s="36">
-        <v>1</v>
+      <c r="F22" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="26">
+        <v>1</v>
+      </c>
+      <c r="H22" s="26">
+        <v>0</v>
+      </c>
+      <c r="I22" s="26">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="26" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>90</v>
@@ -9582,10 +9582,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="26" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>90</v>
@@ -9611,10 +9611,10 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="26" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>90</v>
@@ -9640,10 +9640,10 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="26" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>90</v>
@@ -9669,25 +9669,25 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="26" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>90</v>
+        <v>187</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>116</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="F27" s="26" t="s">
-        <v>104</v>
+        <v>189</v>
       </c>
       <c r="G27" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="26">
         <v>0</v>
@@ -9698,10 +9698,10 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="26" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>187</v>
@@ -9727,10 +9727,10 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="26" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>187</v>
@@ -9756,10 +9756,10 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="26" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>187</v>
@@ -9785,10 +9785,10 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="26" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>187</v>
@@ -9814,28 +9814,28 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="26" t="s">
-        <v>197</v>
+        <v>134</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>196</v>
+        <v>133</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>187</v>
+        <v>94</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>188</v>
+        <v>111</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="G32" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="26">
         <v>0</v>
@@ -9843,13 +9843,13 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>132</v>
@@ -9857,31 +9857,31 @@
       <c r="E33" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="F33" s="26" t="s">
-        <v>104</v>
+      <c r="F33" s="36" t="s">
+        <v>98</v>
       </c>
       <c r="G33" s="26">
         <v>1</v>
       </c>
       <c r="H33" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="26" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="E34" s="26" t="s">
         <v>111</v>
@@ -9901,10 +9901,10 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="26" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C35" s="26" t="s">
         <v>144</v>
@@ -9930,10 +9930,10 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="26" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C36" s="26" t="s">
         <v>144</v>
@@ -9959,13 +9959,13 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="26" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="D37" s="26" t="s">
         <v>145</v>
@@ -9973,7 +9973,7 @@
       <c r="E37" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="F37" s="36" t="s">
+      <c r="F37" s="26" t="s">
         <v>98</v>
       </c>
       <c r="G37" s="26">
@@ -9988,10 +9988,10 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="26" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C38" s="26" t="s">
         <v>90</v>
@@ -10017,10 +10017,10 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="26" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>90</v>
@@ -10046,13 +10046,13 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="26" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>145</v>
@@ -10060,7 +10060,7 @@
       <c r="E40" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="F40" s="26" t="s">
+      <c r="F40" s="36" t="s">
         <v>98</v>
       </c>
       <c r="G40" s="26">
@@ -10075,16 +10075,16 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="26" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="E41" s="26" t="s">
         <v>111</v>
@@ -10096,7 +10096,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="26">
         <v>1</v>
@@ -10104,28 +10104,28 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="26" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="E42" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="F42" s="36" t="s">
+      <c r="F42" s="26" t="s">
         <v>98</v>
       </c>
       <c r="G42" s="26">
         <v>1</v>
       </c>
       <c r="H42" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="26">
         <v>1</v>
@@ -10133,25 +10133,25 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="26" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="F43" s="26" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G43" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" s="26">
         <v>0</v>
@@ -10162,10 +10162,10 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="26" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C44" s="26" t="s">
         <v>102</v>
@@ -10191,10 +10191,10 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="26" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C45" s="26" t="s">
         <v>102</v>
@@ -10220,22 +10220,22 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="26" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>107</v>
+        <v>200</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>98</v>
+        <v>201</v>
       </c>
       <c r="F46" s="26" t="s">
-        <v>104</v>
+        <v>203</v>
       </c>
       <c r="G46" s="26">
         <v>0</v>
@@ -10249,10 +10249,10 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="26" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C47" s="26" t="s">
         <v>90</v>
@@ -10278,10 +10278,10 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="26" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C48" s="26" t="s">
         <v>90</v>
@@ -10307,10 +10307,10 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="26" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C49" s="26" t="s">
         <v>90</v>
@@ -10336,10 +10336,10 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="26" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C50" s="26" t="s">
         <v>90</v>
@@ -10365,10 +10365,10 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="26" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C51" s="26" t="s">
         <v>90</v>
@@ -10394,10 +10394,10 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C52" s="26" t="s">
         <v>90</v>
@@ -10423,13 +10423,13 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D53" s="26" t="s">
         <v>116</v>
@@ -10452,10 +10452,10 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C54" s="26" t="s">
         <v>97</v>
@@ -10481,10 +10481,10 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="26" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C55" s="26" t="s">
         <v>97</v>
@@ -10510,10 +10510,10 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C56" s="26" t="s">
         <v>97</v>
@@ -10539,10 +10539,10 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="26" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C57" s="26" t="s">
         <v>97</v>
@@ -10568,10 +10568,10 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="26" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C58" s="26" t="s">
         <v>97</v>
@@ -10597,10 +10597,10 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="26" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C59" s="26" t="s">
         <v>97</v>
@@ -10626,13 +10626,13 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="26" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>97</v>
+        <v>165</v>
       </c>
       <c r="D60" s="26" t="s">
         <v>116</v>
@@ -10655,10 +10655,10 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="26" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C61" s="26" t="s">
         <v>165</v>
@@ -10684,10 +10684,10 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="26" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C62" s="26" t="s">
         <v>165</v>
@@ -10713,10 +10713,10 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="26" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C63" s="26" t="s">
         <v>165</v>
@@ -10742,10 +10742,10 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="B64" s="26" t="s">
-        <v>236</v>
+        <v>239</v>
+      </c>
+      <c r="B64" s="27" t="s">
+        <v>238</v>
       </c>
       <c r="C64" s="26" t="s">
         <v>165</v>
@@ -10771,10 +10771,10 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B65" s="27" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C65" s="26" t="s">
         <v>165</v>
@@ -10800,10 +10800,10 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="26" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B66" s="27" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C66" s="26" t="s">
         <v>165</v>
@@ -10829,10 +10829,10 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="26" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C67" s="26" t="s">
         <v>165</v>
@@ -10858,10 +10858,10 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="26" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B68" s="27" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C68" s="26" t="s">
         <v>165</v>
@@ -10887,10 +10887,10 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="26" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C69" s="26" t="s">
         <v>165</v>
@@ -10916,13 +10916,13 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="26" t="s">
-        <v>249</v>
-      </c>
-      <c r="B70" s="27" t="s">
-        <v>248</v>
+        <v>428</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="C70" s="26" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="D70" s="26" t="s">
         <v>116</v>
@@ -10933,25 +10933,25 @@
       <c r="F70" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="G70" s="26">
-        <v>0</v>
-      </c>
-      <c r="H70" s="26">
-        <v>0</v>
-      </c>
-      <c r="I70" s="26">
+      <c r="G70" s="36">
+        <v>0</v>
+      </c>
+      <c r="H70" s="36">
+        <v>0</v>
+      </c>
+      <c r="I70" s="36">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="26" t="s">
-        <v>428</v>
-      </c>
-      <c r="B71" s="26" t="s">
-        <v>427</v>
+        <v>251</v>
+      </c>
+      <c r="B71" s="27" t="s">
+        <v>250</v>
       </c>
       <c r="C71" s="26" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="D71" s="26" t="s">
         <v>116</v>
@@ -10959,25 +10959,25 @@
       <c r="E71" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F71" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="G71" s="36">
-        <v>0</v>
-      </c>
-      <c r="H71" s="36">
-        <v>0</v>
-      </c>
-      <c r="I71" s="36">
+      <c r="F71" s="36" t="s">
+        <v>421</v>
+      </c>
+      <c r="G71" s="26">
+        <v>0</v>
+      </c>
+      <c r="H71" s="26">
+        <v>0</v>
+      </c>
+      <c r="I71" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="26" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C72" s="26" t="s">
         <v>102</v>
@@ -11003,10 +11003,10 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="B73" s="27" t="s">
-        <v>252</v>
+        <v>255</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>254</v>
       </c>
       <c r="C73" s="26" t="s">
         <v>102</v>
@@ -11032,10 +11032,10 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="26" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>102</v>
@@ -11061,10 +11061,10 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="26" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C75" s="26" t="s">
         <v>102</v>
@@ -11090,10 +11090,10 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="26" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C76" s="26" t="s">
         <v>102</v>
@@ -11119,10 +11119,10 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="26" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C77" s="26" t="s">
         <v>102</v>
@@ -11148,10 +11148,10 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="26" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C78" s="26" t="s">
         <v>102</v>
@@ -11177,10 +11177,10 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="26" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C79" s="26" t="s">
         <v>102</v>
@@ -11206,10 +11206,10 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="26" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C80" s="26" t="s">
         <v>102</v>
@@ -11235,10 +11235,10 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="26" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C81" s="26" t="s">
         <v>102</v>
@@ -11264,10 +11264,10 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="26" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C82" s="26" t="s">
         <v>102</v>
@@ -11292,11 +11292,11 @@
       </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="26" t="s">
-        <v>273</v>
-      </c>
-      <c r="B83" s="26" t="s">
-        <v>272</v>
+      <c r="A83" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="B83" s="27" t="s">
+        <v>274</v>
       </c>
       <c r="C83" s="26" t="s">
         <v>102</v>
@@ -11322,10 +11322,10 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="B84" s="27" t="s">
-        <v>274</v>
+        <v>276</v>
+      </c>
+      <c r="B84" s="37" t="s">
+        <v>424</v>
       </c>
       <c r="C84" s="26" t="s">
         <v>102</v>
@@ -11336,8 +11336,8 @@
       <c r="E84" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F84" s="36" t="s">
-        <v>421</v>
+      <c r="F84" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="G84" s="26">
         <v>0</v>
@@ -11350,11 +11350,11 @@
       </c>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="27" t="s">
-        <v>276</v>
-      </c>
-      <c r="B85" s="37" t="s">
-        <v>424</v>
+      <c r="A85" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="B85" s="36" t="s">
+        <v>425</v>
       </c>
       <c r="C85" s="26" t="s">
         <v>102</v>
@@ -11380,13 +11380,13 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="26" t="s">
-        <v>277</v>
-      </c>
-      <c r="B86" s="36" t="s">
-        <v>425</v>
+        <v>279</v>
+      </c>
+      <c r="B86" s="26" t="s">
+        <v>278</v>
       </c>
       <c r="C86" s="26" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D86" s="26" t="s">
         <v>116</v>
@@ -11409,10 +11409,10 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="26" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C87" s="26" t="s">
         <v>97</v>
@@ -11438,10 +11438,10 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="26" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C88" s="26" t="s">
         <v>97</v>
@@ -11452,8 +11452,8 @@
       <c r="E88" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F88" s="26" t="s">
-        <v>203</v>
+      <c r="F88" s="36" t="s">
+        <v>421</v>
       </c>
       <c r="G88" s="26">
         <v>0</v>
@@ -11467,13 +11467,13 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="26" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C89" s="26" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D89" s="26" t="s">
         <v>116</v>
@@ -11481,8 +11481,8 @@
       <c r="E89" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F89" s="36" t="s">
-        <v>421</v>
+      <c r="F89" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="G89" s="26">
         <v>0</v>
@@ -11496,10 +11496,10 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="26" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C90" s="26" t="s">
         <v>90</v>
@@ -11525,10 +11525,10 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="26" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C91" s="26" t="s">
         <v>90</v>
@@ -11554,10 +11554,10 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="26" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C92" s="26" t="s">
         <v>90</v>
@@ -11583,10 +11583,10 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="26" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C93" s="26" t="s">
         <v>90</v>
@@ -11612,10 +11612,10 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="26" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C94" s="26" t="s">
         <v>90</v>
@@ -11641,10 +11641,10 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="26" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C95" s="26" t="s">
         <v>90</v>
@@ -11670,10 +11670,10 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="26" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C96" s="26" t="s">
         <v>90</v>
@@ -11699,10 +11699,10 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="26" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C97" s="26" t="s">
         <v>90</v>
@@ -11713,8 +11713,8 @@
       <c r="E97" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F97" s="26" t="s">
-        <v>203</v>
+      <c r="F97" s="36" t="s">
+        <v>421</v>
       </c>
       <c r="G97" s="26">
         <v>0</v>
@@ -11728,10 +11728,10 @@
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="26" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C98" s="26" t="s">
         <v>90</v>
@@ -11757,10 +11757,10 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="26" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C99" s="26" t="s">
         <v>90</v>
@@ -11786,10 +11786,10 @@
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="26" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B100" s="26" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C100" s="26" t="s">
         <v>90</v>
@@ -11815,10 +11815,10 @@
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="26" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B101" s="26" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C101" s="26" t="s">
         <v>90</v>
@@ -11844,10 +11844,10 @@
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="26" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B102" s="26" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C102" s="26" t="s">
         <v>90</v>
@@ -11873,10 +11873,10 @@
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="26" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C103" s="26" t="s">
         <v>90</v>
@@ -11901,39 +11901,15 @@
       </c>
     </row>
     <row r="104" spans="1:9">
-      <c r="A104" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="B104" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="C104" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D104" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="E104" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="F104" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="G104" s="26">
-        <v>0</v>
-      </c>
-      <c r="H104" s="26">
-        <v>0</v>
-      </c>
-      <c r="I104" s="26">
-        <v>1</v>
-      </c>
+      <c r="D104" s="26"/>
     </row>
     <row r="105" spans="1:9">
       <c r="D105" s="26"/>
     </row>
     <row r="106" spans="1:9">
+      <c r="C106" s="26"/>
       <c r="D106" s="26"/>
+      <c r="E106" s="26"/>
     </row>
     <row r="107" spans="1:9">
       <c r="C107" s="26"/>
@@ -11989,11 +11965,6 @@
       <c r="C117" s="26"/>
       <c r="D117" s="26"/>
       <c r="E117" s="26"/>
-    </row>
-    <row r="118" spans="3:5">
-      <c r="C118" s="26"/>
-      <c r="D118" s="26"/>
-      <c r="E118" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
swapped order in spreadsheet
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -6838,8 +6838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6859,16 +6859,16 @@
     <col min="17" max="19" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="31" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="8.85546875" style="2"/>
-    <col min="38" max="38" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="9.140625" style="2"/>
+    <col min="26" max="26" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
@@ -6933,59 +6933,59 @@
       <c r="U1" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="32" t="s">
+      <c r="V1" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="32" t="s">
+      <c r="AC1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="32" t="s">
+      <c r="AD1" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="32" t="s">
+      <c r="AE1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="32" t="s">
+      <c r="AF1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" s="32" t="s">
+      <c r="AG1" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="22" t="s">
+      <c r="AH1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="22" t="s">
+      <c r="AI1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="22" t="s">
+      <c r="AJ1" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="AE1" s="22" t="s">
+      <c r="AK1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AF1" s="22" t="s">
+      <c r="AL1" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="AG1" s="22" t="s">
+      <c r="AM1" s="22" t="s">
         <v>34</v>
-      </c>
-      <c r="AH1" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI1" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ1" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AK1" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL1" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="AM1" s="23" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
@@ -7714,8 +7714,12 @@
       <c r="S16" s="33"/>
       <c r="T16" s="33"/>
       <c r="U16" s="36"/>
-      <c r="V16" s="33"/>
-      <c r="W16" s="33"/>
+      <c r="V16" s="21">
+        <v>1</v>
+      </c>
+      <c r="W16" s="21">
+        <v>1</v>
+      </c>
       <c r="X16" s="33"/>
       <c r="Y16" s="33"/>
       <c r="Z16" s="33"/>
@@ -7726,12 +7730,8 @@
       <c r="AE16" s="33"/>
       <c r="AF16" s="33"/>
       <c r="AG16" s="36"/>
-      <c r="AH16" s="21">
-        <v>1</v>
-      </c>
-      <c r="AI16" s="21">
-        <v>1</v>
-      </c>
+      <c r="AH16" s="33"/>
+      <c r="AI16" s="33"/>
       <c r="AJ16" s="33"/>
       <c r="AK16" s="33"/>
       <c r="AL16" s="33"/>
@@ -7766,8 +7766,12 @@
       <c r="T17" s="33"/>
       <c r="U17" s="36"/>
       <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
-      <c r="X17" s="33"/>
+      <c r="W17" s="21">
+        <v>1</v>
+      </c>
+      <c r="X17" s="21">
+        <v>1</v>
+      </c>
       <c r="Y17" s="33"/>
       <c r="Z17" s="33"/>
       <c r="AA17" s="36"/>
@@ -7778,12 +7782,8 @@
       <c r="AF17" s="33"/>
       <c r="AG17" s="36"/>
       <c r="AH17" s="33"/>
-      <c r="AI17" s="21">
-        <v>1</v>
-      </c>
-      <c r="AJ17" s="21">
-        <v>1</v>
-      </c>
+      <c r="AI17" s="33"/>
+      <c r="AJ17" s="33"/>
       <c r="AK17" s="33"/>
       <c r="AL17" s="33"/>
       <c r="AM17" s="36"/>
@@ -7818,8 +7818,12 @@
       <c r="U18" s="36"/>
       <c r="V18" s="33"/>
       <c r="W18" s="33"/>
-      <c r="X18" s="33"/>
-      <c r="Y18" s="33"/>
+      <c r="X18" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="21">
+        <v>1</v>
+      </c>
       <c r="Z18" s="33"/>
       <c r="AA18" s="36"/>
       <c r="AB18" s="33"/>
@@ -7830,12 +7834,8 @@
       <c r="AG18" s="36"/>
       <c r="AH18" s="33"/>
       <c r="AI18" s="33"/>
-      <c r="AJ18" s="21">
-        <v>1</v>
-      </c>
-      <c r="AK18" s="21">
-        <v>1</v>
-      </c>
+      <c r="AJ18" s="33"/>
+      <c r="AK18" s="33"/>
       <c r="AL18" s="33"/>
       <c r="AM18" s="36"/>
     </row>
@@ -7870,8 +7870,12 @@
       <c r="V19" s="33"/>
       <c r="W19" s="33"/>
       <c r="X19" s="33"/>
-      <c r="Y19" s="33"/>
-      <c r="Z19" s="33"/>
+      <c r="Y19" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="21">
+        <v>1</v>
+      </c>
       <c r="AA19" s="36"/>
       <c r="AB19" s="33"/>
       <c r="AC19" s="33"/>
@@ -7882,12 +7886,8 @@
       <c r="AH19" s="33"/>
       <c r="AI19" s="33"/>
       <c r="AJ19" s="33"/>
-      <c r="AK19" s="21">
-        <v>1</v>
-      </c>
-      <c r="AL19" s="21">
-        <v>1</v>
-      </c>
+      <c r="AK19" s="33"/>
+      <c r="AL19" s="33"/>
       <c r="AM19" s="36"/>
     </row>
     <row r="20" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
@@ -7922,8 +7922,12 @@
       <c r="W20" s="33"/>
       <c r="X20" s="33"/>
       <c r="Y20" s="33"/>
-      <c r="Z20" s="33"/>
-      <c r="AA20" s="36"/>
+      <c r="Z20" s="21">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="39">
+        <v>1</v>
+      </c>
       <c r="AB20" s="33"/>
       <c r="AC20" s="33"/>
       <c r="AD20" s="33"/>
@@ -7934,12 +7938,8 @@
       <c r="AI20" s="33"/>
       <c r="AJ20" s="33"/>
       <c r="AK20" s="33"/>
-      <c r="AL20" s="21">
-        <v>1</v>
-      </c>
-      <c r="AM20" s="39">
-        <v>1</v>
-      </c>
+      <c r="AL20" s="33"/>
+      <c r="AM20" s="36"/>
     </row>
     <row r="21" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
@@ -7972,7 +7972,9 @@
       <c r="X21" s="34"/>
       <c r="Y21" s="34"/>
       <c r="Z21" s="34"/>
-      <c r="AA21" s="38"/>
+      <c r="AA21" s="37">
+        <v>1</v>
+      </c>
       <c r="AB21" s="34"/>
       <c r="AC21" s="34"/>
       <c r="AD21" s="34"/>
@@ -7984,13 +7986,11 @@
       <c r="AJ21" s="34"/>
       <c r="AK21" s="34"/>
       <c r="AL21" s="34"/>
-      <c r="AM21" s="37">
-        <v>1</v>
-      </c>
+      <c r="AM21" s="38"/>
     </row>
     <row r="22" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>23</v>
+      <c r="A22" s="23" t="s">
+        <v>35</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="36"/>
@@ -8006,8 +8006,12 @@
       <c r="M22" s="33"/>
       <c r="N22" s="33"/>
       <c r="O22" s="36"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
+      <c r="P22" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>1</v>
+      </c>
       <c r="R22" s="33"/>
       <c r="S22" s="33"/>
       <c r="T22" s="33"/>
@@ -8022,26 +8026,22 @@
       <c r="Y22" s="33"/>
       <c r="Z22" s="33"/>
       <c r="AA22" s="36"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="21"/>
+      <c r="AB22" s="33"/>
+      <c r="AC22" s="33"/>
       <c r="AD22" s="33"/>
       <c r="AE22" s="33"/>
       <c r="AF22" s="33"/>
       <c r="AG22" s="36"/>
-      <c r="AH22" s="21">
-        <v>1</v>
-      </c>
-      <c r="AI22" s="21">
-        <v>1</v>
-      </c>
+      <c r="AH22" s="33"/>
+      <c r="AI22" s="33"/>
       <c r="AJ22" s="33"/>
       <c r="AK22" s="33"/>
       <c r="AL22" s="33"/>
       <c r="AM22" s="36"/>
     </row>
     <row r="23" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>24</v>
+      <c r="A23" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="36"/>
@@ -8058,8 +8058,12 @@
       <c r="N23" s="33"/>
       <c r="O23" s="36"/>
       <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-      <c r="R23" s="33"/>
+      <c r="Q23" s="21">
+        <v>1</v>
+      </c>
+      <c r="R23" s="21">
+        <v>1</v>
+      </c>
       <c r="S23" s="33"/>
       <c r="T23" s="33"/>
       <c r="U23" s="36"/>
@@ -8074,25 +8078,21 @@
       <c r="Z23" s="33"/>
       <c r="AA23" s="36"/>
       <c r="AB23" s="33"/>
-      <c r="AC23" s="21"/>
-      <c r="AD23" s="21"/>
+      <c r="AC23" s="33"/>
+      <c r="AD23" s="33"/>
       <c r="AE23" s="33"/>
       <c r="AF23" s="33"/>
       <c r="AG23" s="36"/>
       <c r="AH23" s="33"/>
-      <c r="AI23" s="21">
-        <v>1</v>
-      </c>
-      <c r="AJ23" s="21">
-        <v>1</v>
-      </c>
+      <c r="AI23" s="33"/>
+      <c r="AJ23" s="33"/>
       <c r="AK23" s="33"/>
       <c r="AL23" s="33"/>
       <c r="AM23" s="36"/>
     </row>
     <row r="24" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>25</v>
+      <c r="A24" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="B24" s="33"/>
       <c r="C24" s="36"/>
@@ -8110,14 +8110,16 @@
       <c r="O24" s="36"/>
       <c r="P24" s="33"/>
       <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="33"/>
+      <c r="R24" s="21">
+        <v>1</v>
+      </c>
+      <c r="S24" s="21">
+        <v>1</v>
+      </c>
       <c r="T24" s="33"/>
       <c r="U24" s="36"/>
       <c r="V24" s="33"/>
-      <c r="W24" s="21">
-        <v>1</v>
-      </c>
+      <c r="W24" s="33"/>
       <c r="X24" s="21">
         <v>1</v>
       </c>
@@ -8127,27 +8129,21 @@
       <c r="Z24" s="33"/>
       <c r="AA24" s="36"/>
       <c r="AB24" s="33"/>
-      <c r="AC24" s="21"/>
-      <c r="AD24" s="21"/>
-      <c r="AE24" s="21"/>
+      <c r="AC24" s="33"/>
+      <c r="AD24" s="33"/>
+      <c r="AE24" s="33"/>
       <c r="AF24" s="33"/>
       <c r="AG24" s="36"/>
       <c r="AH24" s="33"/>
-      <c r="AI24" s="21">
-        <v>1</v>
-      </c>
-      <c r="AJ24" s="21">
-        <v>1</v>
-      </c>
-      <c r="AK24" s="21">
-        <v>1</v>
-      </c>
+      <c r="AI24" s="33"/>
+      <c r="AJ24" s="33"/>
+      <c r="AK24" s="33"/>
       <c r="AL24" s="33"/>
       <c r="AM24" s="36"/>
     </row>
     <row r="25" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>26</v>
+      <c r="A25" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="B25" s="33"/>
       <c r="C25" s="36"/>
@@ -8166,14 +8162,16 @@
       <c r="P25" s="33"/>
       <c r="Q25" s="33"/>
       <c r="R25" s="33"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
+      <c r="S25" s="21">
+        <v>1</v>
+      </c>
+      <c r="T25" s="21">
+        <v>1</v>
+      </c>
       <c r="U25" s="36"/>
       <c r="V25" s="33"/>
       <c r="W25" s="33"/>
-      <c r="X25" s="21">
-        <v>1</v>
-      </c>
+      <c r="X25" s="33"/>
       <c r="Y25" s="21">
         <v>1</v>
       </c>
@@ -8183,26 +8181,20 @@
       <c r="AA25" s="36"/>
       <c r="AB25" s="33"/>
       <c r="AC25" s="33"/>
-      <c r="AD25" s="21"/>
-      <c r="AE25" s="21"/>
-      <c r="AF25" s="21"/>
+      <c r="AD25" s="33"/>
+      <c r="AE25" s="33"/>
+      <c r="AF25" s="33"/>
       <c r="AG25" s="36"/>
       <c r="AH25" s="33"/>
       <c r="AI25" s="33"/>
-      <c r="AJ25" s="21">
-        <v>1</v>
-      </c>
-      <c r="AK25" s="21">
-        <v>1</v>
-      </c>
-      <c r="AL25" s="21">
-        <v>1</v>
-      </c>
+      <c r="AJ25" s="33"/>
+      <c r="AK25" s="33"/>
+      <c r="AL25" s="33"/>
       <c r="AM25" s="36"/>
     </row>
     <row r="26" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>27</v>
+      <c r="A26" s="23" t="s">
+        <v>39</v>
       </c>
       <c r="B26" s="33"/>
       <c r="C26" s="36"/>
@@ -8222,14 +8214,16 @@
       <c r="Q26" s="33"/>
       <c r="R26" s="33"/>
       <c r="S26" s="33"/>
-      <c r="T26" s="33"/>
-      <c r="U26" s="36"/>
+      <c r="T26" s="21">
+        <v>1</v>
+      </c>
+      <c r="U26" s="39">
+        <v>1</v>
+      </c>
       <c r="V26" s="33"/>
       <c r="W26" s="33"/>
       <c r="X26" s="33"/>
-      <c r="Y26" s="21">
-        <v>1</v>
-      </c>
+      <c r="Y26" s="33"/>
       <c r="Z26" s="21">
         <v>1</v>
       </c>
@@ -8239,25 +8233,19 @@
       <c r="AB26" s="33"/>
       <c r="AC26" s="33"/>
       <c r="AD26" s="33"/>
-      <c r="AE26" s="21"/>
-      <c r="AF26" s="21"/>
-      <c r="AG26" s="39"/>
+      <c r="AE26" s="33"/>
+      <c r="AF26" s="33"/>
+      <c r="AG26" s="36"/>
       <c r="AH26" s="33"/>
       <c r="AI26" s="33"/>
       <c r="AJ26" s="33"/>
-      <c r="AK26" s="21">
-        <v>1</v>
-      </c>
-      <c r="AL26" s="21">
-        <v>1</v>
-      </c>
-      <c r="AM26" s="39">
-        <v>1</v>
-      </c>
+      <c r="AK26" s="33"/>
+      <c r="AL26" s="33"/>
+      <c r="AM26" s="36"/>
     </row>
     <row r="27" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>28</v>
+      <c r="A27" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="B27" s="34"/>
       <c r="C27" s="38"/>
@@ -8278,14 +8266,14 @@
       <c r="R27" s="34"/>
       <c r="S27" s="34"/>
       <c r="T27" s="34"/>
-      <c r="U27" s="38"/>
+      <c r="U27" s="37">
+        <v>1</v>
+      </c>
       <c r="V27" s="34"/>
       <c r="W27" s="34"/>
       <c r="X27" s="34"/>
       <c r="Y27" s="34"/>
-      <c r="Z27" s="35">
-        <v>1</v>
-      </c>
+      <c r="Z27" s="34"/>
       <c r="AA27" s="37">
         <v>1</v>
       </c>
@@ -8293,22 +8281,18 @@
       <c r="AC27" s="34"/>
       <c r="AD27" s="34"/>
       <c r="AE27" s="34"/>
-      <c r="AF27" s="35"/>
-      <c r="AG27" s="37"/>
+      <c r="AF27" s="34"/>
+      <c r="AG27" s="38"/>
       <c r="AH27" s="34"/>
       <c r="AI27" s="34"/>
       <c r="AJ27" s="34"/>
       <c r="AK27" s="34"/>
-      <c r="AL27" s="35">
-        <v>1</v>
-      </c>
-      <c r="AM27" s="37">
-        <v>1</v>
-      </c>
+      <c r="AL27" s="34"/>
+      <c r="AM27" s="38"/>
     </row>
     <row r="28" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
-        <v>29</v>
+      <c r="A28" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="B28" s="33"/>
       <c r="C28" s="36"/>
@@ -8350,20 +8334,16 @@
       <c r="AE28" s="33"/>
       <c r="AF28" s="33"/>
       <c r="AG28" s="36"/>
-      <c r="AH28" s="21">
-        <v>1</v>
-      </c>
-      <c r="AI28" s="21">
-        <v>1</v>
-      </c>
+      <c r="AH28" s="21"/>
+      <c r="AI28" s="21"/>
       <c r="AJ28" s="33"/>
       <c r="AK28" s="33"/>
       <c r="AL28" s="33"/>
       <c r="AM28" s="36"/>
     </row>
     <row r="29" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>30</v>
+      <c r="A29" s="28" t="s">
+        <v>24</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="36"/>
@@ -8389,7 +8369,9 @@
       <c r="W29" s="21">
         <v>1</v>
       </c>
-      <c r="X29" s="33"/>
+      <c r="X29" s="21">
+        <v>1</v>
+      </c>
       <c r="Y29" s="33"/>
       <c r="Z29" s="33"/>
       <c r="AA29" s="36"/>
@@ -8397,22 +8379,22 @@
       <c r="AC29" s="21">
         <v>1</v>
       </c>
-      <c r="AD29" s="33"/>
+      <c r="AD29" s="21">
+        <v>1</v>
+      </c>
       <c r="AE29" s="33"/>
       <c r="AF29" s="33"/>
       <c r="AG29" s="36"/>
       <c r="AH29" s="33"/>
-      <c r="AI29" s="21">
-        <v>1</v>
-      </c>
-      <c r="AJ29" s="33"/>
+      <c r="AI29" s="21"/>
+      <c r="AJ29" s="21"/>
       <c r="AK29" s="33"/>
       <c r="AL29" s="33"/>
       <c r="AM29" s="36"/>
     </row>
     <row r="30" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>31</v>
+      <c r="A30" s="28" t="s">
+        <v>25</v>
       </c>
       <c r="B30" s="33"/>
       <c r="C30" s="36"/>
@@ -8441,7 +8423,9 @@
       <c r="X30" s="21">
         <v>1</v>
       </c>
-      <c r="Y30" s="33"/>
+      <c r="Y30" s="21">
+        <v>1</v>
+      </c>
       <c r="Z30" s="33"/>
       <c r="AA30" s="36"/>
       <c r="AB30" s="33"/>
@@ -8451,23 +8435,21 @@
       <c r="AD30" s="21">
         <v>1</v>
       </c>
-      <c r="AE30" s="33"/>
+      <c r="AE30" s="21">
+        <v>1</v>
+      </c>
       <c r="AF30" s="33"/>
       <c r="AG30" s="36"/>
       <c r="AH30" s="33"/>
-      <c r="AI30" s="21">
-        <v>1</v>
-      </c>
-      <c r="AJ30" s="21">
-        <v>1</v>
-      </c>
-      <c r="AK30" s="33"/>
+      <c r="AI30" s="21"/>
+      <c r="AJ30" s="21"/>
+      <c r="AK30" s="21"/>
       <c r="AL30" s="33"/>
       <c r="AM30" s="36"/>
     </row>
     <row r="31" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
-        <v>32</v>
+      <c r="A31" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="B31" s="33"/>
       <c r="C31" s="36"/>
@@ -8497,7 +8479,9 @@
       <c r="Y31" s="21">
         <v>1</v>
       </c>
-      <c r="Z31" s="33"/>
+      <c r="Z31" s="21">
+        <v>1</v>
+      </c>
       <c r="AA31" s="36"/>
       <c r="AB31" s="33"/>
       <c r="AC31" s="33"/>
@@ -8507,22 +8491,20 @@
       <c r="AE31" s="21">
         <v>1</v>
       </c>
-      <c r="AF31" s="33"/>
+      <c r="AF31" s="21">
+        <v>1</v>
+      </c>
       <c r="AG31" s="36"/>
       <c r="AH31" s="33"/>
       <c r="AI31" s="33"/>
-      <c r="AJ31" s="21">
-        <v>1</v>
-      </c>
-      <c r="AK31" s="21">
-        <v>1</v>
-      </c>
-      <c r="AL31" s="33"/>
+      <c r="AJ31" s="21"/>
+      <c r="AK31" s="21"/>
+      <c r="AL31" s="21"/>
       <c r="AM31" s="36"/>
     </row>
     <row r="32" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
-        <v>33</v>
+      <c r="A32" s="28" t="s">
+        <v>27</v>
       </c>
       <c r="B32" s="33"/>
       <c r="C32" s="36"/>
@@ -8553,7 +8535,9 @@
       <c r="Z32" s="21">
         <v>1</v>
       </c>
-      <c r="AA32" s="36"/>
+      <c r="AA32" s="39">
+        <v>1</v>
+      </c>
       <c r="AB32" s="33"/>
       <c r="AC32" s="33"/>
       <c r="AD32" s="33"/>
@@ -8563,21 +8547,19 @@
       <c r="AF32" s="21">
         <v>1</v>
       </c>
-      <c r="AG32" s="36"/>
+      <c r="AG32" s="39">
+        <v>1</v>
+      </c>
       <c r="AH32" s="33"/>
       <c r="AI32" s="33"/>
       <c r="AJ32" s="33"/>
-      <c r="AK32" s="21">
-        <v>1</v>
-      </c>
-      <c r="AL32" s="21">
-        <v>1</v>
-      </c>
-      <c r="AM32" s="36"/>
+      <c r="AK32" s="21"/>
+      <c r="AL32" s="21"/>
+      <c r="AM32" s="39"/>
     </row>
     <row r="33" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
-        <v>34</v>
+      <c r="A33" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="B33" s="34"/>
       <c r="C33" s="38"/>
@@ -8623,16 +8605,12 @@
       <c r="AI33" s="34"/>
       <c r="AJ33" s="34"/>
       <c r="AK33" s="34"/>
-      <c r="AL33" s="35">
-        <v>1</v>
-      </c>
-      <c r="AM33" s="37">
-        <v>1</v>
-      </c>
+      <c r="AL33" s="35"/>
+      <c r="AM33" s="37"/>
     </row>
     <row r="34" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
-        <v>35</v>
+      <c r="A34" s="22" t="s">
+        <v>29</v>
       </c>
       <c r="B34" s="33"/>
       <c r="C34" s="36"/>
@@ -8648,24 +8626,28 @@
       <c r="M34" s="33"/>
       <c r="N34" s="33"/>
       <c r="O34" s="36"/>
-      <c r="P34" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="21">
-        <v>1</v>
-      </c>
+      <c r="P34" s="33"/>
+      <c r="Q34" s="33"/>
       <c r="R34" s="33"/>
       <c r="S34" s="33"/>
       <c r="T34" s="33"/>
       <c r="U34" s="36"/>
-      <c r="V34" s="33"/>
-      <c r="W34" s="33"/>
+      <c r="V34" s="21">
+        <v>1</v>
+      </c>
+      <c r="W34" s="21">
+        <v>1</v>
+      </c>
       <c r="X34" s="33"/>
       <c r="Y34" s="33"/>
       <c r="Z34" s="33"/>
       <c r="AA34" s="36"/>
-      <c r="AB34" s="33"/>
-      <c r="AC34" s="33"/>
+      <c r="AB34" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="21">
+        <v>1</v>
+      </c>
       <c r="AD34" s="33"/>
       <c r="AE34" s="33"/>
       <c r="AF34" s="33"/>
@@ -8682,8 +8664,8 @@
       <c r="AM34" s="36"/>
     </row>
     <row r="35" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
-        <v>36</v>
+      <c r="A35" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="36"/>
@@ -8700,23 +8682,23 @@
       <c r="N35" s="33"/>
       <c r="O35" s="36"/>
       <c r="P35" s="33"/>
-      <c r="Q35" s="21">
-        <v>1</v>
-      </c>
-      <c r="R35" s="21">
-        <v>1</v>
-      </c>
+      <c r="Q35" s="33"/>
+      <c r="R35" s="33"/>
       <c r="S35" s="33"/>
       <c r="T35" s="33"/>
       <c r="U35" s="36"/>
       <c r="V35" s="33"/>
-      <c r="W35" s="33"/>
+      <c r="W35" s="21">
+        <v>1</v>
+      </c>
       <c r="X35" s="33"/>
       <c r="Y35" s="33"/>
       <c r="Z35" s="33"/>
       <c r="AA35" s="36"/>
       <c r="AB35" s="33"/>
-      <c r="AC35" s="33"/>
+      <c r="AC35" s="21">
+        <v>1</v>
+      </c>
       <c r="AD35" s="33"/>
       <c r="AE35" s="33"/>
       <c r="AF35" s="33"/>
@@ -8725,16 +8707,14 @@
       <c r="AI35" s="21">
         <v>1</v>
       </c>
-      <c r="AJ35" s="21">
-        <v>1</v>
-      </c>
+      <c r="AJ35" s="33"/>
       <c r="AK35" s="33"/>
       <c r="AL35" s="33"/>
       <c r="AM35" s="36"/>
     </row>
     <row r="36" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
-        <v>37</v>
+      <c r="A36" s="22" t="s">
+        <v>31</v>
       </c>
       <c r="B36" s="33"/>
       <c r="C36" s="36"/>
@@ -8752,40 +8732,44 @@
       <c r="O36" s="36"/>
       <c r="P36" s="33"/>
       <c r="Q36" s="33"/>
-      <c r="R36" s="21">
-        <v>1</v>
-      </c>
-      <c r="S36" s="21">
-        <v>1</v>
-      </c>
+      <c r="R36" s="33"/>
+      <c r="S36" s="33"/>
       <c r="T36" s="33"/>
       <c r="U36" s="36"/>
       <c r="V36" s="33"/>
-      <c r="W36" s="33"/>
-      <c r="X36" s="33"/>
+      <c r="W36" s="21">
+        <v>1</v>
+      </c>
+      <c r="X36" s="21">
+        <v>1</v>
+      </c>
       <c r="Y36" s="33"/>
       <c r="Z36" s="33"/>
       <c r="AA36" s="36"/>
       <c r="AB36" s="33"/>
-      <c r="AC36" s="33"/>
-      <c r="AD36" s="33"/>
+      <c r="AC36" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD36" s="21">
+        <v>1</v>
+      </c>
       <c r="AE36" s="33"/>
       <c r="AF36" s="33"/>
       <c r="AG36" s="36"/>
       <c r="AH36" s="33"/>
-      <c r="AI36" s="33"/>
+      <c r="AI36" s="21">
+        <v>1</v>
+      </c>
       <c r="AJ36" s="21">
         <v>1</v>
       </c>
-      <c r="AK36" s="21">
-        <v>1</v>
-      </c>
+      <c r="AK36" s="33"/>
       <c r="AL36" s="33"/>
       <c r="AM36" s="36"/>
     </row>
     <row r="37" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
-        <v>38</v>
+      <c r="A37" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="B37" s="33"/>
       <c r="C37" s="36"/>
@@ -8804,39 +8788,43 @@
       <c r="P37" s="33"/>
       <c r="Q37" s="33"/>
       <c r="R37" s="33"/>
-      <c r="S37" s="21">
-        <v>1</v>
-      </c>
-      <c r="T37" s="21">
-        <v>1</v>
-      </c>
+      <c r="S37" s="33"/>
+      <c r="T37" s="33"/>
       <c r="U37" s="36"/>
       <c r="V37" s="33"/>
       <c r="W37" s="33"/>
-      <c r="X37" s="33"/>
-      <c r="Y37" s="33"/>
+      <c r="X37" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y37" s="21">
+        <v>1</v>
+      </c>
       <c r="Z37" s="33"/>
       <c r="AA37" s="36"/>
       <c r="AB37" s="33"/>
       <c r="AC37" s="33"/>
-      <c r="AD37" s="33"/>
-      <c r="AE37" s="33"/>
+      <c r="AD37" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE37" s="21">
+        <v>1</v>
+      </c>
       <c r="AF37" s="33"/>
       <c r="AG37" s="36"/>
       <c r="AH37" s="33"/>
       <c r="AI37" s="33"/>
-      <c r="AJ37" s="33"/>
+      <c r="AJ37" s="21">
+        <v>1</v>
+      </c>
       <c r="AK37" s="21">
         <v>1</v>
       </c>
-      <c r="AL37" s="21">
-        <v>1</v>
-      </c>
+      <c r="AL37" s="33"/>
       <c r="AM37" s="36"/>
     </row>
     <row r="38" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
-        <v>39</v>
+      <c r="A38" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="B38" s="33"/>
       <c r="C38" s="36"/>
@@ -8856,38 +8844,42 @@
       <c r="Q38" s="33"/>
       <c r="R38" s="33"/>
       <c r="S38" s="33"/>
-      <c r="T38" s="21">
-        <v>1</v>
-      </c>
-      <c r="U38" s="39">
-        <v>1</v>
-      </c>
+      <c r="T38" s="33"/>
+      <c r="U38" s="36"/>
       <c r="V38" s="33"/>
       <c r="W38" s="33"/>
       <c r="X38" s="33"/>
-      <c r="Y38" s="33"/>
-      <c r="Z38" s="33"/>
+      <c r="Y38" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="21">
+        <v>1</v>
+      </c>
       <c r="AA38" s="36"/>
       <c r="AB38" s="33"/>
       <c r="AC38" s="33"/>
       <c r="AD38" s="33"/>
-      <c r="AE38" s="33"/>
-      <c r="AF38" s="33"/>
+      <c r="AE38" s="21">
+        <v>1</v>
+      </c>
+      <c r="AF38" s="21">
+        <v>1</v>
+      </c>
       <c r="AG38" s="36"/>
       <c r="AH38" s="33"/>
       <c r="AI38" s="33"/>
       <c r="AJ38" s="33"/>
-      <c r="AK38" s="33"/>
+      <c r="AK38" s="21">
+        <v>1</v>
+      </c>
       <c r="AL38" s="21">
         <v>1</v>
       </c>
-      <c r="AM38" s="39">
-        <v>1</v>
-      </c>
+      <c r="AM38" s="36"/>
     </row>
     <row r="39" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
-        <v>40</v>
+      <c r="A39" s="22" t="s">
+        <v>34</v>
       </c>
       <c r="B39" s="34"/>
       <c r="C39" s="38"/>
@@ -8908,26 +8900,34 @@
       <c r="R39" s="34"/>
       <c r="S39" s="34"/>
       <c r="T39" s="34"/>
-      <c r="U39" s="37">
-        <v>1</v>
-      </c>
+      <c r="U39" s="38"/>
       <c r="V39" s="34"/>
       <c r="W39" s="34"/>
       <c r="X39" s="34"/>
       <c r="Y39" s="34"/>
-      <c r="Z39" s="34"/>
-      <c r="AA39" s="38"/>
+      <c r="Z39" s="35">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="37">
+        <v>1</v>
+      </c>
       <c r="AB39" s="34"/>
       <c r="AC39" s="34"/>
       <c r="AD39" s="34"/>
       <c r="AE39" s="34"/>
-      <c r="AF39" s="34"/>
-      <c r="AG39" s="38"/>
+      <c r="AF39" s="35">
+        <v>1</v>
+      </c>
+      <c r="AG39" s="37">
+        <v>1</v>
+      </c>
       <c r="AH39" s="34"/>
       <c r="AI39" s="34"/>
       <c r="AJ39" s="34"/>
       <c r="AK39" s="34"/>
-      <c r="AL39" s="34"/>
+      <c r="AL39" s="35">
+        <v>1</v>
+      </c>
       <c r="AM39" s="37">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
changed numvlmon, and added transnorm parameter
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="432">
   <si>
     <t>Code Label</t>
   </si>
@@ -1309,6 +1309,12 @@
   </si>
   <si>
     <t>3. Update the example spreadsheets (e.g. simple.xlsx, concentrated.xlsx, and generalized.xlsx) in the tests folder to have the correct parameters.</t>
+  </si>
+  <si>
+    <t>transnorm</t>
+  </si>
+  <si>
+    <t>Transmission normalization factor</t>
   </si>
 </sst>
 </file>
@@ -6838,7 +6844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
@@ -8945,11 +8951,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10273,13 +10279,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>202</v>
+        <v>430</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>200</v>
+        <v>431</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>116</v>
@@ -10297,15 +10303,15 @@
         <v>0</v>
       </c>
       <c r="I46" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>90</v>
@@ -10331,10 +10337,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>90</v>
@@ -10360,10 +10366,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>90</v>
@@ -10389,10 +10395,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>90</v>
@@ -10418,10 +10424,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>90</v>
@@ -10447,10 +10453,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>90</v>
@@ -10476,13 +10482,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>116</v>
@@ -10505,10 +10511,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>97</v>
@@ -10534,10 +10540,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>97</v>
@@ -10563,10 +10569,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>97</v>
@@ -10592,10 +10598,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>97</v>
@@ -10621,10 +10627,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>97</v>
@@ -10650,10 +10656,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>97</v>
@@ -10679,13 +10685,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>165</v>
+        <v>97</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>116</v>
@@ -10708,10 +10714,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>165</v>
@@ -10737,10 +10743,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>165</v>
@@ -10766,10 +10772,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>165</v>
@@ -10795,10 +10801,10 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>165</v>
@@ -10824,10 +10830,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>165</v>
@@ -10853,10 +10859,10 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>165</v>
@@ -10882,10 +10888,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>165</v>
@@ -10911,10 +10917,10 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>165</v>
@@ -10940,10 +10946,10 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>165</v>
@@ -10969,13 +10975,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>425</v>
+        <v>249</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>248</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>116</v>
@@ -10986,25 +10992,25 @@
       <c r="F70" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="G70" s="17">
-        <v>0</v>
-      </c>
-      <c r="H70" s="17">
-        <v>0</v>
-      </c>
-      <c r="I70" s="17">
+      <c r="G70" s="7">
+        <v>0</v>
+      </c>
+      <c r="H70" s="7">
+        <v>0</v>
+      </c>
+      <c r="I70" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>250</v>
+        <v>426</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>425</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>116</v>
@@ -11012,25 +11018,25 @@
       <c r="E71" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="F71" s="17" t="s">
-        <v>419</v>
-      </c>
-      <c r="G71" s="7">
-        <v>0</v>
-      </c>
-      <c r="H71" s="7">
-        <v>0</v>
-      </c>
-      <c r="I71" s="7">
+      <c r="F71" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="G71" s="17">
+        <v>0</v>
+      </c>
+      <c r="H71" s="17">
+        <v>0</v>
+      </c>
+      <c r="I71" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>102</v>
@@ -11056,10 +11062,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>252</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>102</v>
@@ -11085,10 +11091,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>102</v>
@@ -11114,10 +11120,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>102</v>
@@ -11143,10 +11149,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>102</v>
@@ -11172,10 +11178,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>102</v>
@@ -11201,10 +11207,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>102</v>
@@ -11230,10 +11236,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>102</v>
@@ -11259,10 +11265,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>102</v>
@@ -11288,10 +11294,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>102</v>
@@ -11317,10 +11323,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>102</v>
@@ -11345,11 +11351,11 @@
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>274</v>
+      <c r="A83" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>272</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>102</v>
@@ -11375,10 +11381,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="B84" s="18" t="s">
-        <v>422</v>
+        <v>275</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>102</v>
@@ -11389,8 +11395,8 @@
       <c r="E84" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="F84" s="7" t="s">
-        <v>203</v>
+      <c r="F84" s="17" t="s">
+        <v>419</v>
       </c>
       <c r="G84" s="7">
         <v>0</v>
@@ -11403,11 +11409,11 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="B85" s="17" t="s">
-        <v>423</v>
+      <c r="A85" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>422</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>102</v>
@@ -11433,13 +11439,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>423</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>116</v>
@@ -11462,10 +11468,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>97</v>
@@ -11491,10 +11497,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>97</v>
@@ -11505,8 +11511,8 @@
       <c r="E88" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="F88" s="17" t="s">
-        <v>419</v>
+      <c r="F88" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="G88" s="7">
         <v>0</v>
@@ -11520,13 +11526,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>116</v>
@@ -11534,8 +11540,8 @@
       <c r="E89" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="F89" s="7" t="s">
-        <v>203</v>
+      <c r="F89" s="17" t="s">
+        <v>419</v>
       </c>
       <c r="G89" s="7">
         <v>0</v>
@@ -11549,10 +11555,10 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>90</v>
@@ -11578,10 +11584,10 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>90</v>
@@ -11607,10 +11613,10 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>90</v>
@@ -11636,10 +11642,10 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>90</v>
@@ -11665,10 +11671,10 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>90</v>
@@ -11694,10 +11700,10 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>90</v>
@@ -11723,10 +11729,10 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>90</v>
@@ -11752,10 +11758,10 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>90</v>
@@ -11766,8 +11772,8 @@
       <c r="E97" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="F97" s="17" t="s">
-        <v>419</v>
+      <c r="F97" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="G97" s="7">
         <v>0</v>
@@ -11781,10 +11787,10 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>90</v>
@@ -11810,10 +11816,10 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>90</v>
@@ -11839,10 +11845,10 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>90</v>
@@ -11868,10 +11874,10 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>90</v>
@@ -11897,10 +11903,10 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>90</v>
@@ -11926,10 +11932,10 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>90</v>
@@ -11954,15 +11960,39 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D104" s="7"/>
+      <c r="A104" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F104" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="G104" s="7">
+        <v>0</v>
+      </c>
+      <c r="H104" s="7">
+        <v>0</v>
+      </c>
+      <c r="I104" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D105" s="7"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C106" s="7"/>
       <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C107" s="7"/>
@@ -12018,6 +12048,11 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
+    </row>
+    <row r="118" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C118" s="7"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixing bugs in spreadsheet
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="435">
   <si>
     <t>Code Label</t>
   </si>
@@ -531,9 +531,6 @@
     <t>Viral load monitoring (number/year)</t>
   </si>
   <si>
-    <t>freqvlmon</t>
-  </si>
-  <si>
     <t>Loss to follow-up rate (per year)</t>
   </si>
   <si>
@@ -1315,6 +1312,18 @@
   </si>
   <si>
     <t>Transmission normalization factor</t>
+  </si>
+  <si>
+    <t>matrix</t>
+  </si>
+  <si>
+    <t>partcas</t>
+  </si>
+  <si>
+    <t>condomreg</t>
+  </si>
+  <si>
+    <t>optprev</t>
   </si>
 </sst>
 </file>
@@ -6367,38 +6376,38 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B1" t="s">
         <v>399</v>
       </c>
-      <c r="B1" t="s">
-        <v>400</v>
-      </c>
       <c r="C1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -6406,7 +6415,7 @@
         <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -6414,7 +6423,7 @@
         <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -6422,7 +6431,7 @@
         <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -6430,7 +6439,7 @@
         <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -6438,7 +6447,7 @@
         <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -6446,7 +6455,7 @@
         <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -6454,7 +6463,7 @@
         <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -6462,7 +6471,7 @@
         <v>166</v>
       </c>
       <c r="B23" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -6470,7 +6479,7 @@
         <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -6478,15 +6487,15 @@
         <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B26" t="s">
         <v>412</v>
-      </c>
-      <c r="B26" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -6494,7 +6503,7 @@
         <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -8953,7 +8962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
@@ -8989,10 +8998,10 @@
         <v>82</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>417</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>418</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>84</v>
@@ -9035,7 +9044,7 @@
         <v>96</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>97</v>
@@ -9064,7 +9073,7 @@
         <v>99</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>97</v>
@@ -9409,10 +9418,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>94</v>
@@ -9496,10 +9505,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>102</v>
@@ -9525,10 +9534,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>102</v>
@@ -9554,7 +9563,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>169</v>
@@ -9583,10 +9592,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>90</v>
@@ -9612,10 +9621,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>90</v>
@@ -9641,10 +9650,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>90</v>
@@ -9670,10 +9679,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>90</v>
@@ -9699,10 +9708,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>90</v>
@@ -9728,22 +9737,22 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E27" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="G27" s="7">
         <v>0</v>
@@ -9757,22 +9766,22 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E28" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="G28" s="7">
         <v>0</v>
@@ -9786,22 +9795,22 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E29" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="G29" s="7">
         <v>0</v>
@@ -9815,22 +9824,22 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E30" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="G30" s="7">
         <v>0</v>
@@ -9844,22 +9853,22 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E31" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="G31" s="7">
         <v>0</v>
@@ -10279,10 +10288,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>430</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>431</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>97</v>
@@ -10291,10 +10300,10 @@
         <v>116</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G46" s="7">
         <v>0</v>
@@ -10308,10 +10317,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>90</v>
@@ -10320,10 +10329,10 @@
         <v>116</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G47" s="7">
         <v>0</v>
@@ -10337,10 +10346,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>90</v>
@@ -10349,10 +10358,10 @@
         <v>116</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G48" s="7">
         <v>0</v>
@@ -10366,10 +10375,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>90</v>
@@ -10378,10 +10387,10 @@
         <v>116</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G49" s="7">
         <v>0</v>
@@ -10395,10 +10404,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>90</v>
@@ -10407,10 +10416,10 @@
         <v>116</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G50" s="7">
         <v>0</v>
@@ -10424,10 +10433,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>90</v>
@@ -10436,10 +10445,10 @@
         <v>116</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G51" s="7">
         <v>0</v>
@@ -10453,10 +10462,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>90</v>
@@ -10465,10 +10474,10 @@
         <v>116</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G52" s="7">
         <v>0</v>
@@ -10482,10 +10491,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>90</v>
@@ -10494,10 +10503,10 @@
         <v>116</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G53" s="7">
         <v>0</v>
@@ -10511,10 +10520,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>97</v>
@@ -10523,10 +10532,10 @@
         <v>116</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G54" s="7">
         <v>0</v>
@@ -10540,10 +10549,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>97</v>
@@ -10552,10 +10561,10 @@
         <v>116</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G55" s="7">
         <v>0</v>
@@ -10569,10 +10578,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>97</v>
@@ -10581,10 +10590,10 @@
         <v>116</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G56" s="7">
         <v>0</v>
@@ -10598,10 +10607,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>97</v>
@@ -10610,10 +10619,10 @@
         <v>116</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G57" s="7">
         <v>0</v>
@@ -10627,10 +10636,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>97</v>
@@ -10639,10 +10648,10 @@
         <v>116</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G58" s="7">
         <v>0</v>
@@ -10656,10 +10665,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>97</v>
@@ -10668,10 +10677,10 @@
         <v>116</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G59" s="7">
         <v>0</v>
@@ -10685,10 +10694,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>97</v>
@@ -10697,10 +10706,10 @@
         <v>116</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G60" s="7">
         <v>0</v>
@@ -10714,10 +10723,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>165</v>
@@ -10726,10 +10735,10 @@
         <v>116</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G61" s="7">
         <v>0</v>
@@ -10743,10 +10752,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>165</v>
@@ -10755,10 +10764,10 @@
         <v>116</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G62" s="7">
         <v>0</v>
@@ -10772,10 +10781,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>165</v>
@@ -10784,10 +10793,10 @@
         <v>116</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G63" s="7">
         <v>0</v>
@@ -10801,10 +10810,10 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>165</v>
@@ -10813,10 +10822,10 @@
         <v>116</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G64" s="7">
         <v>0</v>
@@ -10830,10 +10839,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>165</v>
@@ -10842,10 +10851,10 @@
         <v>116</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G65" s="7">
         <v>0</v>
@@ -10859,10 +10868,10 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>165</v>
@@ -10871,10 +10880,10 @@
         <v>116</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G66" s="7">
         <v>0</v>
@@ -10888,10 +10897,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>165</v>
@@ -10900,10 +10909,10 @@
         <v>116</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G67" s="7">
         <v>0</v>
@@ -10917,10 +10926,10 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>165</v>
@@ -10929,10 +10938,10 @@
         <v>116</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G68" s="7">
         <v>0</v>
@@ -10946,10 +10955,10 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>165</v>
@@ -10958,10 +10967,10 @@
         <v>116</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G69" s="7">
         <v>0</v>
@@ -10975,10 +10984,10 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>165</v>
@@ -10987,10 +10996,10 @@
         <v>116</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G70" s="7">
         <v>0</v>
@@ -11004,10 +11013,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>144</v>
@@ -11016,10 +11025,10 @@
         <v>116</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G71" s="17">
         <v>0</v>
@@ -11033,10 +11042,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>102</v>
@@ -11045,10 +11054,10 @@
         <v>116</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G72" s="7">
         <v>0</v>
@@ -11062,10 +11071,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>102</v>
@@ -11074,10 +11083,10 @@
         <v>116</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G73" s="7">
         <v>0</v>
@@ -11091,10 +11100,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>102</v>
@@ -11103,10 +11112,10 @@
         <v>116</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G74" s="7">
         <v>0</v>
@@ -11120,10 +11129,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>102</v>
@@ -11132,10 +11141,10 @@
         <v>116</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G75" s="7">
         <v>0</v>
@@ -11149,10 +11158,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>102</v>
@@ -11161,10 +11170,10 @@
         <v>116</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G76" s="7">
         <v>0</v>
@@ -11178,10 +11187,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>102</v>
@@ -11190,10 +11199,10 @@
         <v>116</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G77" s="7">
         <v>0</v>
@@ -11207,10 +11216,10 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>102</v>
@@ -11219,10 +11228,10 @@
         <v>116</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G78" s="7">
         <v>0</v>
@@ -11236,10 +11245,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>102</v>
@@ -11248,10 +11257,10 @@
         <v>116</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G79" s="7">
         <v>0</v>
@@ -11265,10 +11274,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>102</v>
@@ -11277,10 +11286,10 @@
         <v>116</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F80" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G80" s="7">
         <v>0</v>
@@ -11294,10 +11303,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>102</v>
@@ -11306,10 +11315,10 @@
         <v>116</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G81" s="7">
         <v>0</v>
@@ -11323,10 +11332,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>102</v>
@@ -11335,10 +11344,10 @@
         <v>116</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G82" s="7">
         <v>0</v>
@@ -11352,10 +11361,10 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>102</v>
@@ -11364,10 +11373,10 @@
         <v>116</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G83" s="7">
         <v>0</v>
@@ -11381,10 +11390,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>102</v>
@@ -11393,10 +11402,10 @@
         <v>116</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G84" s="7">
         <v>0</v>
@@ -11410,10 +11419,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>102</v>
@@ -11422,10 +11431,10 @@
         <v>116</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G85" s="7">
         <v>0</v>
@@ -11439,10 +11448,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>102</v>
@@ -11451,10 +11460,10 @@
         <v>116</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G86" s="7">
         <v>0</v>
@@ -11468,10 +11477,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>97</v>
@@ -11480,10 +11489,10 @@
         <v>116</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G87" s="7">
         <v>0</v>
@@ -11497,10 +11506,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>97</v>
@@ -11509,10 +11518,10 @@
         <v>116</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G88" s="7">
         <v>0</v>
@@ -11526,10 +11535,10 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>97</v>
@@ -11538,10 +11547,10 @@
         <v>116</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G89" s="7">
         <v>0</v>
@@ -11555,10 +11564,10 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>90</v>
@@ -11567,10 +11576,10 @@
         <v>116</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G90" s="7">
         <v>0</v>
@@ -11584,10 +11593,10 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>90</v>
@@ -11596,10 +11605,10 @@
         <v>116</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G91" s="7">
         <v>0</v>
@@ -11613,10 +11622,10 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>90</v>
@@ -11625,10 +11634,10 @@
         <v>116</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G92" s="7">
         <v>0</v>
@@ -11642,10 +11651,10 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>90</v>
@@ -11654,10 +11663,10 @@
         <v>116</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G93" s="7">
         <v>0</v>
@@ -11671,10 +11680,10 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>90</v>
@@ -11683,10 +11692,10 @@
         <v>116</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G94" s="7">
         <v>0</v>
@@ -11700,10 +11709,10 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>90</v>
@@ -11712,10 +11721,10 @@
         <v>116</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G95" s="7">
         <v>0</v>
@@ -11729,10 +11738,10 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>90</v>
@@ -11741,10 +11750,10 @@
         <v>116</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G96" s="7">
         <v>0</v>
@@ -11758,10 +11767,10 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>90</v>
@@ -11770,10 +11779,10 @@
         <v>116</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G97" s="7">
         <v>0</v>
@@ -11787,10 +11796,10 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>90</v>
@@ -11799,10 +11808,10 @@
         <v>116</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G98" s="7">
         <v>0</v>
@@ -11816,10 +11825,10 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>90</v>
@@ -11828,10 +11837,10 @@
         <v>116</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G99" s="7">
         <v>0</v>
@@ -11845,10 +11854,10 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>90</v>
@@ -11857,10 +11866,10 @@
         <v>116</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F100" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G100" s="7">
         <v>0</v>
@@ -11874,10 +11883,10 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>90</v>
@@ -11886,10 +11895,10 @@
         <v>116</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F101" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G101" s="7">
         <v>0</v>
@@ -11903,10 +11912,10 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>90</v>
@@ -11915,10 +11924,10 @@
         <v>116</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F102" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G102" s="7">
         <v>0</v>
@@ -11932,10 +11941,10 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>90</v>
@@ -11944,10 +11953,10 @@
         <v>116</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F103" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G103" s="7">
         <v>0</v>
@@ -11961,10 +11970,10 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>90</v>
@@ -11973,10 +11982,10 @@
         <v>116</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F104" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G104" s="7">
         <v>0</v>
@@ -12069,8 +12078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12083,10 +12092,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>79</v>
@@ -12095,18 +12104,18 @@
         <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B2" t="s">
         <v>98</v>
@@ -12114,19 +12123,22 @@
       <c r="C2" t="s">
         <v>91</v>
       </c>
+      <c r="D2" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B3" t="s">
         <v>333</v>
       </c>
-      <c r="B3" t="s">
-        <v>334</v>
-      </c>
       <c r="C3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D3" t="s">
-        <v>333</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -12134,21 +12146,18 @@
         <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C4" t="s">
         <v>93</v>
       </c>
-      <c r="D4" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C5" t="s">
         <v>110</v>
@@ -12156,10 +12165,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C6" t="s">
         <v>118</v>
@@ -12167,10 +12176,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C7" t="s">
         <v>120</v>
@@ -12178,10 +12187,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C8" t="s">
         <v>113</v>
@@ -12189,10 +12198,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C9" t="s">
         <v>115</v>
@@ -12200,10 +12209,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C10" t="s">
         <v>122</v>
@@ -12211,21 +12220,21 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C12" t="s">
         <v>140</v>
@@ -12233,10 +12242,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C13" t="s">
         <v>124</v>
@@ -12244,10 +12253,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C14" t="s">
         <v>128</v>
@@ -12255,10 +12264,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C15" t="s">
         <v>126</v>
@@ -12266,142 +12275,142 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C19" t="s">
-        <v>316</v>
+        <v>434</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B21" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B23" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B24" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C24" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C28" t="s">
         <v>164</v>
@@ -12409,10 +12418,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C29" t="s">
         <v>168</v>
@@ -12420,43 +12429,43 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C32" t="s">
-        <v>170</v>
+        <v>423</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C33" t="s">
         <v>143</v>
@@ -12464,10 +12473,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C34" t="s">
         <v>148</v>
@@ -12475,10 +12484,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C35" t="s">
         <v>151</v>
@@ -12486,21 +12495,21 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B36" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C36" t="s">
-        <v>151</v>
+        <v>433</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B37" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C37" t="s">
         <v>159</v>
@@ -12508,10 +12517,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B38" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C38" t="s">
         <v>162</v>
@@ -12519,10 +12528,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B39" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C39" t="s">
         <v>131</v>
@@ -12530,10 +12539,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B40" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C40" t="s">
         <v>154</v>
@@ -12541,10 +12550,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B41" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C41" t="s">
         <v>138</v>
@@ -12552,10 +12561,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B42" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C42" t="s">
         <v>136</v>
@@ -12563,54 +12572,54 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B43" t="s">
-        <v>335</v>
+        <v>431</v>
       </c>
       <c r="C43" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B44" t="s">
-        <v>335</v>
+        <v>431</v>
       </c>
       <c r="C44" t="s">
-        <v>325</v>
+        <v>432</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B45" t="s">
-        <v>335</v>
+        <v>431</v>
       </c>
       <c r="C45" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B46" t="s">
-        <v>335</v>
+        <v>431</v>
       </c>
       <c r="C46" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B47" t="s">
-        <v>335</v>
+        <v>431</v>
       </c>
       <c r="C47" t="s">
         <v>108</v>
@@ -12618,10 +12627,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B48" t="s">
-        <v>335</v>
+        <v>431</v>
       </c>
       <c r="C48" t="s">
         <v>106</v>
@@ -12629,13 +12638,13 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B49" t="s">
-        <v>335</v>
+        <v>431</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -12648,8 +12657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12661,7 +12670,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>79</v>
@@ -12670,27 +12679,27 @@
         <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>349</v>
-      </c>
       <c r="G1" s="19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D2" s="11">
         <v>4.0000000000000002E-4</v>
@@ -12708,13 +12717,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D3" s="11">
         <v>8.0000000000000004E-4</v>
@@ -12732,13 +12741,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D4" s="11">
         <v>1.1000000000000001E-3</v>
@@ -12756,13 +12765,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D5" s="11">
         <v>1.38E-2</v>
@@ -12780,13 +12789,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D6" s="11">
         <v>8.0000000000000002E-3</v>
@@ -12804,13 +12813,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D7" s="11">
         <v>0.36699999999999999</v>
@@ -12828,13 +12837,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D8" s="11">
         <v>0.20499999999999999</v>
@@ -12852,13 +12861,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D9">
         <v>5.6</v>
@@ -12876,13 +12885,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -12900,13 +12909,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -12924,13 +12933,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -12948,13 +12957,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D13">
         <v>3.49</v>
@@ -12972,13 +12981,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D14">
         <v>7.17</v>
@@ -12996,13 +13005,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D15">
         <v>0.24</v>
@@ -13020,13 +13029,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D16">
         <v>0.95</v>
@@ -13044,13 +13053,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -13068,13 +13077,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D18">
         <v>3.74</v>
@@ -13092,13 +13101,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D19">
         <v>1.5</v>
@@ -13116,13 +13125,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D20">
         <v>2.2000000000000002</v>
@@ -13140,13 +13149,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D21">
         <v>1.42</v>
@@ -13164,13 +13173,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D22">
         <v>2.14</v>
@@ -13188,13 +13197,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D23">
         <v>0.66</v>
@@ -13212,13 +13221,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D24">
         <v>0.2</v>
@@ -13236,13 +13245,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -13260,13 +13269,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D26" s="11">
         <v>2.5999999999999999E-2</v>
@@ -13284,13 +13293,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D27" s="11">
         <v>0.15</v>
@@ -13308,13 +13317,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D28" s="11">
         <v>0.1</v>
@@ -13332,13 +13341,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D29" s="11">
         <v>5.2999999999999999E-2</v>
@@ -13356,13 +13365,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D30" s="11">
         <v>0.16200000000000001</v>
@@ -13380,13 +13389,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D31" s="11">
         <v>0.11700000000000001</v>
@@ -13404,13 +13413,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D32" s="11">
         <v>0.09</v>
@@ -13428,13 +13437,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D33" s="11">
         <v>0.111</v>
@@ -13452,13 +13461,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D34" s="11">
         <v>0.16</v>
@@ -13476,13 +13485,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D35" s="11">
         <v>3.5999999999999999E-3</v>
@@ -13500,13 +13509,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D36" s="11">
         <v>3.5999999999999999E-3</v>
@@ -13524,13 +13533,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D37" s="11">
         <v>5.7999999999999996E-3</v>
@@ -13548,13 +13557,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D38" s="11">
         <v>8.8000000000000005E-3</v>
@@ -13572,13 +13581,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D39" s="11">
         <v>5.8999999999999997E-2</v>
@@ -13596,13 +13605,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D40" s="11">
         <v>0.32300000000000001</v>
@@ -13620,13 +13629,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D41" s="11">
         <v>0.23</v>
@@ -13644,13 +13653,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D42" s="11">
         <v>0.48780000000000001</v>
@@ -13668,13 +13677,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D43" s="11">
         <v>2.17</v>
@@ -13692,13 +13701,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D44" s="13">
         <v>0.95</v>
@@ -13716,13 +13725,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D45" s="13">
         <v>0.57999999999999996</v>
@@ -13740,13 +13749,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D46" s="13">
         <v>0</v>
@@ -13764,13 +13773,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D47" s="13">
         <v>2.65</v>
@@ -13788,13 +13797,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D48" s="13">
         <v>0.54</v>
@@ -13812,13 +13821,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D49" s="13">
         <v>0.9</v>
@@ -13836,13 +13845,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D50" s="13">
         <v>0.73</v>
@@ -13860,13 +13869,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D51" s="13">
         <v>0.5</v>
@@ -13884,13 +13893,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D52" s="13">
         <v>0.92</v>
@@ -13908,13 +13917,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D53">
         <v>0.15</v>
@@ -13932,13 +13941,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D54">
         <v>0.01</v>
@@ -13956,13 +13965,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D55">
         <v>0.02</v>
@@ -13980,13 +13989,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D56">
         <v>7.0000000000000007E-2</v>
@@ -14004,13 +14013,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D57">
         <v>0.27</v>
@@ -14028,13 +14037,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D58">
         <v>0.55000000000000004</v>
@@ -14052,13 +14061,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B59" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C59" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D59">
         <v>0.05</v>

</xml_diff>

<commit_message>
starting to add required info to spreadsheet
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="438">
   <si>
     <t>Code Label</t>
   </si>
@@ -1311,9 +1311,6 @@
     <t>transnorm</t>
   </si>
   <si>
-    <t>Transmission normalization factor</t>
-  </si>
-  <si>
     <t>matrix</t>
   </si>
   <si>
@@ -1327,6 +1324,15 @@
   </si>
   <si>
     <t>checkupper</t>
+  </si>
+  <si>
+    <t>Normalization factor for transmissibility</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>percentage</t>
   </si>
 </sst>
 </file>
@@ -8966,8 +8972,8 @@
   <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L65" sqref="L65"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10294,7 +10300,7 @@
         <v>429</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>97</v>
@@ -12081,8 +12087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12108,7 +12114,7 @@
         <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>330</v>
@@ -12369,7 +12375,7 @@
         <v>334</v>
       </c>
       <c r="C19" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -12607,7 +12613,7 @@
         <v>334</v>
       </c>
       <c r="C36" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -12702,7 +12708,7 @@
         <v>343</v>
       </c>
       <c r="B43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C43" t="s">
         <v>324</v>
@@ -12716,10 +12722,10 @@
         <v>343</v>
       </c>
       <c r="B44" t="s">
+        <v>430</v>
+      </c>
+      <c r="C44" t="s">
         <v>431</v>
-      </c>
-      <c r="C44" t="s">
-        <v>432</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -12730,7 +12736,7 @@
         <v>343</v>
       </c>
       <c r="B45" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C45" t="s">
         <v>325</v>
@@ -12744,7 +12750,7 @@
         <v>343</v>
       </c>
       <c r="B46" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C46" t="s">
         <v>326</v>
@@ -12758,7 +12764,7 @@
         <v>343</v>
       </c>
       <c r="B47" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C47" t="s">
         <v>108</v>
@@ -12772,7 +12778,7 @@
         <v>343</v>
       </c>
       <c r="B48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C48" t="s">
         <v>106</v>
@@ -12786,7 +12792,7 @@
         <v>343</v>
       </c>
       <c r="B49" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C49" t="s">
         <v>101</v>
@@ -12803,10 +12809,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12814,9 +12820,10 @@
     <col min="1" max="1" width="62.5703125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>344</v>
       </c>
@@ -12838,8 +12845,11 @@
       <c r="G1" s="19" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>345</v>
       </c>
@@ -12862,8 +12872,11 @@
         <f>AND(D2&gt;=E2, D2&lt;=F2)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>345</v>
       </c>
@@ -12886,8 +12899,11 @@
         <f t="shared" ref="G3:G59" si="0">AND(D3&gt;=E3, D3&lt;=F3)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>345</v>
       </c>
@@ -12910,8 +12926,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>345</v>
       </c>
@@ -12934,8 +12953,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>345</v>
       </c>
@@ -12958,8 +12980,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>345</v>
       </c>
@@ -12982,8 +13007,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>345</v>
       </c>
@@ -13006,8 +13034,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>396</v>
       </c>
@@ -13030,8 +13061,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>396</v>
       </c>
@@ -13054,8 +13088,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>396</v>
       </c>
@@ -13078,8 +13115,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>396</v>
       </c>
@@ -13102,8 +13142,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>396</v>
       </c>
@@ -13126,8 +13169,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>396</v>
       </c>
@@ -13150,8 +13196,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>395</v>
       </c>
@@ -13174,8 +13223,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>395</v>
       </c>
@@ -13198,8 +13250,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>395</v>
       </c>
@@ -13222,8 +13277,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>395</v>
       </c>
@@ -13246,8 +13304,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>395</v>
       </c>
@@ -13270,8 +13331,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>394</v>
       </c>
@@ -13294,8 +13358,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>394</v>
       </c>
@@ -13318,8 +13385,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>394</v>
       </c>
@@ -13342,8 +13412,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>394</v>
       </c>
@@ -13366,8 +13439,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>394</v>
       </c>
@@ -13390,8 +13466,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>394</v>
       </c>
@@ -13414,8 +13493,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>393</v>
       </c>
@@ -13438,8 +13520,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>393</v>
       </c>
@@ -13462,8 +13547,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>393</v>
       </c>
@@ -13486,8 +13574,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>393</v>
       </c>
@@ -13510,8 +13601,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>393</v>
       </c>
@@ -13534,8 +13628,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>393</v>
       </c>
@@ -13558,8 +13655,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>393</v>
       </c>
@@ -13582,8 +13682,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>393</v>
       </c>
@@ -13606,8 +13709,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>393</v>
       </c>
@@ -13630,8 +13736,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>392</v>
       </c>
@@ -13654,8 +13763,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>392</v>
       </c>
@@ -13678,8 +13790,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>392</v>
       </c>
@@ -13702,8 +13817,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>392</v>
       </c>
@@ -13726,8 +13844,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>392</v>
       </c>
@@ -13750,8 +13871,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>392</v>
       </c>
@@ -13774,8 +13898,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>392</v>
       </c>
@@ -13798,8 +13925,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>392</v>
       </c>
@@ -13822,8 +13952,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>392</v>
       </c>
@@ -13846,8 +13979,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>391</v>
       </c>
@@ -13870,8 +14006,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>391</v>
       </c>
@@ -13894,8 +14033,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>391</v>
       </c>
@@ -13918,8 +14060,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>391</v>
       </c>
@@ -13942,8 +14087,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>391</v>
       </c>
@@ -13966,8 +14114,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>391</v>
       </c>
@@ -13990,8 +14141,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>391</v>
       </c>
@@ -14014,8 +14168,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>391</v>
       </c>
@@ -14038,8 +14195,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>391</v>
       </c>
@@ -14062,8 +14222,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>390</v>
       </c>
@@ -14086,8 +14249,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>390</v>
       </c>
@@ -14110,8 +14276,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>390</v>
       </c>
@@ -14134,8 +14303,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>390</v>
       </c>
@@ -14158,8 +14330,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>390</v>
       </c>
@@ -14182,8 +14357,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>390</v>
       </c>
@@ -14206,8 +14384,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>390</v>
       </c>
@@ -14229,6 +14410,9 @@
       <c r="G59" s="20" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on other sheets...getting close to being done
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="440">
   <si>
     <t>Code Label</t>
   </si>
@@ -1336,6 +1336,9 @@
   </si>
   <si>
     <t>decimal</t>
+  </si>
+  <si>
+    <t>general</t>
   </si>
 </sst>
 </file>
@@ -12090,8 +12093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12101,6 +12104,7 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -12156,6 +12160,9 @@
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="G3" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -12173,6 +12180,9 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="G4" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -12187,6 +12197,9 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="G5" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -12201,6 +12214,9 @@
       <c r="E6">
         <v>1</v>
       </c>
+      <c r="G6" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -12215,6 +12231,9 @@
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="G7" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -12229,6 +12248,9 @@
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="G8" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -12243,6 +12265,9 @@
       <c r="E9">
         <v>1</v>
       </c>
+      <c r="G9" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -12257,6 +12282,9 @@
       <c r="E10">
         <v>0</v>
       </c>
+      <c r="G10" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -12271,6 +12299,9 @@
       <c r="E11">
         <v>0</v>
       </c>
+      <c r="G11" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -12285,6 +12316,9 @@
       <c r="E12">
         <v>1</v>
       </c>
+      <c r="G12" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -12299,6 +12333,9 @@
       <c r="E13">
         <v>0</v>
       </c>
+      <c r="G13" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -12313,6 +12350,9 @@
       <c r="E14">
         <v>0</v>
       </c>
+      <c r="G14" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -12327,6 +12367,9 @@
       <c r="E15">
         <v>1</v>
       </c>
+      <c r="G15" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -12341,8 +12384,11 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>339</v>
       </c>
@@ -12355,8 +12401,11 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>339</v>
       </c>
@@ -12369,8 +12418,11 @@
       <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>339</v>
       </c>
@@ -12383,8 +12435,11 @@
       <c r="E19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>339</v>
       </c>
@@ -12397,8 +12452,11 @@
       <c r="E20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>339</v>
       </c>
@@ -12411,8 +12469,11 @@
       <c r="E21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>339</v>
       </c>
@@ -12425,8 +12486,11 @@
       <c r="E22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>339</v>
       </c>
@@ -12439,8 +12503,11 @@
       <c r="E23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>339</v>
       </c>
@@ -12453,8 +12520,11 @@
       <c r="E24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>339</v>
       </c>
@@ -12467,8 +12537,11 @@
       <c r="E25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>339</v>
       </c>
@@ -12481,8 +12554,11 @@
       <c r="E26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>339</v>
       </c>
@@ -12495,8 +12571,11 @@
       <c r="E27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>340</v>
       </c>
@@ -12509,8 +12588,11 @@
       <c r="E28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>340</v>
       </c>
@@ -12523,8 +12605,11 @@
       <c r="E29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>340</v>
       </c>
@@ -12537,8 +12622,11 @@
       <c r="E30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>340</v>
       </c>
@@ -12551,8 +12639,11 @@
       <c r="E31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>340</v>
       </c>
@@ -12565,8 +12656,11 @@
       <c r="E32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>341</v>
       </c>
@@ -12579,8 +12673,11 @@
       <c r="E33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>341</v>
       </c>
@@ -12593,8 +12690,11 @@
       <c r="E34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>341</v>
       </c>
@@ -12607,8 +12707,11 @@
       <c r="E35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>341</v>
       </c>
@@ -12621,8 +12724,11 @@
       <c r="E36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>341</v>
       </c>
@@ -12635,8 +12741,11 @@
       <c r="E37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>341</v>
       </c>
@@ -12649,8 +12758,11 @@
       <c r="E38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>341</v>
       </c>
@@ -12663,8 +12775,11 @@
       <c r="E39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>342</v>
       </c>
@@ -12677,8 +12792,11 @@
       <c r="E40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>342</v>
       </c>
@@ -12691,8 +12809,11 @@
       <c r="E41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>342</v>
       </c>
@@ -12705,8 +12826,11 @@
       <c r="E42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>343</v>
       </c>
@@ -12719,8 +12843,11 @@
       <c r="E43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>343</v>
       </c>
@@ -12733,8 +12860,11 @@
       <c r="E44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>343</v>
       </c>
@@ -12747,8 +12877,11 @@
       <c r="E45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>343</v>
       </c>
@@ -12761,8 +12894,11 @@
       <c r="E46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>343</v>
       </c>
@@ -12775,8 +12911,11 @@
       <c r="E47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>343</v>
       </c>
@@ -12789,8 +12928,11 @@
       <c r="E48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>343</v>
       </c>
@@ -12802,6 +12944,9 @@
       </c>
       <c r="E49">
         <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -12814,8 +12959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
format is a dangerous word
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="441">
   <si>
     <t>Code Label</t>
   </si>
@@ -1339,6 +1339,9 @@
   </si>
   <si>
     <t>general</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -12094,7 +12097,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12142,6 +12145,21 @@
       </c>
       <c r="C2" t="s">
         <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E2" t="s">
+        <v>440</v>
+      </c>
+      <c r="F2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G2" t="s">
+        <v>440</v>
+      </c>
+      <c r="H2" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
massive reorganization one more...
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="484">
   <si>
     <t>Code Label</t>
   </si>
@@ -1317,9 +1317,6 @@
     <t>optprev</t>
   </si>
   <si>
-    <t>checkupper</t>
-  </si>
-  <si>
     <t>Normalization factor for transmissibility</t>
   </si>
   <si>
@@ -1338,12 +1335,6 @@
     <t>rowformat</t>
   </si>
   <si>
-    <t>range1</t>
-  </si>
-  <si>
-    <t>range2</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
@@ -1468,6 +1459,18 @@
   </si>
   <si>
     <t>Percentage of people who receptively shared a needle/syringe at last injection</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>rownames</t>
+  </si>
+  <si>
+    <t>colnames</t>
   </si>
 </sst>
 </file>
@@ -8097,7 +8100,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8174,6 +8177,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6302">
     <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
@@ -17385,11 +17391,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17406,7 +17412,7 @@
     <col min="10" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>79</v>
       </c>
@@ -17434,8 +17440,9 @@
       <c r="I1" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="42"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>89</v>
       </c>
@@ -17464,7 +17471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>96</v>
       </c>
@@ -17493,7 +17500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>99</v>
       </c>
@@ -17522,7 +17529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>93</v>
       </c>
@@ -17551,7 +17558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>110</v>
       </c>
@@ -17580,7 +17587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>113</v>
       </c>
@@ -17609,7 +17616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>115</v>
       </c>
@@ -17638,7 +17645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>118</v>
       </c>
@@ -17667,7 +17674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>120</v>
       </c>
@@ -17696,7 +17703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>122</v>
       </c>
@@ -17725,7 +17732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>124</v>
       </c>
@@ -17754,7 +17761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>140</v>
       </c>
@@ -17783,7 +17790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>126</v>
       </c>
@@ -17812,7 +17819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>128</v>
       </c>
@@ -17841,7 +17848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>198</v>
       </c>
@@ -18716,7 +18723,7 @@
         <v>427</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>97</v>
@@ -20490,7 +20497,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -20501,11 +20508,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20513,12 +20520,13 @@
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="76.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="76.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>327</v>
       </c>
@@ -20529,25 +20537,22 @@
         <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>432</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>437</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>438</v>
+        <v>328</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>328</v>
+        <v>482</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>329</v>
       </c>
@@ -20558,25 +20563,22 @@
         <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="H2" t="s">
-        <v>441</v>
-      </c>
-      <c r="I2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>330</v>
       </c>
@@ -20586,20 +20588,17 @@
       <c r="C3" t="s">
         <v>333</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" t="s">
+        <v>330</v>
       </c>
       <c r="E3" t="s">
-        <v>330</v>
-      </c>
-      <c r="F3" t="s">
-        <v>436</v>
-      </c>
-      <c r="I3" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+      <c r="H3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -20609,20 +20608,17 @@
       <c r="C4" t="s">
         <v>93</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="41" t="s">
+      <c r="D4" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="F4" t="s">
-        <v>437</v>
-      </c>
-      <c r="I4" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>436</v>
+      </c>
+      <c r="H4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>334</v>
       </c>
@@ -20632,20 +20628,17 @@
       <c r="C5" t="s">
         <v>110</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>451</v>
-      </c>
-      <c r="F5" t="s">
-        <v>436</v>
-      </c>
-      <c r="I5" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="41" t="s">
+        <v>448</v>
+      </c>
+      <c r="E5" t="s">
+        <v>435</v>
+      </c>
+      <c r="H5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>334</v>
       </c>
@@ -20655,20 +20648,17 @@
       <c r="C6" t="s">
         <v>118</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>452</v>
-      </c>
-      <c r="F6" t="s">
-        <v>436</v>
-      </c>
-      <c r="I6" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="41" t="s">
+        <v>449</v>
+      </c>
+      <c r="E6" t="s">
+        <v>435</v>
+      </c>
+      <c r="H6" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>334</v>
       </c>
@@ -20678,20 +20668,17 @@
       <c r="C7" t="s">
         <v>120</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="41" t="s">
+      <c r="D7" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="F7" t="s">
-        <v>436</v>
-      </c>
-      <c r="I7" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>435</v>
+      </c>
+      <c r="H7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>336</v>
       </c>
@@ -20701,20 +20688,17 @@
       <c r="C8" t="s">
         <v>113</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>453</v>
-      </c>
-      <c r="F8" t="s">
-        <v>435</v>
-      </c>
-      <c r="I8" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="41" t="s">
+        <v>450</v>
+      </c>
+      <c r="E8" t="s">
+        <v>434</v>
+      </c>
+      <c r="H8" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>336</v>
       </c>
@@ -20724,20 +20708,17 @@
       <c r="C9" t="s">
         <v>115</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="41" t="s">
-        <v>454</v>
-      </c>
-      <c r="F9" t="s">
-        <v>435</v>
-      </c>
-      <c r="I9" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="41" t="s">
+        <v>451</v>
+      </c>
+      <c r="E9" t="s">
+        <v>434</v>
+      </c>
+      <c r="H9" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>336</v>
       </c>
@@ -20747,20 +20728,17 @@
       <c r="C10" t="s">
         <v>122</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="41" t="s">
+      <c r="D10" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="F10" t="s">
-        <v>437</v>
-      </c>
-      <c r="I10" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>436</v>
+      </c>
+      <c r="H10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>336</v>
       </c>
@@ -20770,20 +20748,17 @@
       <c r="C11" t="s">
         <v>198</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="41" t="s">
+      <c r="D11" s="41" t="s">
         <v>197</v>
       </c>
-      <c r="F11" t="s">
-        <v>437</v>
-      </c>
-      <c r="I11" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>436</v>
+      </c>
+      <c r="H11" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>336</v>
       </c>
@@ -20793,20 +20768,17 @@
       <c r="C12" t="s">
         <v>140</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>455</v>
-      </c>
-      <c r="F12" t="s">
-        <v>435</v>
-      </c>
-      <c r="I12" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="41" t="s">
+        <v>452</v>
+      </c>
+      <c r="E12" t="s">
+        <v>434</v>
+      </c>
+      <c r="H12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>336</v>
       </c>
@@ -20816,20 +20788,17 @@
       <c r="C13" t="s">
         <v>124</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>456</v>
-      </c>
-      <c r="F13" t="s">
-        <v>437</v>
-      </c>
-      <c r="I13" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="41" t="s">
+        <v>453</v>
+      </c>
+      <c r="E13" t="s">
+        <v>436</v>
+      </c>
+      <c r="H13" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>336</v>
       </c>
@@ -20839,20 +20808,17 @@
       <c r="C14" t="s">
         <v>128</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="41" t="s">
-        <v>457</v>
-      </c>
-      <c r="F14" t="s">
-        <v>434</v>
-      </c>
-      <c r="I14" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="41" t="s">
+        <v>454</v>
+      </c>
+      <c r="E14" t="s">
+        <v>433</v>
+      </c>
+      <c r="H14" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>336</v>
       </c>
@@ -20862,20 +20828,17 @@
       <c r="C15" t="s">
         <v>126</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>458</v>
-      </c>
-      <c r="F15" t="s">
-        <v>435</v>
-      </c>
-      <c r="I15" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="41" t="s">
+        <v>455</v>
+      </c>
+      <c r="E15" t="s">
+        <v>434</v>
+      </c>
+      <c r="H15" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>337</v>
       </c>
@@ -20885,20 +20848,17 @@
       <c r="C16" t="s">
         <v>313</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>459</v>
-      </c>
-      <c r="F16" t="s">
-        <v>437</v>
-      </c>
-      <c r="I16" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="41" t="s">
+        <v>456</v>
+      </c>
+      <c r="E16" t="s">
+        <v>436</v>
+      </c>
+      <c r="H16" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>337</v>
       </c>
@@ -20908,20 +20868,17 @@
       <c r="C17" t="s">
         <v>314</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>460</v>
-      </c>
-      <c r="F17" t="s">
-        <v>437</v>
-      </c>
-      <c r="I17" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="41" t="s">
+        <v>457</v>
+      </c>
+      <c r="E17" t="s">
+        <v>436</v>
+      </c>
+      <c r="H17" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>337</v>
       </c>
@@ -20931,20 +20888,17 @@
       <c r="C18" t="s">
         <v>315</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="41" t="s">
-        <v>461</v>
-      </c>
-      <c r="F18" t="s">
-        <v>437</v>
-      </c>
-      <c r="I18" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="41" t="s">
+        <v>458</v>
+      </c>
+      <c r="E18" t="s">
+        <v>436</v>
+      </c>
+      <c r="H18" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>337</v>
       </c>
@@ -20954,20 +20908,17 @@
       <c r="C19" t="s">
         <v>431</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>462</v>
-      </c>
-      <c r="F19" t="s">
-        <v>435</v>
-      </c>
-      <c r="I19" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="41" t="s">
+        <v>459</v>
+      </c>
+      <c r="E19" t="s">
+        <v>434</v>
+      </c>
+      <c r="H19" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>337</v>
       </c>
@@ -20977,20 +20928,17 @@
       <c r="C20" t="s">
         <v>316</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>463</v>
-      </c>
-      <c r="F20" t="s">
-        <v>437</v>
-      </c>
-      <c r="I20" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="41" t="s">
+        <v>460</v>
+      </c>
+      <c r="E20" t="s">
+        <v>436</v>
+      </c>
+      <c r="H20" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>337</v>
       </c>
@@ -21000,20 +20948,17 @@
       <c r="C21" t="s">
         <v>317</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>464</v>
-      </c>
-      <c r="F21" t="s">
-        <v>437</v>
-      </c>
-      <c r="I21" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="41" t="s">
+        <v>461</v>
+      </c>
+      <c r="E21" t="s">
+        <v>436</v>
+      </c>
+      <c r="H21" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>337</v>
       </c>
@@ -21023,20 +20968,17 @@
       <c r="C22" t="s">
         <v>318</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>465</v>
-      </c>
-      <c r="F22" t="s">
-        <v>437</v>
-      </c>
-      <c r="I22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="41" t="s">
+        <v>462</v>
+      </c>
+      <c r="E22" t="s">
+        <v>436</v>
+      </c>
+      <c r="H22" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>337</v>
       </c>
@@ -21046,20 +20988,17 @@
       <c r="C23" t="s">
         <v>319</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="41" t="s">
-        <v>466</v>
-      </c>
-      <c r="F23" t="s">
-        <v>435</v>
-      </c>
-      <c r="I23" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="41" t="s">
+        <v>463</v>
+      </c>
+      <c r="E23" t="s">
+        <v>434</v>
+      </c>
+      <c r="H23" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>337</v>
       </c>
@@ -21069,20 +21008,17 @@
       <c r="C24" t="s">
         <v>320</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="41" t="s">
-        <v>467</v>
-      </c>
-      <c r="F24" t="s">
-        <v>435</v>
-      </c>
-      <c r="I24" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="41" t="s">
+        <v>464</v>
+      </c>
+      <c r="E24" t="s">
+        <v>434</v>
+      </c>
+      <c r="H24" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>337</v>
       </c>
@@ -21092,20 +21028,17 @@
       <c r="C25" t="s">
         <v>321</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" s="41" t="s">
-        <v>468</v>
-      </c>
-      <c r="F25" t="s">
-        <v>435</v>
-      </c>
-      <c r="I25" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="41" t="s">
+        <v>465</v>
+      </c>
+      <c r="E25" t="s">
+        <v>434</v>
+      </c>
+      <c r="H25" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>337</v>
       </c>
@@ -21115,20 +21048,17 @@
       <c r="C26" t="s">
         <v>322</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" s="41" t="s">
-        <v>469</v>
-      </c>
-      <c r="F26" t="s">
-        <v>435</v>
-      </c>
-      <c r="I26" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="41" t="s">
+        <v>466</v>
+      </c>
+      <c r="E26" t="s">
+        <v>434</v>
+      </c>
+      <c r="H26" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>337</v>
       </c>
@@ -21138,20 +21068,17 @@
       <c r="C27" t="s">
         <v>323</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" s="41" t="s">
-        <v>470</v>
-      </c>
-      <c r="F27" t="s">
-        <v>435</v>
-      </c>
-      <c r="I27" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="41" t="s">
+        <v>467</v>
+      </c>
+      <c r="E27" t="s">
+        <v>434</v>
+      </c>
+      <c r="H27" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>338</v>
       </c>
@@ -21161,20 +21088,17 @@
       <c r="C28" t="s">
         <v>164</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28" s="41" t="s">
+      <c r="D28" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="F28" t="s">
-        <v>437</v>
-      </c>
-      <c r="I28" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>436</v>
+      </c>
+      <c r="H28" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>338</v>
       </c>
@@ -21184,20 +21108,17 @@
       <c r="C29" t="s">
         <v>168</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29" s="41" t="s">
+      <c r="D29" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="F29" t="s">
-        <v>437</v>
-      </c>
-      <c r="I29" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>436</v>
+      </c>
+      <c r="H29" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>338</v>
       </c>
@@ -21207,20 +21128,17 @@
       <c r="C30" t="s">
         <v>171</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="41" t="s">
-        <v>471</v>
-      </c>
-      <c r="F30" t="s">
-        <v>435</v>
-      </c>
-      <c r="I30" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="41" t="s">
+        <v>468</v>
+      </c>
+      <c r="E30" t="s">
+        <v>434</v>
+      </c>
+      <c r="H30" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>338</v>
       </c>
@@ -21230,20 +21148,17 @@
       <c r="C31" t="s">
         <v>173</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" s="41" t="s">
-        <v>472</v>
-      </c>
-      <c r="F31" t="s">
-        <v>435</v>
-      </c>
-      <c r="I31" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="41" t="s">
+        <v>469</v>
+      </c>
+      <c r="E31" t="s">
+        <v>434</v>
+      </c>
+      <c r="H31" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>338</v>
       </c>
@@ -21253,20 +21168,17 @@
       <c r="C32" t="s">
         <v>421</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32" s="41" t="s">
+      <c r="D32" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="F32" t="s">
-        <v>437</v>
-      </c>
-      <c r="I32" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>436</v>
+      </c>
+      <c r="H32" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>339</v>
       </c>
@@ -21276,20 +21188,17 @@
       <c r="C33" t="s">
         <v>143</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33" s="41" t="s">
-        <v>473</v>
-      </c>
-      <c r="F33" t="s">
-        <v>437</v>
-      </c>
-      <c r="I33" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="41" t="s">
+        <v>470</v>
+      </c>
+      <c r="E33" t="s">
+        <v>436</v>
+      </c>
+      <c r="H33" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>339</v>
       </c>
@@ -21299,20 +21208,17 @@
       <c r="C34" t="s">
         <v>148</v>
       </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34" s="41" t="s">
-        <v>474</v>
-      </c>
-      <c r="F34" t="s">
-        <v>437</v>
-      </c>
-      <c r="I34" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="41" t="s">
+        <v>471</v>
+      </c>
+      <c r="E34" t="s">
+        <v>436</v>
+      </c>
+      <c r="H34" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>339</v>
       </c>
@@ -21322,20 +21228,17 @@
       <c r="C35" t="s">
         <v>151</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35" s="41" t="s">
-        <v>475</v>
-      </c>
-      <c r="F35" t="s">
-        <v>437</v>
-      </c>
-      <c r="I35" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="41" t="s">
+        <v>472</v>
+      </c>
+      <c r="E35" t="s">
+        <v>436</v>
+      </c>
+      <c r="H35" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>339</v>
       </c>
@@ -21345,20 +21248,17 @@
       <c r="C36" t="s">
         <v>430</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" s="41" t="s">
-        <v>476</v>
-      </c>
-      <c r="F36" t="s">
-        <v>435</v>
-      </c>
-      <c r="I36" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D36" s="41" t="s">
+        <v>473</v>
+      </c>
+      <c r="E36" t="s">
+        <v>434</v>
+      </c>
+      <c r="H36" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>339</v>
       </c>
@@ -21368,20 +21268,17 @@
       <c r="C37" t="s">
         <v>159</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="41" t="s">
-        <v>477</v>
-      </c>
-      <c r="F37" t="s">
-        <v>435</v>
-      </c>
-      <c r="I37" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D37" s="41" t="s">
+        <v>474</v>
+      </c>
+      <c r="E37" t="s">
+        <v>434</v>
+      </c>
+      <c r="H37" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>339</v>
       </c>
@@ -21391,20 +21288,17 @@
       <c r="C38" t="s">
         <v>162</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" s="41" t="s">
-        <v>478</v>
-      </c>
-      <c r="F38" t="s">
-        <v>435</v>
-      </c>
-      <c r="I38" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D38" s="41" t="s">
+        <v>475</v>
+      </c>
+      <c r="E38" t="s">
+        <v>434</v>
+      </c>
+      <c r="H38" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>339</v>
       </c>
@@ -21414,20 +21308,17 @@
       <c r="C39" t="s">
         <v>131</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" s="41" t="s">
-        <v>479</v>
-      </c>
-      <c r="F39" t="s">
-        <v>435</v>
-      </c>
-      <c r="I39" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D39" s="41" t="s">
+        <v>476</v>
+      </c>
+      <c r="E39" t="s">
+        <v>434</v>
+      </c>
+      <c r="H39" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>340</v>
       </c>
@@ -21437,20 +21328,23 @@
       <c r="C40" t="s">
         <v>154</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40" s="41" t="s">
-        <v>480</v>
+      <c r="D40" s="41" t="s">
+        <v>477</v>
+      </c>
+      <c r="E40" t="s">
+        <v>436</v>
       </c>
       <c r="F40" t="s">
-        <v>437</v>
-      </c>
-      <c r="I40" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+      <c r="G40" t="s">
+        <v>440</v>
+      </c>
+      <c r="H40" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>340</v>
       </c>
@@ -21460,20 +21354,23 @@
       <c r="C41" t="s">
         <v>138</v>
       </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" s="41" t="s">
-        <v>482</v>
+      <c r="D41" s="41" t="s">
+        <v>479</v>
+      </c>
+      <c r="E41" t="s">
+        <v>434</v>
       </c>
       <c r="F41" t="s">
-        <v>435</v>
-      </c>
-      <c r="I41" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+      <c r="G41" t="s">
+        <v>440</v>
+      </c>
+      <c r="H41" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>340</v>
       </c>
@@ -21483,20 +21380,23 @@
       <c r="C42" t="s">
         <v>136</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42" s="41" t="s">
+      <c r="D42" s="41" t="s">
+        <v>478</v>
+      </c>
+      <c r="E42" t="s">
+        <v>436</v>
+      </c>
+      <c r="F42" t="s">
         <v>481</v>
       </c>
-      <c r="F42" t="s">
-        <v>437</v>
-      </c>
-      <c r="I42" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>480</v>
+      </c>
+      <c r="H42" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>341</v>
       </c>
@@ -21506,23 +21406,23 @@
       <c r="C43" t="s">
         <v>324</v>
       </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43" s="41" t="s">
-        <v>444</v>
+      <c r="D43" s="41" t="s">
+        <v>441</v>
+      </c>
+      <c r="E43" t="s">
+        <v>436</v>
       </c>
       <c r="F43" t="s">
-        <v>437</v>
+        <v>428</v>
+      </c>
+      <c r="G43" t="s">
+        <v>440</v>
       </c>
       <c r="H43" t="s">
-        <v>443</v>
-      </c>
-      <c r="I43" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>341</v>
       </c>
@@ -21532,23 +21432,23 @@
       <c r="C44" t="s">
         <v>429</v>
       </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44" s="41" t="s">
-        <v>445</v>
+      <c r="D44" s="41" t="s">
+        <v>442</v>
+      </c>
+      <c r="E44" t="s">
+        <v>436</v>
       </c>
       <c r="F44" t="s">
-        <v>437</v>
+        <v>428</v>
+      </c>
+      <c r="G44" t="s">
+        <v>440</v>
       </c>
       <c r="H44" t="s">
-        <v>443</v>
-      </c>
-      <c r="I44" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>341</v>
       </c>
@@ -21558,23 +21458,23 @@
       <c r="C45" t="s">
         <v>325</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45" s="41" t="s">
-        <v>446</v>
+      <c r="D45" s="41" t="s">
+        <v>443</v>
+      </c>
+      <c r="E45" t="s">
+        <v>436</v>
       </c>
       <c r="F45" t="s">
-        <v>437</v>
+        <v>428</v>
+      </c>
+      <c r="G45" t="s">
+        <v>440</v>
       </c>
       <c r="H45" t="s">
-        <v>443</v>
-      </c>
-      <c r="I45" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>341</v>
       </c>
@@ -21584,23 +21484,23 @@
       <c r="C46" t="s">
         <v>326</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46" s="41" t="s">
-        <v>447</v>
+      <c r="D46" s="41" t="s">
+        <v>444</v>
+      </c>
+      <c r="E46" t="s">
+        <v>436</v>
       </c>
       <c r="F46" t="s">
-        <v>437</v>
+        <v>428</v>
+      </c>
+      <c r="G46" t="s">
+        <v>440</v>
       </c>
       <c r="H46" t="s">
-        <v>443</v>
-      </c>
-      <c r="I46" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>341</v>
       </c>
@@ -21610,23 +21510,23 @@
       <c r="C47" t="s">
         <v>108</v>
       </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47" s="41" t="s">
-        <v>448</v>
+      <c r="D47" s="41" t="s">
+        <v>445</v>
+      </c>
+      <c r="E47" t="s">
+        <v>436</v>
       </c>
       <c r="F47" t="s">
-        <v>437</v>
+        <v>428</v>
+      </c>
+      <c r="G47" t="s">
+        <v>439</v>
       </c>
       <c r="H47" t="s">
-        <v>442</v>
-      </c>
-      <c r="I47" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>341</v>
       </c>
@@ -21636,23 +21536,23 @@
       <c r="C48" t="s">
         <v>106</v>
       </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48" s="41" t="s">
-        <v>449</v>
+      <c r="D48" s="41" t="s">
+        <v>446</v>
+      </c>
+      <c r="E48" t="s">
+        <v>436</v>
       </c>
       <c r="F48" t="s">
-        <v>437</v>
+        <v>428</v>
+      </c>
+      <c r="G48" t="s">
+        <v>440</v>
       </c>
       <c r="H48" t="s">
-        <v>443</v>
-      </c>
-      <c r="I48" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>341</v>
       </c>
@@ -21662,20 +21562,20 @@
       <c r="C49" t="s">
         <v>101</v>
       </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49" s="41" t="s">
-        <v>450</v>
+      <c r="D49" s="41" t="s">
+        <v>447</v>
+      </c>
+      <c r="E49" t="s">
+        <v>436</v>
       </c>
       <c r="F49" t="s">
-        <v>437</v>
+        <v>428</v>
+      </c>
+      <c r="G49" t="s">
+        <v>440</v>
       </c>
       <c r="H49" t="s">
-        <v>443</v>
-      </c>
-      <c r="I49" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -21689,7 +21589,7 @@
   <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21697,7 +21597,7 @@
     <col min="1" max="1" width="62.5703125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -21719,11 +21619,11 @@
       <c r="F1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>395</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -21745,12 +21645,12 @@
       <c r="F2" s="11">
         <v>1.4E-3</v>
       </c>
-      <c r="G2" s="20" t="b">
+      <c r="G2" t="s">
+        <v>435</v>
+      </c>
+      <c r="H2" s="20" t="b">
         <f>AND(D2&gt;=E2, D2&lt;=F2)</f>
         <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -21772,12 +21672,12 @@
       <c r="F3" s="11">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="G3" s="20" t="b">
-        <f t="shared" ref="G3:G59" si="0">AND(D3&gt;=E3, D3&lt;=F3)</f>
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>436</v>
+      <c r="G3" t="s">
+        <v>435</v>
+      </c>
+      <c r="H3" s="20" t="b">
+        <f>AND(D3&gt;=E3, D3&lt;=F3)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -21799,12 +21699,12 @@
       <c r="F4" s="11">
         <v>2.8E-3</v>
       </c>
-      <c r="G4" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>436</v>
+      <c r="G4" t="s">
+        <v>435</v>
+      </c>
+      <c r="H4" s="20" t="b">
+        <f>AND(D4&gt;=E4, D4&lt;=F4)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -21826,12 +21726,12 @@
       <c r="F5" s="11">
         <v>1.8599999999999998E-2</v>
       </c>
-      <c r="G5" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>436</v>
+      <c r="G5" t="s">
+        <v>435</v>
+      </c>
+      <c r="H5" s="20" t="b">
+        <f>AND(D5&gt;=E5, D5&lt;=F5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -21853,12 +21753,12 @@
       <c r="F6" s="11">
         <v>2.4E-2</v>
       </c>
-      <c r="G6" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>436</v>
+      <c r="G6" t="s">
+        <v>435</v>
+      </c>
+      <c r="H6" s="20" t="b">
+        <f>AND(D6&gt;=E6, D6&lt;=F6)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -21880,12 +21780,12 @@
       <c r="F7" s="11">
         <v>0.44</v>
       </c>
-      <c r="G7" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>436</v>
+      <c r="G7" t="s">
+        <v>435</v>
+      </c>
+      <c r="H7" s="20" t="b">
+        <f>AND(D7&gt;=E7, D7&lt;=F7)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -21907,12 +21807,12 @@
       <c r="F8" s="11">
         <v>0.27</v>
       </c>
-      <c r="G8" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>436</v>
+      <c r="G8" t="s">
+        <v>435</v>
+      </c>
+      <c r="H8" s="20" t="b">
+        <f>AND(D8&gt;=E8, D8&lt;=F8)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -21934,12 +21834,12 @@
       <c r="F9">
         <v>9.1</v>
       </c>
-      <c r="G9" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>434</v>
+      <c r="G9" t="s">
+        <v>433</v>
+      </c>
+      <c r="H9" s="20" t="b">
+        <f>AND(D9&gt;=E9, D9&lt;=F9)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -21961,12 +21861,12 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
-        <v>434</v>
+      <c r="G10" t="s">
+        <v>433</v>
+      </c>
+      <c r="H10" s="20" t="b">
+        <f>AND(D10&gt;=E10, D10&lt;=F10)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -21988,12 +21888,12 @@
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>434</v>
+      <c r="G11" t="s">
+        <v>433</v>
+      </c>
+      <c r="H11" s="20" t="b">
+        <f>AND(D11&gt;=E11, D11&lt;=F11)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -22015,12 +21915,12 @@
       <c r="F12">
         <v>1</v>
       </c>
-      <c r="G12" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>434</v>
+      <c r="G12" t="s">
+        <v>433</v>
+      </c>
+      <c r="H12" s="20" t="b">
+        <f>AND(D12&gt;=E12, D12&lt;=F12)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -22042,12 +21942,12 @@
       <c r="F13">
         <v>6.92</v>
       </c>
-      <c r="G13" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>434</v>
+      <c r="G13" t="s">
+        <v>433</v>
+      </c>
+      <c r="H13" s="20" t="b">
+        <f>AND(D13&gt;=E13, D13&lt;=F13)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -22069,12 +21969,12 @@
       <c r="F14">
         <v>12.08</v>
       </c>
-      <c r="G14" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>434</v>
+      <c r="G14" t="s">
+        <v>433</v>
+      </c>
+      <c r="H14" s="20" t="b">
+        <f>AND(D14&gt;=E14, D14&lt;=F14)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -22096,12 +21996,12 @@
       <c r="F15">
         <v>0.5</v>
       </c>
-      <c r="G15" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>434</v>
+      <c r="G15" t="s">
+        <v>433</v>
+      </c>
+      <c r="H15" s="20" t="b">
+        <f>AND(D15&gt;=E15, D15&lt;=F15)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -22123,12 +22023,12 @@
       <c r="F16">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G16" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>434</v>
+      <c r="G16" t="s">
+        <v>433</v>
+      </c>
+      <c r="H16" s="20" t="b">
+        <f>AND(D16&gt;=E16, D16&lt;=F16)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -22150,12 +22050,12 @@
       <c r="F17">
         <v>3.16</v>
       </c>
-      <c r="G17" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>434</v>
+      <c r="G17" t="s">
+        <v>433</v>
+      </c>
+      <c r="H17" s="20" t="b">
+        <f>AND(D17&gt;=E17, D17&lt;=F17)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -22177,12 +22077,12 @@
       <c r="F18">
         <v>4</v>
       </c>
-      <c r="G18" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>434</v>
+      <c r="G18" t="s">
+        <v>433</v>
+      </c>
+      <c r="H18" s="20" t="b">
+        <f>AND(D18&gt;=E18, D18&lt;=F18)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -22204,12 +22104,12 @@
       <c r="F19">
         <v>2.25</v>
       </c>
-      <c r="G19" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>434</v>
+      <c r="G19" t="s">
+        <v>433</v>
+      </c>
+      <c r="H19" s="20" t="b">
+        <f>AND(D19&gt;=E19, D19&lt;=F19)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -22231,12 +22131,12 @@
       <c r="F20">
         <v>7.28</v>
       </c>
-      <c r="G20" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H20" t="s">
-        <v>434</v>
+      <c r="G20" t="s">
+        <v>433</v>
+      </c>
+      <c r="H20" s="20" t="b">
+        <f>AND(D20&gt;=E20, D20&lt;=F20)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -22258,12 +22158,12 @@
       <c r="F21">
         <v>3.42</v>
       </c>
-      <c r="G21" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>434</v>
+      <c r="G21" t="s">
+        <v>433</v>
+      </c>
+      <c r="H21" s="20" t="b">
+        <f>AND(D21&gt;=E21, D21&lt;=F21)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -22285,12 +22185,12 @@
       <c r="F22">
         <v>3.58</v>
       </c>
-      <c r="G22" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>434</v>
+      <c r="G22" t="s">
+        <v>433</v>
+      </c>
+      <c r="H22" s="20" t="b">
+        <f>AND(D22&gt;=E22, D22&lt;=F22)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -22312,12 +22212,12 @@
       <c r="F23">
         <v>0.94</v>
       </c>
-      <c r="G23" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>434</v>
+      <c r="G23" t="s">
+        <v>433</v>
+      </c>
+      <c r="H23" s="20" t="b">
+        <f>AND(D23&gt;=E23, D23&lt;=F23)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -22339,12 +22239,12 @@
       <c r="F24">
         <v>0.3</v>
       </c>
-      <c r="G24" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
-        <v>434</v>
+      <c r="G24" t="s">
+        <v>433</v>
+      </c>
+      <c r="H24" s="20" t="b">
+        <f>AND(D24&gt;=E24, D24&lt;=F24)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -22366,12 +22266,12 @@
       <c r="F25">
         <v>2.5</v>
       </c>
-      <c r="G25" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>434</v>
+      <c r="G25" t="s">
+        <v>433</v>
+      </c>
+      <c r="H25" s="20" t="b">
+        <f>AND(D25&gt;=E25, D25&lt;=F25)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -22393,12 +22293,12 @@
       <c r="F26" s="11">
         <v>0.27500000000000002</v>
       </c>
-      <c r="G26" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H26" t="s">
-        <v>435</v>
+      <c r="G26" t="s">
+        <v>434</v>
+      </c>
+      <c r="H26" s="20" t="b">
+        <f>AND(D26&gt;=E26, D26&lt;=F26)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -22420,12 +22320,12 @@
       <c r="F27" s="11">
         <v>0.88500000000000001</v>
       </c>
-      <c r="G27" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H27" t="s">
-        <v>435</v>
+      <c r="G27" t="s">
+        <v>434</v>
+      </c>
+      <c r="H27" s="20" t="b">
+        <f>AND(D27&gt;=E27, D27&lt;=F27)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -22447,12 +22347,12 @@
       <c r="F28" s="11">
         <v>0.87</v>
       </c>
-      <c r="G28" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H28" t="s">
-        <v>435</v>
+      <c r="G28" t="s">
+        <v>434</v>
+      </c>
+      <c r="H28" s="20" t="b">
+        <f>AND(D28&gt;=E28, D28&lt;=F28)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -22474,12 +22374,12 @@
       <c r="F29" s="11">
         <v>0.82699999999999996</v>
       </c>
-      <c r="G29" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
-        <v>435</v>
+      <c r="G29" t="s">
+        <v>434</v>
+      </c>
+      <c r="H29" s="20" t="b">
+        <f>AND(D29&gt;=E29, D29&lt;=F29)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -22501,12 +22401,12 @@
       <c r="F30" s="11">
         <v>0.86899999999999999</v>
       </c>
-      <c r="G30" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H30" t="s">
-        <v>435</v>
+      <c r="G30" t="s">
+        <v>434</v>
+      </c>
+      <c r="H30" s="20" t="b">
+        <f>AND(D30&gt;=E30, D30&lt;=F30)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -22528,12 +22428,12 @@
       <c r="F31" s="11">
         <v>0.68600000000000005</v>
       </c>
-      <c r="G31" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H31" t="s">
-        <v>435</v>
+      <c r="G31" t="s">
+        <v>434</v>
+      </c>
+      <c r="H31" s="20" t="b">
+        <f>AND(D31&gt;=E31, D31&lt;=F31)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -22555,12 +22455,12 @@
       <c r="F32" s="11">
         <v>0.72299999999999998</v>
       </c>
-      <c r="G32" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H32" t="s">
-        <v>435</v>
+      <c r="G32" t="s">
+        <v>434</v>
+      </c>
+      <c r="H32" s="20" t="b">
+        <f>AND(D32&gt;=E32, D32&lt;=F32)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -22582,12 +22482,12 @@
       <c r="F33" s="11">
         <v>0.56299999999999994</v>
       </c>
-      <c r="G33" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H33" t="s">
-        <v>435</v>
+      <c r="G33" t="s">
+        <v>434</v>
+      </c>
+      <c r="H33" s="20" t="b">
+        <f>AND(D33&gt;=E33, D33&lt;=F33)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -22609,12 +22509,12 @@
       <c r="F34" s="11">
         <v>0.26</v>
       </c>
-      <c r="G34" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
-        <v>435</v>
+      <c r="G34" t="s">
+        <v>434</v>
+      </c>
+      <c r="H34" s="20" t="b">
+        <f>AND(D34&gt;=E34, D34&lt;=F34)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -22636,12 +22536,12 @@
       <c r="F35" s="11">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="G35" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H35" t="s">
-        <v>436</v>
+      <c r="G35" t="s">
+        <v>435</v>
+      </c>
+      <c r="H35" s="20" t="b">
+        <f>AND(D35&gt;=E35, D35&lt;=F35)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -22663,12 +22563,12 @@
       <c r="F36" s="11">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="G36" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H36" t="s">
-        <v>436</v>
+      <c r="G36" t="s">
+        <v>435</v>
+      </c>
+      <c r="H36" s="20" t="b">
+        <f>AND(D36&gt;=E36, D36&lt;=F36)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -22690,12 +22590,12 @@
       <c r="F37" s="11">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="G37" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
-        <v>436</v>
+      <c r="G37" t="s">
+        <v>435</v>
+      </c>
+      <c r="H37" s="20" t="b">
+        <f>AND(D37&gt;=E37, D37&lt;=F37)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -22717,12 +22617,12 @@
       <c r="F38" s="11">
         <v>1.01E-2</v>
       </c>
-      <c r="G38" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H38" t="s">
-        <v>436</v>
+      <c r="G38" t="s">
+        <v>435</v>
+      </c>
+      <c r="H38" s="20" t="b">
+        <f>AND(D38&gt;=E38, D38&lt;=F38)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -22744,12 +22644,12 @@
       <c r="F39" s="11">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="G39" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
-        <v>436</v>
+      <c r="G39" t="s">
+        <v>435</v>
+      </c>
+      <c r="H39" s="20" t="b">
+        <f>AND(D39&gt;=E39, D39&lt;=F39)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -22771,12 +22671,12 @@
       <c r="F40" s="11">
         <v>0.432</v>
       </c>
-      <c r="G40" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H40" t="s">
-        <v>436</v>
+      <c r="G40" t="s">
+        <v>435</v>
+      </c>
+      <c r="H40" s="20" t="b">
+        <f>AND(D40&gt;=E40, D40&lt;=F40)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -22798,12 +22698,12 @@
       <c r="F41" s="11">
         <v>0.3</v>
       </c>
-      <c r="G41" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H41" t="s">
-        <v>435</v>
+      <c r="G41" t="s">
+        <v>434</v>
+      </c>
+      <c r="H41" s="20" t="b">
+        <f>AND(D41&gt;=E41, D41&lt;=F41)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -22825,12 +22725,12 @@
       <c r="F42" s="11">
         <v>0.8417</v>
       </c>
-      <c r="G42" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H42" t="s">
-        <v>435</v>
+      <c r="G42" t="s">
+        <v>434</v>
+      </c>
+      <c r="H42" s="20" t="b">
+        <f>AND(D42&gt;=E42, D42&lt;=F42)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -22852,12 +22752,12 @@
       <c r="F43" s="11">
         <v>3.71</v>
       </c>
-      <c r="G43" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H43" t="s">
-        <v>435</v>
+      <c r="G43" t="s">
+        <v>434</v>
+      </c>
+      <c r="H43" s="20" t="b">
+        <f>AND(D43&gt;=E43, D43&lt;=F43)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -22879,12 +22779,12 @@
       <c r="F44" s="13">
         <v>0.98</v>
       </c>
-      <c r="G44" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H44" t="s">
-        <v>435</v>
+      <c r="G44" t="s">
+        <v>434</v>
+      </c>
+      <c r="H44" s="20" t="b">
+        <f>AND(D44&gt;=E44, D44&lt;=F44)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -22906,12 +22806,12 @@
       <c r="F45" s="13">
         <v>0.67</v>
       </c>
-      <c r="G45" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H45" t="s">
-        <v>435</v>
+      <c r="G45" t="s">
+        <v>434</v>
+      </c>
+      <c r="H45" s="20" t="b">
+        <f>AND(D45&gt;=E45, D45&lt;=F45)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -22933,12 +22833,12 @@
       <c r="F46" s="13">
         <v>0.68</v>
       </c>
-      <c r="G46" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H46" t="s">
-        <v>435</v>
+      <c r="G46" t="s">
+        <v>434</v>
+      </c>
+      <c r="H46" s="20" t="b">
+        <f>AND(D46&gt;=E46, D46&lt;=F46)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -22960,12 +22860,12 @@
       <c r="F47" s="13">
         <v>5.19</v>
       </c>
-      <c r="G47" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H47" t="s">
-        <v>435</v>
+      <c r="G47" t="s">
+        <v>434</v>
+      </c>
+      <c r="H47" s="20" t="b">
+        <f>AND(D47&gt;=E47, D47&lt;=F47)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -22987,12 +22887,12 @@
       <c r="F48" s="13">
         <v>0.68</v>
       </c>
-      <c r="G48" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H48" t="s">
-        <v>435</v>
+      <c r="G48" t="s">
+        <v>434</v>
+      </c>
+      <c r="H48" s="20" t="b">
+        <f>AND(D48&gt;=E48, D48&lt;=F48)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -23014,12 +22914,12 @@
       <c r="F49" s="13">
         <v>0.93</v>
       </c>
-      <c r="G49" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H49" t="s">
-        <v>435</v>
+      <c r="G49" t="s">
+        <v>434</v>
+      </c>
+      <c r="H49" s="20" t="b">
+        <f>AND(D49&gt;=E49, D49&lt;=F49)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -23041,12 +22941,12 @@
       <c r="F50" s="13">
         <v>0.8</v>
       </c>
-      <c r="G50" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H50" t="s">
-        <v>435</v>
+      <c r="G50" t="s">
+        <v>434</v>
+      </c>
+      <c r="H50" s="20" t="b">
+        <f>AND(D50&gt;=E50, D50&lt;=F50)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -23068,12 +22968,12 @@
       <c r="F51" s="13">
         <v>0.8</v>
       </c>
-      <c r="G51" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H51" t="s">
-        <v>435</v>
+      <c r="G51" t="s">
+        <v>434</v>
+      </c>
+      <c r="H51" s="20" t="b">
+        <f>AND(D51&gt;=E51, D51&lt;=F51)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -23095,12 +22995,12 @@
       <c r="F52" s="13">
         <v>0.95</v>
       </c>
-      <c r="G52" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H52" t="s">
-        <v>435</v>
+      <c r="G52" t="s">
+        <v>434</v>
+      </c>
+      <c r="H52" s="20" t="b">
+        <f>AND(D52&gt;=E52, D52&lt;=F52)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -23122,12 +23022,12 @@
       <c r="F53">
         <v>0.21</v>
       </c>
-      <c r="G53" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H53" t="s">
-        <v>434</v>
+      <c r="G53" t="s">
+        <v>433</v>
+      </c>
+      <c r="H53" s="20" t="b">
+        <f>AND(D53&gt;=E53, D53&lt;=F53)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -23149,12 +23049,12 @@
       <c r="F54">
         <v>0.01</v>
       </c>
-      <c r="G54" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H54" t="s">
-        <v>434</v>
+      <c r="G54" t="s">
+        <v>433</v>
+      </c>
+      <c r="H54" s="20" t="b">
+        <f>AND(D54&gt;=E54, D54&lt;=F54)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -23176,12 +23076,12 @@
       <c r="F55">
         <v>0.03</v>
       </c>
-      <c r="G55" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H55" t="s">
-        <v>434</v>
+      <c r="G55" t="s">
+        <v>433</v>
+      </c>
+      <c r="H55" s="20" t="b">
+        <f>AND(D55&gt;=E55, D55&lt;=F55)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -23203,12 +23103,12 @@
       <c r="F56">
         <v>0.09</v>
       </c>
-      <c r="G56" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H56" t="s">
-        <v>434</v>
+      <c r="G56" t="s">
+        <v>433</v>
+      </c>
+      <c r="H56" s="20" t="b">
+        <f>AND(D56&gt;=E56, D56&lt;=F56)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -23230,12 +23130,12 @@
       <c r="F57">
         <v>0.47</v>
       </c>
-      <c r="G57" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H57" t="s">
-        <v>434</v>
+      <c r="G57" t="s">
+        <v>433</v>
+      </c>
+      <c r="H57" s="20" t="b">
+        <f>AND(D57&gt;=E57, D57&lt;=F57)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -23257,12 +23157,12 @@
       <c r="F58">
         <v>0.72</v>
       </c>
-      <c r="G58" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H58" t="s">
-        <v>434</v>
+      <c r="G58" t="s">
+        <v>433</v>
+      </c>
+      <c r="H58" s="20" t="b">
+        <f>AND(D58&gt;=E58, D58&lt;=F58)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -23284,12 +23184,12 @@
       <c r="F59">
         <v>0.08</v>
       </c>
-      <c r="G59" s="20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H59" t="s">
-        <v>434</v>
+      <c r="G59" t="s">
+        <v>433</v>
+      </c>
+      <c r="H59" s="20" t="b">
+        <f>AND(D59&gt;=E59, D59&lt;=F59)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
going well with the cutting!
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="486">
   <si>
     <t>Code Label</t>
   </si>
@@ -1461,6 +1461,9 @@
     <t>Percentage of people who receptively shared a needle/syringe at last injection</t>
   </si>
   <si>
+    <t>average</t>
+  </si>
+  <si>
     <t>total</t>
   </si>
   <si>
@@ -1471,6 +1474,9 @@
   </si>
   <si>
     <t>colnames</t>
+  </si>
+  <si>
+    <t>males</t>
   </si>
 </sst>
 </file>
@@ -20511,8 +20517,8 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20546,10 +20552,10 @@
         <v>328</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -21094,6 +21100,12 @@
       <c r="E28" t="s">
         <v>436</v>
       </c>
+      <c r="F28" t="s">
+        <v>482</v>
+      </c>
+      <c r="G28" t="s">
+        <v>440</v>
+      </c>
       <c r="H28" t="s">
         <v>438</v>
       </c>
@@ -21114,6 +21126,12 @@
       <c r="E29" t="s">
         <v>436</v>
       </c>
+      <c r="F29" t="s">
+        <v>482</v>
+      </c>
+      <c r="G29" t="s">
+        <v>480</v>
+      </c>
       <c r="H29" t="s">
         <v>438</v>
       </c>
@@ -21134,6 +21152,12 @@
       <c r="E30" t="s">
         <v>434</v>
       </c>
+      <c r="F30" t="s">
+        <v>482</v>
+      </c>
+      <c r="G30" t="s">
+        <v>440</v>
+      </c>
       <c r="H30" t="s">
         <v>438</v>
       </c>
@@ -21154,6 +21178,12 @@
       <c r="E31" t="s">
         <v>434</v>
       </c>
+      <c r="F31" t="s">
+        <v>482</v>
+      </c>
+      <c r="G31" t="s">
+        <v>480</v>
+      </c>
       <c r="H31" t="s">
         <v>438</v>
       </c>
@@ -21174,6 +21204,12 @@
       <c r="E32" t="s">
         <v>436</v>
       </c>
+      <c r="F32" t="s">
+        <v>482</v>
+      </c>
+      <c r="G32" t="s">
+        <v>481</v>
+      </c>
       <c r="H32" t="s">
         <v>438</v>
       </c>
@@ -21194,6 +21230,12 @@
       <c r="E33" t="s">
         <v>436</v>
       </c>
+      <c r="F33" t="s">
+        <v>482</v>
+      </c>
+      <c r="G33" t="s">
+        <v>440</v>
+      </c>
       <c r="H33" t="s">
         <v>438</v>
       </c>
@@ -21214,6 +21256,12 @@
       <c r="E34" t="s">
         <v>436</v>
       </c>
+      <c r="F34" t="s">
+        <v>482</v>
+      </c>
+      <c r="G34" t="s">
+        <v>440</v>
+      </c>
       <c r="H34" t="s">
         <v>438</v>
       </c>
@@ -21234,6 +21282,12 @@
       <c r="E35" t="s">
         <v>436</v>
       </c>
+      <c r="F35" t="s">
+        <v>482</v>
+      </c>
+      <c r="G35" t="s">
+        <v>440</v>
+      </c>
       <c r="H35" t="s">
         <v>438</v>
       </c>
@@ -21254,6 +21308,12 @@
       <c r="E36" t="s">
         <v>434</v>
       </c>
+      <c r="F36" t="s">
+        <v>482</v>
+      </c>
+      <c r="G36" t="s">
+        <v>440</v>
+      </c>
       <c r="H36" t="s">
         <v>438</v>
       </c>
@@ -21274,6 +21334,12 @@
       <c r="E37" t="s">
         <v>434</v>
       </c>
+      <c r="F37" t="s">
+        <v>482</v>
+      </c>
+      <c r="G37" t="s">
+        <v>440</v>
+      </c>
       <c r="H37" t="s">
         <v>438</v>
       </c>
@@ -21294,6 +21360,12 @@
       <c r="E38" t="s">
         <v>434</v>
       </c>
+      <c r="F38" t="s">
+        <v>482</v>
+      </c>
+      <c r="G38" t="s">
+        <v>440</v>
+      </c>
       <c r="H38" t="s">
         <v>438</v>
       </c>
@@ -21314,6 +21386,12 @@
       <c r="E39" t="s">
         <v>434</v>
       </c>
+      <c r="F39" t="s">
+        <v>482</v>
+      </c>
+      <c r="G39" t="s">
+        <v>485</v>
+      </c>
       <c r="H39" t="s">
         <v>438</v>
       </c>
@@ -21335,7 +21413,7 @@
         <v>436</v>
       </c>
       <c r="F40" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G40" t="s">
         <v>440</v>
@@ -21361,7 +21439,7 @@
         <v>434</v>
       </c>
       <c r="F41" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G41" t="s">
         <v>440</v>
@@ -21387,10 +21465,10 @@
         <v>436</v>
       </c>
       <c r="F42" t="s">
+        <v>482</v>
+      </c>
+      <c r="G42" t="s">
         <v>481</v>
-      </c>
-      <c r="G42" t="s">
-        <v>480</v>
       </c>
       <c r="H42" t="s">
         <v>438</v>

</xml_diff>

<commit_message>
so many underutilized methods
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="486">
   <si>
     <t>Code Label</t>
   </si>
@@ -20517,8 +20517,8 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20640,6 +20640,12 @@
       <c r="E5" t="s">
         <v>435</v>
       </c>
+      <c r="F5" t="s">
+        <v>482</v>
+      </c>
+      <c r="G5" t="s">
+        <v>440</v>
+      </c>
       <c r="H5" t="s">
         <v>438</v>
       </c>
@@ -20660,6 +20666,12 @@
       <c r="E6" t="s">
         <v>435</v>
       </c>
+      <c r="F6" t="s">
+        <v>482</v>
+      </c>
+      <c r="G6" t="s">
+        <v>440</v>
+      </c>
       <c r="H6" t="s">
         <v>438</v>
       </c>
@@ -20680,6 +20692,12 @@
       <c r="E7" t="s">
         <v>435</v>
       </c>
+      <c r="F7" t="s">
+        <v>482</v>
+      </c>
+      <c r="G7" t="s">
+        <v>440</v>
+      </c>
       <c r="H7" t="s">
         <v>438</v>
       </c>
@@ -20700,6 +20718,12 @@
       <c r="E8" t="s">
         <v>434</v>
       </c>
+      <c r="F8" t="s">
+        <v>482</v>
+      </c>
+      <c r="G8" t="s">
+        <v>440</v>
+      </c>
       <c r="H8" t="s">
         <v>438</v>
       </c>
@@ -20720,6 +20744,12 @@
       <c r="E9" t="s">
         <v>434</v>
       </c>
+      <c r="F9" t="s">
+        <v>482</v>
+      </c>
+      <c r="G9" t="s">
+        <v>480</v>
+      </c>
       <c r="H9" t="s">
         <v>438</v>
       </c>
@@ -20740,6 +20770,12 @@
       <c r="E10" t="s">
         <v>436</v>
       </c>
+      <c r="F10" t="s">
+        <v>482</v>
+      </c>
+      <c r="G10" t="s">
+        <v>481</v>
+      </c>
       <c r="H10" t="s">
         <v>438</v>
       </c>
@@ -20760,6 +20796,12 @@
       <c r="E11" t="s">
         <v>436</v>
       </c>
+      <c r="F11" t="s">
+        <v>482</v>
+      </c>
+      <c r="G11" t="s">
+        <v>481</v>
+      </c>
       <c r="H11" t="s">
         <v>438</v>
       </c>
@@ -20780,6 +20822,12 @@
       <c r="E12" t="s">
         <v>434</v>
       </c>
+      <c r="F12" t="s">
+        <v>482</v>
+      </c>
+      <c r="G12" t="s">
+        <v>440</v>
+      </c>
       <c r="H12" t="s">
         <v>438</v>
       </c>
@@ -20800,6 +20848,12 @@
       <c r="E13" t="s">
         <v>436</v>
       </c>
+      <c r="F13" t="s">
+        <v>482</v>
+      </c>
+      <c r="G13" t="s">
+        <v>481</v>
+      </c>
       <c r="H13" t="s">
         <v>438</v>
       </c>
@@ -20820,6 +20874,12 @@
       <c r="E14" t="s">
         <v>433</v>
       </c>
+      <c r="F14" t="s">
+        <v>482</v>
+      </c>
+      <c r="G14" t="s">
+        <v>439</v>
+      </c>
       <c r="H14" t="s">
         <v>438</v>
       </c>
@@ -20840,6 +20900,12 @@
       <c r="E15" t="s">
         <v>434</v>
       </c>
+      <c r="F15" t="s">
+        <v>482</v>
+      </c>
+      <c r="G15" t="s">
+        <v>480</v>
+      </c>
       <c r="H15" t="s">
         <v>438</v>
       </c>
@@ -20860,6 +20926,12 @@
       <c r="E16" t="s">
         <v>436</v>
       </c>
+      <c r="F16" t="s">
+        <v>482</v>
+      </c>
+      <c r="G16" t="s">
+        <v>481</v>
+      </c>
       <c r="H16" t="s">
         <v>438</v>
       </c>
@@ -20880,6 +20952,12 @@
       <c r="E17" t="s">
         <v>436</v>
       </c>
+      <c r="F17" t="s">
+        <v>482</v>
+      </c>
+      <c r="G17" t="s">
+        <v>481</v>
+      </c>
       <c r="H17" t="s">
         <v>438</v>
       </c>
@@ -20900,6 +20978,12 @@
       <c r="E18" t="s">
         <v>436</v>
       </c>
+      <c r="F18" t="s">
+        <v>482</v>
+      </c>
+      <c r="G18" t="s">
+        <v>481</v>
+      </c>
       <c r="H18" t="s">
         <v>438</v>
       </c>
@@ -20920,6 +21004,12 @@
       <c r="E19" t="s">
         <v>434</v>
       </c>
+      <c r="F19" t="s">
+        <v>482</v>
+      </c>
+      <c r="G19" t="s">
+        <v>481</v>
+      </c>
       <c r="H19" t="s">
         <v>438</v>
       </c>
@@ -20940,6 +21030,12 @@
       <c r="E20" t="s">
         <v>436</v>
       </c>
+      <c r="F20" t="s">
+        <v>482</v>
+      </c>
+      <c r="G20" t="s">
+        <v>481</v>
+      </c>
       <c r="H20" t="s">
         <v>438</v>
       </c>
@@ -20960,6 +21056,12 @@
       <c r="E21" t="s">
         <v>436</v>
       </c>
+      <c r="F21" t="s">
+        <v>482</v>
+      </c>
+      <c r="G21" t="s">
+        <v>481</v>
+      </c>
       <c r="H21" t="s">
         <v>438</v>
       </c>
@@ -20980,6 +21082,12 @@
       <c r="E22" t="s">
         <v>436</v>
       </c>
+      <c r="F22" t="s">
+        <v>482</v>
+      </c>
+      <c r="G22" t="s">
+        <v>481</v>
+      </c>
       <c r="H22" t="s">
         <v>438</v>
       </c>
@@ -21000,6 +21108,12 @@
       <c r="E23" t="s">
         <v>434</v>
       </c>
+      <c r="F23" t="s">
+        <v>482</v>
+      </c>
+      <c r="G23" t="s">
+        <v>480</v>
+      </c>
       <c r="H23" t="s">
         <v>438</v>
       </c>
@@ -21020,6 +21134,12 @@
       <c r="E24" t="s">
         <v>434</v>
       </c>
+      <c r="F24" t="s">
+        <v>482</v>
+      </c>
+      <c r="G24" t="s">
+        <v>480</v>
+      </c>
       <c r="H24" t="s">
         <v>438</v>
       </c>
@@ -21040,6 +21160,12 @@
       <c r="E25" t="s">
         <v>434</v>
       </c>
+      <c r="F25" t="s">
+        <v>482</v>
+      </c>
+      <c r="G25" t="s">
+        <v>480</v>
+      </c>
       <c r="H25" t="s">
         <v>438</v>
       </c>
@@ -21060,6 +21186,12 @@
       <c r="E26" t="s">
         <v>434</v>
       </c>
+      <c r="F26" t="s">
+        <v>482</v>
+      </c>
+      <c r="G26" t="s">
+        <v>480</v>
+      </c>
       <c r="H26" t="s">
         <v>438</v>
       </c>
@@ -21079,6 +21211,12 @@
       </c>
       <c r="E27" t="s">
         <v>434</v>
+      </c>
+      <c r="F27" t="s">
+        <v>482</v>
+      </c>
+      <c r="G27" t="s">
+        <v>480</v>
       </c>
       <c r="H27" t="s">
         <v>438</v>

</xml_diff>

<commit_message>
all working, but very slow
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="483">
   <si>
     <t>Code Label</t>
   </si>
@@ -1005,9 +1005,6 @@
     <t>sheet</t>
   </si>
   <si>
-    <t>method</t>
-  </si>
-  <si>
     <t>Populations</t>
   </si>
   <si>
@@ -1467,13 +1464,7 @@
     <t>total</t>
   </si>
   <si>
-    <t>years</t>
-  </si>
-  <si>
     <t>rownames</t>
-  </si>
-  <si>
-    <t>colnames</t>
   </si>
   <si>
     <t>males</t>
@@ -14813,38 +14804,38 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B1" t="s">
         <v>396</v>
       </c>
-      <c r="B1" t="s">
-        <v>397</v>
-      </c>
       <c r="C1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -14852,7 +14843,7 @@
         <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -14860,7 +14851,7 @@
         <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -14868,7 +14859,7 @@
         <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -14876,7 +14867,7 @@
         <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -14884,7 +14875,7 @@
         <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -14892,7 +14883,7 @@
         <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -14900,7 +14891,7 @@
         <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -14908,7 +14899,7 @@
         <v>166</v>
       </c>
       <c r="B23" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -14916,7 +14907,7 @@
         <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -14924,15 +14915,15 @@
         <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B26" t="s">
         <v>409</v>
-      </c>
-      <c r="B26" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -14940,7 +14931,7 @@
         <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -17435,10 +17426,10 @@
         <v>82</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>414</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>415</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>84</v>
@@ -17482,7 +17473,7 @@
         <v>96</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>97</v>
@@ -17511,7 +17502,7 @@
         <v>99</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>97</v>
@@ -18001,7 +17992,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>169</v>
@@ -18726,10 +18717,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>97</v>
@@ -19451,10 +19442,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>144</v>
@@ -19495,7 +19486,7 @@
         <v>200</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G72" s="7">
         <v>0</v>
@@ -19524,7 +19515,7 @@
         <v>200</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G73" s="7">
         <v>0</v>
@@ -19553,7 +19544,7 @@
         <v>200</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G74" s="7">
         <v>0</v>
@@ -19582,7 +19573,7 @@
         <v>200</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G75" s="7">
         <v>0</v>
@@ -19611,7 +19602,7 @@
         <v>200</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G76" s="7">
         <v>0</v>
@@ -19640,7 +19631,7 @@
         <v>200</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G77" s="7">
         <v>0</v>
@@ -19669,7 +19660,7 @@
         <v>200</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G78" s="7">
         <v>0</v>
@@ -19698,7 +19689,7 @@
         <v>200</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G79" s="7">
         <v>0</v>
@@ -19727,7 +19718,7 @@
         <v>200</v>
       </c>
       <c r="F80" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G80" s="7">
         <v>0</v>
@@ -19756,7 +19747,7 @@
         <v>200</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G81" s="7">
         <v>0</v>
@@ -19785,7 +19776,7 @@
         <v>200</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G82" s="7">
         <v>0</v>
@@ -19814,7 +19805,7 @@
         <v>200</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G83" s="7">
         <v>0</v>
@@ -19843,7 +19834,7 @@
         <v>200</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G84" s="7">
         <v>0</v>
@@ -19860,7 +19851,7 @@
         <v>275</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>102</v>
@@ -19889,7 +19880,7 @@
         <v>276</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>102</v>
@@ -19988,7 +19979,7 @@
         <v>200</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G89" s="7">
         <v>0</v>
@@ -20249,7 +20240,7 @@
         <v>200</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G98" s="7">
         <v>0</v>
@@ -20278,7 +20269,7 @@
         <v>200</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G99" s="7">
         <v>0</v>
@@ -20307,7 +20298,7 @@
         <v>200</v>
       </c>
       <c r="F100" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G100" s="7">
         <v>0</v>
@@ -20336,7 +20327,7 @@
         <v>200</v>
       </c>
       <c r="F101" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G101" s="7">
         <v>0</v>
@@ -20365,7 +20356,7 @@
         <v>200</v>
       </c>
       <c r="F102" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G102" s="7">
         <v>0</v>
@@ -20394,7 +20385,7 @@
         <v>200</v>
       </c>
       <c r="F103" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G103" s="7">
         <v>0</v>
@@ -20423,7 +20414,7 @@
         <v>200</v>
       </c>
       <c r="F104" s="17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G104" s="7">
         <v>0</v>
@@ -20514,11 +20505,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20528,16 +20519,15 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="76.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>327</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>79</v>
@@ -20546,21 +20536,15 @@
         <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>328</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>329</v>
       </c>
       <c r="B2" t="s">
         <v>98</v>
@@ -20569,47 +20553,41 @@
         <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F2" t="s">
-        <v>438</v>
-      </c>
-      <c r="G2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" t="s">
         <v>330</v>
       </c>
-      <c r="B3" t="s">
-        <v>331</v>
-      </c>
       <c r="C3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E3" t="s">
-        <v>435</v>
-      </c>
-      <c r="H3" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+      <c r="F3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C4" t="s">
         <v>93</v>
@@ -20618,70 +20596,58 @@
         <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>436</v>
-      </c>
-      <c r="H4" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+      <c r="F4" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C5" t="s">
         <v>110</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F5" t="s">
-        <v>482</v>
-      </c>
-      <c r="G5" t="s">
-        <v>440</v>
-      </c>
-      <c r="H5" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C6" t="s">
         <v>118</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F6" t="s">
-        <v>482</v>
-      </c>
-      <c r="G6" t="s">
-        <v>440</v>
-      </c>
-      <c r="H6" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C7" t="s">
         <v>120</v>
@@ -20690,76 +20656,58 @@
         <v>119</v>
       </c>
       <c r="E7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F7" t="s">
-        <v>482</v>
-      </c>
-      <c r="G7" t="s">
-        <v>440</v>
-      </c>
-      <c r="H7" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C8" t="s">
         <v>113</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F8" t="s">
-        <v>482</v>
-      </c>
-      <c r="G8" t="s">
-        <v>440</v>
-      </c>
-      <c r="H8" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C9" t="s">
         <v>115</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F9" t="s">
-        <v>482</v>
-      </c>
-      <c r="G9" t="s">
-        <v>480</v>
-      </c>
-      <c r="H9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C10" t="s">
         <v>122</v>
@@ -20768,24 +20716,18 @@
         <v>121</v>
       </c>
       <c r="E10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F10" t="s">
-        <v>482</v>
-      </c>
-      <c r="G10" t="s">
-        <v>481</v>
-      </c>
-      <c r="H10" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C11" t="s">
         <v>198</v>
@@ -20794,440 +20736,338 @@
         <v>197</v>
       </c>
       <c r="E11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F11" t="s">
-        <v>482</v>
-      </c>
-      <c r="G11" t="s">
-        <v>481</v>
-      </c>
-      <c r="H11" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C12" t="s">
         <v>140</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F12" t="s">
-        <v>482</v>
-      </c>
-      <c r="G12" t="s">
-        <v>440</v>
-      </c>
-      <c r="H12" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C13" t="s">
         <v>124</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F13" t="s">
-        <v>482</v>
-      </c>
-      <c r="G13" t="s">
-        <v>481</v>
-      </c>
-      <c r="H13" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C14" t="s">
         <v>128</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F14" t="s">
-        <v>482</v>
-      </c>
-      <c r="G14" t="s">
-        <v>439</v>
-      </c>
-      <c r="H14" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C15" t="s">
         <v>126</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F15" t="s">
-        <v>482</v>
-      </c>
-      <c r="G15" t="s">
-        <v>480</v>
-      </c>
-      <c r="H15" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B16" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C16" t="s">
         <v>313</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F16" t="s">
-        <v>482</v>
-      </c>
-      <c r="G16" t="s">
-        <v>481</v>
-      </c>
-      <c r="H16" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C17" t="s">
         <v>314</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F17" t="s">
-        <v>482</v>
-      </c>
-      <c r="G17" t="s">
-        <v>481</v>
-      </c>
-      <c r="H17" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C18" t="s">
         <v>315</v>
       </c>
       <c r="D18" s="41" t="s">
+        <v>457</v>
+      </c>
+      <c r="E18" t="s">
+        <v>435</v>
+      </c>
+      <c r="F18" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>336</v>
+      </c>
+      <c r="B19" t="s">
+        <v>331</v>
+      </c>
+      <c r="C19" t="s">
+        <v>430</v>
+      </c>
+      <c r="D19" s="41" t="s">
         <v>458</v>
       </c>
-      <c r="E18" t="s">
-        <v>436</v>
-      </c>
-      <c r="F18" t="s">
-        <v>482</v>
-      </c>
-      <c r="G18" t="s">
-        <v>481</v>
-      </c>
-      <c r="H18" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>337</v>
-      </c>
-      <c r="B19" t="s">
-        <v>332</v>
-      </c>
-      <c r="C19" t="s">
-        <v>431</v>
-      </c>
-      <c r="D19" s="41" t="s">
-        <v>459</v>
-      </c>
       <c r="E19" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F19" t="s">
-        <v>482</v>
-      </c>
-      <c r="G19" t="s">
-        <v>481</v>
-      </c>
-      <c r="H19" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C20" t="s">
         <v>316</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F20" t="s">
-        <v>482</v>
-      </c>
-      <c r="G20" t="s">
-        <v>481</v>
-      </c>
-      <c r="H20" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C21" t="s">
         <v>317</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E21" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F21" t="s">
-        <v>482</v>
-      </c>
-      <c r="G21" t="s">
-        <v>481</v>
-      </c>
-      <c r="H21" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C22" t="s">
         <v>318</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E22" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F22" t="s">
-        <v>482</v>
-      </c>
-      <c r="G22" t="s">
-        <v>481</v>
-      </c>
-      <c r="H22" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C23" t="s">
         <v>319</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E23" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F23" t="s">
-        <v>482</v>
-      </c>
-      <c r="G23" t="s">
-        <v>480</v>
-      </c>
-      <c r="H23" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C24" t="s">
         <v>320</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E24" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F24" t="s">
-        <v>482</v>
-      </c>
-      <c r="G24" t="s">
-        <v>480</v>
-      </c>
-      <c r="H24" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C25" t="s">
         <v>321</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F25" t="s">
-        <v>482</v>
-      </c>
-      <c r="G25" t="s">
-        <v>480</v>
-      </c>
-      <c r="H25" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B26" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C26" t="s">
         <v>322</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F26" t="s">
-        <v>482</v>
-      </c>
-      <c r="G26" t="s">
-        <v>480</v>
-      </c>
-      <c r="H26" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C27" t="s">
         <v>323</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E27" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F27" t="s">
-        <v>482</v>
-      </c>
-      <c r="G27" t="s">
-        <v>480</v>
-      </c>
-      <c r="H27" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C28" t="s">
         <v>164</v>
@@ -21236,24 +21076,18 @@
         <v>163</v>
       </c>
       <c r="E28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F28" t="s">
-        <v>482</v>
-      </c>
-      <c r="G28" t="s">
-        <v>440</v>
-      </c>
-      <c r="H28" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C29" t="s">
         <v>168</v>
@@ -21262,536 +21096,410 @@
         <v>167</v>
       </c>
       <c r="E29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F29" t="s">
-        <v>482</v>
-      </c>
-      <c r="G29" t="s">
-        <v>480</v>
-      </c>
-      <c r="H29" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C30" t="s">
         <v>171</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E30" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F30" t="s">
-        <v>482</v>
-      </c>
-      <c r="G30" t="s">
-        <v>440</v>
-      </c>
-      <c r="H30" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B31" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C31" t="s">
         <v>173</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E31" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F31" t="s">
-        <v>482</v>
-      </c>
-      <c r="G31" t="s">
-        <v>480</v>
-      </c>
-      <c r="H31" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D32" s="41" t="s">
         <v>169</v>
       </c>
       <c r="E32" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F32" t="s">
-        <v>482</v>
-      </c>
-      <c r="G32" t="s">
-        <v>481</v>
-      </c>
-      <c r="H32" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B33" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C33" t="s">
         <v>143</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F33" t="s">
-        <v>482</v>
-      </c>
-      <c r="G33" t="s">
-        <v>440</v>
-      </c>
-      <c r="H33" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C34" t="s">
         <v>148</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E34" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F34" t="s">
-        <v>482</v>
-      </c>
-      <c r="G34" t="s">
-        <v>440</v>
-      </c>
-      <c r="H34" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B35" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C35" t="s">
         <v>151</v>
       </c>
       <c r="D35" s="41" t="s">
+        <v>471</v>
+      </c>
+      <c r="E35" t="s">
+        <v>435</v>
+      </c>
+      <c r="F35" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>338</v>
+      </c>
+      <c r="B36" t="s">
+        <v>331</v>
+      </c>
+      <c r="C36" t="s">
+        <v>429</v>
+      </c>
+      <c r="D36" s="41" t="s">
         <v>472</v>
       </c>
-      <c r="E35" t="s">
-        <v>436</v>
-      </c>
-      <c r="F35" t="s">
-        <v>482</v>
-      </c>
-      <c r="G35" t="s">
-        <v>440</v>
-      </c>
-      <c r="H35" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>339</v>
-      </c>
-      <c r="B36" t="s">
-        <v>332</v>
-      </c>
-      <c r="C36" t="s">
-        <v>430</v>
-      </c>
-      <c r="D36" s="41" t="s">
-        <v>473</v>
-      </c>
       <c r="E36" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F36" t="s">
-        <v>482</v>
-      </c>
-      <c r="G36" t="s">
-        <v>440</v>
-      </c>
-      <c r="H36" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B37" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C37" t="s">
         <v>159</v>
       </c>
       <c r="D37" s="41" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E37" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F37" t="s">
-        <v>482</v>
-      </c>
-      <c r="G37" t="s">
-        <v>440</v>
-      </c>
-      <c r="H37" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B38" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C38" t="s">
         <v>162</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E38" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F38" t="s">
-        <v>482</v>
-      </c>
-      <c r="G38" t="s">
-        <v>440</v>
-      </c>
-      <c r="H38" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C39" t="s">
         <v>131</v>
       </c>
       <c r="D39" s="41" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E39" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F39" t="s">
         <v>482</v>
       </c>
-      <c r="G39" t="s">
-        <v>485</v>
-      </c>
-      <c r="H39" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B40" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C40" t="s">
         <v>154</v>
       </c>
       <c r="D40" s="41" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E40" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F40" t="s">
-        <v>482</v>
-      </c>
-      <c r="G40" t="s">
-        <v>440</v>
-      </c>
-      <c r="H40" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B41" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C41" t="s">
         <v>138</v>
       </c>
       <c r="D41" s="41" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E41" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F41" t="s">
-        <v>482</v>
-      </c>
-      <c r="G41" t="s">
-        <v>440</v>
-      </c>
-      <c r="H41" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B42" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C42" t="s">
         <v>136</v>
       </c>
       <c r="D42" s="41" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E42" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F42" t="s">
-        <v>482</v>
-      </c>
-      <c r="G42" t="s">
-        <v>481</v>
-      </c>
-      <c r="H42" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B43" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C43" t="s">
         <v>324</v>
       </c>
       <c r="D43" s="41" t="s">
+        <v>440</v>
+      </c>
+      <c r="E43" t="s">
+        <v>435</v>
+      </c>
+      <c r="F43" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>340</v>
+      </c>
+      <c r="B44" t="s">
+        <v>427</v>
+      </c>
+      <c r="C44" t="s">
+        <v>428</v>
+      </c>
+      <c r="D44" s="41" t="s">
         <v>441</v>
       </c>
-      <c r="E43" t="s">
-        <v>436</v>
-      </c>
-      <c r="F43" t="s">
-        <v>428</v>
-      </c>
-      <c r="G43" t="s">
-        <v>440</v>
-      </c>
-      <c r="H43" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>341</v>
-      </c>
-      <c r="B44" t="s">
-        <v>428</v>
-      </c>
-      <c r="C44" t="s">
-        <v>429</v>
-      </c>
-      <c r="D44" s="41" t="s">
-        <v>442</v>
-      </c>
       <c r="E44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F44" t="s">
-        <v>428</v>
-      </c>
-      <c r="G44" t="s">
-        <v>440</v>
-      </c>
-      <c r="H44" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B45" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C45" t="s">
         <v>325</v>
       </c>
       <c r="D45" s="41" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F45" t="s">
-        <v>428</v>
-      </c>
-      <c r="G45" t="s">
-        <v>440</v>
-      </c>
-      <c r="H45" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B46" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C46" t="s">
         <v>326</v>
       </c>
       <c r="D46" s="41" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E46" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F46" t="s">
-        <v>428</v>
-      </c>
-      <c r="G46" t="s">
-        <v>440</v>
-      </c>
-      <c r="H46" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B47" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C47" t="s">
         <v>108</v>
       </c>
       <c r="D47" s="41" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F47" t="s">
-        <v>428</v>
-      </c>
-      <c r="G47" t="s">
-        <v>439</v>
-      </c>
-      <c r="H47" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C48" t="s">
         <v>106</v>
       </c>
       <c r="D48" s="41" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F48" t="s">
-        <v>428</v>
-      </c>
-      <c r="G48" t="s">
-        <v>440</v>
-      </c>
-      <c r="H48" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B49" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C49" t="s">
         <v>101</v>
       </c>
       <c r="D49" s="41" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E49" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F49" t="s">
-        <v>428</v>
-      </c>
-      <c r="G49" t="s">
-        <v>440</v>
-      </c>
-      <c r="H49" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -21818,7 +21526,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>79</v>
@@ -21827,30 +21535,30 @@
         <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B2" t="s">
         <v>201</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D2" s="11">
         <v>4.0000000000000002E-4</v>
@@ -21862,7 +21570,7 @@
         <v>1.4E-3</v>
       </c>
       <c r="G2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H2" s="20" t="b">
         <f>AND(D2&gt;=E2, D2&lt;=F2)</f>
@@ -21871,13 +21579,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B3" t="s">
         <v>204</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D3" s="11">
         <v>8.0000000000000004E-4</v>
@@ -21889,7 +21597,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="G3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H3" s="20" t="b">
         <f>AND(D3&gt;=E3, D3&lt;=F3)</f>
@@ -21898,13 +21606,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B4" t="s">
         <v>206</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D4" s="11">
         <v>1.1000000000000001E-3</v>
@@ -21916,7 +21624,7 @@
         <v>2.8E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H4" s="20" t="b">
         <f>AND(D4&gt;=E4, D4&lt;=F4)</f>
@@ -21925,13 +21633,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B5" t="s">
         <v>208</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D5" s="11">
         <v>1.38E-2</v>
@@ -21943,7 +21651,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
       <c r="G5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H5" s="20" t="b">
         <f>AND(D5&gt;=E5, D5&lt;=F5)</f>
@@ -21952,13 +21660,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B6" t="s">
         <v>210</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D6" s="11">
         <v>8.0000000000000002E-3</v>
@@ -21970,7 +21678,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="G6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H6" s="20" t="b">
         <f>AND(D6&gt;=E6, D6&lt;=F6)</f>
@@ -21979,13 +21687,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B7" t="s">
         <v>212</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D7" s="11">
         <v>0.36699999999999999</v>
@@ -21997,7 +21705,7 @@
         <v>0.44</v>
       </c>
       <c r="G7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H7" s="20" t="b">
         <f>AND(D7&gt;=E7, D7&lt;=F7)</f>
@@ -22006,13 +21714,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B8" t="s">
         <v>214</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D8" s="11">
         <v>0.20499999999999999</v>
@@ -22024,7 +21732,7 @@
         <v>0.27</v>
       </c>
       <c r="G8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H8" s="20" t="b">
         <f>AND(D8&gt;=E8, D8&lt;=F8)</f>
@@ -22033,13 +21741,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>216</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D9">
         <v>5.6</v>
@@ -22051,7 +21759,7 @@
         <v>9.1</v>
       </c>
       <c r="G9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H9" s="20" t="b">
         <f>AND(D9&gt;=E9, D9&lt;=F9)</f>
@@ -22060,13 +21768,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>218</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -22078,7 +21786,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H10" s="20" t="b">
         <f>AND(D10&gt;=E10, D10&lt;=F10)</f>
@@ -22087,13 +21795,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>220</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -22105,7 +21813,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H11" s="20" t="b">
         <f>AND(D11&gt;=E11, D11&lt;=F11)</f>
@@ -22114,13 +21822,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>222</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -22132,7 +21840,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H12" s="20" t="b">
         <f>AND(D12&gt;=E12, D12&lt;=F12)</f>
@@ -22141,13 +21849,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>224</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D13">
         <v>3.49</v>
@@ -22159,7 +21867,7 @@
         <v>6.92</v>
       </c>
       <c r="G13" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H13" s="20" t="b">
         <f>AND(D13&gt;=E13, D13&lt;=F13)</f>
@@ -22168,13 +21876,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>226</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D14">
         <v>7.17</v>
@@ -22186,7 +21894,7 @@
         <v>12.08</v>
       </c>
       <c r="G14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H14" s="20" t="b">
         <f>AND(D14&gt;=E14, D14&lt;=F14)</f>
@@ -22195,13 +21903,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>230</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D15">
         <v>0.24</v>
@@ -22213,7 +21921,7 @@
         <v>0.5</v>
       </c>
       <c r="G15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H15" s="20" t="b">
         <f>AND(D15&gt;=E15, D15&lt;=F15)</f>
@@ -22222,13 +21930,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>232</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D16">
         <v>0.95</v>
@@ -22240,7 +21948,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="G16" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H16" s="20" t="b">
         <f>AND(D16&gt;=E16, D16&lt;=F16)</f>
@@ -22249,13 +21957,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>234</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -22267,7 +21975,7 @@
         <v>3.16</v>
       </c>
       <c r="G17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H17" s="20" t="b">
         <f>AND(D17&gt;=E17, D17&lt;=F17)</f>
@@ -22276,13 +21984,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>236</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D18">
         <v>3.74</v>
@@ -22294,7 +22002,7 @@
         <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H18" s="20" t="b">
         <f>AND(D18&gt;=E18, D18&lt;=F18)</f>
@@ -22303,13 +22011,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>238</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D19">
         <v>1.5</v>
@@ -22321,7 +22029,7 @@
         <v>2.25</v>
       </c>
       <c r="G19" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H19" s="20" t="b">
         <f>AND(D19&gt;=E19, D19&lt;=F19)</f>
@@ -22330,13 +22038,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>240</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D20">
         <v>2.2000000000000002</v>
@@ -22348,7 +22056,7 @@
         <v>7.28</v>
       </c>
       <c r="G20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H20" s="20" t="b">
         <f>AND(D20&gt;=E20, D20&lt;=F20)</f>
@@ -22357,13 +22065,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>242</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D21">
         <v>1.42</v>
@@ -22375,7 +22083,7 @@
         <v>3.42</v>
       </c>
       <c r="G21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H21" s="20" t="b">
         <f>AND(D21&gt;=E21, D21&lt;=F21)</f>
@@ -22384,13 +22092,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>244</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D22">
         <v>2.14</v>
@@ -22402,7 +22110,7 @@
         <v>3.58</v>
       </c>
       <c r="G22" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H22" s="20" t="b">
         <f>AND(D22&gt;=E22, D22&lt;=F22)</f>
@@ -22411,13 +22119,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>246</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D23">
         <v>0.66</v>
@@ -22429,7 +22137,7 @@
         <v>0.94</v>
       </c>
       <c r="G23" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H23" s="20" t="b">
         <f>AND(D23&gt;=E23, D23&lt;=F23)</f>
@@ -22438,7 +22146,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>248</v>
@@ -22456,7 +22164,7 @@
         <v>0.3</v>
       </c>
       <c r="G24" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H24" s="20" t="b">
         <f>AND(D24&gt;=E24, D24&lt;=F24)</f>
@@ -22465,13 +22173,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -22483,7 +22191,7 @@
         <v>2.5</v>
       </c>
       <c r="G25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H25" s="20" t="b">
         <f>AND(D25&gt;=E25, D25&lt;=F25)</f>
@@ -22492,13 +22200,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>250</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D26" s="11">
         <v>2.5999999999999999E-2</v>
@@ -22510,7 +22218,7 @@
         <v>0.27500000000000002</v>
       </c>
       <c r="G26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H26" s="20" t="b">
         <f>AND(D26&gt;=E26, D26&lt;=F26)</f>
@@ -22519,13 +22227,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>252</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D27" s="11">
         <v>0.15</v>
@@ -22537,7 +22245,7 @@
         <v>0.88500000000000001</v>
       </c>
       <c r="G27" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H27" s="20" t="b">
         <f>AND(D27&gt;=E27, D27&lt;=F27)</f>
@@ -22546,13 +22254,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>254</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D28" s="11">
         <v>0.1</v>
@@ -22564,7 +22272,7 @@
         <v>0.87</v>
       </c>
       <c r="G28" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H28" s="20" t="b">
         <f>AND(D28&gt;=E28, D28&lt;=F28)</f>
@@ -22573,13 +22281,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>256</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D29" s="11">
         <v>5.2999999999999999E-2</v>
@@ -22591,7 +22299,7 @@
         <v>0.82699999999999996</v>
       </c>
       <c r="G29" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H29" s="20" t="b">
         <f>AND(D29&gt;=E29, D29&lt;=F29)</f>
@@ -22600,13 +22308,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>258</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D30" s="11">
         <v>0.16200000000000001</v>
@@ -22618,7 +22326,7 @@
         <v>0.86899999999999999</v>
       </c>
       <c r="G30" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H30" s="20" t="b">
         <f>AND(D30&gt;=E30, D30&lt;=F30)</f>
@@ -22627,13 +22335,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>260</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D31" s="11">
         <v>0.11700000000000001</v>
@@ -22645,7 +22353,7 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="G31" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H31" s="20" t="b">
         <f>AND(D31&gt;=E31, D31&lt;=F31)</f>
@@ -22654,13 +22362,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>262</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D32" s="11">
         <v>0.09</v>
@@ -22672,7 +22380,7 @@
         <v>0.72299999999999998</v>
       </c>
       <c r="G32" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H32" s="20" t="b">
         <f>AND(D32&gt;=E32, D32&lt;=F32)</f>
@@ -22681,13 +22389,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>264</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D33" s="11">
         <v>0.111</v>
@@ -22699,7 +22407,7 @@
         <v>0.56299999999999994</v>
       </c>
       <c r="G33" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H33" s="20" t="b">
         <f>AND(D33&gt;=E33, D33&lt;=F33)</f>
@@ -22708,7 +22416,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>266</v>
@@ -22726,7 +22434,7 @@
         <v>0.26</v>
       </c>
       <c r="G34" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H34" s="20" t="b">
         <f>AND(D34&gt;=E34, D34&lt;=F34)</f>
@@ -22735,13 +22443,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>268</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D35" s="11">
         <v>3.5999999999999999E-3</v>
@@ -22753,7 +22461,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="G35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H35" s="20" t="b">
         <f>AND(D35&gt;=E35, D35&lt;=F35)</f>
@@ -22762,13 +22470,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>270</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D36" s="11">
         <v>3.5999999999999999E-3</v>
@@ -22780,7 +22488,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="G36" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H36" s="20" t="b">
         <f>AND(D36&gt;=E36, D36&lt;=F36)</f>
@@ -22789,13 +22497,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>272</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D37" s="11">
         <v>5.7999999999999996E-3</v>
@@ -22807,7 +22515,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="G37" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H37" s="20" t="b">
         <f>AND(D37&gt;=E37, D37&lt;=F37)</f>
@@ -22816,13 +22524,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>274</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D38" s="11">
         <v>8.8000000000000005E-3</v>
@@ -22834,7 +22542,7 @@
         <v>1.01E-2</v>
       </c>
       <c r="G38" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H38" s="20" t="b">
         <f>AND(D38&gt;=E38, D38&lt;=F38)</f>
@@ -22843,13 +22551,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>275</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D39" s="11">
         <v>5.8999999999999997E-2</v>
@@ -22861,7 +22569,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="G39" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H39" s="20" t="b">
         <f>AND(D39&gt;=E39, D39&lt;=F39)</f>
@@ -22870,13 +22578,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>276</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D40" s="11">
         <v>0.32300000000000001</v>
@@ -22888,7 +22596,7 @@
         <v>0.432</v>
       </c>
       <c r="G40" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H40" s="20" t="b">
         <f>AND(D40&gt;=E40, D40&lt;=F40)</f>
@@ -22897,13 +22605,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>278</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D41" s="11">
         <v>0.23</v>
@@ -22915,7 +22623,7 @@
         <v>0.3</v>
       </c>
       <c r="G41" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H41" s="20" t="b">
         <f>AND(D41&gt;=E41, D41&lt;=F41)</f>
@@ -22924,13 +22632,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>280</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D42" s="11">
         <v>0.48780000000000001</v>
@@ -22942,7 +22650,7 @@
         <v>0.8417</v>
       </c>
       <c r="G42" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H42" s="20" t="b">
         <f>AND(D42&gt;=E42, D42&lt;=F42)</f>
@@ -22951,13 +22659,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>282</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D43" s="11">
         <v>2.17</v>
@@ -22969,7 +22677,7 @@
         <v>3.71</v>
       </c>
       <c r="G43" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H43" s="20" t="b">
         <f>AND(D43&gt;=E43, D43&lt;=F43)</f>
@@ -22978,13 +22686,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>292</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D44" s="13">
         <v>0.95</v>
@@ -22996,7 +22704,7 @@
         <v>0.98</v>
       </c>
       <c r="G44" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H44" s="20" t="b">
         <f>AND(D44&gt;=E44, D44&lt;=F44)</f>
@@ -23005,13 +22713,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>294</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D45" s="13">
         <v>0.57999999999999996</v>
@@ -23023,7 +22731,7 @@
         <v>0.67</v>
       </c>
       <c r="G45" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H45" s="20" t="b">
         <f>AND(D45&gt;=E45, D45&lt;=F45)</f>
@@ -23032,13 +22740,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>298</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D46" s="13">
         <v>0</v>
@@ -23050,7 +22758,7 @@
         <v>0.68</v>
       </c>
       <c r="G46" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H46" s="20" t="b">
         <f>AND(D46&gt;=E46, D46&lt;=F46)</f>
@@ -23059,13 +22767,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>228</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D47" s="13">
         <v>2.65</v>
@@ -23077,7 +22785,7 @@
         <v>5.19</v>
       </c>
       <c r="G47" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H47" s="20" t="b">
         <f>AND(D47&gt;=E47, D47&lt;=F47)</f>
@@ -23086,13 +22794,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>296</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D48" s="13">
         <v>0.54</v>
@@ -23104,7 +22812,7 @@
         <v>0.68</v>
       </c>
       <c r="G48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H48" s="20" t="b">
         <f>AND(D48&gt;=E48, D48&lt;=F48)</f>
@@ -23113,13 +22821,13 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>288</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D49" s="13">
         <v>0.9</v>
@@ -23131,7 +22839,7 @@
         <v>0.93</v>
       </c>
       <c r="G49" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H49" s="20" t="b">
         <f>AND(D49&gt;=E49, D49&lt;=F49)</f>
@@ -23140,13 +22848,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>290</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D50" s="13">
         <v>0.73</v>
@@ -23158,7 +22866,7 @@
         <v>0.8</v>
       </c>
       <c r="G50" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H50" s="20" t="b">
         <f>AND(D50&gt;=E50, D50&lt;=F50)</f>
@@ -23167,13 +22875,13 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>284</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D51" s="13">
         <v>0.5</v>
@@ -23185,7 +22893,7 @@
         <v>0.8</v>
       </c>
       <c r="G51" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H51" s="20" t="b">
         <f>AND(D51&gt;=E51, D51&lt;=F51)</f>
@@ -23194,13 +22902,13 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>286</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D52" s="13">
         <v>0.92</v>
@@ -23212,7 +22920,7 @@
         <v>0.95</v>
       </c>
       <c r="G52" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H52" s="20" t="b">
         <f>AND(D52&gt;=E52, D52&lt;=F52)</f>
@@ -23221,13 +22929,13 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>300</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D53">
         <v>0.15</v>
@@ -23239,7 +22947,7 @@
         <v>0.21</v>
       </c>
       <c r="G53" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H53" s="20" t="b">
         <f>AND(D53&gt;=E53, D53&lt;=F53)</f>
@@ -23248,13 +22956,13 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>302</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D54">
         <v>0.01</v>
@@ -23266,7 +22974,7 @@
         <v>0.01</v>
       </c>
       <c r="G54" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H54" s="20" t="b">
         <f>AND(D54&gt;=E54, D54&lt;=F54)</f>
@@ -23275,13 +22983,13 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>304</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D55">
         <v>0.02</v>
@@ -23293,7 +23001,7 @@
         <v>0.03</v>
       </c>
       <c r="G55" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H55" s="20" t="b">
         <f>AND(D55&gt;=E55, D55&lt;=F55)</f>
@@ -23302,13 +23010,13 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>306</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D56">
         <v>7.0000000000000007E-2</v>
@@ -23320,7 +23028,7 @@
         <v>0.09</v>
       </c>
       <c r="G56" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H56" s="20" t="b">
         <f>AND(D56&gt;=E56, D56&lt;=F56)</f>
@@ -23329,13 +23037,13 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>308</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D57">
         <v>0.27</v>
@@ -23347,7 +23055,7 @@
         <v>0.47</v>
       </c>
       <c r="G57" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H57" s="20" t="b">
         <f>AND(D57&gt;=E57, D57&lt;=F57)</f>
@@ -23356,13 +23064,13 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>310</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D58">
         <v>0.55000000000000004</v>
@@ -23374,7 +23082,7 @@
         <v>0.72</v>
       </c>
       <c r="G58" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H58" s="20" t="b">
         <f>AND(D58&gt;=E58, D58&lt;=F58)</f>
@@ -23383,13 +23091,13 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B59" t="s">
         <v>312</v>
       </c>
       <c r="C59" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D59">
         <v>0.05</v>
@@ -23401,7 +23109,7 @@
         <v>0.08</v>
       </c>
       <c r="G59" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H59" s="20" t="b">
         <f>AND(D59&gt;=E59, D59&lt;=F59)</f>

</xml_diff>

<commit_message>
swapped order to restore match with spreadsheets
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -17425,7 +17425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
@@ -20542,9 +20542,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20599,19 +20599,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
         <v>328</v>
       </c>
       <c r="C3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D3" t="s">
-        <v>327</v>
+        <v>91</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F3" t="s">
         <v>436</v>
@@ -20619,19 +20619,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>327</v>
       </c>
       <c r="B4" t="s">
         <v>328</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>90</v>
+        <v>330</v>
+      </c>
+      <c r="D4" t="s">
+        <v>327</v>
       </c>
       <c r="E4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F4" t="s">
         <v>436</v>
@@ -21608,7 +21608,7 @@
         <v>432</v>
       </c>
       <c r="H2" s="17" t="b">
-        <f>AND(D2&gt;=E2, D2&lt;=F2)</f>
+        <f t="shared" ref="H2:H33" si="0">AND(D2&gt;=E2, D2&lt;=F2)</f>
         <v>1</v>
       </c>
     </row>
@@ -21635,7 +21635,7 @@
         <v>432</v>
       </c>
       <c r="H3" s="17" t="b">
-        <f>AND(D3&gt;=E3, D3&lt;=F3)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21662,7 +21662,7 @@
         <v>432</v>
       </c>
       <c r="H4" s="17" t="b">
-        <f>AND(D4&gt;=E4, D4&lt;=F4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21689,7 +21689,7 @@
         <v>432</v>
       </c>
       <c r="H5" s="17" t="b">
-        <f>AND(D5&gt;=E5, D5&lt;=F5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21716,7 +21716,7 @@
         <v>432</v>
       </c>
       <c r="H6" s="17" t="b">
-        <f>AND(D6&gt;=E6, D6&lt;=F6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21743,7 +21743,7 @@
         <v>432</v>
       </c>
       <c r="H7" s="17" t="b">
-        <f>AND(D7&gt;=E7, D7&lt;=F7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21770,7 +21770,7 @@
         <v>432</v>
       </c>
       <c r="H8" s="17" t="b">
-        <f>AND(D8&gt;=E8, D8&lt;=F8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21797,7 +21797,7 @@
         <v>430</v>
       </c>
       <c r="H9" s="17" t="b">
-        <f>AND(D9&gt;=E9, D9&lt;=F9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21824,7 +21824,7 @@
         <v>430</v>
       </c>
       <c r="H10" s="17" t="b">
-        <f>AND(D10&gt;=E10, D10&lt;=F10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21851,7 +21851,7 @@
         <v>430</v>
       </c>
       <c r="H11" s="17" t="b">
-        <f>AND(D11&gt;=E11, D11&lt;=F11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21878,7 +21878,7 @@
         <v>430</v>
       </c>
       <c r="H12" s="17" t="b">
-        <f>AND(D12&gt;=E12, D12&lt;=F12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21905,7 +21905,7 @@
         <v>430</v>
       </c>
       <c r="H13" s="17" t="b">
-        <f>AND(D13&gt;=E13, D13&lt;=F13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21932,7 +21932,7 @@
         <v>430</v>
       </c>
       <c r="H14" s="17" t="b">
-        <f>AND(D14&gt;=E14, D14&lt;=F14)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21959,7 +21959,7 @@
         <v>430</v>
       </c>
       <c r="H15" s="17" t="b">
-        <f>AND(D15&gt;=E15, D15&lt;=F15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -21986,7 +21986,7 @@
         <v>430</v>
       </c>
       <c r="H16" s="17" t="b">
-        <f>AND(D16&gt;=E16, D16&lt;=F16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22013,7 +22013,7 @@
         <v>430</v>
       </c>
       <c r="H17" s="17" t="b">
-        <f>AND(D17&gt;=E17, D17&lt;=F17)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22040,7 +22040,7 @@
         <v>430</v>
       </c>
       <c r="H18" s="17" t="b">
-        <f>AND(D18&gt;=E18, D18&lt;=F18)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22067,7 +22067,7 @@
         <v>430</v>
       </c>
       <c r="H19" s="17" t="b">
-        <f>AND(D19&gt;=E19, D19&lt;=F19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22094,7 +22094,7 @@
         <v>430</v>
       </c>
       <c r="H20" s="17" t="b">
-        <f>AND(D20&gt;=E20, D20&lt;=F20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22121,7 +22121,7 @@
         <v>430</v>
       </c>
       <c r="H21" s="17" t="b">
-        <f>AND(D21&gt;=E21, D21&lt;=F21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22148,7 +22148,7 @@
         <v>430</v>
       </c>
       <c r="H22" s="17" t="b">
-        <f>AND(D22&gt;=E22, D22&lt;=F22)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22175,7 +22175,7 @@
         <v>430</v>
       </c>
       <c r="H23" s="17" t="b">
-        <f>AND(D23&gt;=E23, D23&lt;=F23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22202,7 +22202,7 @@
         <v>430</v>
       </c>
       <c r="H24" s="17" t="b">
-        <f>AND(D24&gt;=E24, D24&lt;=F24)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22229,7 +22229,7 @@
         <v>430</v>
       </c>
       <c r="H25" s="17" t="b">
-        <f>AND(D25&gt;=E25, D25&lt;=F25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22256,7 +22256,7 @@
         <v>431</v>
       </c>
       <c r="H26" s="17" t="b">
-        <f>AND(D26&gt;=E26, D26&lt;=F26)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22283,7 +22283,7 @@
         <v>431</v>
       </c>
       <c r="H27" s="17" t="b">
-        <f>AND(D27&gt;=E27, D27&lt;=F27)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22310,7 +22310,7 @@
         <v>431</v>
       </c>
       <c r="H28" s="17" t="b">
-        <f>AND(D28&gt;=E28, D28&lt;=F28)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22337,7 +22337,7 @@
         <v>431</v>
       </c>
       <c r="H29" s="17" t="b">
-        <f>AND(D29&gt;=E29, D29&lt;=F29)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22364,7 +22364,7 @@
         <v>431</v>
       </c>
       <c r="H30" s="17" t="b">
-        <f>AND(D30&gt;=E30, D30&lt;=F30)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22391,7 +22391,7 @@
         <v>431</v>
       </c>
       <c r="H31" s="17" t="b">
-        <f>AND(D31&gt;=E31, D31&lt;=F31)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22418,7 +22418,7 @@
         <v>431</v>
       </c>
       <c r="H32" s="17" t="b">
-        <f>AND(D32&gt;=E32, D32&lt;=F32)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22445,7 +22445,7 @@
         <v>431</v>
       </c>
       <c r="H33" s="17" t="b">
-        <f>AND(D33&gt;=E33, D33&lt;=F33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -22472,7 +22472,7 @@
         <v>431</v>
       </c>
       <c r="H34" s="17" t="b">
-        <f>AND(D34&gt;=E34, D34&lt;=F34)</f>
+        <f t="shared" ref="H34:H59" si="1">AND(D34&gt;=E34, D34&lt;=F34)</f>
         <v>1</v>
       </c>
     </row>
@@ -22499,7 +22499,7 @@
         <v>432</v>
       </c>
       <c r="H35" s="17" t="b">
-        <f>AND(D35&gt;=E35, D35&lt;=F35)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22526,7 +22526,7 @@
         <v>432</v>
       </c>
       <c r="H36" s="17" t="b">
-        <f>AND(D36&gt;=E36, D36&lt;=F36)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I36" s="41"/>
@@ -22554,7 +22554,7 @@
         <v>432</v>
       </c>
       <c r="H37" s="17" t="b">
-        <f>AND(D37&gt;=E37, D37&lt;=F37)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22581,7 +22581,7 @@
         <v>432</v>
       </c>
       <c r="H38" s="17" t="b">
-        <f>AND(D38&gt;=E38, D38&lt;=F38)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22608,7 +22608,7 @@
         <v>432</v>
       </c>
       <c r="H39" s="17" t="b">
-        <f>AND(D39&gt;=E39, D39&lt;=F39)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22635,7 +22635,7 @@
         <v>432</v>
       </c>
       <c r="H40" s="17" t="b">
-        <f>AND(D40&gt;=E40, D40&lt;=F40)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22662,7 +22662,7 @@
         <v>431</v>
       </c>
       <c r="H41" s="17" t="b">
-        <f>AND(D41&gt;=E41, D41&lt;=F41)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22689,7 +22689,7 @@
         <v>431</v>
       </c>
       <c r="H42" s="17" t="b">
-        <f>AND(D42&gt;=E42, D42&lt;=F42)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22716,7 +22716,7 @@
         <v>431</v>
       </c>
       <c r="H43" s="17" t="b">
-        <f>AND(D43&gt;=E43, D43&lt;=F43)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22743,7 +22743,7 @@
         <v>431</v>
       </c>
       <c r="H44" s="17" t="b">
-        <f>AND(D44&gt;=E44, D44&lt;=F44)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22770,7 +22770,7 @@
         <v>431</v>
       </c>
       <c r="H45" s="17" t="b">
-        <f>AND(D45&gt;=E45, D45&lt;=F45)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22797,7 +22797,7 @@
         <v>431</v>
       </c>
       <c r="H46" s="17" t="b">
-        <f>AND(D46&gt;=E46, D46&lt;=F46)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22824,7 +22824,7 @@
         <v>431</v>
       </c>
       <c r="H47" s="17" t="b">
-        <f>AND(D47&gt;=E47, D47&lt;=F47)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22851,7 +22851,7 @@
         <v>431</v>
       </c>
       <c r="H48" s="17" t="b">
-        <f>AND(D48&gt;=E48, D48&lt;=F48)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22878,7 +22878,7 @@
         <v>431</v>
       </c>
       <c r="H49" s="17" t="b">
-        <f>AND(D49&gt;=E49, D49&lt;=F49)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22905,7 +22905,7 @@
         <v>431</v>
       </c>
       <c r="H50" s="17" t="b">
-        <f>AND(D50&gt;=E50, D50&lt;=F50)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22932,7 +22932,7 @@
         <v>431</v>
       </c>
       <c r="H51" s="17" t="b">
-        <f>AND(D51&gt;=E51, D51&lt;=F51)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22959,7 +22959,7 @@
         <v>431</v>
       </c>
       <c r="H52" s="17" t="b">
-        <f>AND(D52&gt;=E52, D52&lt;=F52)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22986,7 +22986,7 @@
         <v>430</v>
       </c>
       <c r="H53" s="17" t="b">
-        <f>AND(D53&gt;=E53, D53&lt;=F53)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -23013,7 +23013,7 @@
         <v>430</v>
       </c>
       <c r="H54" s="17" t="b">
-        <f>AND(D54&gt;=E54, D54&lt;=F54)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -23040,7 +23040,7 @@
         <v>430</v>
       </c>
       <c r="H55" s="17" t="b">
-        <f>AND(D55&gt;=E55, D55&lt;=F55)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -23067,7 +23067,7 @@
         <v>430</v>
       </c>
       <c r="H56" s="17" t="b">
-        <f>AND(D56&gt;=E56, D56&lt;=F56)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -23094,7 +23094,7 @@
         <v>430</v>
       </c>
       <c r="H57" s="17" t="b">
-        <f>AND(D57&gt;=E57, D57&lt;=F57)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -23121,7 +23121,7 @@
         <v>430</v>
       </c>
       <c r="H58" s="17" t="b">
-        <f>AND(D58&gt;=E58, D58&lt;=F58)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -23148,7 +23148,7 @@
         <v>430</v>
       </c>
       <c r="H59" s="17" t="b">
-        <f>AND(D59&gt;=E59, D59&lt;=F59)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
why did that not work
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -1482,7 +1482,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1675,6 +1675,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1821,7 +1837,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6302">
+  <cellStyleXfs count="6412">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -8124,8 +8140,118 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8207,8 +8333,9 @@
     <xf numFmtId="10" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6302">
+  <cellStyles count="6412">
     <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
     <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
     <cellStyle name="60% - Accent5" xfId="6" builtinId="48"/>
@@ -11307,6 +11434,61 @@
     <cellStyle name="Followed Hyperlink" xfId="6297" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6299" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6307" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6309" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6311" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6313" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6343" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6355" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6357" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6359" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6361" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6411" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="70"/>
     <cellStyle name="Followed Hyperlink 11" xfId="71"/>
     <cellStyle name="Followed Hyperlink 12" xfId="72"/>
@@ -14487,6 +14669,61 @@
     <cellStyle name="Hyperlink" xfId="6296" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6298" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6306" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6308" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6310" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6312" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6316" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6318" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6340" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6342" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6344" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6346" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6348" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6350" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6352" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6354" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6356" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6358" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6360" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6362" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6364" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6374" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6376" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6378" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6380" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6382" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6384" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6386" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6388" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6396" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6398" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6400" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6404" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6406" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6408" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6410" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="45"/>
@@ -20542,7 +20779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
@@ -21547,8 +21784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22974,13 +23211,13 @@
         <v>378</v>
       </c>
       <c r="D53" s="43">
-        <v>0.15</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="E53" s="43">
-        <v>0.1</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="F53" s="43">
-        <v>0.21</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="G53" t="s">
         <v>430</v>
@@ -23001,13 +23238,13 @@
         <v>379</v>
       </c>
       <c r="D54" s="43">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E54" s="43">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F54" s="43">
-        <v>0.01</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="G54" t="s">
         <v>430</v>
@@ -23027,14 +23264,14 @@
       <c r="C55" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="D55" s="43">
+      <c r="D55" s="45">
         <v>0.02</v>
       </c>
       <c r="E55" s="43">
-        <v>0.01</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="F55" s="43">
-        <v>0.03</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="G55" t="s">
         <v>430</v>
@@ -23054,14 +23291,14 @@
       <c r="C56" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="D56" s="43">
+      <c r="D56" s="45">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E56" s="43">
-        <v>0.05</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="F56" s="43">
-        <v>0.09</v>
+        <v>9.4E-2</v>
       </c>
       <c r="G56" t="s">
         <v>430</v>
@@ -23082,13 +23319,13 @@
         <v>382</v>
       </c>
       <c r="D57" s="43">
-        <v>0.27</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="E57" s="43">
-        <v>0.11</v>
+        <v>0.114</v>
       </c>
       <c r="F57" s="43">
-        <v>0.47</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="G57" t="s">
         <v>430</v>
@@ -23109,13 +23346,13 @@
         <v>383</v>
       </c>
       <c r="D58" s="43">
-        <v>0.55000000000000004</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="E58" s="43">
-        <v>0.38</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="F58" s="43">
-        <v>0.72</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="G58" t="s">
         <v>430</v>
@@ -23136,13 +23373,13 @@
         <v>384</v>
       </c>
       <c r="D59" s="43">
-        <v>0.05</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E59" s="43">
-        <v>0.03</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="F59" s="43">
-        <v>0.08</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="G59" t="s">
         <v>430</v>

</xml_diff>

<commit_message>
removed mentions of coverage
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="27480" windowHeight="15465" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="483">
   <si>
     <t>Susceptible</t>
   </si>
@@ -1255,9 +1255,6 @@
   </si>
   <si>
     <t>manual</t>
-  </si>
-  <si>
-    <t>targetable</t>
   </si>
   <si>
     <t>advanced</t>
@@ -15092,17 +15089,17 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -15228,10 +15225,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>482</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -17660,11 +17657,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17675,13 +17672,11 @@
     <col min="4" max="4" width="8.5703125" style="5" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="8" customWidth="1"/>
     <col min="6" max="6" width="10" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="7" max="7" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>77</v>
       </c>
@@ -17700,18 +17695,12 @@
       <c r="F1" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>412</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="39"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H1" s="39"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>87</v>
       </c>
@@ -17731,21 +17720,15 @@
         <v>89</v>
       </c>
       <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>95</v>
@@ -17762,19 +17745,13 @@
       <c r="G3" s="6">
         <v>0</v>
       </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>95</v>
@@ -17791,14 +17768,8 @@
       <c r="G4" s="6">
         <v>0</v>
       </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>91</v>
       </c>
@@ -17818,16 +17789,10 @@
         <v>93</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>108</v>
       </c>
@@ -17849,14 +17814,8 @@
       <c r="G6" s="6">
         <v>1</v>
       </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>111</v>
       </c>
@@ -17878,14 +17837,8 @@
       <c r="G7" s="6">
         <v>1</v>
       </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>113</v>
       </c>
@@ -17907,14 +17860,8 @@
       <c r="G8" s="6">
         <v>1</v>
       </c>
-      <c r="H8" s="6">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>116</v>
       </c>
@@ -17936,14 +17883,8 @@
       <c r="G9" s="6">
         <v>1</v>
       </c>
-      <c r="H9" s="6">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>118</v>
       </c>
@@ -17965,14 +17906,8 @@
       <c r="G10" s="6">
         <v>1</v>
       </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>120</v>
       </c>
@@ -17994,14 +17929,8 @@
       <c r="G11" s="6">
         <v>1</v>
       </c>
-      <c r="H11" s="6">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>122</v>
       </c>
@@ -18023,14 +17952,8 @@
       <c r="G12" s="6">
         <v>1</v>
       </c>
-      <c r="H12" s="6">
-        <v>1</v>
-      </c>
-      <c r="I12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>138</v>
       </c>
@@ -18052,14 +17975,8 @@
       <c r="G13" s="6">
         <v>1</v>
       </c>
-      <c r="H13" s="6">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>124</v>
       </c>
@@ -18081,14 +17998,8 @@
       <c r="G14" s="6">
         <v>1</v>
       </c>
-      <c r="H14" s="6">
-        <v>0</v>
-      </c>
-      <c r="I14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>126</v>
       </c>
@@ -18110,14 +18021,8 @@
       <c r="G15" s="6">
         <v>1</v>
       </c>
-      <c r="H15" s="6">
-        <v>0</v>
-      </c>
-      <c r="I15" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>196</v>
       </c>
@@ -18139,14 +18044,8 @@
       <c r="G16" s="6">
         <v>1</v>
       </c>
-      <c r="H16" s="6">
-        <v>0</v>
-      </c>
-      <c r="I16" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>162</v>
       </c>
@@ -18168,14 +18067,8 @@
       <c r="G17" s="6">
         <v>1</v>
       </c>
-      <c r="H17" s="6">
-        <v>0</v>
-      </c>
-      <c r="I17" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>166</v>
       </c>
@@ -18197,14 +18090,8 @@
       <c r="G18" s="6">
         <v>1</v>
       </c>
-      <c r="H18" s="6">
-        <v>0</v>
-      </c>
-      <c r="I18" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>169</v>
       </c>
@@ -18226,14 +18113,8 @@
       <c r="G19" s="6">
         <v>1</v>
       </c>
-      <c r="H19" s="6">
-        <v>0</v>
-      </c>
-      <c r="I19" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>171</v>
       </c>
@@ -18255,16 +18136,10 @@
       <c r="G20" s="6">
         <v>1</v>
       </c>
-      <c r="H20" s="6">
-        <v>0</v>
-      </c>
-      <c r="I20" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>167</v>
@@ -18284,14 +18159,8 @@
       <c r="G21" s="14">
         <v>1</v>
       </c>
-      <c r="H21" s="14">
-        <v>1</v>
-      </c>
-      <c r="I21" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>173</v>
       </c>
@@ -18311,16 +18180,10 @@
         <v>102</v>
       </c>
       <c r="G22" s="6">
-        <v>1</v>
-      </c>
-      <c r="H22" s="6">
         <v>0</v>
       </c>
-      <c r="I22" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>175</v>
       </c>
@@ -18340,16 +18203,10 @@
         <v>102</v>
       </c>
       <c r="G23" s="6">
-        <v>1</v>
-      </c>
-      <c r="H23" s="6">
         <v>0</v>
       </c>
-      <c r="I23" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>177</v>
       </c>
@@ -18369,16 +18226,10 @@
         <v>102</v>
       </c>
       <c r="G24" s="6">
-        <v>1</v>
-      </c>
-      <c r="H24" s="6">
         <v>0</v>
       </c>
-      <c r="I24" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>179</v>
       </c>
@@ -18398,16 +18249,10 @@
         <v>102</v>
       </c>
       <c r="G25" s="6">
-        <v>1</v>
-      </c>
-      <c r="H25" s="6">
         <v>0</v>
       </c>
-      <c r="I25" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>181</v>
       </c>
@@ -18427,16 +18272,10 @@
         <v>102</v>
       </c>
       <c r="G26" s="6">
-        <v>1</v>
-      </c>
-      <c r="H26" s="6">
         <v>0</v>
       </c>
-      <c r="I26" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>183</v>
       </c>
@@ -18458,14 +18297,8 @@
       <c r="G27" s="6">
         <v>0</v>
       </c>
-      <c r="H27" s="6">
-        <v>0</v>
-      </c>
-      <c r="I27" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>188</v>
       </c>
@@ -18487,14 +18320,8 @@
       <c r="G28" s="6">
         <v>0</v>
       </c>
-      <c r="H28" s="6">
-        <v>0</v>
-      </c>
-      <c r="I28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>190</v>
       </c>
@@ -18516,14 +18343,8 @@
       <c r="G29" s="6">
         <v>0</v>
       </c>
-      <c r="H29" s="6">
-        <v>0</v>
-      </c>
-      <c r="I29" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>192</v>
       </c>
@@ -18545,14 +18366,8 @@
       <c r="G30" s="6">
         <v>0</v>
       </c>
-      <c r="H30" s="6">
-        <v>0</v>
-      </c>
-      <c r="I30" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>194</v>
       </c>
@@ -18574,14 +18389,8 @@
       <c r="G31" s="6">
         <v>0</v>
       </c>
-      <c r="H31" s="6">
-        <v>0</v>
-      </c>
-      <c r="I31" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>132</v>
       </c>
@@ -18601,16 +18410,10 @@
         <v>102</v>
       </c>
       <c r="G32" s="6">
-        <v>1</v>
-      </c>
-      <c r="H32" s="6">
-        <v>1</v>
-      </c>
-      <c r="I32" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>129</v>
       </c>
@@ -18632,14 +18435,8 @@
       <c r="G33" s="6">
         <v>1</v>
       </c>
-      <c r="H33" s="6">
-        <v>0</v>
-      </c>
-      <c r="I33" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>140</v>
       </c>
@@ -18661,14 +18458,8 @@
       <c r="G34" s="6">
         <v>1</v>
       </c>
-      <c r="H34" s="6">
-        <v>0</v>
-      </c>
-      <c r="I34" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>145</v>
       </c>
@@ -18690,14 +18481,8 @@
       <c r="G35" s="6">
         <v>1</v>
       </c>
-      <c r="H35" s="6">
-        <v>0</v>
-      </c>
-      <c r="I35" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>148</v>
       </c>
@@ -18719,14 +18504,8 @@
       <c r="G36" s="6">
         <v>1</v>
       </c>
-      <c r="H36" s="6">
-        <v>0</v>
-      </c>
-      <c r="I36" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>154</v>
       </c>
@@ -18748,14 +18527,8 @@
       <c r="G37" s="6">
         <v>1</v>
       </c>
-      <c r="H37" s="6">
-        <v>0</v>
-      </c>
-      <c r="I37" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>156</v>
       </c>
@@ -18777,14 +18550,8 @@
       <c r="G38" s="6">
         <v>1</v>
       </c>
-      <c r="H38" s="6">
-        <v>0</v>
-      </c>
-      <c r="I38" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>159</v>
       </c>
@@ -18806,14 +18573,8 @@
       <c r="G39" s="6">
         <v>1</v>
       </c>
-      <c r="H39" s="6">
-        <v>0</v>
-      </c>
-      <c r="I39" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>151</v>
       </c>
@@ -18835,14 +18596,8 @@
       <c r="G40" s="6">
         <v>1</v>
       </c>
-      <c r="H40" s="6">
-        <v>0</v>
-      </c>
-      <c r="I40" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>134</v>
       </c>
@@ -18864,14 +18619,8 @@
       <c r="G41" s="6">
         <v>1</v>
       </c>
-      <c r="H41" s="6">
-        <v>1</v>
-      </c>
-      <c r="I41" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>136</v>
       </c>
@@ -18893,14 +18642,8 @@
       <c r="G42" s="6">
         <v>1</v>
       </c>
-      <c r="H42" s="6">
-        <v>0</v>
-      </c>
-      <c r="I42" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>99</v>
       </c>
@@ -18920,16 +18663,10 @@
         <v>102</v>
       </c>
       <c r="G43" s="6">
-        <v>0</v>
-      </c>
-      <c r="H43" s="6">
-        <v>0</v>
-      </c>
-      <c r="I43" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>104</v>
       </c>
@@ -18949,16 +18686,10 @@
         <v>102</v>
       </c>
       <c r="G44" s="6">
-        <v>0</v>
-      </c>
-      <c r="H44" s="6">
-        <v>0</v>
-      </c>
-      <c r="I44" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>106</v>
       </c>
@@ -18978,21 +18709,15 @@
         <v>102</v>
       </c>
       <c r="G45" s="6">
-        <v>0</v>
-      </c>
-      <c r="H45" s="6">
-        <v>0</v>
-      </c>
-      <c r="I45" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>95</v>
@@ -19009,14 +18734,8 @@
       <c r="G46" s="6">
         <v>0</v>
       </c>
-      <c r="H46" s="6">
-        <v>0</v>
-      </c>
-      <c r="I46" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>199</v>
       </c>
@@ -19036,16 +18755,10 @@
         <v>200</v>
       </c>
       <c r="G47" s="6">
-        <v>0</v>
-      </c>
-      <c r="H47" s="6">
-        <v>0</v>
-      </c>
-      <c r="I47" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>202</v>
       </c>
@@ -19065,16 +18778,10 @@
         <v>200</v>
       </c>
       <c r="G48" s="6">
-        <v>0</v>
-      </c>
-      <c r="H48" s="6">
-        <v>0</v>
-      </c>
-      <c r="I48" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>204</v>
       </c>
@@ -19094,16 +18801,10 @@
         <v>200</v>
       </c>
       <c r="G49" s="6">
-        <v>0</v>
-      </c>
-      <c r="H49" s="6">
-        <v>0</v>
-      </c>
-      <c r="I49" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>206</v>
       </c>
@@ -19123,16 +18824,10 @@
         <v>200</v>
       </c>
       <c r="G50" s="6">
-        <v>0</v>
-      </c>
-      <c r="H50" s="6">
-        <v>0</v>
-      </c>
-      <c r="I50" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>208</v>
       </c>
@@ -19152,16 +18847,10 @@
         <v>200</v>
       </c>
       <c r="G51" s="6">
-        <v>0</v>
-      </c>
-      <c r="H51" s="6">
-        <v>0</v>
-      </c>
-      <c r="I51" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>210</v>
       </c>
@@ -19181,16 +18870,10 @@
         <v>200</v>
       </c>
       <c r="G52" s="6">
-        <v>0</v>
-      </c>
-      <c r="H52" s="6">
-        <v>0</v>
-      </c>
-      <c r="I52" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>212</v>
       </c>
@@ -19210,16 +18893,10 @@
         <v>200</v>
       </c>
       <c r="G53" s="6">
-        <v>0</v>
-      </c>
-      <c r="H53" s="6">
-        <v>0</v>
-      </c>
-      <c r="I53" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>214</v>
       </c>
@@ -19239,16 +18916,10 @@
         <v>200</v>
       </c>
       <c r="G54" s="6">
-        <v>0</v>
-      </c>
-      <c r="H54" s="6">
-        <v>0</v>
-      </c>
-      <c r="I54" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>216</v>
       </c>
@@ -19268,16 +18939,10 @@
         <v>200</v>
       </c>
       <c r="G55" s="6">
-        <v>0</v>
-      </c>
-      <c r="H55" s="6">
-        <v>0</v>
-      </c>
-      <c r="I55" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>218</v>
       </c>
@@ -19297,16 +18962,10 @@
         <v>200</v>
       </c>
       <c r="G56" s="6">
-        <v>0</v>
-      </c>
-      <c r="H56" s="6">
-        <v>0</v>
-      </c>
-      <c r="I56" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>220</v>
       </c>
@@ -19326,16 +18985,10 @@
         <v>200</v>
       </c>
       <c r="G57" s="6">
-        <v>0</v>
-      </c>
-      <c r="H57" s="6">
-        <v>0</v>
-      </c>
-      <c r="I57" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>222</v>
       </c>
@@ -19355,16 +19008,10 @@
         <v>200</v>
       </c>
       <c r="G58" s="6">
-        <v>0</v>
-      </c>
-      <c r="H58" s="6">
-        <v>0</v>
-      </c>
-      <c r="I58" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>224</v>
       </c>
@@ -19384,16 +19031,10 @@
         <v>200</v>
       </c>
       <c r="G59" s="6">
-        <v>0</v>
-      </c>
-      <c r="H59" s="6">
-        <v>0</v>
-      </c>
-      <c r="I59" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>226</v>
       </c>
@@ -19413,16 +19054,10 @@
         <v>200</v>
       </c>
       <c r="G60" s="6">
-        <v>0</v>
-      </c>
-      <c r="H60" s="6">
-        <v>0</v>
-      </c>
-      <c r="I60" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>228</v>
       </c>
@@ -19442,16 +19077,10 @@
         <v>200</v>
       </c>
       <c r="G61" s="6">
-        <v>0</v>
-      </c>
-      <c r="H61" s="6">
-        <v>0</v>
-      </c>
-      <c r="I61" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>230</v>
       </c>
@@ -19471,16 +19100,10 @@
         <v>200</v>
       </c>
       <c r="G62" s="6">
-        <v>0</v>
-      </c>
-      <c r="H62" s="6">
-        <v>0</v>
-      </c>
-      <c r="I62" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>232</v>
       </c>
@@ -19500,16 +19123,10 @@
         <v>200</v>
       </c>
       <c r="G63" s="6">
-        <v>0</v>
-      </c>
-      <c r="H63" s="6">
-        <v>0</v>
-      </c>
-      <c r="I63" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>234</v>
       </c>
@@ -19529,16 +19146,10 @@
         <v>200</v>
       </c>
       <c r="G64" s="6">
-        <v>0</v>
-      </c>
-      <c r="H64" s="6">
-        <v>0</v>
-      </c>
-      <c r="I64" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>236</v>
       </c>
@@ -19558,16 +19169,10 @@
         <v>200</v>
       </c>
       <c r="G65" s="6">
-        <v>0</v>
-      </c>
-      <c r="H65" s="6">
-        <v>0</v>
-      </c>
-      <c r="I65" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>238</v>
       </c>
@@ -19587,16 +19192,10 @@
         <v>200</v>
       </c>
       <c r="G66" s="6">
-        <v>0</v>
-      </c>
-      <c r="H66" s="6">
-        <v>0</v>
-      </c>
-      <c r="I66" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>240</v>
       </c>
@@ -19616,16 +19215,10 @@
         <v>200</v>
       </c>
       <c r="G67" s="6">
-        <v>0</v>
-      </c>
-      <c r="H67" s="6">
-        <v>0</v>
-      </c>
-      <c r="I67" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>242</v>
       </c>
@@ -19645,16 +19238,10 @@
         <v>200</v>
       </c>
       <c r="G68" s="6">
-        <v>0</v>
-      </c>
-      <c r="H68" s="6">
-        <v>0</v>
-      </c>
-      <c r="I68" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>244</v>
       </c>
@@ -19674,16 +19261,10 @@
         <v>200</v>
       </c>
       <c r="G69" s="6">
-        <v>0</v>
-      </c>
-      <c r="H69" s="6">
-        <v>0</v>
-      </c>
-      <c r="I69" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>246</v>
       </c>
@@ -19703,21 +19284,15 @@
         <v>200</v>
       </c>
       <c r="G70" s="6">
-        <v>0</v>
-      </c>
-      <c r="H70" s="6">
-        <v>0</v>
-      </c>
-      <c r="I70" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>142</v>
@@ -19732,16 +19307,10 @@
         <v>200</v>
       </c>
       <c r="G71" s="14">
-        <v>0</v>
-      </c>
-      <c r="H71" s="14">
-        <v>0</v>
-      </c>
-      <c r="I71" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>248</v>
       </c>
@@ -19758,19 +19327,13 @@
         <v>198</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G72" s="6">
-        <v>0</v>
-      </c>
-      <c r="H72" s="6">
-        <v>0</v>
-      </c>
-      <c r="I72" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>250</v>
       </c>
@@ -19787,19 +19350,13 @@
         <v>198</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G73" s="6">
-        <v>0</v>
-      </c>
-      <c r="H73" s="6">
-        <v>0</v>
-      </c>
-      <c r="I73" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>252</v>
       </c>
@@ -19816,19 +19373,13 @@
         <v>198</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G74" s="6">
-        <v>0</v>
-      </c>
-      <c r="H74" s="6">
-        <v>0</v>
-      </c>
-      <c r="I74" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>254</v>
       </c>
@@ -19845,19 +19396,13 @@
         <v>198</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G75" s="6">
-        <v>0</v>
-      </c>
-      <c r="H75" s="6">
-        <v>0</v>
-      </c>
-      <c r="I75" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>256</v>
       </c>
@@ -19874,19 +19419,13 @@
         <v>198</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G76" s="6">
-        <v>0</v>
-      </c>
-      <c r="H76" s="6">
-        <v>0</v>
-      </c>
-      <c r="I76" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>258</v>
       </c>
@@ -19903,19 +19442,13 @@
         <v>198</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G77" s="6">
-        <v>0</v>
-      </c>
-      <c r="H77" s="6">
-        <v>0</v>
-      </c>
-      <c r="I77" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>260</v>
       </c>
@@ -19932,19 +19465,13 @@
         <v>198</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G78" s="6">
-        <v>0</v>
-      </c>
-      <c r="H78" s="6">
-        <v>0</v>
-      </c>
-      <c r="I78" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>262</v>
       </c>
@@ -19961,19 +19488,13 @@
         <v>198</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G79" s="6">
-        <v>0</v>
-      </c>
-      <c r="H79" s="6">
-        <v>0</v>
-      </c>
-      <c r="I79" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>264</v>
       </c>
@@ -19990,19 +19511,13 @@
         <v>198</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G80" s="6">
-        <v>0</v>
-      </c>
-      <c r="H80" s="6">
-        <v>0</v>
-      </c>
-      <c r="I80" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>266</v>
       </c>
@@ -20019,19 +19534,13 @@
         <v>198</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G81" s="6">
-        <v>0</v>
-      </c>
-      <c r="H81" s="6">
-        <v>0</v>
-      </c>
-      <c r="I81" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>268</v>
       </c>
@@ -20048,19 +19557,13 @@
         <v>198</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G82" s="6">
-        <v>0</v>
-      </c>
-      <c r="H82" s="6">
-        <v>0</v>
-      </c>
-      <c r="I82" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>270</v>
       </c>
@@ -20077,19 +19580,13 @@
         <v>198</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G83" s="6">
-        <v>0</v>
-      </c>
-      <c r="H83" s="6">
-        <v>0</v>
-      </c>
-      <c r="I83" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>272</v>
       </c>
@@ -20106,24 +19603,18 @@
         <v>198</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G84" s="6">
-        <v>0</v>
-      </c>
-      <c r="H84" s="6">
-        <v>0</v>
-      </c>
-      <c r="I84" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>273</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>100</v>
@@ -20138,21 +19629,15 @@
         <v>200</v>
       </c>
       <c r="G85" s="6">
-        <v>0</v>
-      </c>
-      <c r="H85" s="6">
-        <v>0</v>
-      </c>
-      <c r="I85" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>274</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>100</v>
@@ -20167,16 +19652,10 @@
         <v>200</v>
       </c>
       <c r="G86" s="6">
-        <v>0</v>
-      </c>
-      <c r="H86" s="6">
-        <v>0</v>
-      </c>
-      <c r="I86" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>276</v>
       </c>
@@ -20196,16 +19675,10 @@
         <v>200</v>
       </c>
       <c r="G87" s="6">
-        <v>0</v>
-      </c>
-      <c r="H87" s="6">
-        <v>0</v>
-      </c>
-      <c r="I87" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>278</v>
       </c>
@@ -20225,16 +19698,10 @@
         <v>200</v>
       </c>
       <c r="G88" s="6">
-        <v>0</v>
-      </c>
-      <c r="H88" s="6">
-        <v>0</v>
-      </c>
-      <c r="I88" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>280</v>
       </c>
@@ -20251,19 +19718,13 @@
         <v>198</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G89" s="6">
-        <v>0</v>
-      </c>
-      <c r="H89" s="6">
-        <v>0</v>
-      </c>
-      <c r="I89" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>282</v>
       </c>
@@ -20283,16 +19744,10 @@
         <v>200</v>
       </c>
       <c r="G90" s="6">
-        <v>0</v>
-      </c>
-      <c r="H90" s="6">
-        <v>0</v>
-      </c>
-      <c r="I90" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>284</v>
       </c>
@@ -20312,16 +19767,10 @@
         <v>200</v>
       </c>
       <c r="G91" s="6">
-        <v>0</v>
-      </c>
-      <c r="H91" s="6">
-        <v>0</v>
-      </c>
-      <c r="I91" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>286</v>
       </c>
@@ -20341,16 +19790,10 @@
         <v>200</v>
       </c>
       <c r="G92" s="6">
-        <v>0</v>
-      </c>
-      <c r="H92" s="6">
-        <v>0</v>
-      </c>
-      <c r="I92" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>288</v>
       </c>
@@ -20370,16 +19813,10 @@
         <v>200</v>
       </c>
       <c r="G93" s="6">
-        <v>0</v>
-      </c>
-      <c r="H93" s="6">
-        <v>0</v>
-      </c>
-      <c r="I93" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>290</v>
       </c>
@@ -20399,16 +19836,10 @@
         <v>200</v>
       </c>
       <c r="G94" s="6">
-        <v>0</v>
-      </c>
-      <c r="H94" s="6">
-        <v>0</v>
-      </c>
-      <c r="I94" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>292</v>
       </c>
@@ -20428,16 +19859,10 @@
         <v>200</v>
       </c>
       <c r="G95" s="6">
-        <v>0</v>
-      </c>
-      <c r="H95" s="6">
-        <v>0</v>
-      </c>
-      <c r="I95" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>294</v>
       </c>
@@ -20457,16 +19882,10 @@
         <v>200</v>
       </c>
       <c r="G96" s="6">
-        <v>0</v>
-      </c>
-      <c r="H96" s="6">
-        <v>0</v>
-      </c>
-      <c r="I96" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>296</v>
       </c>
@@ -20486,16 +19905,10 @@
         <v>200</v>
       </c>
       <c r="G97" s="6">
-        <v>0</v>
-      </c>
-      <c r="H97" s="6">
-        <v>0</v>
-      </c>
-      <c r="I97" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>298</v>
       </c>
@@ -20512,19 +19925,13 @@
         <v>198</v>
       </c>
       <c r="F98" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G98" s="6">
-        <v>0</v>
-      </c>
-      <c r="H98" s="6">
-        <v>0</v>
-      </c>
-      <c r="I98" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>300</v>
       </c>
@@ -20541,19 +19948,13 @@
         <v>198</v>
       </c>
       <c r="F99" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G99" s="6">
-        <v>0</v>
-      </c>
-      <c r="H99" s="6">
-        <v>0</v>
-      </c>
-      <c r="I99" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>302</v>
       </c>
@@ -20570,19 +19971,13 @@
         <v>198</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G100" s="6">
-        <v>0</v>
-      </c>
-      <c r="H100" s="6">
-        <v>0</v>
-      </c>
-      <c r="I100" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>304</v>
       </c>
@@ -20599,19 +19994,13 @@
         <v>198</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G101" s="6">
-        <v>0</v>
-      </c>
-      <c r="H101" s="6">
-        <v>0</v>
-      </c>
-      <c r="I101" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>306</v>
       </c>
@@ -20628,19 +20017,13 @@
         <v>198</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G102" s="6">
-        <v>0</v>
-      </c>
-      <c r="H102" s="6">
-        <v>0</v>
-      </c>
-      <c r="I102" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>308</v>
       </c>
@@ -20657,19 +20040,13 @@
         <v>198</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G103" s="6">
-        <v>0</v>
-      </c>
-      <c r="H103" s="6">
-        <v>0</v>
-      </c>
-      <c r="I103" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>310</v>
       </c>
@@ -20686,50 +20063,44 @@
         <v>198</v>
       </c>
       <c r="F104" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G104" s="6">
-        <v>0</v>
-      </c>
-      <c r="H104" s="6">
-        <v>0</v>
-      </c>
-      <c r="I104" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D105" s="6"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D106" s="6"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
       <c r="E107" s="6"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
       <c r="E109" s="6"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C110" s="6"/>
       <c r="D110" s="6"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
       <c r="E111" s="6"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
       <c r="E112" s="6"/>
@@ -20808,10 +20179,10 @@
         <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -20825,13 +20196,13 @@
         <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -20848,10 +20219,10 @@
         <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -20868,10 +20239,10 @@
         <v>327</v>
       </c>
       <c r="E4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -20885,13 +20256,13 @@
         <v>108</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -20905,13 +20276,13 @@
         <v>116</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -20928,10 +20299,10 @@
         <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -20945,13 +20316,13 @@
         <v>111</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -20965,13 +20336,13 @@
         <v>113</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -20988,10 +20359,10 @@
         <v>119</v>
       </c>
       <c r="E10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -21008,10 +20379,10 @@
         <v>195</v>
       </c>
       <c r="E11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -21025,13 +20396,13 @@
         <v>138</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -21045,13 +20416,13 @@
         <v>122</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E13" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F13" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -21065,13 +20436,13 @@
         <v>126</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -21085,13 +20456,13 @@
         <v>124</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F15" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -21105,13 +20476,13 @@
         <v>311</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E16" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F16" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -21125,13 +20496,13 @@
         <v>312</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -21145,13 +20516,13 @@
         <v>313</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E18" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F18" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -21162,16 +20533,16 @@
         <v>329</v>
       </c>
       <c r="C19" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E19" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F19" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -21185,13 +20556,13 @@
         <v>314</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F20" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -21205,13 +20576,13 @@
         <v>315</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F21" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -21225,13 +20596,13 @@
         <v>316</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E22" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -21245,13 +20616,13 @@
         <v>317</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E23" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F23" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -21265,13 +20636,13 @@
         <v>318</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E24" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F24" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -21285,13 +20656,13 @@
         <v>319</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E25" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F25" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -21305,13 +20676,13 @@
         <v>320</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F26" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -21325,13 +20696,13 @@
         <v>321</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E27" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F27" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -21348,10 +20719,10 @@
         <v>161</v>
       </c>
       <c r="E28" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -21368,10 +20739,10 @@
         <v>165</v>
       </c>
       <c r="E29" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -21385,13 +20756,13 @@
         <v>169</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E30" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -21405,13 +20776,13 @@
         <v>171</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E31" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F31" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -21422,16 +20793,16 @@
         <v>329</v>
       </c>
       <c r="C32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D32" s="38" t="s">
         <v>167</v>
       </c>
       <c r="E32" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F32" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -21445,13 +20816,13 @@
         <v>141</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E33" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -21465,13 +20836,13 @@
         <v>146</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E34" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F34" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -21485,13 +20856,13 @@
         <v>149</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F35" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -21502,16 +20873,16 @@
         <v>329</v>
       </c>
       <c r="C36" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -21525,13 +20896,13 @@
         <v>157</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E37" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F37" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -21545,13 +20916,13 @@
         <v>160</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E38" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F38" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -21565,13 +20936,13 @@
         <v>129</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E39" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F39" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -21585,13 +20956,13 @@
         <v>152</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E40" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F40" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -21605,13 +20976,13 @@
         <v>136</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E41" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F41" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -21625,13 +20996,13 @@
         <v>134</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E42" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -21639,19 +21010,19 @@
         <v>338</v>
       </c>
       <c r="B43" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C43" t="s">
         <v>322</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E43" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -21659,19 +21030,19 @@
         <v>338</v>
       </c>
       <c r="B44" t="s">
+        <v>424</v>
+      </c>
+      <c r="C44" t="s">
         <v>425</v>
       </c>
-      <c r="C44" t="s">
-        <v>426</v>
-      </c>
       <c r="D44" s="38" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E44" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -21679,19 +21050,19 @@
         <v>338</v>
       </c>
       <c r="B45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C45" t="s">
         <v>323</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E45" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -21699,19 +21070,19 @@
         <v>338</v>
       </c>
       <c r="B46" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C46" t="s">
         <v>324</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E46" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F46" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -21719,19 +21090,19 @@
         <v>338</v>
       </c>
       <c r="B47" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C47" t="s">
         <v>106</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F47" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -21739,19 +21110,19 @@
         <v>338</v>
       </c>
       <c r="B48" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C48" t="s">
         <v>104</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -21759,19 +21130,19 @@
         <v>338</v>
       </c>
       <c r="B49" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C49" t="s">
         <v>99</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E49" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F49" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -21784,7 +21155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
@@ -21816,7 +21187,7 @@
         <v>343</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>392</v>
@@ -21842,7 +21213,7 @@
         <v>1.4E-3</v>
       </c>
       <c r="G2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H2" s="17" t="b">
         <f t="shared" ref="H2:H33" si="0">AND(D2&gt;=E2, D2&lt;=F2)</f>
@@ -21869,7 +21240,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="G3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H3" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21896,7 +21267,7 @@
         <v>2.8E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H4" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21923,7 +21294,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
       <c r="G5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H5" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21950,7 +21321,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="G6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H6" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21977,7 +21348,7 @@
         <v>0.44</v>
       </c>
       <c r="G7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H7" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22004,7 +21375,7 @@
         <v>0.27</v>
       </c>
       <c r="G8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H8" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22031,7 +21402,7 @@
         <v>9.1</v>
       </c>
       <c r="G9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H9" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22058,7 +21429,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H10" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22085,7 +21456,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H11" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22112,7 +21483,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H12" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22139,7 +21510,7 @@
         <v>6.92</v>
       </c>
       <c r="G13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H13" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22166,7 +21537,7 @@
         <v>12.08</v>
       </c>
       <c r="G14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H14" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22193,7 +21564,7 @@
         <v>0.5</v>
       </c>
       <c r="G15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H15" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22220,7 +21591,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="G16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H16" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22247,7 +21618,7 @@
         <v>3.16</v>
       </c>
       <c r="G17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H17" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22274,7 +21645,7 @@
         <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H18" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22301,7 +21672,7 @@
         <v>2.25</v>
       </c>
       <c r="G19" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H19" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22328,7 +21699,7 @@
         <v>7.28</v>
       </c>
       <c r="G20" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H20" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22355,7 +21726,7 @@
         <v>3.42</v>
       </c>
       <c r="G21" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H21" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22382,7 +21753,7 @@
         <v>3.58</v>
       </c>
       <c r="G22" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H22" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22409,7 +21780,7 @@
         <v>0.94</v>
       </c>
       <c r="G23" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H23" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22436,7 +21807,7 @@
         <v>0.3</v>
       </c>
       <c r="G24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H24" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22448,10 +21819,10 @@
         <v>389</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D25" s="43">
         <v>2</v>
@@ -22463,7 +21834,7 @@
         <v>2.5</v>
       </c>
       <c r="G25" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H25" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22490,7 +21861,7 @@
         <v>0.27500000000000002</v>
       </c>
       <c r="G26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H26" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22517,7 +21888,7 @@
         <v>0.88500000000000001</v>
       </c>
       <c r="G27" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H27" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22544,7 +21915,7 @@
         <v>0.87</v>
       </c>
       <c r="G28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H28" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22571,7 +21942,7 @@
         <v>0.82699999999999996</v>
       </c>
       <c r="G29" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H29" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22598,7 +21969,7 @@
         <v>0.86899999999999999</v>
       </c>
       <c r="G30" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H30" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22625,7 +21996,7 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="G31" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H31" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22652,7 +22023,7 @@
         <v>0.72299999999999998</v>
       </c>
       <c r="G32" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H32" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22679,7 +22050,7 @@
         <v>0.56299999999999994</v>
       </c>
       <c r="G33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H33" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22706,7 +22077,7 @@
         <v>0.26</v>
       </c>
       <c r="G34" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H34" s="17" t="b">
         <f t="shared" ref="H34:H59" si="1">AND(D34&gt;=E34, D34&lt;=F34)</f>
@@ -22733,7 +22104,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="G35" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H35" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22760,7 +22131,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="G36" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H36" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22788,7 +22159,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="G37" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H37" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22815,7 +22186,7 @@
         <v>1.01E-2</v>
       </c>
       <c r="G38" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H38" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22842,7 +22213,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="G39" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H39" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22869,7 +22240,7 @@
         <v>0.432</v>
       </c>
       <c r="G40" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H40" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22896,7 +22267,7 @@
         <v>0.3</v>
       </c>
       <c r="G41" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H41" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22923,7 +22294,7 @@
         <v>0.8417</v>
       </c>
       <c r="G42" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H42" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22950,7 +22321,7 @@
         <v>3.71</v>
       </c>
       <c r="G43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H43" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22977,7 +22348,7 @@
         <v>0.98</v>
       </c>
       <c r="G44" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H44" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23004,7 +22375,7 @@
         <v>0.67</v>
       </c>
       <c r="G45" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H45" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23031,7 +22402,7 @@
         <v>0.68</v>
       </c>
       <c r="G46" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H46" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23058,7 +22429,7 @@
         <v>5.19</v>
       </c>
       <c r="G47" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H47" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23085,7 +22456,7 @@
         <v>0.68</v>
       </c>
       <c r="G48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H48" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23112,7 +22483,7 @@
         <v>0.93</v>
       </c>
       <c r="G49" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H49" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23139,7 +22510,7 @@
         <v>0.8</v>
       </c>
       <c r="G50" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H50" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23166,7 +22537,7 @@
         <v>0.8</v>
       </c>
       <c r="G51" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H51" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23193,7 +22564,7 @@
         <v>0.95</v>
       </c>
       <c r="G52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H52" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23220,7 +22591,7 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="G53" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H53" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23247,7 +22618,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="G54" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H54" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23274,7 +22645,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="G55" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H55" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23301,7 +22672,7 @@
         <v>9.4E-2</v>
       </c>
       <c r="G56" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H56" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23328,7 +22699,7 @@
         <v>0.47399999999999998</v>
       </c>
       <c r="G57" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H57" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23355,7 +22726,7 @@
         <v>0.71499999999999997</v>
       </c>
       <c r="G58" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H58" s="17" t="b">
         <f t="shared" si="1"/>
@@ -23382,7 +22753,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="G59" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H59" s="17" t="b">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
make treatfail appear in man cal
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/optima/optima/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27480" windowHeight="15460" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27480" windowHeight="15460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -16,11 +21,11 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -14748,17 +14753,7 @@
     <cellStyle name="Percent 3" xfId="162"/>
     <cellStyle name="Percent 4" xfId="47"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -15077,13 +15072,13 @@
       <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>383</v>
       </c>
@@ -15094,32 +15089,32 @@
         <v>393</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>77</v>
       </c>
@@ -15127,7 +15122,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -15135,7 +15130,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
@@ -15143,7 +15138,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
@@ -15151,7 +15146,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>80</v>
       </c>
@@ -15159,7 +15154,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>395</v>
       </c>
@@ -15167,7 +15162,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>81</v>
       </c>
@@ -15178,11 +15173,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -15194,13 +15184,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
     <col min="2" max="2" width="48.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
         <v>465</v>
       </c>
@@ -15208,7 +15198,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -15216,7 +15206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -15224,7 +15214,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -15232,7 +15222,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -15240,7 +15230,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -15248,7 +15238,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -15256,7 +15246,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -15264,7 +15254,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -15272,7 +15262,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -15280,7 +15270,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -15288,7 +15278,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -15296,7 +15286,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -15304,7 +15294,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -15312,7 +15302,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -15320,7 +15310,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -15328,7 +15318,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -15336,7 +15326,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -15344,7 +15334,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -15352,7 +15342,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -15360,7 +15350,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -15368,7 +15358,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -15376,7 +15366,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -15384,7 +15374,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -15392,7 +15382,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -15400,7 +15390,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -15408,7 +15398,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -15416,7 +15406,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -15424,7 +15414,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -15432,7 +15422,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -15440,7 +15430,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -15448,7 +15438,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -15456,7 +15446,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -15464,7 +15454,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -15472,7 +15462,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -15480,7 +15470,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -15488,7 +15478,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -15496,7 +15486,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
@@ -15504,7 +15494,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
@@ -15515,11 +15505,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -15527,11 +15512,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="AJ23" sqref="AJ23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -15560,7 +15545,7 @@
     <col min="39" max="39" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" s="21"/>
       <c r="B1" s="37" t="s">
         <v>1</v>
@@ -15677,7 +15662,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="16">
+    <row r="2" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
@@ -15724,7 +15709,7 @@
       <c r="AL2" s="30"/>
       <c r="AM2" s="33"/>
     </row>
-    <row r="3" spans="1:39" ht="16">
+    <row r="3" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>2</v>
       </c>
@@ -15771,7 +15756,7 @@
       <c r="AL3" s="31"/>
       <c r="AM3" s="35"/>
     </row>
-    <row r="4" spans="1:39" ht="16">
+    <row r="4" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
@@ -15822,7 +15807,7 @@
       <c r="AL4" s="30"/>
       <c r="AM4" s="33"/>
     </row>
-    <row r="5" spans="1:39" ht="16">
+    <row r="5" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>4</v>
       </c>
@@ -15873,7 +15858,7 @@
       <c r="AL5" s="30"/>
       <c r="AM5" s="33"/>
     </row>
-    <row r="6" spans="1:39" ht="16">
+    <row r="6" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>5</v>
       </c>
@@ -15924,7 +15909,7 @@
       <c r="AL6" s="30"/>
       <c r="AM6" s="33"/>
     </row>
-    <row r="7" spans="1:39" ht="16">
+    <row r="7" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>6</v>
       </c>
@@ -15975,7 +15960,7 @@
       <c r="AL7" s="30"/>
       <c r="AM7" s="33"/>
     </row>
-    <row r="8" spans="1:39" ht="16">
+    <row r="8" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>7</v>
       </c>
@@ -16026,7 +16011,7 @@
       <c r="AL8" s="30"/>
       <c r="AM8" s="33"/>
     </row>
-    <row r="9" spans="1:39" ht="16">
+    <row r="9" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>8</v>
       </c>
@@ -16073,7 +16058,7 @@
       <c r="AL9" s="31"/>
       <c r="AM9" s="35"/>
     </row>
-    <row r="10" spans="1:39" ht="16">
+    <row r="10" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
@@ -16124,7 +16109,7 @@
       <c r="AL10" s="30"/>
       <c r="AM10" s="33"/>
     </row>
-    <row r="11" spans="1:39" ht="16">
+    <row r="11" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>10</v>
       </c>
@@ -16175,7 +16160,7 @@
       <c r="AL11" s="30"/>
       <c r="AM11" s="33"/>
     </row>
-    <row r="12" spans="1:39" ht="16">
+    <row r="12" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>11</v>
       </c>
@@ -16226,7 +16211,7 @@
       <c r="AL12" s="30"/>
       <c r="AM12" s="33"/>
     </row>
-    <row r="13" spans="1:39" ht="16">
+    <row r="13" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>12</v>
       </c>
@@ -16277,7 +16262,7 @@
       <c r="AL13" s="30"/>
       <c r="AM13" s="33"/>
     </row>
-    <row r="14" spans="1:39" ht="16">
+    <row r="14" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>13</v>
       </c>
@@ -16328,7 +16313,7 @@
       <c r="AL14" s="30"/>
       <c r="AM14" s="33"/>
     </row>
-    <row r="15" spans="1:39" ht="16">
+    <row r="15" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>14</v>
       </c>
@@ -16375,7 +16360,7 @@
       <c r="AL15" s="31"/>
       <c r="AM15" s="35"/>
     </row>
-    <row r="16" spans="1:39" ht="16">
+    <row r="16" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>15</v>
       </c>
@@ -16426,7 +16411,7 @@
       <c r="AL16" s="30"/>
       <c r="AM16" s="33"/>
     </row>
-    <row r="17" spans="1:39" ht="16">
+    <row r="17" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>16</v>
       </c>
@@ -16477,7 +16462,7 @@
       <c r="AL17" s="30"/>
       <c r="AM17" s="33"/>
     </row>
-    <row r="18" spans="1:39" ht="16">
+    <row r="18" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
         <v>17</v>
       </c>
@@ -16528,7 +16513,7 @@
       <c r="AL18" s="30"/>
       <c r="AM18" s="33"/>
     </row>
-    <row r="19" spans="1:39" ht="16">
+    <row r="19" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
         <v>18</v>
       </c>
@@ -16579,7 +16564,7 @@
       <c r="AL19" s="30"/>
       <c r="AM19" s="33"/>
     </row>
-    <row r="20" spans="1:39" ht="16">
+    <row r="20" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
         <v>19</v>
       </c>
@@ -16630,7 +16615,7 @@
       <c r="AL20" s="30"/>
       <c r="AM20" s="33"/>
     </row>
-    <row r="21" spans="1:39" ht="16">
+    <row r="21" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>20</v>
       </c>
@@ -16677,7 +16662,7 @@
       <c r="AL21" s="31"/>
       <c r="AM21" s="35"/>
     </row>
-    <row r="22" spans="1:39" ht="16">
+    <row r="22" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>33</v>
       </c>
@@ -16728,7 +16713,7 @@
       <c r="AL22" s="30"/>
       <c r="AM22" s="33"/>
     </row>
-    <row r="23" spans="1:39" ht="16">
+    <row r="23" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>34</v>
       </c>
@@ -16779,7 +16764,7 @@
       <c r="AL23" s="30"/>
       <c r="AM23" s="33"/>
     </row>
-    <row r="24" spans="1:39" ht="16">
+    <row r="24" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>35</v>
       </c>
@@ -16830,7 +16815,7 @@
       <c r="AL24" s="30"/>
       <c r="AM24" s="33"/>
     </row>
-    <row r="25" spans="1:39" ht="16">
+    <row r="25" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>36</v>
       </c>
@@ -16881,7 +16866,7 @@
       <c r="AL25" s="30"/>
       <c r="AM25" s="33"/>
     </row>
-    <row r="26" spans="1:39" ht="16">
+    <row r="26" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
         <v>37</v>
       </c>
@@ -16932,7 +16917,7 @@
       <c r="AL26" s="30"/>
       <c r="AM26" s="33"/>
     </row>
-    <row r="27" spans="1:39" ht="16">
+    <row r="27" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>38</v>
       </c>
@@ -16979,7 +16964,7 @@
       <c r="AL27" s="31"/>
       <c r="AM27" s="35"/>
     </row>
-    <row r="28" spans="1:39" ht="16">
+    <row r="28" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="25" t="s">
         <v>21</v>
       </c>
@@ -17034,7 +17019,7 @@
       <c r="AL28" s="30"/>
       <c r="AM28" s="33"/>
     </row>
-    <row r="29" spans="1:39" ht="16">
+    <row r="29" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
         <v>22</v>
       </c>
@@ -17089,7 +17074,7 @@
       <c r="AL29" s="30"/>
       <c r="AM29" s="33"/>
     </row>
-    <row r="30" spans="1:39" ht="16">
+    <row r="30" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
         <v>23</v>
       </c>
@@ -17150,7 +17135,7 @@
       <c r="AL30" s="30"/>
       <c r="AM30" s="33"/>
     </row>
-    <row r="31" spans="1:39" ht="16">
+    <row r="31" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
         <v>24</v>
       </c>
@@ -17211,7 +17196,7 @@
       </c>
       <c r="AM31" s="33"/>
     </row>
-    <row r="32" spans="1:39" ht="16">
+    <row r="32" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
         <v>25</v>
       </c>
@@ -17272,7 +17257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="16">
+    <row r="33" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
         <v>26</v>
       </c>
@@ -17327,7 +17312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="16">
+    <row r="34" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>27</v>
       </c>
@@ -17382,7 +17367,7 @@
       <c r="AL34" s="30"/>
       <c r="AM34" s="33"/>
     </row>
-    <row r="35" spans="1:39" ht="16">
+    <row r="35" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>28</v>
       </c>
@@ -17431,7 +17416,7 @@
       <c r="AL35" s="30"/>
       <c r="AM35" s="33"/>
     </row>
-    <row r="36" spans="1:39" ht="16">
+    <row r="36" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
         <v>29</v>
       </c>
@@ -17486,7 +17471,7 @@
       <c r="AL36" s="30"/>
       <c r="AM36" s="33"/>
     </row>
-    <row r="37" spans="1:39" ht="16">
+    <row r="37" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>30</v>
       </c>
@@ -17541,7 +17526,7 @@
       <c r="AL37" s="30"/>
       <c r="AM37" s="33"/>
     </row>
-    <row r="38" spans="1:39" ht="16">
+    <row r="38" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>31</v>
       </c>
@@ -17596,7 +17581,7 @@
       </c>
       <c r="AM38" s="33"/>
     </row>
-    <row r="39" spans="1:39" ht="16">
+    <row r="39" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
         <v>32</v>
       </c>
@@ -17653,17 +17638,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AM39">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -17671,12 +17651,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="68.5" style="6" customWidth="1"/>
@@ -17688,7 +17668,7 @@
     <col min="8" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>77</v>
       </c>
@@ -17712,7 +17692,7 @@
       </c>
       <c r="H1" s="39"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>83</v>
       </c>
@@ -17735,7 +17715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>90</v>
       </c>
@@ -17758,7 +17738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>93</v>
       </c>
@@ -17781,7 +17761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>87</v>
       </c>
@@ -17804,7 +17784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>104</v>
       </c>
@@ -17827,7 +17807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>107</v>
       </c>
@@ -17850,7 +17830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>109</v>
       </c>
@@ -17873,7 +17853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>112</v>
       </c>
@@ -17896,7 +17876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>114</v>
       </c>
@@ -17919,7 +17899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>116</v>
       </c>
@@ -17942,7 +17922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>118</v>
       </c>
@@ -17965,7 +17945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>134</v>
       </c>
@@ -17988,7 +17968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>120</v>
       </c>
@@ -18011,7 +17991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>122</v>
       </c>
@@ -18034,7 +18014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>186</v>
       </c>
@@ -18057,7 +18037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>158</v>
       </c>
@@ -18080,7 +18060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>161</v>
       </c>
@@ -18103,7 +18083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>164</v>
       </c>
@@ -18126,7 +18106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>166</v>
       </c>
@@ -18149,7 +18129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>401</v>
       </c>
@@ -18172,7 +18152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>167</v>
       </c>
@@ -18195,7 +18175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>168</v>
       </c>
@@ -18218,7 +18198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>169</v>
       </c>
@@ -18241,7 +18221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>170</v>
       </c>
@@ -18264,7 +18244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>171</v>
       </c>
@@ -18287,7 +18267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>173</v>
       </c>
@@ -18310,7 +18290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>178</v>
       </c>
@@ -18333,7 +18313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>180</v>
       </c>
@@ -18356,7 +18336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>182</v>
       </c>
@@ -18379,7 +18359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>184</v>
       </c>
@@ -18402,7 +18382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>128</v>
       </c>
@@ -18425,7 +18405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>125</v>
       </c>
@@ -18448,7 +18428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>136</v>
       </c>
@@ -18471,7 +18451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>141</v>
       </c>
@@ -18494,7 +18474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>144</v>
       </c>
@@ -18517,7 +18497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>150</v>
       </c>
@@ -18540,7 +18520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>152</v>
       </c>
@@ -18563,7 +18543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>155</v>
       </c>
@@ -18586,7 +18566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>147</v>
       </c>
@@ -18609,7 +18589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>130</v>
       </c>
@@ -18632,7 +18612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>132</v>
       </c>
@@ -18655,7 +18635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>95</v>
       </c>
@@ -18678,7 +18658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>100</v>
       </c>
@@ -18701,7 +18681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>102</v>
       </c>
@@ -18724,7 +18704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>407</v>
       </c>
@@ -18747,7 +18727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>189</v>
       </c>
@@ -18770,7 +18750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>192</v>
       </c>
@@ -18793,7 +18773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>194</v>
       </c>
@@ -18816,7 +18796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>196</v>
       </c>
@@ -18839,7 +18819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>198</v>
       </c>
@@ -18862,7 +18842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>200</v>
       </c>
@@ -18885,7 +18865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>202</v>
       </c>
@@ -18908,7 +18888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>204</v>
       </c>
@@ -18931,7 +18911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>206</v>
       </c>
@@ -18954,7 +18934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>208</v>
       </c>
@@ -18977,7 +18957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>210</v>
       </c>
@@ -19000,7 +18980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>212</v>
       </c>
@@ -19023,7 +19003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>214</v>
       </c>
@@ -19046,7 +19026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>216</v>
       </c>
@@ -19069,7 +19049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>218</v>
       </c>
@@ -19092,7 +19072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>220</v>
       </c>
@@ -19115,7 +19095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>222</v>
       </c>
@@ -19138,7 +19118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>224</v>
       </c>
@@ -19161,7 +19141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>226</v>
       </c>
@@ -19184,7 +19164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>228</v>
       </c>
@@ -19207,7 +19187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>230</v>
       </c>
@@ -19230,7 +19210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>232</v>
       </c>
@@ -19253,7 +19233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>234</v>
       </c>
@@ -19276,7 +19256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>236</v>
       </c>
@@ -19299,7 +19279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>403</v>
       </c>
@@ -19322,7 +19302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>238</v>
       </c>
@@ -19345,7 +19325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>240</v>
       </c>
@@ -19368,7 +19348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>242</v>
       </c>
@@ -19391,7 +19371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>244</v>
       </c>
@@ -19414,7 +19394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>246</v>
       </c>
@@ -19437,7 +19417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>248</v>
       </c>
@@ -19460,7 +19440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>250</v>
       </c>
@@ -19483,7 +19463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>252</v>
       </c>
@@ -19506,7 +19486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>254</v>
       </c>
@@ -19522,14 +19502,14 @@
       <c r="E80" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F80" s="14" t="s">
-        <v>396</v>
+      <c r="F80" s="38" t="s">
+        <v>190</v>
       </c>
       <c r="G80" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>256</v>
       </c>
@@ -19552,7 +19532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>258</v>
       </c>
@@ -19575,7 +19555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>260</v>
       </c>
@@ -19598,7 +19578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>262</v>
       </c>
@@ -19621,7 +19601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>263</v>
       </c>
@@ -19644,7 +19624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>264</v>
       </c>
@@ -19667,7 +19647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>266</v>
       </c>
@@ -19690,7 +19670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>268</v>
       </c>
@@ -19713,7 +19693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
         <v>270</v>
       </c>
@@ -19736,7 +19716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
         <v>272</v>
       </c>
@@ -19759,7 +19739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>274</v>
       </c>
@@ -19782,7 +19762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>276</v>
       </c>
@@ -19805,7 +19785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
         <v>278</v>
       </c>
@@ -19828,7 +19808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>280</v>
       </c>
@@ -19851,7 +19831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>282</v>
       </c>
@@ -19874,7 +19854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
         <v>284</v>
       </c>
@@ -19897,7 +19877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
         <v>286</v>
       </c>
@@ -19920,7 +19900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>288</v>
       </c>
@@ -19943,7 +19923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>290</v>
       </c>
@@ -19966,7 +19946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>292</v>
       </c>
@@ -19989,7 +19969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>294</v>
       </c>
@@ -20012,7 +19992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>296</v>
       </c>
@@ -20035,7 +20015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>298</v>
       </c>
@@ -20058,7 +20038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>300</v>
       </c>
@@ -20081,68 +20061,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D105" s="6"/>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D106" s="6"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
       <c r="E107" s="6"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
       <c r="E109" s="6"/>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C110" s="6"/>
       <c r="D110" s="6"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
       <c r="E111" s="6"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
       <c r="E112" s="6"/>
     </row>
-    <row r="113" spans="3:5">
+    <row r="113" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C113" s="6"/>
       <c r="D113" s="6"/>
       <c r="E113" s="6"/>
     </row>
-    <row r="114" spans="3:5">
+    <row r="114" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
       <c r="E114" s="6"/>
     </row>
-    <row r="115" spans="3:5">
+    <row r="115" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C115" s="6"/>
       <c r="D115" s="6"/>
       <c r="E115" s="6"/>
     </row>
-    <row r="116" spans="3:5">
+    <row r="116" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
       <c r="E116" s="6"/>
     </row>
-    <row r="117" spans="3:5">
+    <row r="117" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C117" s="6"/>
       <c r="D117" s="6"/>
       <c r="E117" s="6"/>
     </row>
-    <row r="118" spans="3:5">
+    <row r="118" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C118" s="6"/>
       <c r="D118" s="6"/>
       <c r="E118" s="6"/>
@@ -20150,11 +20130,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -20167,7 +20142,7 @@
       <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
@@ -20177,7 +20152,7 @@
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>315</v>
       </c>
@@ -20197,7 +20172,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>316</v>
       </c>
@@ -20217,7 +20192,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -20237,7 +20212,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>317</v>
       </c>
@@ -20257,7 +20232,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>321</v>
       </c>
@@ -20277,7 +20252,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>321</v>
       </c>
@@ -20297,7 +20272,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>321</v>
       </c>
@@ -20317,7 +20292,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>323</v>
       </c>
@@ -20337,7 +20312,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>323</v>
       </c>
@@ -20357,7 +20332,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>323</v>
       </c>
@@ -20377,7 +20352,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>323</v>
       </c>
@@ -20397,7 +20372,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>323</v>
       </c>
@@ -20417,7 +20392,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>323</v>
       </c>
@@ -20437,7 +20412,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>323</v>
       </c>
@@ -20457,7 +20432,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>323</v>
       </c>
@@ -20477,7 +20452,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>324</v>
       </c>
@@ -20497,7 +20472,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>324</v>
       </c>
@@ -20517,7 +20492,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>324</v>
       </c>
@@ -20537,7 +20512,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>324</v>
       </c>
@@ -20557,7 +20532,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>324</v>
       </c>
@@ -20577,7 +20552,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>324</v>
       </c>
@@ -20597,7 +20572,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>324</v>
       </c>
@@ -20617,7 +20592,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>324</v>
       </c>
@@ -20637,7 +20612,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>324</v>
       </c>
@@ -20657,7 +20632,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>324</v>
       </c>
@@ -20677,7 +20652,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>324</v>
       </c>
@@ -20697,7 +20672,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>324</v>
       </c>
@@ -20717,7 +20692,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>325</v>
       </c>
@@ -20737,7 +20712,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>325</v>
       </c>
@@ -20757,7 +20732,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>325</v>
       </c>
@@ -20777,7 +20752,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>325</v>
       </c>
@@ -20797,7 +20772,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>325</v>
       </c>
@@ -20817,7 +20792,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>326</v>
       </c>
@@ -20837,7 +20812,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>326</v>
       </c>
@@ -20857,7 +20832,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>326</v>
       </c>
@@ -20877,7 +20852,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>326</v>
       </c>
@@ -20897,7 +20872,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>326</v>
       </c>
@@ -20917,7 +20892,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>326</v>
       </c>
@@ -20937,7 +20912,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>326</v>
       </c>
@@ -20957,7 +20932,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>327</v>
       </c>
@@ -20977,7 +20952,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>327</v>
       </c>
@@ -20997,7 +20972,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>327</v>
       </c>
@@ -21017,7 +20992,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>328</v>
       </c>
@@ -21037,7 +21012,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>328</v>
       </c>
@@ -21057,7 +21032,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>328</v>
       </c>
@@ -21077,7 +21052,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>328</v>
       </c>
@@ -21097,7 +21072,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>328</v>
       </c>
@@ -21117,7 +21092,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>328</v>
       </c>
@@ -21137,7 +21112,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>328</v>
       </c>
@@ -21160,11 +21135,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -21176,7 +21146,7 @@
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="62.5" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -21184,7 +21154,7 @@
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>329</v>
       </c>
@@ -21210,7 +21180,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>330</v>
       </c>
@@ -21237,7 +21207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>330</v>
       </c>
@@ -21264,7 +21234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>330</v>
       </c>
@@ -21291,7 +21261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>330</v>
       </c>
@@ -21318,7 +21288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>330</v>
       </c>
@@ -21345,7 +21315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>330</v>
       </c>
@@ -21372,7 +21342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>330</v>
       </c>
@@ -21399,7 +21369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>381</v>
       </c>
@@ -21426,7 +21396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>381</v>
       </c>
@@ -21453,7 +21423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>381</v>
       </c>
@@ -21480,7 +21450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>381</v>
       </c>
@@ -21507,7 +21477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>381</v>
       </c>
@@ -21534,7 +21504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>381</v>
       </c>
@@ -21561,7 +21531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>380</v>
       </c>
@@ -21588,7 +21558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>380</v>
       </c>
@@ -21615,7 +21585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>380</v>
       </c>
@@ -21642,7 +21612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>380</v>
       </c>
@@ -21669,7 +21639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>380</v>
       </c>
@@ -21696,7 +21666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>379</v>
       </c>
@@ -21723,7 +21693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>379</v>
       </c>
@@ -21750,7 +21720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>379</v>
       </c>
@@ -21777,7 +21747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>379</v>
       </c>
@@ -21804,7 +21774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>379</v>
       </c>
@@ -21831,7 +21801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>379</v>
       </c>
@@ -21858,7 +21828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>378</v>
       </c>
@@ -21885,7 +21855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>378</v>
       </c>
@@ -21912,7 +21882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>378</v>
       </c>
@@ -21939,7 +21909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>378</v>
       </c>
@@ -21966,7 +21936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>378</v>
       </c>
@@ -21993,7 +21963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>378</v>
       </c>
@@ -22020,7 +21990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>378</v>
       </c>
@@ -22047,7 +22017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>378</v>
       </c>
@@ -22074,7 +22044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>378</v>
       </c>
@@ -22101,7 +22071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>377</v>
       </c>
@@ -22128,7 +22098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>377</v>
       </c>
@@ -22156,7 +22126,7 @@
       </c>
       <c r="I36" s="41"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>377</v>
       </c>
@@ -22183,7 +22153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>377</v>
       </c>
@@ -22210,7 +22180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>377</v>
       </c>
@@ -22237,7 +22207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>377</v>
       </c>
@@ -22264,7 +22234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>377</v>
       </c>
@@ -22291,7 +22261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>377</v>
       </c>
@@ -22318,7 +22288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>377</v>
       </c>
@@ -22345,7 +22315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>376</v>
       </c>
@@ -22372,7 +22342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>376</v>
       </c>
@@ -22399,7 +22369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>376</v>
       </c>
@@ -22426,7 +22396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>376</v>
       </c>
@@ -22453,7 +22423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>376</v>
       </c>
@@ -22480,7 +22450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>376</v>
       </c>
@@ -22507,7 +22477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>376</v>
       </c>
@@ -22534,7 +22504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>376</v>
       </c>
@@ -22561,7 +22531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>376</v>
       </c>
@@ -22588,7 +22558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>375</v>
       </c>
@@ -22615,7 +22585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>375</v>
       </c>
@@ -22642,7 +22612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>375</v>
       </c>
@@ -22669,7 +22639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>375</v>
       </c>
@@ -22696,7 +22666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>375</v>
       </c>
@@ -22723,7 +22693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>375</v>
       </c>
@@ -22750,7 +22720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>375</v>
       </c>
@@ -22780,10 +22750,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove from pars and loadspreadsheet
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27480" windowHeight="15460" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27480" windowHeight="15460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="471">
   <si>
     <t>Susceptible</t>
   </si>
@@ -587,12 +587,6 @@
   </si>
   <si>
     <t>fixproppmtct</t>
-  </si>
-  <si>
-    <t>Unit cost of treatment</t>
-  </si>
-  <si>
-    <t>costtx</t>
   </si>
   <si>
     <t>Male-female insertive transmissibility (per act)</t>
@@ -15080,38 +15074,38 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -15119,7 +15113,7 @@
         <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -15127,7 +15121,7 @@
         <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -15135,7 +15129,7 @@
         <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -15143,7 +15137,7 @@
         <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -15151,15 +15145,15 @@
         <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -15167,7 +15161,7 @@
         <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -15192,10 +15186,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -17649,11 +17643,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H118"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17685,7 +17679,7 @@
         <v>80</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>81</v>
@@ -17720,7 +17714,7 @@
         <v>90</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>91</v>
@@ -17743,7 +17737,7 @@
         <v>93</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>91</v>
@@ -18016,21 +18010,21 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="6" t="s">
         <v>92</v>
       </c>
       <c r="G16" s="6">
@@ -18039,16 +18033,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>159</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>105</v>
@@ -18062,16 +18056,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>160</v>
+        <v>164</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>159</v>
+        <v>96</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>105</v>
@@ -18085,16 +18079,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>105</v>
@@ -18108,13 +18102,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>165</v>
+        <v>399</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>110</v>
@@ -18122,22 +18116,22 @@
       <c r="E20" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>162</v>
+        <v>466</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>110</v>
@@ -18145,19 +18139,19 @@
       <c r="E21" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="14">
-        <v>1</v>
+      <c r="F21" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>84</v>
@@ -18177,10 +18171,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>84</v>
@@ -18200,10 +18194,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>84</v>
@@ -18223,10 +18217,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>84</v>
@@ -18246,22 +18240,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>472</v>
+        <v>172</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>98</v>
+        <v>176</v>
       </c>
       <c r="G26" s="6">
         <v>0</v>
@@ -18269,10 +18263,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>174</v>
@@ -18292,10 +18286,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>174</v>
@@ -18315,10 +18309,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>174</v>
@@ -18338,10 +18332,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>174</v>
@@ -18361,22 +18355,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>183</v>
+        <v>127</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>175</v>
+        <v>105</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>176</v>
+        <v>98</v>
       </c>
       <c r="G31" s="6">
         <v>0</v>
@@ -18384,13 +18378,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>126</v>
@@ -18398,25 +18392,25 @@
       <c r="E32" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>98</v>
+      <c r="F32" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="G32" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>105</v>
@@ -18430,10 +18424,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>138</v>
@@ -18453,10 +18447,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>138</v>
@@ -18476,13 +18470,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>139</v>
@@ -18490,7 +18484,7 @@
       <c r="E36" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="6" t="s">
         <v>92</v>
       </c>
       <c r="G36" s="6">
@@ -18499,10 +18493,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>84</v>
@@ -18522,10 +18516,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>84</v>
@@ -18545,13 +18539,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>139</v>
@@ -18559,7 +18553,7 @@
       <c r="E39" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="14" t="s">
         <v>92</v>
       </c>
       <c r="G39" s="6">
@@ -18568,16 +18562,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>105</v>
@@ -18591,21 +18585,21 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="6" t="s">
         <v>92</v>
       </c>
       <c r="G41" s="6">
@@ -18614,22 +18608,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G42" s="6">
         <v>1</v>
@@ -18637,10 +18631,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>96</v>
@@ -18660,10 +18654,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>96</v>
@@ -18683,56 +18677,56 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>102</v>
+        <v>405</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>101</v>
+        <v>410</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>98</v>
+        <v>188</v>
       </c>
       <c r="G45" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>407</v>
+        <v>187</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>412</v>
+        <v>185</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E46" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>190</v>
-      </c>
       <c r="G46" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>84</v>
@@ -18741,10 +18735,10 @@
         <v>110</v>
       </c>
       <c r="E47" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G47" s="6">
         <v>1</v>
@@ -18764,10 +18758,10 @@
         <v>110</v>
       </c>
       <c r="E48" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G48" s="6">
         <v>1</v>
@@ -18787,10 +18781,10 @@
         <v>110</v>
       </c>
       <c r="E49" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G49" s="6">
         <v>1</v>
@@ -18810,10 +18804,10 @@
         <v>110</v>
       </c>
       <c r="E50" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G50" s="6">
         <v>1</v>
@@ -18833,10 +18827,10 @@
         <v>110</v>
       </c>
       <c r="E51" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G51" s="6">
         <v>1</v>
@@ -18856,10 +18850,10 @@
         <v>110</v>
       </c>
       <c r="E52" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G52" s="6">
         <v>1</v>
@@ -18873,16 +18867,16 @@
         <v>201</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E53" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G53" s="6">
         <v>1</v>
@@ -18902,10 +18896,10 @@
         <v>110</v>
       </c>
       <c r="E54" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G54" s="6">
         <v>1</v>
@@ -18925,10 +18919,10 @@
         <v>110</v>
       </c>
       <c r="E55" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G55" s="6">
         <v>1</v>
@@ -18948,10 +18942,10 @@
         <v>110</v>
       </c>
       <c r="E56" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F56" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G56" s="6">
         <v>1</v>
@@ -18971,10 +18965,10 @@
         <v>110</v>
       </c>
       <c r="E57" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F57" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G57" s="6">
         <v>1</v>
@@ -18994,10 +18988,10 @@
         <v>110</v>
       </c>
       <c r="E58" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F58" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G58" s="6">
         <v>1</v>
@@ -19017,10 +19011,10 @@
         <v>110</v>
       </c>
       <c r="E59" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F59" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G59" s="6">
         <v>1</v>
@@ -19034,16 +19028,16 @@
         <v>215</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E60" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F60" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G60" s="6">
         <v>1</v>
@@ -19063,10 +19057,10 @@
         <v>110</v>
       </c>
       <c r="E61" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F61" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G61" s="6">
         <v>1</v>
@@ -19086,10 +19080,10 @@
         <v>110</v>
       </c>
       <c r="E62" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F62" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G62" s="6">
         <v>1</v>
@@ -19109,10 +19103,10 @@
         <v>110</v>
       </c>
       <c r="E63" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F63" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G63" s="6">
         <v>1</v>
@@ -19122,7 +19116,7 @@
       <c r="A64" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="7" t="s">
         <v>223</v>
       </c>
       <c r="C64" s="6" t="s">
@@ -19132,10 +19126,10 @@
         <v>110</v>
       </c>
       <c r="E64" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F64" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G64" s="6">
         <v>1</v>
@@ -19155,10 +19149,10 @@
         <v>110</v>
       </c>
       <c r="E65" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F65" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G65" s="6">
         <v>1</v>
@@ -19178,10 +19172,10 @@
         <v>110</v>
       </c>
       <c r="E66" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F66" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G66" s="6">
         <v>1</v>
@@ -19201,10 +19195,10 @@
         <v>110</v>
       </c>
       <c r="E67" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F67" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G67" s="6">
         <v>1</v>
@@ -19224,10 +19218,10 @@
         <v>110</v>
       </c>
       <c r="E68" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F68" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G68" s="6">
         <v>1</v>
@@ -19247,10 +19241,10 @@
         <v>110</v>
       </c>
       <c r="E69" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F69" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G69" s="6">
         <v>1</v>
@@ -19258,47 +19252,47 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>235</v>
+        <v>401</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>400</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E70" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F70" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F70" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G70" s="6">
+      <c r="G70" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>138</v>
+        <v>236</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C71" s="38" t="s">
+        <v>84</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G71" s="14">
+        <v>186</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="G71" s="6">
         <v>1</v>
       </c>
     </row>
@@ -19316,10 +19310,10 @@
         <v>110</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G72" s="6">
         <v>1</v>
@@ -19329,7 +19323,7 @@
       <c r="A73" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="6" t="s">
         <v>239</v>
       </c>
       <c r="C73" s="38" t="s">
@@ -19339,10 +19333,10 @@
         <v>110</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G73" s="6">
         <v>1</v>
@@ -19362,10 +19356,10 @@
         <v>110</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G74" s="6">
         <v>1</v>
@@ -19385,10 +19379,10 @@
         <v>110</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G75" s="6">
         <v>1</v>
@@ -19408,10 +19402,10 @@
         <v>110</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G76" s="6">
         <v>1</v>
@@ -19431,10 +19425,10 @@
         <v>110</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G77" s="6">
         <v>1</v>
@@ -19454,10 +19448,10 @@
         <v>110</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G78" s="6">
         <v>1</v>
@@ -19470,17 +19464,17 @@
       <c r="B79" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C79" s="38" t="s">
-        <v>84</v>
+      <c r="C79" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F79" s="14" t="s">
-        <v>396</v>
+        <v>186</v>
+      </c>
+      <c r="F79" s="38" t="s">
+        <v>394</v>
       </c>
       <c r="G79" s="6">
         <v>1</v>
@@ -19500,10 +19494,10 @@
         <v>110</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F80" s="38" t="s">
-        <v>396</v>
+        <v>186</v>
+      </c>
+      <c r="F80" s="14" t="s">
+        <v>394</v>
       </c>
       <c r="G80" s="6">
         <v>1</v>
@@ -19523,10 +19517,10 @@
         <v>110</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G81" s="6">
         <v>1</v>
@@ -19546,20 +19540,20 @@
         <v>110</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G82" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B83" s="7" t="s">
         <v>259</v>
       </c>
       <c r="C83" s="6" t="s">
@@ -19569,10 +19563,10 @@
         <v>110</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G83" s="6">
         <v>1</v>
@@ -19580,10 +19574,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="B84" s="7" t="s">
         <v>261</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>397</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>96</v>
@@ -19592,21 +19586,21 @@
         <v>110</v>
       </c>
       <c r="E84" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F84" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F84" s="14" t="s">
-        <v>396</v>
-      </c>
       <c r="G84" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="B85" s="15" t="s">
-        <v>399</v>
+      <c r="A85" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>398</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>96</v>
@@ -19615,10 +19609,10 @@
         <v>110</v>
       </c>
       <c r="E85" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F85" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F85" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G85" s="6">
         <v>1</v>
@@ -19628,20 +19622,20 @@
       <c r="A86" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="B86" s="14" t="s">
-        <v>400</v>
+      <c r="B86" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E86" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F86" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F86" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G86" s="6">
         <v>1</v>
@@ -19661,10 +19655,10 @@
         <v>110</v>
       </c>
       <c r="E87" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F87" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G87" s="6">
         <v>1</v>
@@ -19684,10 +19678,10 @@
         <v>110</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>394</v>
       </c>
       <c r="G88" s="6">
         <v>1</v>
@@ -19701,16 +19695,16 @@
         <v>269</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E89" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F89" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F89" s="14" t="s">
-        <v>396</v>
       </c>
       <c r="G89" s="6">
         <v>1</v>
@@ -19730,10 +19724,10 @@
         <v>110</v>
       </c>
       <c r="E90" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F90" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F90" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G90" s="6">
         <v>1</v>
@@ -19753,10 +19747,10 @@
         <v>110</v>
       </c>
       <c r="E91" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F91" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F91" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G91" s="6">
         <v>1</v>
@@ -19776,10 +19770,10 @@
         <v>110</v>
       </c>
       <c r="E92" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F92" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G92" s="6">
         <v>1</v>
@@ -19799,10 +19793,10 @@
         <v>110</v>
       </c>
       <c r="E93" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F93" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G93" s="6">
         <v>1</v>
@@ -19822,10 +19816,10 @@
         <v>110</v>
       </c>
       <c r="E94" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F94" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F94" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G94" s="6">
         <v>1</v>
@@ -19845,10 +19839,10 @@
         <v>110</v>
       </c>
       <c r="E95" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F95" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G95" s="6">
         <v>1</v>
@@ -19868,10 +19862,10 @@
         <v>110</v>
       </c>
       <c r="E96" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F96" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G96" s="6">
         <v>1</v>
@@ -19891,10 +19885,10 @@
         <v>110</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F97" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="F97" s="14" t="s">
+        <v>394</v>
       </c>
       <c r="G97" s="6">
         <v>1</v>
@@ -19914,10 +19908,10 @@
         <v>110</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F98" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G98" s="6">
         <v>1</v>
@@ -19937,10 +19931,10 @@
         <v>110</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F99" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G99" s="6">
         <v>1</v>
@@ -19960,10 +19954,10 @@
         <v>110</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G100" s="6">
         <v>1</v>
@@ -19983,10 +19977,10 @@
         <v>110</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G101" s="6">
         <v>1</v>
@@ -20006,10 +20000,10 @@
         <v>110</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G102" s="6">
         <v>1</v>
@@ -20029,43 +20023,25 @@
         <v>110</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G103" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E104" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F104" s="14" t="s">
-        <v>396</v>
-      </c>
-      <c r="G104" s="6">
-        <v>1</v>
-      </c>
+      <c r="D104" s="6"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D105" s="6"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C106" s="6"/>
       <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C107" s="6"/>
@@ -20121,11 +20097,6 @@
       <c r="C117" s="6"/>
       <c r="D117" s="6"/>
       <c r="E117" s="6"/>
-    </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C118" s="6"/>
-      <c r="D118" s="6"/>
-      <c r="E118" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20137,7 +20108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
@@ -20154,10 +20125,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>77</v>
@@ -20166,15 +20137,15 @@
         <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s">
         <v>92</v>
@@ -20183,13 +20154,13 @@
         <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="E2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -20197,7 +20168,7 @@
         <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C3" t="s">
         <v>87</v>
@@ -20206,78 +20177,78 @@
         <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F3" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B4" t="s">
+        <v>316</v>
+      </c>
+      <c r="C4" t="s">
         <v>318</v>
       </c>
-      <c r="C4" t="s">
-        <v>320</v>
-      </c>
       <c r="D4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C5" t="s">
         <v>104</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C6" t="s">
         <v>112</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C7" t="s">
         <v>114</v>
@@ -20286,58 +20257,58 @@
         <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C8" t="s">
         <v>107</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E8" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C9" t="s">
         <v>109</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E9" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F9" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C10" t="s">
         <v>116</v>
@@ -20346,338 +20317,338 @@
         <v>115</v>
       </c>
       <c r="E10" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C11" t="s">
         <v>134</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E11" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F11" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C12" t="s">
         <v>118</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E12" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F12" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C13" t="s">
         <v>122</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F13" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C14" t="s">
         <v>120</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E14" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F14" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E15" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F15" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C16" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E16" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F16" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B17" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C17" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E17" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B18" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C18" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E18" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F18" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E19" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F19" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E20" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F20" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E21" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F21" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B22" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C22" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E22" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F22" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B23" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E23" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F23" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E24" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F24" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B25" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E25" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F25" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C26" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E26" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F26" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B27" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C27" t="s">
         <v>158</v>
@@ -20686,18 +20657,18 @@
         <v>157</v>
       </c>
       <c r="E27" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F27" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B28" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C28" t="s">
         <v>161</v>
@@ -20706,410 +20677,410 @@
         <v>160</v>
       </c>
       <c r="E28" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B29" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C29" t="s">
         <v>164</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E29" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B30" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C30" t="s">
         <v>166</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E30" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F30" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B31" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D31" s="38" t="s">
         <v>162</v>
       </c>
       <c r="E31" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F31" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B32" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C32" t="s">
         <v>137</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E32" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F32" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B33" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C33" t="s">
         <v>142</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E33" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F33" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B34" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C34" t="s">
         <v>145</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E34" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F34" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B35" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C35" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E35" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F35" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B36" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C36" t="s">
         <v>153</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E36" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F36" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B37" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C37" t="s">
         <v>156</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E37" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F37" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B38" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C38" t="s">
         <v>125</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E38" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F38" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B39" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C39" t="s">
         <v>148</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E39" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F39" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B40" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C40" t="s">
         <v>132</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E40" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F40" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B41" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C41" t="s">
         <v>130</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E41" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F41" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B42" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C42" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E42" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F42" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B43" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C43" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E43" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F43" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B44" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C44" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E44" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F44" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B45" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C45" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E45" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F45" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B46" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C46" t="s">
         <v>102</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E46" t="s">
+        <v>414</v>
+      </c>
+      <c r="F46" t="s">
         <v>416</v>
-      </c>
-      <c r="F46" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B47" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C47" t="s">
         <v>100</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E47" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F47" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B48" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C48" t="s">
         <v>95</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E48" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F48" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -21136,7 +21107,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>77</v>
@@ -21145,30 +21116,30 @@
         <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>333</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D2" s="42">
         <v>4.0000000000000002E-4</v>
@@ -21180,7 +21151,7 @@
         <v>1.4E-3</v>
       </c>
       <c r="G2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H2" s="17" t="b">
         <f t="shared" ref="H2:H33" si="0">AND(D2&gt;=E2, D2&lt;=F2)</f>
@@ -21189,13 +21160,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D3" s="42">
         <v>8.0000000000000004E-4</v>
@@ -21207,7 +21178,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="G3" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H3" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21216,13 +21187,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D4" s="42">
         <v>1.1000000000000001E-3</v>
@@ -21234,7 +21205,7 @@
         <v>2.8E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H4" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21243,13 +21214,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D5" s="42">
         <v>1.38E-2</v>
@@ -21261,7 +21232,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
       <c r="G5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H5" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21270,13 +21241,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D6" s="42">
         <v>8.0000000000000002E-3</v>
@@ -21288,7 +21259,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="G6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H6" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21297,13 +21268,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D7" s="42">
         <v>0.36699999999999999</v>
@@ -21315,7 +21286,7 @@
         <v>0.44</v>
       </c>
       <c r="G7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H7" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21324,13 +21295,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D8" s="42">
         <v>0.20499999999999999</v>
@@ -21342,7 +21313,7 @@
         <v>0.27</v>
       </c>
       <c r="G8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H8" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21351,13 +21322,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D9" s="43">
         <v>5.6</v>
@@ -21369,7 +21340,7 @@
         <v>9.1</v>
       </c>
       <c r="G9" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H9" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21378,13 +21349,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D10" s="43">
         <v>1</v>
@@ -21396,7 +21367,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H10" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21405,13 +21376,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D11" s="43">
         <v>1</v>
@@ -21423,7 +21394,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H11" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21432,13 +21403,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D12" s="43">
         <v>1</v>
@@ -21450,7 +21421,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H12" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21459,13 +21430,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D13" s="43">
         <v>3.49</v>
@@ -21477,7 +21448,7 @@
         <v>6.92</v>
       </c>
       <c r="G13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H13" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21486,13 +21457,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D14" s="43">
         <v>7.17</v>
@@ -21504,7 +21475,7 @@
         <v>12.08</v>
       </c>
       <c r="G14" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H14" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21513,13 +21484,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D15" s="43">
         <v>0.24</v>
@@ -21531,7 +21502,7 @@
         <v>0.5</v>
       </c>
       <c r="G15" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H15" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21540,13 +21511,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D16" s="43">
         <v>0.95</v>
@@ -21558,7 +21529,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="G16" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H16" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21567,13 +21538,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D17" s="43">
         <v>3</v>
@@ -21585,7 +21556,7 @@
         <v>3.16</v>
       </c>
       <c r="G17" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H17" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21594,13 +21565,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D18" s="43">
         <v>3.74</v>
@@ -21612,7 +21583,7 @@
         <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H18" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21621,13 +21592,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D19" s="43">
         <v>1.5</v>
@@ -21639,7 +21610,7 @@
         <v>2.25</v>
       </c>
       <c r="G19" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H19" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21648,13 +21619,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D20" s="43">
         <v>2.2000000000000002</v>
@@ -21666,7 +21637,7 @@
         <v>7.28</v>
       </c>
       <c r="G20" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H20" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21675,13 +21646,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D21" s="43">
         <v>1.42</v>
@@ -21693,7 +21664,7 @@
         <v>3.42</v>
       </c>
       <c r="G21" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H21" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21702,13 +21673,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D22" s="43">
         <v>2.14</v>
@@ -21720,7 +21691,7 @@
         <v>3.58</v>
       </c>
       <c r="G22" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H22" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21729,13 +21700,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D23" s="43">
         <v>0.66</v>
@@ -21747,7 +21718,7 @@
         <v>0.94</v>
       </c>
       <c r="G23" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H23" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21756,13 +21727,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D24" s="43">
         <v>0.2</v>
@@ -21774,7 +21745,7 @@
         <v>0.3</v>
       </c>
       <c r="G24" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H24" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21783,13 +21754,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D25" s="43">
         <v>2</v>
@@ -21801,7 +21772,7 @@
         <v>2.5</v>
       </c>
       <c r="G25" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H25" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21810,13 +21781,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D26" s="42">
         <v>2.5999999999999999E-2</v>
@@ -21828,7 +21799,7 @@
         <v>0.27500000000000002</v>
       </c>
       <c r="G26" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H26" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21837,13 +21808,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D27" s="42">
         <v>0.15</v>
@@ -21855,7 +21826,7 @@
         <v>0.88500000000000001</v>
       </c>
       <c r="G27" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H27" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21864,13 +21835,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D28" s="42">
         <v>0.1</v>
@@ -21882,7 +21853,7 @@
         <v>0.87</v>
       </c>
       <c r="G28" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H28" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21891,13 +21862,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D29" s="42">
         <v>5.2999999999999999E-2</v>
@@ -21909,7 +21880,7 @@
         <v>0.82699999999999996</v>
       </c>
       <c r="G29" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H29" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21918,13 +21889,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D30" s="42">
         <v>0.16200000000000001</v>
@@ -21936,7 +21907,7 @@
         <v>0.86899999999999999</v>
       </c>
       <c r="G30" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H30" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21945,13 +21916,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D31" s="42">
         <v>0.11700000000000001</v>
@@ -21963,7 +21934,7 @@
         <v>0.68600000000000005</v>
       </c>
       <c r="G31" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H31" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21972,13 +21943,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D32" s="42">
         <v>0.09</v>
@@ -21990,7 +21961,7 @@
         <v>0.72299999999999998</v>
       </c>
       <c r="G32" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H32" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21999,13 +21970,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D33" s="42">
         <v>0.111</v>
@@ -22017,7 +21988,7 @@
         <v>0.56299999999999994</v>
       </c>
       <c r="G33" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H33" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22026,13 +21997,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D34" s="42">
         <v>0.16</v>
@@ -22044,7 +22015,7 @@
         <v>0.26</v>
       </c>
       <c r="G34" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H34" s="17" t="b">
         <f t="shared" ref="H34:H59" si="1">AND(D34&gt;=E34, D34&lt;=F34)</f>
@@ -22053,13 +22024,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D35" s="42">
         <v>3.5999999999999999E-3</v>
@@ -22071,7 +22042,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="G35" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H35" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22080,13 +22051,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D36" s="42">
         <v>3.5999999999999999E-3</v>
@@ -22098,7 +22069,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="G36" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H36" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22108,13 +22079,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D37" s="42">
         <v>5.7999999999999996E-3</v>
@@ -22126,7 +22097,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="G37" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H37" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22135,13 +22106,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D38" s="42">
         <v>8.8000000000000005E-3</v>
@@ -22153,7 +22124,7 @@
         <v>1.01E-2</v>
       </c>
       <c r="G38" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H38" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22162,13 +22133,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D39" s="42">
         <v>5.8999999999999997E-2</v>
@@ -22180,7 +22151,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="G39" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H39" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22189,13 +22160,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D40" s="42">
         <v>0.32300000000000001</v>
@@ -22207,7 +22178,7 @@
         <v>0.432</v>
       </c>
       <c r="G40" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H40" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22216,13 +22187,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D41" s="42">
         <v>0.23</v>
@@ -22234,7 +22205,7 @@
         <v>0.3</v>
       </c>
       <c r="G41" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H41" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22243,13 +22214,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D42" s="42">
         <v>0.48780000000000001</v>
@@ -22261,7 +22232,7 @@
         <v>0.8417</v>
       </c>
       <c r="G42" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H42" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22270,13 +22241,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D43" s="42">
         <v>2.17</v>
@@ -22288,7 +22259,7 @@
         <v>3.71</v>
       </c>
       <c r="G43" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H43" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22297,13 +22268,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D44" s="44">
         <v>0.95</v>
@@ -22315,7 +22286,7 @@
         <v>0.98</v>
       </c>
       <c r="G44" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H44" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22324,13 +22295,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D45" s="44">
         <v>0.57999999999999996</v>
@@ -22342,7 +22313,7 @@
         <v>0.67</v>
       </c>
       <c r="G45" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H45" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22351,13 +22322,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D46" s="44">
         <v>0</v>
@@ -22369,7 +22340,7 @@
         <v>0.68</v>
       </c>
       <c r="G46" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H46" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22378,13 +22349,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D47" s="44">
         <v>2.65</v>
@@ -22396,7 +22367,7 @@
         <v>5.19</v>
       </c>
       <c r="G47" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H47" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22405,13 +22376,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D48" s="44">
         <v>0.54</v>
@@ -22423,7 +22394,7 @@
         <v>0.68</v>
       </c>
       <c r="G48" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H48" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22432,13 +22403,13 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D49" s="44">
         <v>0.9</v>
@@ -22450,7 +22421,7 @@
         <v>0.93</v>
       </c>
       <c r="G49" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H49" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22459,13 +22430,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D50" s="44">
         <v>0.73</v>
@@ -22477,7 +22448,7 @@
         <v>0.8</v>
       </c>
       <c r="G50" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H50" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22486,13 +22457,13 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D51" s="44">
         <v>0.5</v>
@@ -22504,7 +22475,7 @@
         <v>0.8</v>
       </c>
       <c r="G51" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H51" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22513,13 +22484,13 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D52" s="44">
         <v>0.92</v>
@@ -22531,7 +22502,7 @@
         <v>0.95</v>
       </c>
       <c r="G52" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H52" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22540,13 +22511,13 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D53" s="43">
         <v>0.14599999999999999</v>
@@ -22558,7 +22529,7 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="G53" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H53" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22567,13 +22538,13 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D54" s="43">
         <v>8.0000000000000002E-3</v>
@@ -22585,7 +22556,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="G54" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H54" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22594,13 +22565,13 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D55" s="45">
         <v>0.02</v>
@@ -22612,7 +22583,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="G55" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H55" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22621,13 +22592,13 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D56" s="45">
         <v>7.0000000000000007E-2</v>
@@ -22639,7 +22610,7 @@
         <v>9.4E-2</v>
       </c>
       <c r="G56" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H56" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22648,13 +22619,13 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D57" s="43">
         <v>0.26500000000000001</v>
@@ -22666,7 +22637,7 @@
         <v>0.47399999999999998</v>
       </c>
       <c r="G57" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H57" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22675,13 +22646,13 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D58" s="43">
         <v>0.54700000000000004</v>
@@ -22693,7 +22664,7 @@
         <v>0.71499999999999997</v>
       </c>
       <c r="G58" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H58" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22702,13 +22673,13 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B59" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C59" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D59" s="43">
         <v>5.2999999999999999E-2</v>
@@ -22720,7 +22691,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="G59" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H59" s="17" t="b">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
change model logic and add migration
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27480" windowHeight="15460" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27480" windowHeight="15460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="476">
   <si>
     <t>Susceptible</t>
   </si>
@@ -17662,11 +17662,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H120"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22:B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A82" sqref="A82:XFD82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19547,10 +19547,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>96</v>
@@ -19561,7 +19561,7 @@
       <c r="E82" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F82" s="38" t="s">
+      <c r="F82" s="14" t="s">
         <v>391</v>
       </c>
       <c r="G82" s="6">
@@ -19570,10 +19570,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>96</v>
@@ -19593,10 +19593,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>96</v>
@@ -19615,11 +19615,11 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>256</v>
+      <c r="A85" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>258</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>96</v>
@@ -19639,10 +19639,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>258</v>
+        <v>260</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>96</v>
@@ -19653,19 +19653,19 @@
       <c r="E86" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F86" s="14" t="s">
-        <v>391</v>
+      <c r="F86" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="G86" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="B87" s="15" t="s">
-        <v>394</v>
+      <c r="A87" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>395</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>96</v>
@@ -19685,13 +19685,13 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="B88" s="14" t="s">
-        <v>395</v>
+        <v>263</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>262</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>110</v>
@@ -19708,10 +19708,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>91</v>
@@ -19731,10 +19731,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>91</v>
@@ -19745,8 +19745,8 @@
       <c r="E90" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F90" s="6" t="s">
-        <v>187</v>
+      <c r="F90" s="14" t="s">
+        <v>391</v>
       </c>
       <c r="G90" s="6">
         <v>1</v>
@@ -19754,13 +19754,13 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>110</v>
@@ -19768,8 +19768,8 @@
       <c r="E91" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F91" s="14" t="s">
-        <v>391</v>
+      <c r="F91" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="G91" s="6">
         <v>1</v>
@@ -19777,10 +19777,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>84</v>
@@ -19800,10 +19800,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>84</v>
@@ -19823,10 +19823,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>272</v>
+        <v>472</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>84</v>
@@ -19846,10 +19846,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>472</v>
+        <v>275</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>84</v>
@@ -19869,10 +19869,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>84</v>
@@ -19892,10 +19892,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>84</v>
@@ -19915,10 +19915,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>84</v>
@@ -19938,10 +19938,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>84</v>
@@ -19952,8 +19952,8 @@
       <c r="E99" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F99" s="6" t="s">
-        <v>187</v>
+      <c r="F99" s="14" t="s">
+        <v>391</v>
       </c>
       <c r="G99" s="6">
         <v>1</v>
@@ -19961,10 +19961,10 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>84</v>
@@ -19984,10 +19984,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>84</v>
@@ -20007,10 +20007,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>84</v>
@@ -20030,10 +20030,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>84</v>
@@ -20053,10 +20053,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>84</v>
@@ -20076,10 +20076,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>84</v>
@@ -20098,33 +20098,15 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D106" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E106" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F106" s="14" t="s">
-        <v>391</v>
-      </c>
-      <c r="G106" s="6">
-        <v>1</v>
-      </c>
+      <c r="D106" s="6"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D107" s="6"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C108" s="6"/>
       <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C109" s="6"/>
@@ -20180,11 +20162,6 @@
       <c r="C119" s="6"/>
       <c r="D119" s="6"/>
       <c r="E119" s="6"/>
-    </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20196,9 +20173,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
renamed people > exposure events
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="27480" windowHeight="15465" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="27480" windowHeight="15465" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -1439,13 +1439,13 @@
     <t>ARV-based prophylaxis</t>
   </si>
   <si>
-    <t>Proportion of people covered by ARV-based prophylaxis</t>
-  </si>
-  <si>
     <t>Efficacy of ARV-based prophylaxis</t>
   </si>
   <si>
     <t>Percentage of people covered by ARV-based prophylaxis</t>
+  </si>
+  <si>
+    <t>Proportion of exposure events covered by ARV-based prophylaxis</t>
   </si>
 </sst>
 </file>
@@ -17580,7 +17580,7 @@
       </c>
       <c r="AM38" s="33"/>
     </row>
-    <row r="39" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>32</v>
       </c>
@@ -17650,9 +17650,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17972,7 +17972,7 @@
         <v>133</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>84</v>
@@ -19789,7 +19789,7 @@
         <v>274</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>84</v>
@@ -20362,7 +20362,7 @@
         <v>133</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E11" t="s">
         <v>409</v>
@@ -21121,7 +21121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change required vl per sk mail
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27480" windowHeight="15460" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27480" windowHeight="15460" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -17664,8 +17664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A82" sqref="A82:XFD82"/>
     </sheetView>
   </sheetViews>
@@ -21198,8 +21198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21868,13 +21868,13 @@
         <v>397</v>
       </c>
       <c r="D25" s="43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="F25" s="43">
         <v>1.5</v>
-      </c>
-      <c r="F25" s="43">
-        <v>2.5</v>
       </c>
       <c r="G25" t="s">
         <v>408</v>

</xml_diff>

<commit_message>
add col to input sheet
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/optima/optima/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0122FF-0018-094C-8CD4-76FE5651C808}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="27480" windowHeight="15465" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27480" windowHeight="15460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <sheet name="Data inputs" sheetId="4" r:id="rId5"/>
     <sheet name="Data constants" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="475">
   <si>
     <t>Susceptible</t>
   </si>
@@ -1443,16 +1449,22 @@
   </si>
   <si>
     <t>regainvs</t>
+  </si>
+  <si>
+    <t>progdefault</t>
+  </si>
+  <si>
+    <t>lower</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -1860,20 +1872,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1973,21 +1985,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -8239,7 +8251,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8313,33 +8325,34 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6424">
     <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
     <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
     <cellStyle name="60% - Accent5" xfId="6" builtinId="48"/>
     <cellStyle name="Accent5" xfId="3" builtinId="45"/>
-    <cellStyle name="Comma 2" xfId="51"/>
-    <cellStyle name="Comma 2 2" xfId="166"/>
-    <cellStyle name="Comma 2 3" xfId="59"/>
-    <cellStyle name="Comma 2 4" xfId="173"/>
-    <cellStyle name="Comma 3" xfId="57"/>
-    <cellStyle name="Comma 3 2" xfId="171"/>
-    <cellStyle name="Comma 4" xfId="161"/>
-    <cellStyle name="Comma 5" xfId="159"/>
-    <cellStyle name="Comma 6" xfId="46"/>
-    <cellStyle name="Explanatory Text 2" xfId="53"/>
-    <cellStyle name="Explanatory Text 3" xfId="163"/>
-    <cellStyle name="Explanatory Text 4" xfId="48"/>
+    <cellStyle name="Comma 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 2 2" xfId="166" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Comma 2 3" xfId="59" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Comma 2 4" xfId="173" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Comma 3" xfId="57" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Comma 3 2" xfId="171" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Comma 4" xfId="161" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Comma 5" xfId="159" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Comma 6" xfId="46" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="53" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Explanatory Text 3" xfId="163" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Explanatory Text 4" xfId="48" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
@@ -11483,103 +11496,103 @@
     <cellStyle name="Followed Hyperlink" xfId="6419" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6421" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6423" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink 10" xfId="70"/>
-    <cellStyle name="Followed Hyperlink 11" xfId="71"/>
-    <cellStyle name="Followed Hyperlink 12" xfId="72"/>
-    <cellStyle name="Followed Hyperlink 13" xfId="73"/>
-    <cellStyle name="Followed Hyperlink 14" xfId="74"/>
-    <cellStyle name="Followed Hyperlink 15" xfId="75"/>
-    <cellStyle name="Followed Hyperlink 16" xfId="76"/>
-    <cellStyle name="Followed Hyperlink 17" xfId="77"/>
-    <cellStyle name="Followed Hyperlink 18" xfId="78"/>
-    <cellStyle name="Followed Hyperlink 19" xfId="79"/>
-    <cellStyle name="Followed Hyperlink 2" xfId="62"/>
-    <cellStyle name="Followed Hyperlink 20" xfId="80"/>
-    <cellStyle name="Followed Hyperlink 21" xfId="81"/>
-    <cellStyle name="Followed Hyperlink 22" xfId="82"/>
-    <cellStyle name="Followed Hyperlink 23" xfId="83"/>
-    <cellStyle name="Followed Hyperlink 24" xfId="84"/>
-    <cellStyle name="Followed Hyperlink 25" xfId="85"/>
-    <cellStyle name="Followed Hyperlink 26" xfId="86"/>
-    <cellStyle name="Followed Hyperlink 27" xfId="87"/>
-    <cellStyle name="Followed Hyperlink 28" xfId="88"/>
-    <cellStyle name="Followed Hyperlink 29" xfId="89"/>
-    <cellStyle name="Followed Hyperlink 3" xfId="63"/>
-    <cellStyle name="Followed Hyperlink 30" xfId="90"/>
-    <cellStyle name="Followed Hyperlink 31" xfId="91"/>
-    <cellStyle name="Followed Hyperlink 32" xfId="92"/>
-    <cellStyle name="Followed Hyperlink 33" xfId="93"/>
-    <cellStyle name="Followed Hyperlink 34" xfId="94"/>
-    <cellStyle name="Followed Hyperlink 35" xfId="95"/>
-    <cellStyle name="Followed Hyperlink 36" xfId="96"/>
-    <cellStyle name="Followed Hyperlink 37" xfId="97"/>
-    <cellStyle name="Followed Hyperlink 38" xfId="98"/>
-    <cellStyle name="Followed Hyperlink 39" xfId="99"/>
-    <cellStyle name="Followed Hyperlink 4" xfId="64"/>
-    <cellStyle name="Followed Hyperlink 40" xfId="100"/>
-    <cellStyle name="Followed Hyperlink 41" xfId="101"/>
-    <cellStyle name="Followed Hyperlink 42" xfId="102"/>
-    <cellStyle name="Followed Hyperlink 43" xfId="103"/>
-    <cellStyle name="Followed Hyperlink 44" xfId="104"/>
-    <cellStyle name="Followed Hyperlink 45" xfId="105"/>
-    <cellStyle name="Followed Hyperlink 46" xfId="106"/>
-    <cellStyle name="Followed Hyperlink 47" xfId="107"/>
-    <cellStyle name="Followed Hyperlink 48" xfId="108"/>
-    <cellStyle name="Followed Hyperlink 49" xfId="109"/>
-    <cellStyle name="Followed Hyperlink 5" xfId="65"/>
-    <cellStyle name="Followed Hyperlink 50" xfId="110"/>
-    <cellStyle name="Followed Hyperlink 51" xfId="111"/>
-    <cellStyle name="Followed Hyperlink 52" xfId="112"/>
-    <cellStyle name="Followed Hyperlink 53" xfId="113"/>
-    <cellStyle name="Followed Hyperlink 54" xfId="114"/>
-    <cellStyle name="Followed Hyperlink 55" xfId="115"/>
-    <cellStyle name="Followed Hyperlink 56" xfId="116"/>
-    <cellStyle name="Followed Hyperlink 57" xfId="117"/>
-    <cellStyle name="Followed Hyperlink 58" xfId="118"/>
-    <cellStyle name="Followed Hyperlink 59" xfId="119"/>
-    <cellStyle name="Followed Hyperlink 6" xfId="66"/>
-    <cellStyle name="Followed Hyperlink 60" xfId="120"/>
-    <cellStyle name="Followed Hyperlink 61" xfId="121"/>
-    <cellStyle name="Followed Hyperlink 62" xfId="122"/>
-    <cellStyle name="Followed Hyperlink 63" xfId="123"/>
-    <cellStyle name="Followed Hyperlink 64" xfId="124"/>
-    <cellStyle name="Followed Hyperlink 65" xfId="125"/>
-    <cellStyle name="Followed Hyperlink 66" xfId="126"/>
-    <cellStyle name="Followed Hyperlink 67" xfId="127"/>
-    <cellStyle name="Followed Hyperlink 68" xfId="128"/>
-    <cellStyle name="Followed Hyperlink 69" xfId="129"/>
-    <cellStyle name="Followed Hyperlink 7" xfId="67"/>
-    <cellStyle name="Followed Hyperlink 70" xfId="130"/>
-    <cellStyle name="Followed Hyperlink 71" xfId="131"/>
-    <cellStyle name="Followed Hyperlink 72" xfId="132"/>
-    <cellStyle name="Followed Hyperlink 73" xfId="133"/>
-    <cellStyle name="Followed Hyperlink 74" xfId="134"/>
-    <cellStyle name="Followed Hyperlink 75" xfId="135"/>
-    <cellStyle name="Followed Hyperlink 76" xfId="136"/>
-    <cellStyle name="Followed Hyperlink 77" xfId="137"/>
-    <cellStyle name="Followed Hyperlink 78" xfId="138"/>
-    <cellStyle name="Followed Hyperlink 79" xfId="139"/>
-    <cellStyle name="Followed Hyperlink 8" xfId="68"/>
-    <cellStyle name="Followed Hyperlink 80" xfId="140"/>
-    <cellStyle name="Followed Hyperlink 81" xfId="141"/>
-    <cellStyle name="Followed Hyperlink 82" xfId="142"/>
-    <cellStyle name="Followed Hyperlink 83" xfId="143"/>
-    <cellStyle name="Followed Hyperlink 84" xfId="144"/>
-    <cellStyle name="Followed Hyperlink 85" xfId="145"/>
-    <cellStyle name="Followed Hyperlink 86" xfId="146"/>
-    <cellStyle name="Followed Hyperlink 87" xfId="147"/>
-    <cellStyle name="Followed Hyperlink 88" xfId="148"/>
-    <cellStyle name="Followed Hyperlink 89" xfId="149"/>
-    <cellStyle name="Followed Hyperlink 9" xfId="69"/>
-    <cellStyle name="Followed Hyperlink 90" xfId="150"/>
-    <cellStyle name="Followed Hyperlink 91" xfId="151"/>
-    <cellStyle name="Followed Hyperlink 92" xfId="152"/>
-    <cellStyle name="Followed Hyperlink 93" xfId="153"/>
-    <cellStyle name="Followed Hyperlink 94" xfId="154"/>
-    <cellStyle name="Followed Hyperlink 95" xfId="155"/>
-    <cellStyle name="Followed Hyperlink 96" xfId="156"/>
-    <cellStyle name="Followed Hyperlink 97" xfId="157"/>
-    <cellStyle name="Followed Hyperlink 98" xfId="158"/>
+    <cellStyle name="Followed Hyperlink 10" xfId="70" xr:uid="{00000000-0005-0000-0000-0000570C0000}"/>
+    <cellStyle name="Followed Hyperlink 11" xfId="71" xr:uid="{00000000-0005-0000-0000-0000580C0000}"/>
+    <cellStyle name="Followed Hyperlink 12" xfId="72" xr:uid="{00000000-0005-0000-0000-0000590C0000}"/>
+    <cellStyle name="Followed Hyperlink 13" xfId="73" xr:uid="{00000000-0005-0000-0000-00005A0C0000}"/>
+    <cellStyle name="Followed Hyperlink 14" xfId="74" xr:uid="{00000000-0005-0000-0000-00005B0C0000}"/>
+    <cellStyle name="Followed Hyperlink 15" xfId="75" xr:uid="{00000000-0005-0000-0000-00005C0C0000}"/>
+    <cellStyle name="Followed Hyperlink 16" xfId="76" xr:uid="{00000000-0005-0000-0000-00005D0C0000}"/>
+    <cellStyle name="Followed Hyperlink 17" xfId="77" xr:uid="{00000000-0005-0000-0000-00005E0C0000}"/>
+    <cellStyle name="Followed Hyperlink 18" xfId="78" xr:uid="{00000000-0005-0000-0000-00005F0C0000}"/>
+    <cellStyle name="Followed Hyperlink 19" xfId="79" xr:uid="{00000000-0005-0000-0000-0000600C0000}"/>
+    <cellStyle name="Followed Hyperlink 2" xfId="62" xr:uid="{00000000-0005-0000-0000-0000610C0000}"/>
+    <cellStyle name="Followed Hyperlink 20" xfId="80" xr:uid="{00000000-0005-0000-0000-0000620C0000}"/>
+    <cellStyle name="Followed Hyperlink 21" xfId="81" xr:uid="{00000000-0005-0000-0000-0000630C0000}"/>
+    <cellStyle name="Followed Hyperlink 22" xfId="82" xr:uid="{00000000-0005-0000-0000-0000640C0000}"/>
+    <cellStyle name="Followed Hyperlink 23" xfId="83" xr:uid="{00000000-0005-0000-0000-0000650C0000}"/>
+    <cellStyle name="Followed Hyperlink 24" xfId="84" xr:uid="{00000000-0005-0000-0000-0000660C0000}"/>
+    <cellStyle name="Followed Hyperlink 25" xfId="85" xr:uid="{00000000-0005-0000-0000-0000670C0000}"/>
+    <cellStyle name="Followed Hyperlink 26" xfId="86" xr:uid="{00000000-0005-0000-0000-0000680C0000}"/>
+    <cellStyle name="Followed Hyperlink 27" xfId="87" xr:uid="{00000000-0005-0000-0000-0000690C0000}"/>
+    <cellStyle name="Followed Hyperlink 28" xfId="88" xr:uid="{00000000-0005-0000-0000-00006A0C0000}"/>
+    <cellStyle name="Followed Hyperlink 29" xfId="89" xr:uid="{00000000-0005-0000-0000-00006B0C0000}"/>
+    <cellStyle name="Followed Hyperlink 3" xfId="63" xr:uid="{00000000-0005-0000-0000-00006C0C0000}"/>
+    <cellStyle name="Followed Hyperlink 30" xfId="90" xr:uid="{00000000-0005-0000-0000-00006D0C0000}"/>
+    <cellStyle name="Followed Hyperlink 31" xfId="91" xr:uid="{00000000-0005-0000-0000-00006E0C0000}"/>
+    <cellStyle name="Followed Hyperlink 32" xfId="92" xr:uid="{00000000-0005-0000-0000-00006F0C0000}"/>
+    <cellStyle name="Followed Hyperlink 33" xfId="93" xr:uid="{00000000-0005-0000-0000-0000700C0000}"/>
+    <cellStyle name="Followed Hyperlink 34" xfId="94" xr:uid="{00000000-0005-0000-0000-0000710C0000}"/>
+    <cellStyle name="Followed Hyperlink 35" xfId="95" xr:uid="{00000000-0005-0000-0000-0000720C0000}"/>
+    <cellStyle name="Followed Hyperlink 36" xfId="96" xr:uid="{00000000-0005-0000-0000-0000730C0000}"/>
+    <cellStyle name="Followed Hyperlink 37" xfId="97" xr:uid="{00000000-0005-0000-0000-0000740C0000}"/>
+    <cellStyle name="Followed Hyperlink 38" xfId="98" xr:uid="{00000000-0005-0000-0000-0000750C0000}"/>
+    <cellStyle name="Followed Hyperlink 39" xfId="99" xr:uid="{00000000-0005-0000-0000-0000760C0000}"/>
+    <cellStyle name="Followed Hyperlink 4" xfId="64" xr:uid="{00000000-0005-0000-0000-0000770C0000}"/>
+    <cellStyle name="Followed Hyperlink 40" xfId="100" xr:uid="{00000000-0005-0000-0000-0000780C0000}"/>
+    <cellStyle name="Followed Hyperlink 41" xfId="101" xr:uid="{00000000-0005-0000-0000-0000790C0000}"/>
+    <cellStyle name="Followed Hyperlink 42" xfId="102" xr:uid="{00000000-0005-0000-0000-00007A0C0000}"/>
+    <cellStyle name="Followed Hyperlink 43" xfId="103" xr:uid="{00000000-0005-0000-0000-00007B0C0000}"/>
+    <cellStyle name="Followed Hyperlink 44" xfId="104" xr:uid="{00000000-0005-0000-0000-00007C0C0000}"/>
+    <cellStyle name="Followed Hyperlink 45" xfId="105" xr:uid="{00000000-0005-0000-0000-00007D0C0000}"/>
+    <cellStyle name="Followed Hyperlink 46" xfId="106" xr:uid="{00000000-0005-0000-0000-00007E0C0000}"/>
+    <cellStyle name="Followed Hyperlink 47" xfId="107" xr:uid="{00000000-0005-0000-0000-00007F0C0000}"/>
+    <cellStyle name="Followed Hyperlink 48" xfId="108" xr:uid="{00000000-0005-0000-0000-0000800C0000}"/>
+    <cellStyle name="Followed Hyperlink 49" xfId="109" xr:uid="{00000000-0005-0000-0000-0000810C0000}"/>
+    <cellStyle name="Followed Hyperlink 5" xfId="65" xr:uid="{00000000-0005-0000-0000-0000820C0000}"/>
+    <cellStyle name="Followed Hyperlink 50" xfId="110" xr:uid="{00000000-0005-0000-0000-0000830C0000}"/>
+    <cellStyle name="Followed Hyperlink 51" xfId="111" xr:uid="{00000000-0005-0000-0000-0000840C0000}"/>
+    <cellStyle name="Followed Hyperlink 52" xfId="112" xr:uid="{00000000-0005-0000-0000-0000850C0000}"/>
+    <cellStyle name="Followed Hyperlink 53" xfId="113" xr:uid="{00000000-0005-0000-0000-0000860C0000}"/>
+    <cellStyle name="Followed Hyperlink 54" xfId="114" xr:uid="{00000000-0005-0000-0000-0000870C0000}"/>
+    <cellStyle name="Followed Hyperlink 55" xfId="115" xr:uid="{00000000-0005-0000-0000-0000880C0000}"/>
+    <cellStyle name="Followed Hyperlink 56" xfId="116" xr:uid="{00000000-0005-0000-0000-0000890C0000}"/>
+    <cellStyle name="Followed Hyperlink 57" xfId="117" xr:uid="{00000000-0005-0000-0000-00008A0C0000}"/>
+    <cellStyle name="Followed Hyperlink 58" xfId="118" xr:uid="{00000000-0005-0000-0000-00008B0C0000}"/>
+    <cellStyle name="Followed Hyperlink 59" xfId="119" xr:uid="{00000000-0005-0000-0000-00008C0C0000}"/>
+    <cellStyle name="Followed Hyperlink 6" xfId="66" xr:uid="{00000000-0005-0000-0000-00008D0C0000}"/>
+    <cellStyle name="Followed Hyperlink 60" xfId="120" xr:uid="{00000000-0005-0000-0000-00008E0C0000}"/>
+    <cellStyle name="Followed Hyperlink 61" xfId="121" xr:uid="{00000000-0005-0000-0000-00008F0C0000}"/>
+    <cellStyle name="Followed Hyperlink 62" xfId="122" xr:uid="{00000000-0005-0000-0000-0000900C0000}"/>
+    <cellStyle name="Followed Hyperlink 63" xfId="123" xr:uid="{00000000-0005-0000-0000-0000910C0000}"/>
+    <cellStyle name="Followed Hyperlink 64" xfId="124" xr:uid="{00000000-0005-0000-0000-0000920C0000}"/>
+    <cellStyle name="Followed Hyperlink 65" xfId="125" xr:uid="{00000000-0005-0000-0000-0000930C0000}"/>
+    <cellStyle name="Followed Hyperlink 66" xfId="126" xr:uid="{00000000-0005-0000-0000-0000940C0000}"/>
+    <cellStyle name="Followed Hyperlink 67" xfId="127" xr:uid="{00000000-0005-0000-0000-0000950C0000}"/>
+    <cellStyle name="Followed Hyperlink 68" xfId="128" xr:uid="{00000000-0005-0000-0000-0000960C0000}"/>
+    <cellStyle name="Followed Hyperlink 69" xfId="129" xr:uid="{00000000-0005-0000-0000-0000970C0000}"/>
+    <cellStyle name="Followed Hyperlink 7" xfId="67" xr:uid="{00000000-0005-0000-0000-0000980C0000}"/>
+    <cellStyle name="Followed Hyperlink 70" xfId="130" xr:uid="{00000000-0005-0000-0000-0000990C0000}"/>
+    <cellStyle name="Followed Hyperlink 71" xfId="131" xr:uid="{00000000-0005-0000-0000-00009A0C0000}"/>
+    <cellStyle name="Followed Hyperlink 72" xfId="132" xr:uid="{00000000-0005-0000-0000-00009B0C0000}"/>
+    <cellStyle name="Followed Hyperlink 73" xfId="133" xr:uid="{00000000-0005-0000-0000-00009C0C0000}"/>
+    <cellStyle name="Followed Hyperlink 74" xfId="134" xr:uid="{00000000-0005-0000-0000-00009D0C0000}"/>
+    <cellStyle name="Followed Hyperlink 75" xfId="135" xr:uid="{00000000-0005-0000-0000-00009E0C0000}"/>
+    <cellStyle name="Followed Hyperlink 76" xfId="136" xr:uid="{00000000-0005-0000-0000-00009F0C0000}"/>
+    <cellStyle name="Followed Hyperlink 77" xfId="137" xr:uid="{00000000-0005-0000-0000-0000A00C0000}"/>
+    <cellStyle name="Followed Hyperlink 78" xfId="138" xr:uid="{00000000-0005-0000-0000-0000A10C0000}"/>
+    <cellStyle name="Followed Hyperlink 79" xfId="139" xr:uid="{00000000-0005-0000-0000-0000A20C0000}"/>
+    <cellStyle name="Followed Hyperlink 8" xfId="68" xr:uid="{00000000-0005-0000-0000-0000A30C0000}"/>
+    <cellStyle name="Followed Hyperlink 80" xfId="140" xr:uid="{00000000-0005-0000-0000-0000A40C0000}"/>
+    <cellStyle name="Followed Hyperlink 81" xfId="141" xr:uid="{00000000-0005-0000-0000-0000A50C0000}"/>
+    <cellStyle name="Followed Hyperlink 82" xfId="142" xr:uid="{00000000-0005-0000-0000-0000A60C0000}"/>
+    <cellStyle name="Followed Hyperlink 83" xfId="143" xr:uid="{00000000-0005-0000-0000-0000A70C0000}"/>
+    <cellStyle name="Followed Hyperlink 84" xfId="144" xr:uid="{00000000-0005-0000-0000-0000A80C0000}"/>
+    <cellStyle name="Followed Hyperlink 85" xfId="145" xr:uid="{00000000-0005-0000-0000-0000A90C0000}"/>
+    <cellStyle name="Followed Hyperlink 86" xfId="146" xr:uid="{00000000-0005-0000-0000-0000AA0C0000}"/>
+    <cellStyle name="Followed Hyperlink 87" xfId="147" xr:uid="{00000000-0005-0000-0000-0000AB0C0000}"/>
+    <cellStyle name="Followed Hyperlink 88" xfId="148" xr:uid="{00000000-0005-0000-0000-0000AC0C0000}"/>
+    <cellStyle name="Followed Hyperlink 89" xfId="149" xr:uid="{00000000-0005-0000-0000-0000AD0C0000}"/>
+    <cellStyle name="Followed Hyperlink 9" xfId="69" xr:uid="{00000000-0005-0000-0000-0000AE0C0000}"/>
+    <cellStyle name="Followed Hyperlink 90" xfId="150" xr:uid="{00000000-0005-0000-0000-0000AF0C0000}"/>
+    <cellStyle name="Followed Hyperlink 91" xfId="151" xr:uid="{00000000-0005-0000-0000-0000B00C0000}"/>
+    <cellStyle name="Followed Hyperlink 92" xfId="152" xr:uid="{00000000-0005-0000-0000-0000B10C0000}"/>
+    <cellStyle name="Followed Hyperlink 93" xfId="153" xr:uid="{00000000-0005-0000-0000-0000B20C0000}"/>
+    <cellStyle name="Followed Hyperlink 94" xfId="154" xr:uid="{00000000-0005-0000-0000-0000B30C0000}"/>
+    <cellStyle name="Followed Hyperlink 95" xfId="155" xr:uid="{00000000-0005-0000-0000-0000B40C0000}"/>
+    <cellStyle name="Followed Hyperlink 96" xfId="156" xr:uid="{00000000-0005-0000-0000-0000B50C0000}"/>
+    <cellStyle name="Followed Hyperlink 97" xfId="157" xr:uid="{00000000-0005-0000-0000-0000B60C0000}"/>
+    <cellStyle name="Followed Hyperlink 98" xfId="158" xr:uid="{00000000-0005-0000-0000-0000B70C0000}"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
@@ -14726,28 +14739,28 @@
     <cellStyle name="Hyperlink" xfId="6422" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="45"/>
-    <cellStyle name="Normal 2" xfId="49"/>
-    <cellStyle name="Normal 2 2" xfId="164"/>
-    <cellStyle name="Normal 2 3" xfId="60"/>
-    <cellStyle name="Normal 3" xfId="50"/>
-    <cellStyle name="Normal 3 2" xfId="165"/>
-    <cellStyle name="Normal 3 3" xfId="61"/>
-    <cellStyle name="Normal 4" xfId="56"/>
-    <cellStyle name="Normal 4 2" xfId="170"/>
-    <cellStyle name="Normal 5" xfId="55"/>
-    <cellStyle name="Normal 5 2" xfId="169"/>
-    <cellStyle name="Normal 5 2 2" xfId="644"/>
-    <cellStyle name="Normal 6" xfId="160"/>
-    <cellStyle name="Normal 7" xfId="54"/>
-    <cellStyle name="Normal 8" xfId="168"/>
-    <cellStyle name="Normal 9" xfId="264"/>
-    <cellStyle name="Percent 2" xfId="52"/>
-    <cellStyle name="Percent 2 2" xfId="167"/>
-    <cellStyle name="Percent 2 3" xfId="58"/>
-    <cellStyle name="Percent 2 4" xfId="172"/>
-    <cellStyle name="Percent 3" xfId="162"/>
-    <cellStyle name="Percent 4" xfId="47"/>
+    <cellStyle name="Normal 10" xfId="45" xr:uid="{00000000-0005-0000-0000-000002190000}"/>
+    <cellStyle name="Normal 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000003190000}"/>
+    <cellStyle name="Normal 2 2" xfId="164" xr:uid="{00000000-0005-0000-0000-000004190000}"/>
+    <cellStyle name="Normal 2 3" xfId="60" xr:uid="{00000000-0005-0000-0000-000005190000}"/>
+    <cellStyle name="Normal 3" xfId="50" xr:uid="{00000000-0005-0000-0000-000006190000}"/>
+    <cellStyle name="Normal 3 2" xfId="165" xr:uid="{00000000-0005-0000-0000-000007190000}"/>
+    <cellStyle name="Normal 3 3" xfId="61" xr:uid="{00000000-0005-0000-0000-000008190000}"/>
+    <cellStyle name="Normal 4" xfId="56" xr:uid="{00000000-0005-0000-0000-000009190000}"/>
+    <cellStyle name="Normal 4 2" xfId="170" xr:uid="{00000000-0005-0000-0000-00000A190000}"/>
+    <cellStyle name="Normal 5" xfId="55" xr:uid="{00000000-0005-0000-0000-00000B190000}"/>
+    <cellStyle name="Normal 5 2" xfId="169" xr:uid="{00000000-0005-0000-0000-00000C190000}"/>
+    <cellStyle name="Normal 5 2 2" xfId="644" xr:uid="{00000000-0005-0000-0000-00000D190000}"/>
+    <cellStyle name="Normal 6" xfId="160" xr:uid="{00000000-0005-0000-0000-00000E190000}"/>
+    <cellStyle name="Normal 7" xfId="54" xr:uid="{00000000-0005-0000-0000-00000F190000}"/>
+    <cellStyle name="Normal 8" xfId="168" xr:uid="{00000000-0005-0000-0000-000010190000}"/>
+    <cellStyle name="Normal 9" xfId="264" xr:uid="{00000000-0005-0000-0000-000011190000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000012190000}"/>
+    <cellStyle name="Percent 2 2" xfId="167" xr:uid="{00000000-0005-0000-0000-000013190000}"/>
+    <cellStyle name="Percent 2 3" xfId="58" xr:uid="{00000000-0005-0000-0000-000014190000}"/>
+    <cellStyle name="Percent 2 4" xfId="172" xr:uid="{00000000-0005-0000-0000-000015190000}"/>
+    <cellStyle name="Percent 3" xfId="162" xr:uid="{00000000-0005-0000-0000-000016190000}"/>
+    <cellStyle name="Percent 4" xfId="47" xr:uid="{00000000-0005-0000-0000-000017190000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -14770,6 +14783,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -15061,17 +15077,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -15173,24 +15189,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>456</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>457</v>
       </c>
     </row>
@@ -15505,40 +15521,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AM39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AM39" sqref="AM39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="8.85546875" style="2"/>
-    <col min="26" max="26" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="8.83203125" style="2"/>
+    <col min="26" max="26" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="31" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="34" max="37" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.2">
@@ -15658,7 +15674,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
@@ -15705,7 +15721,7 @@
       <c r="AL2" s="30"/>
       <c r="AM2" s="33"/>
     </row>
-    <row r="3" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>2</v>
       </c>
@@ -15752,7 +15768,7 @@
       <c r="AL3" s="31"/>
       <c r="AM3" s="35"/>
     </row>
-    <row r="4" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
@@ -15803,7 +15819,7 @@
       <c r="AL4" s="30"/>
       <c r="AM4" s="33"/>
     </row>
-    <row r="5" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>4</v>
       </c>
@@ -15854,7 +15870,7 @@
       <c r="AL5" s="30"/>
       <c r="AM5" s="33"/>
     </row>
-    <row r="6" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>5</v>
       </c>
@@ -15905,7 +15921,7 @@
       <c r="AL6" s="30"/>
       <c r="AM6" s="33"/>
     </row>
-    <row r="7" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>6</v>
       </c>
@@ -15956,7 +15972,7 @@
       <c r="AL7" s="30"/>
       <c r="AM7" s="33"/>
     </row>
-    <row r="8" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>7</v>
       </c>
@@ -16007,7 +16023,7 @@
       <c r="AL8" s="30"/>
       <c r="AM8" s="33"/>
     </row>
-    <row r="9" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>8</v>
       </c>
@@ -16054,7 +16070,7 @@
       <c r="AL9" s="31"/>
       <c r="AM9" s="35"/>
     </row>
-    <row r="10" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
@@ -16105,7 +16121,7 @@
       <c r="AL10" s="30"/>
       <c r="AM10" s="33"/>
     </row>
-    <row r="11" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>10</v>
       </c>
@@ -16156,7 +16172,7 @@
       <c r="AL11" s="30"/>
       <c r="AM11" s="33"/>
     </row>
-    <row r="12" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>11</v>
       </c>
@@ -16207,7 +16223,7 @@
       <c r="AL12" s="30"/>
       <c r="AM12" s="33"/>
     </row>
-    <row r="13" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>12</v>
       </c>
@@ -16258,7 +16274,7 @@
       <c r="AL13" s="30"/>
       <c r="AM13" s="33"/>
     </row>
-    <row r="14" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>13</v>
       </c>
@@ -16309,7 +16325,7 @@
       <c r="AL14" s="30"/>
       <c r="AM14" s="33"/>
     </row>
-    <row r="15" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>14</v>
       </c>
@@ -16356,7 +16372,7 @@
       <c r="AL15" s="31"/>
       <c r="AM15" s="35"/>
     </row>
-    <row r="16" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>15</v>
       </c>
@@ -16407,7 +16423,7 @@
       <c r="AL16" s="30"/>
       <c r="AM16" s="33"/>
     </row>
-    <row r="17" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>16</v>
       </c>
@@ -16458,7 +16474,7 @@
       <c r="AL17" s="30"/>
       <c r="AM17" s="33"/>
     </row>
-    <row r="18" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
         <v>17</v>
       </c>
@@ -16509,7 +16525,7 @@
       <c r="AL18" s="30"/>
       <c r="AM18" s="33"/>
     </row>
-    <row r="19" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
         <v>18</v>
       </c>
@@ -16560,7 +16576,7 @@
       <c r="AL19" s="30"/>
       <c r="AM19" s="33"/>
     </row>
-    <row r="20" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
         <v>19</v>
       </c>
@@ -16611,7 +16627,7 @@
       <c r="AL20" s="30"/>
       <c r="AM20" s="33"/>
     </row>
-    <row r="21" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>20</v>
       </c>
@@ -16658,7 +16674,7 @@
       <c r="AL21" s="31"/>
       <c r="AM21" s="35"/>
     </row>
-    <row r="22" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>33</v>
       </c>
@@ -16709,7 +16725,7 @@
       <c r="AL22" s="30"/>
       <c r="AM22" s="33"/>
     </row>
-    <row r="23" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>34</v>
       </c>
@@ -16760,7 +16776,7 @@
       <c r="AL23" s="30"/>
       <c r="AM23" s="33"/>
     </row>
-    <row r="24" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>35</v>
       </c>
@@ -16811,7 +16827,7 @@
       <c r="AL24" s="30"/>
       <c r="AM24" s="33"/>
     </row>
-    <row r="25" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>36</v>
       </c>
@@ -16862,7 +16878,7 @@
       <c r="AL25" s="30"/>
       <c r="AM25" s="33"/>
     </row>
-    <row r="26" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
         <v>37</v>
       </c>
@@ -16913,7 +16929,7 @@
       <c r="AL26" s="30"/>
       <c r="AM26" s="33"/>
     </row>
-    <row r="27" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>38</v>
       </c>
@@ -16960,7 +16976,7 @@
       <c r="AL27" s="31"/>
       <c r="AM27" s="35"/>
     </row>
-    <row r="28" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="25" t="s">
         <v>21</v>
       </c>
@@ -17015,7 +17031,7 @@
       <c r="AL28" s="30"/>
       <c r="AM28" s="33"/>
     </row>
-    <row r="29" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
         <v>22</v>
       </c>
@@ -17070,7 +17086,7 @@
       <c r="AL29" s="30"/>
       <c r="AM29" s="33"/>
     </row>
-    <row r="30" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
         <v>23</v>
       </c>
@@ -17131,7 +17147,7 @@
       <c r="AL30" s="30"/>
       <c r="AM30" s="33"/>
     </row>
-    <row r="31" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
         <v>24</v>
       </c>
@@ -17192,7 +17208,7 @@
       </c>
       <c r="AM31" s="33"/>
     </row>
-    <row r="32" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
         <v>25</v>
       </c>
@@ -17253,7 +17269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
         <v>26</v>
       </c>
@@ -17308,7 +17324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>27</v>
       </c>
@@ -17363,7 +17379,7 @@
       <c r="AL34" s="30"/>
       <c r="AM34" s="33"/>
     </row>
-    <row r="35" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>28</v>
       </c>
@@ -17412,7 +17428,7 @@
       <c r="AL35" s="30"/>
       <c r="AM35" s="33"/>
     </row>
-    <row r="36" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
         <v>29</v>
       </c>
@@ -17467,7 +17483,7 @@
       <c r="AL36" s="30"/>
       <c r="AM36" s="33"/>
     </row>
-    <row r="37" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>30</v>
       </c>
@@ -17522,7 +17538,7 @@
       <c r="AL37" s="30"/>
       <c r="AM37" s="33"/>
     </row>
-    <row r="38" spans="1:39" ht="17.100000000000001" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>31</v>
       </c>
@@ -17577,7 +17593,7 @@
       </c>
       <c r="AM38" s="33"/>
     </row>
-    <row r="39" spans="1:39" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
         <v>32</v>
       </c>
@@ -17644,24 +17660,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" activeCellId="1" sqref="H35:H42 H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="68.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="68.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="10" style="6" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="6"/>
+    <col min="7" max="7" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -17686,7 +17703,9 @@
       <c r="G1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="39"/>
+      <c r="H1" s="45" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -17710,6 +17729,7 @@
       <c r="G2" s="6">
         <v>1</v>
       </c>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
@@ -17733,6 +17753,7 @@
       <c r="G3" s="6">
         <v>0</v>
       </c>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
@@ -17756,6 +17777,7 @@
       <c r="G4" s="6">
         <v>0</v>
       </c>
+      <c r="H4" s="38"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -17779,6 +17801,7 @@
       <c r="G5" s="6">
         <v>1</v>
       </c>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -17802,6 +17825,7 @@
       <c r="G6" s="6">
         <v>1</v>
       </c>
+      <c r="H6" s="38"/>
     </row>
     <row r="7" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
@@ -17848,6 +17872,9 @@
       <c r="G8" s="6">
         <v>1</v>
       </c>
+      <c r="H8" s="38" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
@@ -17871,6 +17898,9 @@
       <c r="G9" s="6">
         <v>1</v>
       </c>
+      <c r="H9" s="38" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
@@ -17894,6 +17924,7 @@
       <c r="G10" s="6">
         <v>1</v>
       </c>
+      <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
@@ -17917,6 +17948,7 @@
       <c r="G11" s="6">
         <v>1</v>
       </c>
+      <c r="H11" s="38"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
@@ -17940,6 +17972,9 @@
       <c r="G12" s="6">
         <v>1</v>
       </c>
+      <c r="H12" s="38" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
@@ -17963,6 +17998,9 @@
       <c r="G13" s="6">
         <v>1</v>
       </c>
+      <c r="H13" s="38" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
@@ -17986,6 +18024,9 @@
       <c r="G14" s="6">
         <v>1</v>
       </c>
+      <c r="H14" s="38" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
@@ -18009,6 +18050,7 @@
       <c r="G15" s="6">
         <v>1</v>
       </c>
+      <c r="H15" s="38"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -18032,8 +18074,9 @@
       <c r="G16" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="38"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>157</v>
       </c>
@@ -18055,8 +18098,9 @@
       <c r="G17" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="38"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>160</v>
       </c>
@@ -18078,8 +18122,9 @@
       <c r="G18" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="38"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>163</v>
       </c>
@@ -18101,8 +18146,9 @@
       <c r="G19" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="38"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>165</v>
       </c>
@@ -18124,8 +18170,9 @@
       <c r="G20" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="38"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>395</v>
       </c>
@@ -18147,8 +18194,11 @@
       <c r="G21" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="38" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
         <v>472</v>
       </c>
@@ -18170,8 +18220,11 @@
       <c r="G22" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="38" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
         <v>251</v>
       </c>
@@ -18194,7 +18247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>166</v>
       </c>
@@ -18216,8 +18269,9 @@
       <c r="G24" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="38"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>167</v>
       </c>
@@ -18239,8 +18293,9 @@
       <c r="G25" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="38"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>168</v>
       </c>
@@ -18262,8 +18317,9 @@
       <c r="G26" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="38"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>169</v>
       </c>
@@ -18285,8 +18341,9 @@
       <c r="G27" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="38"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>170</v>
       </c>
@@ -18308,8 +18365,9 @@
       <c r="G28" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="38"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>172</v>
       </c>
@@ -18332,7 +18390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>177</v>
       </c>
@@ -18355,7 +18413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>179</v>
       </c>
@@ -18378,7 +18436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>181</v>
       </c>
@@ -18401,7 +18459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>183</v>
       </c>
@@ -18424,7 +18482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>128</v>
       </c>
@@ -18447,7 +18505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>125</v>
       </c>
@@ -18469,8 +18527,9 @@
       <c r="G35" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" s="38"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>135</v>
       </c>
@@ -18492,8 +18551,9 @@
       <c r="G36" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" s="46"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>140</v>
       </c>
@@ -18515,8 +18575,9 @@
       <c r="G37" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" s="46"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>143</v>
       </c>
@@ -18538,8 +18599,9 @@
       <c r="G38" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" s="46"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>149</v>
       </c>
@@ -18561,8 +18623,9 @@
       <c r="G39" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" s="46"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>151</v>
       </c>
@@ -18584,8 +18647,9 @@
       <c r="G40" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" s="46"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>154</v>
       </c>
@@ -18607,8 +18671,9 @@
       <c r="G41" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" s="46"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>146</v>
       </c>
@@ -18630,8 +18695,9 @@
       <c r="G42" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" s="46"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>130</v>
       </c>
@@ -18653,8 +18719,11 @@
       <c r="G43" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" s="46" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>132</v>
       </c>
@@ -18676,8 +18745,9 @@
       <c r="G44" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="46"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>95</v>
       </c>
@@ -18700,7 +18770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>100</v>
       </c>
@@ -18723,7 +18793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>102</v>
       </c>
@@ -18746,7 +18816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>401</v>
       </c>
@@ -18769,7 +18839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>186</v>
       </c>
@@ -18792,7 +18862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>189</v>
       </c>
@@ -18815,7 +18885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>191</v>
       </c>
@@ -18838,7 +18908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>193</v>
       </c>
@@ -18861,7 +18931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>195</v>
       </c>
@@ -18884,7 +18954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>197</v>
       </c>
@@ -18907,7 +18977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>199</v>
       </c>
@@ -18930,7 +19000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>201</v>
       </c>
@@ -18953,7 +19023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>203</v>
       </c>
@@ -18976,7 +19046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>205</v>
       </c>
@@ -18999,7 +19069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>207</v>
       </c>
@@ -19022,7 +19092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>209</v>
       </c>
@@ -19045,7 +19115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>211</v>
       </c>
@@ -19068,7 +19138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>213</v>
       </c>
@@ -19091,7 +19161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>215</v>
       </c>
@@ -19114,7 +19184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>217</v>
       </c>
@@ -19137,7 +19207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>219</v>
       </c>
@@ -19160,7 +19230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>221</v>
       </c>
@@ -19183,7 +19253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>223</v>
       </c>
@@ -19206,7 +19276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>225</v>
       </c>
@@ -19229,7 +19299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>227</v>
       </c>
@@ -19252,7 +19322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>229</v>
       </c>
@@ -19275,7 +19345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>231</v>
       </c>
@@ -19298,7 +19368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>233</v>
       </c>
@@ -19321,7 +19391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>397</v>
       </c>
@@ -19344,7 +19414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>235</v>
       </c>
@@ -19367,7 +19437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>237</v>
       </c>
@@ -19390,7 +19460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>239</v>
       </c>
@@ -19413,7 +19483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>241</v>
       </c>
@@ -19436,7 +19506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>243</v>
       </c>
@@ -19459,7 +19529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>245</v>
       </c>
@@ -19482,7 +19552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>247</v>
       </c>
@@ -19505,7 +19575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>249</v>
       </c>
@@ -19528,7 +19598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>253</v>
       </c>
@@ -19551,7 +19621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>255</v>
       </c>
@@ -19574,7 +19644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>257</v>
       </c>
@@ -19597,7 +19667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>259</v>
       </c>
@@ -19620,7 +19690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>260</v>
       </c>
@@ -19643,7 +19713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>261</v>
       </c>
@@ -19666,7 +19736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>263</v>
       </c>
@@ -19689,7 +19759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
         <v>265</v>
       </c>
@@ -19712,7 +19782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
         <v>267</v>
       </c>
@@ -19735,7 +19805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>269</v>
       </c>
@@ -19758,7 +19828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>271</v>
       </c>
@@ -19781,7 +19851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
         <v>273</v>
       </c>
@@ -19804,7 +19874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>274</v>
       </c>
@@ -19827,7 +19897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>276</v>
       </c>
@@ -19850,7 +19920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
         <v>278</v>
       </c>
@@ -19873,7 +19943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
         <v>280</v>
       </c>
@@ -19896,7 +19966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>282</v>
       </c>
@@ -19919,7 +19989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>284</v>
       </c>
@@ -19942,7 +20012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>286</v>
       </c>
@@ -19965,7 +20035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>288</v>
       </c>
@@ -19988,7 +20058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>290</v>
       </c>
@@ -20011,7 +20081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>292</v>
       </c>
@@ -20034,7 +20104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>294</v>
       </c>
@@ -20057,7 +20127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>296</v>
       </c>
@@ -20080,68 +20150,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D106" s="6"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D107" s="6"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
       <c r="E109" s="6"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C110" s="6"/>
       <c r="D110" s="6"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
       <c r="E111" s="6"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
       <c r="E112" s="6"/>
     </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C113" s="6"/>
       <c r="D113" s="6"/>
       <c r="E113" s="6"/>
     </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
       <c r="E114" s="6"/>
     </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C115" s="6"/>
       <c r="D115" s="6"/>
       <c r="E115" s="6"/>
     </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
       <c r="E116" s="6"/>
     </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C117" s="6"/>
       <c r="D117" s="6"/>
       <c r="E117" s="6"/>
     </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C118" s="6"/>
       <c r="D118" s="6"/>
       <c r="E118" s="6"/>
     </row>
-    <row r="119" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C119" s="6"/>
       <c r="D119" s="6"/>
       <c r="E119" s="6"/>
@@ -20153,22 +20223,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="76.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -21158,16 +21228,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="62.28515625" customWidth="1"/>
+    <col min="1" max="1" width="62.33203125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
@@ -21209,13 +21279,13 @@
       <c r="C2" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="41">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="41">
         <v>1E-4</v>
       </c>
-      <c r="F2" s="42">
+      <c r="F2" s="41">
         <v>1.4E-3</v>
       </c>
       <c r="G2" t="s">
@@ -21236,13 +21306,13 @@
       <c r="C3" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="41">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="41">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="41">
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="G3" t="s">
@@ -21263,13 +21333,13 @@
       <c r="C4" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="41">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="41">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="41">
         <v>2.8E-3</v>
       </c>
       <c r="G4" t="s">
@@ -21290,13 +21360,13 @@
       <c r="C5" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="41">
         <v>1.38E-2</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="41">
         <v>1.0200000000000001E-2</v>
       </c>
-      <c r="F5" s="42">
+      <c r="F5" s="41">
         <v>1.8599999999999998E-2</v>
       </c>
       <c r="G5" t="s">
@@ -21317,13 +21387,13 @@
       <c r="C6" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="41">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="41">
         <v>6.3E-3</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="41">
         <v>2.4E-2</v>
       </c>
       <c r="G6" t="s">
@@ -21344,13 +21414,13 @@
       <c r="C7" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="41">
         <v>0.36699999999999999</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="41">
         <v>0.29399999999999998</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="41">
         <v>0.44</v>
       </c>
       <c r="G7" t="s">
@@ -21371,13 +21441,13 @@
       <c r="C8" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="41">
         <v>0.20499999999999999</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="41">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8" s="41">
         <v>0.27</v>
       </c>
       <c r="G8" t="s">
@@ -21398,13 +21468,13 @@
       <c r="C9" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="42">
         <v>5.6</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="42">
         <v>3.3</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="42">
         <v>9.1</v>
       </c>
       <c r="G9" t="s">
@@ -21425,13 +21495,13 @@
       <c r="C10" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D10" s="43">
-        <v>1</v>
-      </c>
-      <c r="E10" s="43">
-        <v>1</v>
-      </c>
-      <c r="F10" s="43">
+      <c r="D10" s="42">
+        <v>1</v>
+      </c>
+      <c r="E10" s="42">
+        <v>1</v>
+      </c>
+      <c r="F10" s="42">
         <v>1</v>
       </c>
       <c r="G10" t="s">
@@ -21452,13 +21522,13 @@
       <c r="C11" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D11" s="43">
-        <v>1</v>
-      </c>
-      <c r="E11" s="43">
-        <v>1</v>
-      </c>
-      <c r="F11" s="43">
+      <c r="D11" s="42">
+        <v>1</v>
+      </c>
+      <c r="E11" s="42">
+        <v>1</v>
+      </c>
+      <c r="F11" s="42">
         <v>1</v>
       </c>
       <c r="G11" t="s">
@@ -21479,13 +21549,13 @@
       <c r="C12" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="D12" s="43">
-        <v>1</v>
-      </c>
-      <c r="E12" s="43">
-        <v>1</v>
-      </c>
-      <c r="F12" s="43">
+      <c r="D12" s="42">
+        <v>1</v>
+      </c>
+      <c r="E12" s="42">
+        <v>1</v>
+      </c>
+      <c r="F12" s="42">
         <v>1</v>
       </c>
       <c r="G12" t="s">
@@ -21506,13 +21576,13 @@
       <c r="C13" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="42">
         <v>3.49</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="42">
         <v>1.76</v>
       </c>
-      <c r="F13" s="43">
+      <c r="F13" s="42">
         <v>6.92</v>
       </c>
       <c r="G13" t="s">
@@ -21533,13 +21603,13 @@
       <c r="C14" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="42">
         <v>7.17</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="42">
         <v>3.9</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="42">
         <v>12.08</v>
       </c>
       <c r="G14" t="s">
@@ -21560,13 +21630,13 @@
       <c r="C15" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="42">
         <v>0.24</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="42">
         <v>0.1</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="42">
         <v>0.5</v>
       </c>
       <c r="G15" t="s">
@@ -21587,13 +21657,13 @@
       <c r="C16" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="42">
         <v>0.95</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="42">
         <v>0.62</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="42">
         <v>1.1599999999999999</v>
       </c>
       <c r="G16" t="s">
@@ -21614,13 +21684,13 @@
       <c r="C17" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="42">
         <v>3</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="42">
         <v>2.83</v>
       </c>
-      <c r="F17" s="43">
+      <c r="F17" s="42">
         <v>3.16</v>
       </c>
       <c r="G17" t="s">
@@ -21641,13 +21711,13 @@
       <c r="C18" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="42">
         <v>3.74</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="42">
         <v>3.48</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="42">
         <v>4</v>
       </c>
       <c r="G18" t="s">
@@ -21668,13 +21738,13 @@
       <c r="C19" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="42">
         <v>1.5</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="42">
         <v>1.1299999999999999</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="42">
         <v>2.25</v>
       </c>
       <c r="G19" t="s">
@@ -21695,13 +21765,13 @@
       <c r="C20" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E20" s="43">
+      <c r="E20" s="42">
         <v>1.07</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="42">
         <v>7.28</v>
       </c>
       <c r="G20" t="s">
@@ -21722,13 +21792,13 @@
       <c r="C21" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="42">
         <v>1.42</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E21" s="42">
         <v>0.9</v>
       </c>
-      <c r="F21" s="43">
+      <c r="F21" s="42">
         <v>3.42</v>
       </c>
       <c r="G21" t="s">
@@ -21749,13 +21819,13 @@
       <c r="C22" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="42">
         <v>2.14</v>
       </c>
-      <c r="E22" s="43">
+      <c r="E22" s="42">
         <v>1.39</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="42">
         <v>3.58</v>
       </c>
       <c r="G22" t="s">
@@ -21776,13 +21846,13 @@
       <c r="C23" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="D23" s="43">
+      <c r="D23" s="42">
         <v>0.66</v>
       </c>
-      <c r="E23" s="43">
+      <c r="E23" s="42">
         <v>0.51</v>
       </c>
-      <c r="F23" s="43">
+      <c r="F23" s="42">
         <v>0.94</v>
       </c>
       <c r="G23" t="s">
@@ -21803,13 +21873,13 @@
       <c r="C24" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D24" s="43">
+      <c r="D24" s="42">
         <v>0.2</v>
       </c>
-      <c r="E24" s="43">
+      <c r="E24" s="42">
         <v>0.1</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="42">
         <v>0.3</v>
       </c>
       <c r="G24" t="s">
@@ -21830,13 +21900,13 @@
       <c r="C25" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="D25" s="43">
-        <v>1</v>
-      </c>
-      <c r="E25" s="43">
+      <c r="D25" s="42">
+        <v>1</v>
+      </c>
+      <c r="E25" s="42">
         <v>0.5</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="42">
         <v>1.5</v>
       </c>
       <c r="G25" t="s">
@@ -21857,13 +21927,13 @@
       <c r="C26" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="41">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="E26" s="42">
+      <c r="E26" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F26" s="42">
+      <c r="F26" s="41">
         <v>0.27500000000000002</v>
       </c>
       <c r="G26" t="s">
@@ -21884,13 +21954,13 @@
       <c r="C27" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="D27" s="42">
+      <c r="D27" s="41">
         <v>0.15</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="41">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="F27" s="42">
+      <c r="F27" s="41">
         <v>0.88500000000000001</v>
       </c>
       <c r="G27" t="s">
@@ -21911,13 +21981,13 @@
       <c r="C28" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="D28" s="42">
+      <c r="D28" s="41">
         <v>0.1</v>
       </c>
-      <c r="E28" s="42">
+      <c r="E28" s="41">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="F28" s="42">
+      <c r="F28" s="41">
         <v>0.87</v>
       </c>
       <c r="G28" t="s">
@@ -21938,13 +22008,13 @@
       <c r="C29" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="D29" s="42">
+      <c r="D29" s="41">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="E29" s="42">
+      <c r="E29" s="41">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F29" s="42">
+      <c r="F29" s="41">
         <v>0.82699999999999996</v>
       </c>
       <c r="G29" t="s">
@@ -21965,13 +22035,13 @@
       <c r="C30" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="D30" s="42">
+      <c r="D30" s="41">
         <v>0.16200000000000001</v>
       </c>
-      <c r="E30" s="42">
+      <c r="E30" s="41">
         <v>0.05</v>
       </c>
-      <c r="F30" s="42">
+      <c r="F30" s="41">
         <v>0.86899999999999999</v>
       </c>
       <c r="G30" t="s">
@@ -21992,13 +22062,13 @@
       <c r="C31" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="D31" s="42">
+      <c r="D31" s="41">
         <v>0.11700000000000001</v>
       </c>
-      <c r="E31" s="42">
+      <c r="E31" s="41">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="F31" s="42">
+      <c r="F31" s="41">
         <v>0.68600000000000005</v>
       </c>
       <c r="G31" t="s">
@@ -22019,13 +22089,13 @@
       <c r="C32" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="D32" s="42">
+      <c r="D32" s="41">
         <v>0.09</v>
       </c>
-      <c r="E32" s="42">
+      <c r="E32" s="41">
         <v>1.9E-2</v>
       </c>
-      <c r="F32" s="42">
+      <c r="F32" s="41">
         <v>0.72299999999999998</v>
       </c>
       <c r="G32" t="s">
@@ -22046,13 +22116,13 @@
       <c r="C33" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="D33" s="42">
+      <c r="D33" s="41">
         <v>0.111</v>
       </c>
-      <c r="E33" s="42">
+      <c r="E33" s="41">
         <v>4.7E-2</v>
       </c>
-      <c r="F33" s="42">
+      <c r="F33" s="41">
         <v>0.56299999999999994</v>
       </c>
       <c r="G33" t="s">
@@ -22073,13 +22143,13 @@
       <c r="C34" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="D34" s="42">
+      <c r="D34" s="41">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E34" s="42">
+      <c r="E34" s="41">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="F34" s="42">
+      <c r="F34" s="41">
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="G34" t="s">
@@ -22100,13 +22170,13 @@
       <c r="C35" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="41">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E35" s="42">
+      <c r="E35" s="41">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="F35" s="42">
+      <c r="F35" s="41">
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="G35" t="s">
@@ -22116,7 +22186,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I35" s="41"/>
+      <c r="I35" s="40"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
@@ -22128,13 +22198,13 @@
       <c r="C36" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="D36" s="42">
+      <c r="D36" s="41">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="E36" s="42">
+      <c r="E36" s="41">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="F36" s="42">
+      <c r="F36" s="41">
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="G36" t="s">
@@ -22155,13 +22225,13 @@
       <c r="C37" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="D37" s="42">
+      <c r="D37" s="41">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="E37" s="42">
+      <c r="E37" s="41">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="F37" s="42">
+      <c r="F37" s="41">
         <v>1.01E-2</v>
       </c>
       <c r="G37" t="s">
@@ -22182,13 +22252,13 @@
       <c r="C38" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="D38" s="42">
+      <c r="D38" s="41">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="E38" s="42">
+      <c r="E38" s="41">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F38" s="42">
+      <c r="F38" s="41">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="G38" t="s">
@@ -22209,13 +22279,13 @@
       <c r="C39" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="D39" s="42">
+      <c r="D39" s="41">
         <v>0.32300000000000001</v>
       </c>
-      <c r="E39" s="42">
+      <c r="E39" s="41">
         <v>0.29599999999999999</v>
       </c>
-      <c r="F39" s="42">
+      <c r="F39" s="41">
         <v>0.432</v>
       </c>
       <c r="G39" t="s">
@@ -22236,13 +22306,13 @@
       <c r="C40" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="D40" s="42">
+      <c r="D40" s="41">
         <v>0.23</v>
       </c>
-      <c r="E40" s="42">
+      <c r="E40" s="41">
         <v>0.15</v>
       </c>
-      <c r="F40" s="42">
+      <c r="F40" s="41">
         <v>0.3</v>
       </c>
       <c r="G40" t="s">
@@ -22263,13 +22333,13 @@
       <c r="C41" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D41" s="42">
+      <c r="D41" s="41">
         <v>0.48780000000000001</v>
       </c>
-      <c r="E41" s="42">
+      <c r="E41" s="41">
         <v>0.28349999999999997</v>
       </c>
-      <c r="F41" s="42">
+      <c r="F41" s="41">
         <v>0.8417</v>
       </c>
       <c r="G41" t="s">
@@ -22290,13 +22360,13 @@
       <c r="C42" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="D42" s="42">
+      <c r="D42" s="41">
         <v>2.17</v>
       </c>
-      <c r="E42" s="42">
+      <c r="E42" s="41">
         <v>1.27</v>
       </c>
-      <c r="F42" s="42">
+      <c r="F42" s="41">
         <v>3.71</v>
       </c>
       <c r="G42" t="s">
@@ -22307,7 +22377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>370</v>
       </c>
@@ -22317,13 +22387,13 @@
       <c r="C43" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="D43" s="44">
+      <c r="D43" s="43">
         <v>0.95</v>
       </c>
-      <c r="E43" s="44">
+      <c r="E43" s="43">
         <v>0.8</v>
       </c>
-      <c r="F43" s="44">
+      <c r="F43" s="43">
         <v>0.98</v>
       </c>
       <c r="G43" t="s">
@@ -22334,7 +22404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>370</v>
       </c>
@@ -22344,13 +22414,13 @@
       <c r="C44" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="D44" s="44">
+      <c r="D44" s="43">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E44" s="44">
+      <c r="E44" s="43">
         <v>0.47</v>
       </c>
-      <c r="F44" s="44">
+      <c r="F44" s="43">
         <v>0.67</v>
       </c>
       <c r="G44" t="s">
@@ -22361,7 +22431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>370</v>
       </c>
@@ -22371,13 +22441,13 @@
       <c r="C45" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="D45" s="44">
+      <c r="D45" s="43">
         <v>0</v>
       </c>
-      <c r="E45" s="44">
+      <c r="E45" s="43">
         <v>0</v>
       </c>
-      <c r="F45" s="44">
+      <c r="F45" s="43">
         <v>0.68</v>
       </c>
       <c r="G45" t="s">
@@ -22388,7 +22458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>370</v>
       </c>
@@ -22398,13 +22468,13 @@
       <c r="C46" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="D46" s="44">
+      <c r="D46" s="43">
         <v>2.65</v>
       </c>
-      <c r="E46" s="44">
+      <c r="E46" s="43">
         <v>1.35</v>
       </c>
-      <c r="F46" s="44">
+      <c r="F46" s="43">
         <v>5.19</v>
       </c>
       <c r="G46" t="s">
@@ -22415,7 +22485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>370</v>
       </c>
@@ -22425,13 +22495,13 @@
       <c r="C47" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="D47" s="44">
+      <c r="D47" s="43">
         <v>0.54</v>
       </c>
-      <c r="E47" s="44">
+      <c r="E47" s="43">
         <v>0.33</v>
       </c>
-      <c r="F47" s="44">
+      <c r="F47" s="43">
         <v>0.68</v>
       </c>
       <c r="G47" t="s">
@@ -22442,7 +22512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>370</v>
       </c>
@@ -22452,13 +22522,13 @@
       <c r="C48" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D48" s="44">
+      <c r="D48" s="43">
         <v>0.9</v>
       </c>
-      <c r="E48" s="44">
+      <c r="E48" s="43">
         <v>0.82</v>
       </c>
-      <c r="F48" s="44">
+      <c r="F48" s="43">
         <v>0.93</v>
       </c>
       <c r="G48" t="s">
@@ -22469,7 +22539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>370</v>
       </c>
@@ -22479,13 +22549,13 @@
       <c r="C49" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="D49" s="44">
+      <c r="D49" s="43">
         <v>0.73</v>
       </c>
-      <c r="E49" s="44">
+      <c r="E49" s="43">
         <v>0.65</v>
       </c>
-      <c r="F49" s="44">
+      <c r="F49" s="43">
         <v>0.8</v>
       </c>
       <c r="G49" t="s">
@@ -22496,7 +22566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>370</v>
       </c>
@@ -22506,13 +22576,13 @@
       <c r="C50" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="D50" s="44">
+      <c r="D50" s="43">
         <v>0.5</v>
       </c>
-      <c r="E50" s="44">
+      <c r="E50" s="43">
         <v>0.3</v>
       </c>
-      <c r="F50" s="44">
+      <c r="F50" s="43">
         <v>0.8</v>
       </c>
       <c r="G50" t="s">
@@ -22523,7 +22593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>370</v>
       </c>
@@ -22533,13 +22603,13 @@
       <c r="C51" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="D51" s="44">
+      <c r="D51" s="43">
         <v>0.92</v>
       </c>
-      <c r="E51" s="44">
+      <c r="E51" s="43">
         <v>0.8</v>
       </c>
-      <c r="F51" s="44">
+      <c r="F51" s="43">
         <v>0.95</v>
       </c>
       <c r="G51" t="s">
@@ -22550,7 +22620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>369</v>
       </c>
@@ -22560,13 +22630,13 @@
       <c r="C52" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="D52" s="43">
+      <c r="D52" s="42">
         <v>0.14599999999999999</v>
       </c>
-      <c r="E52" s="43">
+      <c r="E52" s="42">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="F52" s="43">
+      <c r="F52" s="42">
         <v>0.20499999999999999</v>
       </c>
       <c r="G52" t="s">
@@ -22577,7 +22647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>369</v>
       </c>
@@ -22587,13 +22657,13 @@
       <c r="C53" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D53" s="43">
+      <c r="D53" s="42">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E53" s="43">
+      <c r="E53" s="42">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F53" s="43">
+      <c r="F53" s="42">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="G53" t="s">
@@ -22604,7 +22674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>369</v>
       </c>
@@ -22614,13 +22684,13 @@
       <c r="C54" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="D54" s="45">
+      <c r="D54" s="44">
         <v>0.02</v>
       </c>
-      <c r="E54" s="43">
+      <c r="E54" s="42">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F54" s="43">
+      <c r="F54" s="42">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="G54" t="s">
@@ -22631,7 +22701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>369</v>
       </c>
@@ -22641,13 +22711,13 @@
       <c r="C55" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="D55" s="45">
+      <c r="D55" s="44">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E55" s="43">
+      <c r="E55" s="42">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="F55" s="43">
+      <c r="F55" s="42">
         <v>9.4E-2</v>
       </c>
       <c r="G55" t="s">
@@ -22658,7 +22728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>369</v>
       </c>
@@ -22668,13 +22738,13 @@
       <c r="C56" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="D56" s="43">
+      <c r="D56" s="42">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E56" s="43">
+      <c r="E56" s="42">
         <v>0.114</v>
       </c>
-      <c r="F56" s="43">
+      <c r="F56" s="42">
         <v>0.47399999999999998</v>
       </c>
       <c r="G56" t="s">
@@ -22685,7 +22755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>369</v>
       </c>
@@ -22695,13 +22765,13 @@
       <c r="C57" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="D57" s="43">
+      <c r="D57" s="42">
         <v>0.54700000000000004</v>
       </c>
-      <c r="E57" s="43">
+      <c r="E57" s="42">
         <v>0.38200000000000001</v>
       </c>
-      <c r="F57" s="43">
+      <c r="F57" s="42">
         <v>0.71499999999999997</v>
       </c>
       <c r="G57" t="s">
@@ -22712,7 +22782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>369</v>
       </c>
@@ -22722,13 +22792,13 @@
       <c r="C58" t="s">
         <v>368</v>
       </c>
-      <c r="D58" s="43">
+      <c r="D58" s="42">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="E58" s="43">
+      <c r="E58" s="42">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="F58" s="43">
+      <c r="F58" s="42">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="G58" t="s">

</xml_diff>

<commit_message>
Update data with new pars to allow a spreadsheet to be exported
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rowan.martin-hughes\Documents\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541F8C14-2106-4A2E-97FE-64078561E8B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8808EB-BC23-4DBF-BBCE-96D06226EA04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9720" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="482">
   <si>
     <t>Susceptible</t>
   </si>
@@ -1480,13 +1480,10 @@
     <t>Proportion of exposure events covered by ARV-based post-exposure prophylaxis</t>
   </si>
   <si>
-    <t>Proportion of exposure events covered by ARV-based prophylaxis</t>
-  </si>
-  <si>
-    <t>Percentage of people covered by ARV-based post-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Percentage of people covered by ARV-based pre-exposure prophylaxis</t>
+    <t>Proportion of exposure events covered by ARV-based pre-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Number of voluntary medical male circumcisions</t>
   </si>
 </sst>
 </file>
@@ -15113,7 +15110,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17696,8 +17693,8 @@
   <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20270,56 +20267,16 @@
       <c r="D112" s="6"/>
       <c r="E112" s="6"/>
     </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C113" s="6"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="6"/>
-    </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C114" s="6"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="6"/>
-    </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="6"/>
-    </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="6"/>
-    </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C117" s="6"/>
-      <c r="D117" s="6"/>
-      <c r="E117" s="6"/>
-    </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C118" s="6"/>
-      <c r="D118" s="6"/>
-      <c r="E118" s="6"/>
-    </row>
-    <row r="119" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C119" s="6"/>
-      <c r="D119" s="6"/>
-      <c r="E119" s="6"/>
-    </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="6"/>
-    </row>
-    <row r="121" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="6"/>
-    </row>
-    <row r="122" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="6"/>
-    </row>
+    <row r="113" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -20328,11 +20285,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20533,10 +20490,10 @@
         <v>314</v>
       </c>
       <c r="C10" t="s">
-        <v>471</v>
+        <v>133</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E10" t="s">
         <v>408</v>
@@ -20553,10 +20510,10 @@
         <v>314</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>471</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E11" t="s">
         <v>408</v>
@@ -21167,22 +21124,22 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B42" t="s">
         <v>314</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>449</v>
+        <v>481</v>
       </c>
       <c r="E42" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F42" t="s">
-        <v>413</v>
+        <v>455</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -21193,13 +21150,13 @@
         <v>314</v>
       </c>
       <c r="C43" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E43" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="F43" t="s">
         <v>413</v>
@@ -21213,36 +21170,36 @@
         <v>314</v>
       </c>
       <c r="C44" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E44" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F44" t="s">
-        <v>453</v>
+        <v>413</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B45" t="s">
-        <v>402</v>
+        <v>314</v>
       </c>
       <c r="C45" t="s">
-        <v>308</v>
+        <v>130</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>414</v>
+        <v>450</v>
       </c>
       <c r="E45" t="s">
         <v>410</v>
       </c>
       <c r="F45" t="s">
-        <v>413</v>
+        <v>453</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -21253,10 +21210,10 @@
         <v>402</v>
       </c>
       <c r="C46" t="s">
-        <v>403</v>
+        <v>308</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E46" t="s">
         <v>410</v>
@@ -21273,10 +21230,10 @@
         <v>402</v>
       </c>
       <c r="C47" t="s">
-        <v>309</v>
+        <v>403</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E47" t="s">
         <v>410</v>
@@ -21293,10 +21250,10 @@
         <v>402</v>
       </c>
       <c r="C48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E48" t="s">
         <v>410</v>
@@ -21313,16 +21270,16 @@
         <v>402</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>310</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E49" t="s">
         <v>410</v>
       </c>
       <c r="F49" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -21333,16 +21290,16 @@
         <v>402</v>
       </c>
       <c r="C50" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E50" t="s">
         <v>410</v>
       </c>
       <c r="F50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -21353,15 +21310,35 @@
         <v>402</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E51" t="s">
         <v>410</v>
       </c>
       <c r="F51" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>323</v>
+      </c>
+      <c r="B52" t="s">
+        <v>402</v>
+      </c>
+      <c r="C52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="38" t="s">
+        <v>420</v>
+      </c>
+      <c r="E52" t="s">
+        <v>410</v>
+      </c>
+      <c r="F52" t="s">
         <v>413</v>
       </c>
     </row>
@@ -21375,8 +21352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22688,25 +22665,25 @@
         <v>370</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>472</v>
+        <v>274</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D49" s="43">
-        <v>0.73</v>
+        <v>0.95</v>
       </c>
       <c r="E49" s="43">
-        <v>0.65</v>
+        <v>0.92</v>
       </c>
       <c r="F49" s="43">
-        <v>0.8</v>
+        <v>0.97</v>
       </c>
       <c r="G49" t="s">
         <v>408</v>
       </c>
       <c r="H49" s="17" t="b">
-        <f t="shared" ref="H49" si="2">AND(D49&gt;=E49, D49&lt;=F49)</f>
+        <f>AND(D49&gt;=E49, D49&lt;=F49)</f>
         <v>1</v>
       </c>
     </row>
@@ -22715,25 +22692,25 @@
         <v>370</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>274</v>
+        <v>472</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D50" s="43">
-        <v>0.95</v>
+        <v>0.73</v>
       </c>
       <c r="E50" s="43">
-        <v>0.92</v>
+        <v>0.65</v>
       </c>
       <c r="F50" s="43">
-        <v>0.97</v>
+        <v>0.8</v>
       </c>
       <c r="G50" t="s">
         <v>408</v>
       </c>
       <c r="H50" s="17" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H50" si="2">AND(D50&gt;=E50, D50&lt;=F50)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update default model inputs and 3 demo databooks to have GBD 2019 disutility weights for HIV
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rowan.martin-hughes\Documents\GitHub\optima\optima\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8167ECB-EDE3-4DC6-8406-967256D93508}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C29AE6-5069-4309-9A37-F930C70BBFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Data inputs" sheetId="4" r:id="rId5"/>
     <sheet name="Data constants" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -17693,9 +17693,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21355,8 +21355,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22782,13 +22782,13 @@
         <v>355</v>
       </c>
       <c r="D53" s="42">
-        <v>0.14599999999999999</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="E53" s="42">
-        <v>9.6000000000000002E-2</v>
+        <v>0.121</v>
       </c>
       <c r="F53" s="42">
-        <v>0.20499999999999999</v>
+        <v>0.249</v>
       </c>
       <c r="G53" t="s">
         <v>400</v>
@@ -22809,13 +22809,13 @@
         <v>356</v>
       </c>
       <c r="D54" s="42">
-        <v>8.0000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E54" s="42">
-        <v>5.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="F54" s="42">
-        <v>1.0999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="G54" t="s">
         <v>400</v>
@@ -22836,13 +22836,13 @@
         <v>357</v>
       </c>
       <c r="D55" s="44">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E55" s="42">
-        <v>1.2999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="F55" s="42">
-        <v>2.9000000000000001E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G55" t="s">
         <v>400</v>
@@ -22863,13 +22863,13 @@
         <v>358</v>
       </c>
       <c r="D56" s="44">
-        <v>7.0000000000000007E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E56" s="42">
-        <v>4.8000000000000001E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F56" s="42">
-        <v>9.4E-2</v>
+        <v>0.107</v>
       </c>
       <c r="G56" t="s">
         <v>400</v>
@@ -22890,13 +22890,13 @@
         <v>359</v>
       </c>
       <c r="D57" s="42">
-        <v>0.26500000000000001</v>
+        <v>0.28899999999999998</v>
       </c>
       <c r="E57" s="42">
-        <v>0.114</v>
+        <v>0.128</v>
       </c>
       <c r="F57" s="42">
-        <v>0.47399999999999998</v>
+        <v>0.499</v>
       </c>
       <c r="G57" t="s">
         <v>400</v>
@@ -22917,13 +22917,13 @@
         <v>360</v>
       </c>
       <c r="D58" s="42">
-        <v>0.54700000000000004</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="E58" s="42">
-        <v>0.38200000000000001</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="F58" s="42">
-        <v>0.71499999999999997</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="G58" t="s">
         <v>400</v>
@@ -22944,13 +22944,13 @@
         <v>361</v>
       </c>
       <c r="D59" s="42">
-        <v>5.2999999999999999E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="E59" s="42">
-        <v>3.4000000000000002E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="F59" s="42">
-        <v>7.9000000000000001E-2</v>
+        <v>0.111</v>
       </c>
       <c r="G59" t="s">
         <v>400</v>

</xml_diff>

<commit_message>
Add non-uniform ageing rates
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C29AE6-5069-4309-9A37-F930C70BBFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C91A0F1-CB24-4886-9E88-2C18F33FD91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="484">
   <si>
     <t>Susceptible</t>
   </si>
@@ -1481,6 +1481,15 @@
   </si>
   <si>
     <t>Percentage of males who have been traditionally circumcised</t>
+  </si>
+  <si>
+    <t>agerate</t>
+  </si>
+  <si>
+    <t>Ageing rate (per year)</t>
+  </si>
+  <si>
+    <t>Percentage of people who age into the next age category per year</t>
   </si>
 </sst>
 </file>
@@ -17691,17 +17700,17 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:H122"/>
+  <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="68.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" style="6" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" style="5" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="8" customWidth="1"/>
@@ -17833,96 +17842,93 @@
       </c>
       <c r="H5" s="38"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>481</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>482</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="G6" s="6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="38"/>
+    </row>
+    <row r="8" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
         <v>457</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B8" s="38" t="s">
         <v>458</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C8" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D8" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E8" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F8" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="38">
+      <c r="G8" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="6" t="s">
         <v>92</v>
       </c>
       <c r="G9" s="6">
@@ -17934,16 +17940,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>105</v>
@@ -17954,14 +17960,16 @@
       <c r="G10" s="6">
         <v>1</v>
       </c>
-      <c r="H10" s="38"/>
+      <c r="H10" s="38">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>84</v>
@@ -17982,16 +17990,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>105</v>
@@ -18002,16 +18010,14 @@
       <c r="G12" s="6">
         <v>1</v>
       </c>
-      <c r="H12" s="38">
-        <v>0</v>
-      </c>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>88</v>
@@ -18032,52 +18038,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>464</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>472</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="38" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>105</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="6">
         <v>1</v>
       </c>
       <c r="H14" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="C15" s="6" t="s">
+    <row r="15" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>464</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>472</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="38" t="s">
         <v>105</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="38">
         <v>1</v>
       </c>
       <c r="H15" s="38">
@@ -18086,16 +18092,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>119</v>
+        <v>473</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>105</v>
@@ -18106,20 +18112,22 @@
       <c r="G16" s="6">
         <v>1</v>
       </c>
-      <c r="H16" s="38"/>
+      <c r="H16" s="38">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>105</v>
@@ -18134,21 +18142,21 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="14" t="s">
         <v>92</v>
       </c>
       <c r="G18" s="6">
@@ -18158,16 +18166,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>156</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>105</v>
@@ -18182,16 +18190,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>105</v>
@@ -18206,16 +18214,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>105</v>
@@ -18228,69 +18236,67 @@
       </c>
       <c r="H21" s="38"/>
     </row>
-    <row r="22" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1</v>
+      </c>
+      <c r="H22" s="38"/>
+    </row>
+    <row r="23" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
         <v>470</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B23" s="38" t="s">
         <v>471</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C23" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D23" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E23" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="F22" s="38" t="s">
+      <c r="F23" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="G22" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="G23" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="14">
-        <v>1</v>
-      </c>
-      <c r="H23" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
-        <v>461</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>460</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="6" t="s">
         <v>105</v>
       </c>
       <c r="F24" s="14" t="s">
@@ -18305,10 +18311,10 @@
     </row>
     <row r="25" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
-        <v>244</v>
+        <v>461</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>243</v>
+        <v>460</v>
       </c>
       <c r="C25" s="38" t="s">
         <v>96</v>
@@ -18325,37 +18331,39 @@
       <c r="G25" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>452</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="H25" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G26" s="6">
-        <v>0</v>
-      </c>
-      <c r="H26" s="38"/>
+      <c r="F26" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>84</v>
@@ -18376,10 +18384,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>84</v>
@@ -18400,10 +18408,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>84</v>
@@ -18424,10 +18432,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>84</v>
@@ -18448,33 +18456,34 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>475</v>
+        <v>456</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>170</v>
+        <v>84</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>171</v>
+        <v>105</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>172</v>
+        <v>98</v>
       </c>
       <c r="G31" s="6">
         <v>0</v>
       </c>
+      <c r="H31" s="38"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>170</v>
@@ -18494,10 +18503,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>170</v>
@@ -18517,10 +18526,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>170</v>
@@ -18540,10 +18549,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>170</v>
@@ -18563,36 +18572,36 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>126</v>
+        <v>176</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>88</v>
+        <v>170</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>105</v>
+        <v>171</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>98</v>
+        <v>172</v>
       </c>
       <c r="G36" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>125</v>
@@ -18600,26 +18609,25 @@
       <c r="E37" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F37" s="14" t="s">
-        <v>92</v>
+      <c r="F37" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="G37" s="6">
         <v>1</v>
       </c>
-      <c r="H37" s="38"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>132</v>
+        <v>480</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>105</v>
@@ -18630,14 +18638,14 @@
       <c r="G38" s="6">
         <v>1</v>
       </c>
-      <c r="H38" s="46"/>
+      <c r="H38" s="38"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>135</v>
@@ -18658,10 +18666,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>135</v>
@@ -18682,13 +18690,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>136</v>
@@ -18696,7 +18704,7 @@
       <c r="E41" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" s="14" t="s">
         <v>92</v>
       </c>
       <c r="G41" s="6">
@@ -18706,10 +18714,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>84</v>
@@ -18730,10 +18738,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>84</v>
@@ -18754,13 +18762,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>136</v>
@@ -18768,7 +18776,7 @@
       <c r="E44" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="6" t="s">
         <v>92</v>
       </c>
       <c r="G44" s="6">
@@ -18778,16 +18786,16 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>105</v>
@@ -18798,63 +18806,64 @@
       <c r="G45" s="6">
         <v>1</v>
       </c>
-      <c r="H45" s="46" t="s">
-        <v>463</v>
-      </c>
+      <c r="H45" s="46"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F46" s="14" t="s">
         <v>92</v>
       </c>
       <c r="G46" s="6">
         <v>1</v>
       </c>
-      <c r="H46" s="46"/>
+      <c r="H46" s="46" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E47" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="G47" s="6">
         <v>1</v>
       </c>
+      <c r="H47" s="46"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>96</v>
@@ -18874,10 +18883,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>96</v>
@@ -18897,36 +18906,36 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>394</v>
+        <v>102</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>399</v>
+        <v>101</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>180</v>
+        <v>98</v>
       </c>
       <c r="G50" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>179</v>
+        <v>394</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>177</v>
+        <v>399</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>110</v>
@@ -18938,15 +18947,15 @@
         <v>180</v>
       </c>
       <c r="G51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>84</v>
@@ -18966,10 +18975,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>84</v>
@@ -18989,10 +18998,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>84</v>
@@ -19012,10 +19021,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>84</v>
@@ -19035,10 +19044,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>84</v>
@@ -19058,10 +19067,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>84</v>
@@ -19081,13 +19090,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>110</v>
@@ -19104,10 +19113,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>91</v>
@@ -19127,10 +19136,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>91</v>
@@ -19150,10 +19159,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>91</v>
@@ -19173,10 +19182,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>91</v>
@@ -19196,10 +19205,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>91</v>
@@ -19219,10 +19228,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>91</v>
@@ -19242,13 +19251,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>110</v>
@@ -19265,10 +19274,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>156</v>
@@ -19288,10 +19297,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>156</v>
@@ -19311,10 +19320,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>156</v>
@@ -19334,10 +19343,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>156</v>
@@ -19357,10 +19366,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>156</v>
@@ -19380,10 +19389,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>156</v>
@@ -19403,10 +19412,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>156</v>
@@ -19426,10 +19435,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>156</v>
@@ -19449,10 +19458,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>156</v>
@@ -19472,13 +19481,13 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>389</v>
+        <v>226</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>110</v>
@@ -19489,19 +19498,19 @@
       <c r="F75" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G75" s="14">
+      <c r="G75" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C76" s="38" t="s">
-        <v>84</v>
+        <v>390</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>110</v>
@@ -19509,19 +19518,19 @@
       <c r="E76" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F76" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="G76" s="6">
+      <c r="F76" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="G76" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C77" s="38" t="s">
         <v>84</v>
@@ -19541,10 +19550,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>229</v>
       </c>
       <c r="C78" s="38" t="s">
         <v>84</v>
@@ -19564,10 +19573,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C79" s="38" t="s">
         <v>84</v>
@@ -19587,10 +19596,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C80" s="38" t="s">
         <v>84</v>
@@ -19610,10 +19619,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C81" s="38" t="s">
         <v>84</v>
@@ -19633,10 +19642,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C82" s="38" t="s">
         <v>84</v>
@@ -19656,10 +19665,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C83" s="38" t="s">
         <v>84</v>
@@ -19679,13 +19688,13 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>96</v>
+        <v>241</v>
+      </c>
+      <c r="C84" s="38" t="s">
+        <v>84</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>110</v>
@@ -19702,10 +19711,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>96</v>
@@ -19725,10 +19734,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>96</v>
@@ -19747,11 +19756,11 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>251</v>
+      <c r="A87" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>249</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>96</v>
@@ -19771,10 +19780,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B88" s="15" t="s">
-        <v>386</v>
+        <v>252</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>251</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>96</v>
@@ -19785,19 +19794,19 @@
       <c r="E88" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F88" s="6" t="s">
-        <v>180</v>
+      <c r="F88" s="14" t="s">
+        <v>383</v>
       </c>
       <c r="G88" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>387</v>
+      <c r="A89" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>386</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>96</v>
@@ -19817,13 +19826,13 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>387</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>110</v>
@@ -19840,10 +19849,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>91</v>
@@ -19863,10 +19872,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>91</v>
@@ -19877,8 +19886,8 @@
       <c r="E92" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F92" s="14" t="s">
-        <v>383</v>
+      <c r="F92" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="G92" s="6">
         <v>1</v>
@@ -19886,13 +19895,13 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>110</v>
@@ -19900,8 +19909,8 @@
       <c r="E93" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F93" s="6" t="s">
-        <v>180</v>
+      <c r="F93" s="14" t="s">
+        <v>383</v>
       </c>
       <c r="G93" s="6">
         <v>1</v>
@@ -19909,10 +19918,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>84</v>
@@ -19932,10 +19941,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>84</v>
@@ -19953,58 +19962,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="38" t="s">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="G96" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="38" t="s">
         <v>465</v>
       </c>
-      <c r="B96" s="38" t="s">
+      <c r="B97" s="38" t="s">
         <v>466</v>
       </c>
-      <c r="C96" s="38" t="s">
+      <c r="C97" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D96" s="38" t="s">
+      <c r="D97" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="E96" s="38" t="s">
+      <c r="E97" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="F96" s="38" t="s">
+      <c r="F97" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="G96" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E97" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="F97" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="G97" s="6">
+      <c r="G97" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>268</v>
+        <v>467</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>84</v>
@@ -20024,10 +20033,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>84</v>
@@ -20047,10 +20056,10 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>84</v>
@@ -20070,10 +20079,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>84</v>
@@ -20093,10 +20102,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>84</v>
@@ -20107,8 +20116,8 @@
       <c r="E102" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F102" s="14" t="s">
-        <v>383</v>
+      <c r="F102" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="G102" s="6">
         <v>1</v>
@@ -20116,10 +20125,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>84</v>
@@ -20139,10 +20148,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>84</v>
@@ -20162,10 +20171,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>84</v>
@@ -20185,10 +20194,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>84</v>
@@ -20208,10 +20217,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>84</v>
@@ -20231,10 +20240,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>84</v>
@@ -20253,15 +20262,33 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D109" s="6"/>
+      <c r="A109" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F109" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="G109" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D110" s="6"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C111" s="6"/>
       <c r="D111" s="6"/>
-      <c r="E111" s="6"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C112" s="6"/>
@@ -20278,6 +20305,7 @@
     <row r="120" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="121" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="122" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -20287,11 +20315,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20372,10 +20400,10 @@
         <v>307</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>481</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>414</v>
+        <v>483</v>
       </c>
       <c r="E4" t="s">
         <v>401</v>
@@ -20392,13 +20420,13 @@
         <v>307</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F5" t="s">
         <v>406</v>
@@ -20412,10 +20440,10 @@
         <v>307</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>113</v>
+        <v>415</v>
       </c>
       <c r="E6" t="s">
         <v>402</v>
@@ -20426,19 +20454,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B7" t="s">
         <v>307</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>416</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>451</v>
+        <v>402</v>
       </c>
       <c r="F7" t="s">
         <v>406</v>
@@ -20452,16 +20480,16 @@
         <v>307</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E8" t="s">
         <v>451</v>
       </c>
       <c r="F8" t="s">
-        <v>445</v>
+        <v>406</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -20472,16 +20500,16 @@
         <v>307</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>115</v>
+        <v>417</v>
       </c>
       <c r="E9" t="s">
-        <v>403</v>
+        <v>451</v>
       </c>
       <c r="F9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -20492,16 +20520,16 @@
         <v>307</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>473</v>
+        <v>115</v>
       </c>
       <c r="E10" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="F10" t="s">
-        <v>406</v>
+        <v>446</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -20512,10 +20540,10 @@
         <v>307</v>
       </c>
       <c r="C11" t="s">
-        <v>464</v>
+        <v>131</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E11" t="s">
         <v>401</v>
@@ -20532,16 +20560,16 @@
         <v>307</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>464</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>418</v>
+        <v>472</v>
       </c>
       <c r="E12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F12" t="s">
-        <v>446</v>
+        <v>406</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -20552,16 +20580,16 @@
         <v>307</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E13" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="F13" t="s">
-        <v>405</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -20572,36 +20600,36 @@
         <v>307</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F14" t="s">
-        <v>445</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B15" t="s">
         <v>307</v>
       </c>
       <c r="C15" t="s">
-        <v>290</v>
+        <v>120</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F15" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -20612,10 +20640,10 @@
         <v>307</v>
       </c>
       <c r="C16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E16" t="s">
         <v>403</v>
@@ -20632,10 +20660,10 @@
         <v>307</v>
       </c>
       <c r="C17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E17" t="s">
         <v>403</v>
@@ -20652,13 +20680,13 @@
         <v>307</v>
       </c>
       <c r="C18" t="s">
-        <v>398</v>
+        <v>292</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E18" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="F18" t="s">
         <v>459</v>
@@ -20672,13 +20700,13 @@
         <v>307</v>
       </c>
       <c r="C19" t="s">
-        <v>293</v>
+        <v>398</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F19" t="s">
         <v>459</v>
@@ -20692,10 +20720,10 @@
         <v>307</v>
       </c>
       <c r="C20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E20" t="s">
         <v>403</v>
@@ -20712,10 +20740,10 @@
         <v>307</v>
       </c>
       <c r="C21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E21" t="s">
         <v>403</v>
@@ -20732,13 +20760,13 @@
         <v>307</v>
       </c>
       <c r="C22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E22" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="F22" t="s">
         <v>459</v>
@@ -20752,10 +20780,10 @@
         <v>307</v>
       </c>
       <c r="C23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E23" t="s">
         <v>401</v>
@@ -20772,10 +20800,10 @@
         <v>307</v>
       </c>
       <c r="C24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E24" t="s">
         <v>401</v>
@@ -20792,10 +20820,10 @@
         <v>307</v>
       </c>
       <c r="C25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E25" t="s">
         <v>401</v>
@@ -20812,10 +20840,10 @@
         <v>307</v>
       </c>
       <c r="C26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E26" t="s">
         <v>401</v>
@@ -20826,22 +20854,22 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B27" t="s">
         <v>307</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>300</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>154</v>
+        <v>432</v>
       </c>
       <c r="E27" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F27" t="s">
-        <v>406</v>
+        <v>459</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -20852,16 +20880,16 @@
         <v>307</v>
       </c>
       <c r="C28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E28" t="s">
         <v>403</v>
       </c>
       <c r="F28" t="s">
-        <v>445</v>
+        <v>406</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -20872,16 +20900,16 @@
         <v>307</v>
       </c>
       <c r="C29" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>433</v>
+        <v>157</v>
       </c>
       <c r="E29" t="s">
-        <v>451</v>
+        <v>403</v>
       </c>
       <c r="F29" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -20892,16 +20920,16 @@
         <v>307</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E30" t="s">
         <v>451</v>
       </c>
       <c r="F30" t="s">
-        <v>445</v>
+        <v>406</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -20912,16 +20940,16 @@
         <v>307</v>
       </c>
       <c r="C31" t="s">
-        <v>470</v>
+        <v>163</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>471</v>
+        <v>434</v>
       </c>
       <c r="E31" t="s">
-        <v>403</v>
+        <v>451</v>
       </c>
       <c r="F31" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -20932,16 +20960,16 @@
         <v>307</v>
       </c>
       <c r="C32" t="s">
-        <v>388</v>
+        <v>470</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>159</v>
+        <v>471</v>
       </c>
       <c r="E32" t="s">
         <v>403</v>
       </c>
       <c r="F32" t="s">
-        <v>446</v>
+        <v>406</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -20951,11 +20979,11 @@
       <c r="B33" t="s">
         <v>307</v>
       </c>
-      <c r="C33" s="38" t="s">
-        <v>461</v>
+      <c r="C33" t="s">
+        <v>388</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>460</v>
+        <v>159</v>
       </c>
       <c r="E33" t="s">
         <v>403</v>
@@ -20971,11 +20999,11 @@
       <c r="B34" t="s">
         <v>307</v>
       </c>
-      <c r="C34" t="s">
-        <v>244</v>
+      <c r="C34" s="38" t="s">
+        <v>461</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>243</v>
+        <v>460</v>
       </c>
       <c r="E34" t="s">
         <v>403</v>
@@ -20986,22 +21014,22 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B35" t="s">
         <v>307</v>
       </c>
       <c r="C35" t="s">
-        <v>134</v>
+        <v>244</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>435</v>
+        <v>243</v>
       </c>
       <c r="E35" t="s">
         <v>403</v>
       </c>
       <c r="F35" t="s">
-        <v>406</v>
+        <v>446</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -21012,10 +21040,10 @@
         <v>307</v>
       </c>
       <c r="C36" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E36" t="s">
         <v>403</v>
@@ -21032,10 +21060,10 @@
         <v>307</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E37" t="s">
         <v>403</v>
@@ -21052,13 +21080,13 @@
         <v>307</v>
       </c>
       <c r="C38" t="s">
-        <v>397</v>
+        <v>142</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E38" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="F38" t="s">
         <v>406</v>
@@ -21072,10 +21100,10 @@
         <v>307</v>
       </c>
       <c r="C39" t="s">
-        <v>150</v>
+        <v>397</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E39" t="s">
         <v>401</v>
@@ -21092,10 +21120,10 @@
         <v>307</v>
       </c>
       <c r="C40" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E40" t="s">
         <v>401</v>
@@ -21112,16 +21140,16 @@
         <v>307</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E41" t="s">
         <v>401</v>
       </c>
       <c r="F41" t="s">
-        <v>448</v>
+        <v>406</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -21132,10 +21160,10 @@
         <v>307</v>
       </c>
       <c r="C42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>474</v>
+        <v>441</v>
       </c>
       <c r="E42" t="s">
         <v>401</v>
@@ -21146,22 +21174,22 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B43" t="s">
         <v>307</v>
       </c>
       <c r="C43" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>442</v>
+        <v>474</v>
       </c>
       <c r="E43" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F43" t="s">
-        <v>406</v>
+        <v>448</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -21172,13 +21200,13 @@
         <v>307</v>
       </c>
       <c r="C44" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E44" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="F44" t="s">
         <v>406</v>
@@ -21192,36 +21220,36 @@
         <v>307</v>
       </c>
       <c r="C45" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E45" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F45" t="s">
-        <v>446</v>
+        <v>406</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B46" t="s">
-        <v>395</v>
+        <v>307</v>
       </c>
       <c r="C46" t="s">
-        <v>301</v>
+        <v>128</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>407</v>
+        <v>443</v>
       </c>
       <c r="E46" t="s">
         <v>403</v>
       </c>
       <c r="F46" t="s">
-        <v>406</v>
+        <v>446</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -21232,10 +21260,10 @@
         <v>395</v>
       </c>
       <c r="C47" t="s">
-        <v>396</v>
+        <v>301</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E47" t="s">
         <v>403</v>
@@ -21252,10 +21280,10 @@
         <v>395</v>
       </c>
       <c r="C48" t="s">
-        <v>302</v>
+        <v>396</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E48" t="s">
         <v>403</v>
@@ -21272,10 +21300,10 @@
         <v>395</v>
       </c>
       <c r="C49" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E49" t="s">
         <v>403</v>
@@ -21292,16 +21320,16 @@
         <v>395</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>303</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E50" t="s">
         <v>403</v>
       </c>
       <c r="F50" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -21312,16 +21340,16 @@
         <v>395</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E51" t="s">
         <v>403</v>
       </c>
       <c r="F51" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -21332,15 +21360,35 @@
         <v>395</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E52" t="s">
         <v>403</v>
       </c>
       <c r="F52" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>316</v>
+      </c>
+      <c r="B53" t="s">
+        <v>395</v>
+      </c>
+      <c r="C53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" s="38" t="s">
+        <v>413</v>
+      </c>
+      <c r="E53" t="s">
+        <v>403</v>
+      </c>
+      <c r="F53" t="s">
         <v>406</v>
       </c>
     </row>
@@ -21355,7 +21403,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Migration for 2.10.5 to be more consistent in databook inputs with UNAIDS terminology
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C91A0F1-CB24-4886-9E88-2C18F33FD91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0F1221-B1FD-491C-A8B8-B429E176BD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1324,21 +1324,6 @@
     <t>Number of people initiating ART each year</t>
   </si>
   <si>
-    <t>PLHIV aware of their status (%)</t>
-  </si>
-  <si>
-    <t>Diagnosed PLHIV in care (%)</t>
-  </si>
-  <si>
-    <t>PLHIV in care on treatment (%)</t>
-  </si>
-  <si>
-    <t>Pregnant women on PMTCT (%)</t>
-  </si>
-  <si>
-    <t>People on ART with viral suppression (%)</t>
-  </si>
-  <si>
     <t>Percentage of people in care who are lost to follow-up per year (%/year)</t>
   </si>
   <si>
@@ -1490,6 +1475,21 @@
   </si>
   <si>
     <t>Percentage of people who age into the next age category per year</t>
+  </si>
+  <si>
+    <t>Percent of people living with HIV who know their status</t>
+  </si>
+  <si>
+    <t>Percent of people on ART who achieve viral suppression</t>
+  </si>
+  <si>
+    <t>Percent of people who know their status who are on ART</t>
+  </si>
+  <si>
+    <t>Percent of pregnant women with HIV on PMTCT</t>
+  </si>
+  <si>
+    <t>Percent of people who know their status who are retained in care</t>
   </si>
 </sst>
 </file>
@@ -15241,10 +15241,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -17743,7 +17743,7 @@
         <v>81</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -17844,10 +17844,10 @@
     </row>
     <row r="6" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>96</v>
@@ -17891,10 +17891,10 @@
     </row>
     <row r="8" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>91</v>
@@ -18066,10 +18066,10 @@
     </row>
     <row r="15" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="C15" s="38" t="s">
         <v>84</v>
@@ -18095,7 +18095,7 @@
         <v>131</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>84</v>
@@ -18262,10 +18262,10 @@
     </row>
     <row r="23" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="C23" s="38" t="s">
         <v>156</v>
@@ -18311,10 +18311,10 @@
     </row>
     <row r="25" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="C25" s="38" t="s">
         <v>96</v>
@@ -18363,7 +18363,7 @@
         <v>164</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>84</v>
@@ -18387,7 +18387,7 @@
         <v>165</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>84</v>
@@ -18411,7 +18411,7 @@
         <v>166</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>84</v>
@@ -18435,7 +18435,7 @@
         <v>167</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>84</v>
@@ -18459,7 +18459,7 @@
         <v>168</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>84</v>
@@ -18483,7 +18483,7 @@
         <v>169</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>170</v>
@@ -18506,7 +18506,7 @@
         <v>173</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>170</v>
@@ -18529,7 +18529,7 @@
         <v>174</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>170</v>
@@ -18552,7 +18552,7 @@
         <v>175</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>170</v>
@@ -18575,7 +18575,7 @@
         <v>176</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>170</v>
@@ -18598,7 +18598,7 @@
         <v>126</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>88</v>
@@ -18621,7 +18621,7 @@
         <v>124</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>84</v>
@@ -18831,7 +18831,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="46" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -19987,10 +19987,10 @@
     </row>
     <row r="97" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="38" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="B97" s="38" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="C97" s="38" t="s">
         <v>84</v>
@@ -20013,7 +20013,7 @@
         <v>267</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>84</v>
@@ -20319,7 +20319,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20349,7 +20349,7 @@
         <v>404</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -20400,10 +20400,10 @@
         <v>307</v>
       </c>
       <c r="C4" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="E4" t="s">
         <v>401</v>
@@ -20486,7 +20486,7 @@
         <v>416</v>
       </c>
       <c r="E8" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F8" t="s">
         <v>406</v>
@@ -20506,10 +20506,10 @@
         <v>417</v>
       </c>
       <c r="E9" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F9" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -20529,7 +20529,7 @@
         <v>403</v>
       </c>
       <c r="F10" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -20543,7 +20543,7 @@
         <v>131</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="E11" t="s">
         <v>401</v>
@@ -20560,10 +20560,10 @@
         <v>307</v>
       </c>
       <c r="C12" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E12" t="s">
         <v>401</v>
@@ -20589,7 +20589,7 @@
         <v>403</v>
       </c>
       <c r="F13" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -20629,7 +20629,7 @@
         <v>401</v>
       </c>
       <c r="F15" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -20649,7 +20649,7 @@
         <v>403</v>
       </c>
       <c r="F16" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -20669,7 +20669,7 @@
         <v>403</v>
       </c>
       <c r="F17" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -20689,7 +20689,7 @@
         <v>403</v>
       </c>
       <c r="F18" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -20709,7 +20709,7 @@
         <v>401</v>
       </c>
       <c r="F19" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -20729,7 +20729,7 @@
         <v>403</v>
       </c>
       <c r="F20" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -20749,7 +20749,7 @@
         <v>403</v>
       </c>
       <c r="F21" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -20769,7 +20769,7 @@
         <v>403</v>
       </c>
       <c r="F22" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -20782,14 +20782,14 @@
       <c r="C23" t="s">
         <v>296</v>
       </c>
-      <c r="D23" s="38" t="s">
-        <v>428</v>
+      <c r="D23" t="s">
+        <v>479</v>
       </c>
       <c r="E23" t="s">
         <v>401</v>
       </c>
       <c r="F23" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -20803,13 +20803,13 @@
         <v>297</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>429</v>
+        <v>483</v>
       </c>
       <c r="E24" t="s">
         <v>401</v>
       </c>
       <c r="F24" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -20823,13 +20823,13 @@
         <v>298</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>430</v>
+        <v>481</v>
       </c>
       <c r="E25" t="s">
         <v>401</v>
       </c>
       <c r="F25" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -20843,13 +20843,13 @@
         <v>299</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>431</v>
+        <v>482</v>
       </c>
       <c r="E26" t="s">
         <v>401</v>
       </c>
       <c r="F26" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -20863,13 +20863,13 @@
         <v>300</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>432</v>
+        <v>480</v>
       </c>
       <c r="E27" t="s">
         <v>401</v>
       </c>
       <c r="F27" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -20909,7 +20909,7 @@
         <v>403</v>
       </c>
       <c r="F29" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -20923,10 +20923,10 @@
         <v>161</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="E30" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F30" t="s">
         <v>406</v>
@@ -20943,13 +20943,13 @@
         <v>163</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="E31" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F31" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -20960,10 +20960,10 @@
         <v>307</v>
       </c>
       <c r="C32" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E32" t="s">
         <v>403</v>
@@ -20989,7 +20989,7 @@
         <v>403</v>
       </c>
       <c r="F33" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -21000,16 +21000,16 @@
         <v>307</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="E34" t="s">
         <v>403</v>
       </c>
       <c r="F34" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -21029,7 +21029,7 @@
         <v>403</v>
       </c>
       <c r="F35" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -21043,7 +21043,7 @@
         <v>134</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="E36" t="s">
         <v>403</v>
@@ -21063,7 +21063,7 @@
         <v>139</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E37" t="s">
         <v>403</v>
@@ -21083,7 +21083,7 @@
         <v>142</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="E38" t="s">
         <v>403</v>
@@ -21103,7 +21103,7 @@
         <v>397</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="E39" t="s">
         <v>401</v>
@@ -21123,7 +21123,7 @@
         <v>150</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E40" t="s">
         <v>401</v>
@@ -21143,7 +21143,7 @@
         <v>153</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="E41" t="s">
         <v>401</v>
@@ -21163,13 +21163,13 @@
         <v>124</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E42" t="s">
         <v>401</v>
       </c>
       <c r="F42" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -21183,13 +21183,13 @@
         <v>126</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="E43" t="s">
         <v>401</v>
       </c>
       <c r="F43" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -21203,7 +21203,7 @@
         <v>145</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E44" t="s">
         <v>403</v>
@@ -21223,7 +21223,7 @@
         <v>130</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="E45" t="s">
         <v>401</v>
@@ -21243,13 +21243,13 @@
         <v>128</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="E46" t="s">
         <v>403</v>
       </c>
       <c r="F46" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -21394,7 +21394,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -22719,7 +22719,7 @@
         <v>267</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D49" s="43">
         <v>0.95</v>
@@ -22743,10 +22743,10 @@
         <v>363</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D50" s="43">
         <v>0.73</v>

</xml_diff>

<commit_message>
2.10.7 Remove requiredVL parameter
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0F1221-B1FD-491C-A8B8-B429E176BD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BC0446-2919-4C04-B71D-68C0D8881CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="482">
   <si>
     <t>Susceptible</t>
   </si>
@@ -1205,12 +1205,6 @@
   </si>
   <si>
     <t>numvlmon</t>
-  </si>
-  <si>
-    <t>Number of VL tests recommended per person per year</t>
-  </si>
-  <si>
-    <t>requiredvl</t>
   </si>
   <si>
     <t>1. Update the table on the "Model parameters" sheet.</t>
@@ -15144,17 +15138,17 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -15241,10 +15235,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -17700,11 +17694,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:H123"/>
+  <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17743,7 +17737,7 @@
         <v>81</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -17844,10 +17838,10 @@
     </row>
     <row r="6" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>96</v>
@@ -17891,10 +17885,10 @@
     </row>
     <row r="8" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>91</v>
@@ -18066,10 +18060,10 @@
     </row>
     <row r="15" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C15" s="38" t="s">
         <v>84</v>
@@ -18095,7 +18089,7 @@
         <v>131</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>84</v>
@@ -18262,10 +18256,10 @@
     </row>
     <row r="23" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C23" s="38" t="s">
         <v>156</v>
@@ -18311,10 +18305,10 @@
     </row>
     <row r="25" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C25" s="38" t="s">
         <v>96</v>
@@ -18363,7 +18357,7 @@
         <v>164</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>84</v>
@@ -18387,7 +18381,7 @@
         <v>165</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>84</v>
@@ -18411,7 +18405,7 @@
         <v>166</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>84</v>
@@ -18435,7 +18429,7 @@
         <v>167</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>84</v>
@@ -18459,7 +18453,7 @@
         <v>168</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>84</v>
@@ -18483,7 +18477,7 @@
         <v>169</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>170</v>
@@ -18506,7 +18500,7 @@
         <v>173</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>170</v>
@@ -18529,7 +18523,7 @@
         <v>174</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>170</v>
@@ -18552,7 +18546,7 @@
         <v>175</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>170</v>
@@ -18575,7 +18569,7 @@
         <v>176</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>170</v>
@@ -18598,7 +18592,7 @@
         <v>126</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>88</v>
@@ -18621,7 +18615,7 @@
         <v>124</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>84</v>
@@ -18831,7 +18825,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="46" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -18929,10 +18923,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>91</v>
@@ -19504,13 +19498,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>135</v>
+        <v>228</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C76" s="38" t="s">
+        <v>84</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>110</v>
@@ -19518,19 +19512,19 @@
       <c r="E76" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F76" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="G76" s="14">
+      <c r="F76" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="G76" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C77" s="38" t="s">
         <v>84</v>
@@ -19550,10 +19544,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>229</v>
+        <v>232</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>231</v>
       </c>
       <c r="C78" s="38" t="s">
         <v>84</v>
@@ -19573,10 +19567,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C79" s="38" t="s">
         <v>84</v>
@@ -19596,10 +19590,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C80" s="38" t="s">
         <v>84</v>
@@ -19619,10 +19613,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C81" s="38" t="s">
         <v>84</v>
@@ -19642,10 +19636,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C82" s="38" t="s">
         <v>84</v>
@@ -19665,10 +19659,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C83" s="38" t="s">
         <v>84</v>
@@ -19688,13 +19682,13 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="C84" s="38" t="s">
-        <v>84</v>
+        <v>245</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>110</v>
@@ -19711,10 +19705,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>96</v>
@@ -19734,10 +19728,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>96</v>
@@ -19756,11 +19750,11 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>249</v>
+      <c r="A87" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>251</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>96</v>
@@ -19780,10 +19774,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>251</v>
+        <v>253</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>386</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>96</v>
@@ -19794,19 +19788,19 @@
       <c r="E88" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F88" s="14" t="s">
-        <v>383</v>
+      <c r="F88" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="G88" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B89" s="15" t="s">
-        <v>386</v>
+      <c r="A89" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>387</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>96</v>
@@ -19826,13 +19820,13 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>387</v>
+        <v>256</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>255</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>110</v>
@@ -19849,10 +19843,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>91</v>
@@ -19872,10 +19866,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>91</v>
@@ -19886,8 +19880,8 @@
       <c r="E92" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F92" s="6" t="s">
-        <v>180</v>
+      <c r="F92" s="14" t="s">
+        <v>383</v>
       </c>
       <c r="G92" s="6">
         <v>1</v>
@@ -19895,13 +19889,13 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>110</v>
@@ -19909,8 +19903,8 @@
       <c r="E93" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F93" s="14" t="s">
-        <v>383</v>
+      <c r="F93" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="G93" s="6">
         <v>1</v>
@@ -19918,10 +19912,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>84</v>
@@ -19941,10 +19935,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>84</v>
@@ -19962,58 +19956,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="C96" s="6" t="s">
+    <row r="96" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="38" t="s">
+        <v>458</v>
+      </c>
+      <c r="B96" s="38" t="s">
+        <v>459</v>
+      </c>
+      <c r="C96" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D96" s="6" t="s">
+      <c r="D96" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="E96" s="6" t="s">
+      <c r="E96" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="F96" s="6" t="s">
+      <c r="F96" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="G96" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="38" t="s">
+      <c r="G96" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B97" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B97" s="38" t="s">
-        <v>461</v>
-      </c>
-      <c r="C97" s="38" t="s">
+      <c r="C97" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D97" s="38" t="s">
+      <c r="D97" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E97" s="38" t="s">
+      <c r="E97" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F97" s="38" t="s">
+      <c r="F97" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G97" s="38">
+      <c r="G97" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>462</v>
+        <v>268</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>84</v>
@@ -20033,10 +20027,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>84</v>
@@ -20056,10 +20050,10 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>84</v>
@@ -20079,10 +20073,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>84</v>
@@ -20102,10 +20096,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>84</v>
@@ -20116,8 +20110,8 @@
       <c r="E102" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F102" s="6" t="s">
-        <v>180</v>
+      <c r="F102" s="14" t="s">
+        <v>383</v>
       </c>
       <c r="G102" s="6">
         <v>1</v>
@@ -20125,10 +20119,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>84</v>
@@ -20148,10 +20142,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>84</v>
@@ -20171,10 +20165,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>84</v>
@@ -20194,10 +20188,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>84</v>
@@ -20217,10 +20211,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>84</v>
@@ -20240,10 +20234,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>84</v>
@@ -20262,33 +20256,15 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E109" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="F109" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="G109" s="6">
-        <v>1</v>
-      </c>
+      <c r="D109" s="6"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D110" s="6"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C111" s="6"/>
       <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C112" s="6"/>
@@ -20305,7 +20281,6 @@
     <row r="120" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="121" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="122" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -20317,9 +20292,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20346,10 +20321,10 @@
         <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -20366,10 +20341,10 @@
         <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -20386,10 +20361,10 @@
         <v>305</v>
       </c>
       <c r="E3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -20400,16 +20375,16 @@
         <v>307</v>
       </c>
       <c r="C4" t="s">
+        <v>474</v>
+      </c>
+      <c r="D4" s="38" t="s">
         <v>476</v>
       </c>
-      <c r="D4" s="38" t="s">
-        <v>478</v>
-      </c>
       <c r="E4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -20423,13 +20398,13 @@
         <v>104</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -20443,13 +20418,13 @@
         <v>112</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -20466,10 +20441,10 @@
         <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -20483,13 +20458,13 @@
         <v>107</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E8" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -20503,13 +20478,13 @@
         <v>109</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E9" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F9" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -20526,10 +20501,10 @@
         <v>115</v>
       </c>
       <c r="E10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F10" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -20543,13 +20518,13 @@
         <v>131</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E11" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F11" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -20560,16 +20535,16 @@
         <v>307</v>
       </c>
       <c r="C12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -20583,13 +20558,13 @@
         <v>118</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -20603,13 +20578,13 @@
         <v>122</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F14" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -20623,13 +20598,13 @@
         <v>120</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E15" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F15" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -20643,13 +20618,13 @@
         <v>290</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F16" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -20663,13 +20638,13 @@
         <v>291</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E17" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F17" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -20683,13 +20658,13 @@
         <v>292</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E18" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F18" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -20700,16 +20675,16 @@
         <v>307</v>
       </c>
       <c r="C19" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E19" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -20723,13 +20698,13 @@
         <v>293</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E20" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F20" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -20743,13 +20718,13 @@
         <v>294</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E21" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F21" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -20763,13 +20738,13 @@
         <v>295</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E22" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F22" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -20783,13 +20758,13 @@
         <v>296</v>
       </c>
       <c r="D23" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E23" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F23" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -20803,13 +20778,13 @@
         <v>297</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E24" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F24" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -20823,13 +20798,13 @@
         <v>298</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E25" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F25" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -20843,13 +20818,13 @@
         <v>299</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E26" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F26" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -20863,13 +20838,13 @@
         <v>300</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E27" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F27" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -20886,10 +20861,10 @@
         <v>154</v>
       </c>
       <c r="E28" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F28" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -20906,10 +20881,10 @@
         <v>157</v>
       </c>
       <c r="E29" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F29" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -20923,13 +20898,13 @@
         <v>161</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E30" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F30" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -20943,13 +20918,13 @@
         <v>163</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E31" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F31" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -20960,16 +20935,16 @@
         <v>307</v>
       </c>
       <c r="C32" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E32" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F32" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -20986,10 +20961,10 @@
         <v>159</v>
       </c>
       <c r="E33" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F33" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -21000,16 +20975,16 @@
         <v>307</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E34" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F34" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -21026,10 +21001,10 @@
         <v>243</v>
       </c>
       <c r="E35" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F35" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -21043,13 +21018,13 @@
         <v>134</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E36" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F36" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -21063,13 +21038,13 @@
         <v>139</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E37" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F37" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -21083,13 +21058,13 @@
         <v>142</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E38" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F38" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -21100,16 +21075,16 @@
         <v>307</v>
       </c>
       <c r="C39" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E39" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F39" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -21123,13 +21098,13 @@
         <v>150</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E40" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F40" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -21143,13 +21118,13 @@
         <v>153</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E41" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F41" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -21163,13 +21138,13 @@
         <v>124</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E42" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F42" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -21183,13 +21158,13 @@
         <v>126</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E43" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F43" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -21203,13 +21178,13 @@
         <v>145</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E44" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F44" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -21223,13 +21198,13 @@
         <v>130</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E45" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F45" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -21243,13 +21218,13 @@
         <v>128</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E46" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F46" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -21257,19 +21232,19 @@
         <v>316</v>
       </c>
       <c r="B47" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C47" t="s">
         <v>301</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E47" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F47" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -21277,19 +21252,19 @@
         <v>316</v>
       </c>
       <c r="B48" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C48" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E48" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F48" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -21297,19 +21272,19 @@
         <v>316</v>
       </c>
       <c r="B49" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C49" t="s">
         <v>302</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E49" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F49" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -21317,19 +21292,19 @@
         <v>316</v>
       </c>
       <c r="B50" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C50" t="s">
         <v>303</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E50" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F50" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -21337,19 +21312,19 @@
         <v>316</v>
       </c>
       <c r="B51" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C51" t="s">
         <v>102</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E51" t="s">
+        <v>401</v>
+      </c>
+      <c r="F51" t="s">
         <v>403</v>
-      </c>
-      <c r="F51" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -21357,19 +21332,19 @@
         <v>316</v>
       </c>
       <c r="B52" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C52" t="s">
         <v>100</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E52" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F52" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -21377,19 +21352,19 @@
         <v>316</v>
       </c>
       <c r="B53" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C53" t="s">
         <v>95</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E53" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F53" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -21401,10 +21376,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21435,7 +21410,7 @@
         <v>321</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>369</v>
@@ -21461,10 +21436,10 @@
         <v>1.4E-3</v>
       </c>
       <c r="G2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H2" s="17" t="b">
-        <f t="shared" ref="H2:H33" si="0">AND(D2&gt;=E2, D2&lt;=F2)</f>
+        <f t="shared" ref="H2:H32" si="0">AND(D2&gt;=E2, D2&lt;=F2)</f>
         <v>1</v>
       </c>
     </row>
@@ -21488,7 +21463,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="G3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H3" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21515,7 +21490,7 @@
         <v>2.8E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H4" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21542,7 +21517,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
       <c r="G5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H5" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21569,7 +21544,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="G6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H6" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21596,7 +21571,7 @@
         <v>0.44</v>
       </c>
       <c r="G7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H7" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21623,7 +21598,7 @@
         <v>0.27</v>
       </c>
       <c r="G8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H8" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21650,7 +21625,7 @@
         <v>9.1</v>
       </c>
       <c r="G9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H9" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21677,7 +21652,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H10" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21704,7 +21679,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H11" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21731,7 +21706,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H12" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21758,7 +21733,7 @@
         <v>6.92</v>
       </c>
       <c r="G13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H13" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21785,7 +21760,7 @@
         <v>12.08</v>
       </c>
       <c r="G14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H14" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21812,7 +21787,7 @@
         <v>0.5</v>
       </c>
       <c r="G15" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H15" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21839,7 +21814,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="G16" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H16" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21866,7 +21841,7 @@
         <v>3.16</v>
       </c>
       <c r="G17" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H17" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21893,7 +21868,7 @@
         <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H18" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21920,7 +21895,7 @@
         <v>2.25</v>
       </c>
       <c r="G19" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H19" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21947,7 +21922,7 @@
         <v>7.28</v>
       </c>
       <c r="G20" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H20" s="17" t="b">
         <f t="shared" si="0"/>
@@ -21974,7 +21949,7 @@
         <v>3.42</v>
       </c>
       <c r="G21" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H21" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22001,7 +21976,7 @@
         <v>3.58</v>
       </c>
       <c r="G22" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H22" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22028,7 +22003,7 @@
         <v>0.94</v>
       </c>
       <c r="G23" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H23" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22055,7 +22030,7 @@
         <v>0.3</v>
       </c>
       <c r="G24" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H24" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22063,26 +22038,26 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>390</v>
+      <c r="A25" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="D25" s="42">
-        <v>1</v>
-      </c>
-      <c r="E25" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="F25" s="42">
-        <v>1.5</v>
+        <v>331</v>
+      </c>
+      <c r="D25" s="41">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E25" s="41">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F25" s="41">
+        <v>0.27500000000000002</v>
       </c>
       <c r="G25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H25" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22094,22 +22069,22 @@
         <v>365</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="D26" s="41">
-        <v>2.5999999999999999E-2</v>
+        <v>0.15</v>
       </c>
       <c r="E26" s="41">
-        <v>5.0000000000000001E-3</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="F26" s="41">
-        <v>0.27500000000000002</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="G26" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H26" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22121,22 +22096,22 @@
         <v>365</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D27" s="41">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E27" s="41">
-        <v>3.7999999999999999E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="F27" s="41">
-        <v>0.88500000000000001</v>
+        <v>0.87</v>
       </c>
       <c r="G27" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H27" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22148,22 +22123,22 @@
         <v>365</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D28" s="41">
-        <v>0.1</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E28" s="41">
-        <v>2.1999999999999999E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F28" s="41">
-        <v>0.87</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="G28" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H28" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22175,22 +22150,22 @@
         <v>365</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D29" s="41">
-        <v>5.2999999999999999E-2</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="E29" s="41">
-        <v>8.0000000000000002E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F29" s="41">
-        <v>0.82699999999999996</v>
+        <v>0.86899999999999999</v>
       </c>
       <c r="G29" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H29" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22202,22 +22177,22 @@
         <v>365</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D30" s="41">
-        <v>0.16200000000000001</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="E30" s="41">
-        <v>0.05</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="F30" s="41">
-        <v>0.86899999999999999</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="G30" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H30" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22229,22 +22204,22 @@
         <v>365</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D31" s="41">
-        <v>0.11700000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E31" s="41">
-        <v>3.2000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="F31" s="41">
-        <v>0.68600000000000005</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="G31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H31" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22256,22 +22231,22 @@
         <v>365</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="D32" s="41">
-        <v>0.09</v>
+        <v>0.111</v>
       </c>
       <c r="E32" s="41">
-        <v>1.9E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="F32" s="41">
-        <v>0.72299999999999998</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="G32" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H32" s="17" t="b">
         <f t="shared" si="0"/>
@@ -22279,29 +22254,29 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>365</v>
+      <c r="A33" s="10" t="s">
+        <v>364</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="D33" s="41">
-        <v>0.111</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="E33" s="41">
-        <v>4.7E-2</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="F33" s="41">
-        <v>0.56299999999999994</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="G33" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H33" s="17" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H33:H58" si="1">AND(D33&gt;=E33, D33&lt;=F33)</f>
         <v>1</v>
       </c>
     </row>
@@ -22310,10 +22285,10 @@
         <v>364</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D34" s="41">
         <v>3.5999999999999999E-3</v>
@@ -22325,62 +22300,62 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="G34" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H34" s="17" t="b">
-        <f t="shared" ref="H34:H59" si="1">AND(D34&gt;=E34, D34&lt;=F34)</f>
-        <v>1</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I34" s="40"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>364</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="D35" s="41">
-        <v>3.5999999999999999E-3</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="E35" s="41">
-        <v>2.8999999999999998E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="F35" s="41">
-        <v>4.4000000000000003E-3</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="G35" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H35" s="17" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I35" s="40"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>364</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="D36" s="41">
-        <v>5.7999999999999996E-3</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="E36" s="41">
-        <v>4.7999999999999996E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="F36" s="41">
-        <v>7.1000000000000004E-3</v>
+        <v>1.01E-2</v>
       </c>
       <c r="G36" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H36" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22392,22 +22367,22 @@
         <v>364</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D37" s="41">
-        <v>8.8000000000000005E-3</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="E37" s="41">
-        <v>7.4999999999999997E-3</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="F37" s="41">
-        <v>1.01E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="G37" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H37" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22419,22 +22394,22 @@
         <v>364</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D38" s="41">
-        <v>5.8999999999999997E-2</v>
+        <v>0.32300000000000001</v>
       </c>
       <c r="E38" s="41">
-        <v>5.3999999999999999E-2</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="F38" s="41">
-        <v>7.9000000000000001E-2</v>
+        <v>0.432</v>
       </c>
       <c r="G38" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H38" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22446,22 +22421,22 @@
         <v>364</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="D39" s="41">
-        <v>0.32300000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="E39" s="41">
-        <v>0.29599999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="F39" s="41">
-        <v>0.432</v>
+        <v>0.3</v>
       </c>
       <c r="G39" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="H39" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22473,22 +22448,22 @@
         <v>364</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D40" s="41">
-        <v>0.23</v>
+        <v>0.48780000000000001</v>
       </c>
       <c r="E40" s="41">
-        <v>0.15</v>
+        <v>0.28349999999999997</v>
       </c>
       <c r="F40" s="41">
-        <v>0.3</v>
+        <v>0.8417</v>
       </c>
       <c r="G40" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H40" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22500,22 +22475,22 @@
         <v>364</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D41" s="41">
-        <v>0.48780000000000001</v>
+        <v>2.17</v>
       </c>
       <c r="E41" s="41">
-        <v>0.28349999999999997</v>
+        <v>1.27</v>
       </c>
       <c r="F41" s="41">
-        <v>0.8417</v>
+        <v>3.71</v>
       </c>
       <c r="G41" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H41" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22524,25 +22499,25 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="D42" s="41">
-        <v>2.17</v>
-      </c>
-      <c r="E42" s="41">
-        <v>1.27</v>
-      </c>
-      <c r="F42" s="41">
-        <v>3.71</v>
+        <v>347</v>
+      </c>
+      <c r="D42" s="43">
+        <v>0.95</v>
+      </c>
+      <c r="E42" s="43">
+        <v>0.8</v>
+      </c>
+      <c r="F42" s="43">
+        <v>0.98</v>
       </c>
       <c r="G42" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H42" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22554,22 +22529,22 @@
         <v>363</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D43" s="43">
-        <v>0.95</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E43" s="43">
-        <v>0.8</v>
+        <v>0.47</v>
       </c>
       <c r="F43" s="43">
-        <v>0.98</v>
+        <v>0.67</v>
       </c>
       <c r="G43" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H43" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22581,22 +22556,22 @@
         <v>363</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D44" s="43">
-        <v>0.57999999999999996</v>
+        <v>0</v>
       </c>
       <c r="E44" s="43">
-        <v>0.47</v>
+        <v>0</v>
       </c>
       <c r="F44" s="43">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="G44" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H44" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22608,22 +22583,22 @@
         <v>363</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>275</v>
+        <v>206</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D45" s="43">
-        <v>0</v>
+        <v>2.65</v>
       </c>
       <c r="E45" s="43">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="F45" s="43">
-        <v>0.68</v>
+        <v>5.19</v>
       </c>
       <c r="G45" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H45" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22635,22 +22610,22 @@
         <v>363</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>206</v>
+        <v>273</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D46" s="43">
-        <v>2.65</v>
+        <v>0.54</v>
       </c>
       <c r="E46" s="43">
-        <v>1.35</v>
+        <v>0.33</v>
       </c>
       <c r="F46" s="43">
-        <v>5.19</v>
+        <v>0.68</v>
       </c>
       <c r="G46" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H46" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22662,22 +22637,22 @@
         <v>363</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D47" s="43">
-        <v>0.54</v>
+        <v>0.9</v>
       </c>
       <c r="E47" s="43">
-        <v>0.33</v>
+        <v>0.82</v>
       </c>
       <c r="F47" s="43">
-        <v>0.68</v>
+        <v>0.93</v>
       </c>
       <c r="G47" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H47" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22689,25 +22664,25 @@
         <v>363</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>352</v>
+        <v>462</v>
       </c>
       <c r="D48" s="43">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="E48" s="43">
-        <v>0.82</v>
+        <v>0.92</v>
       </c>
       <c r="F48" s="43">
-        <v>0.93</v>
+        <v>0.97</v>
       </c>
       <c r="G48" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H48" s="17" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(D48&gt;=E48, D48&lt;=F48)</f>
         <v>1</v>
       </c>
     </row>
@@ -22716,25 +22691,25 @@
         <v>363</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>267</v>
+        <v>458</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D49" s="43">
-        <v>0.95</v>
+        <v>0.73</v>
       </c>
       <c r="E49" s="43">
-        <v>0.92</v>
+        <v>0.65</v>
       </c>
       <c r="F49" s="43">
-        <v>0.97</v>
+        <v>0.8</v>
       </c>
       <c r="G49" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H49" s="17" t="b">
-        <f>AND(D49&gt;=E49, D49&lt;=F49)</f>
+        <f t="shared" ref="H49" si="2">AND(D49&gt;=E49, D49&lt;=F49)</f>
         <v>1</v>
       </c>
     </row>
@@ -22743,25 +22718,25 @@
         <v>363</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>460</v>
+        <v>262</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>463</v>
+        <v>353</v>
       </c>
       <c r="D50" s="43">
-        <v>0.73</v>
+        <v>0.5</v>
       </c>
       <c r="E50" s="43">
-        <v>0.65</v>
+        <v>0.3</v>
       </c>
       <c r="F50" s="43">
         <v>0.8</v>
       </c>
       <c r="G50" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H50" s="17" t="b">
-        <f t="shared" ref="H50" si="2">AND(D50&gt;=E50, D50&lt;=F50)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -22770,22 +22745,22 @@
         <v>363</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D51" s="43">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E51" s="43">
-        <v>0.3</v>
+        <v>0.92</v>
       </c>
       <c r="F51" s="43">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H51" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22793,26 +22768,26 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>363</v>
+      <c r="A52" s="3" t="s">
+        <v>362</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="D52" s="43">
-        <v>1</v>
-      </c>
-      <c r="E52" s="43">
-        <v>0.92</v>
-      </c>
-      <c r="F52" s="43">
-        <v>1</v>
+        <v>355</v>
+      </c>
+      <c r="D52" s="42">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="E52" s="42">
+        <v>0.121</v>
+      </c>
+      <c r="F52" s="42">
+        <v>0.249</v>
       </c>
       <c r="G52" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H52" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22824,22 +22799,22 @@
         <v>362</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D53" s="42">
-        <v>0.18099999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="E53" s="42">
-        <v>0.121</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="F53" s="42">
-        <v>0.249</v>
+        <v>1.4E-2</v>
       </c>
       <c r="G53" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H53" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22851,22 +22826,22 @@
         <v>362</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="D54" s="42">
-        <v>0.01</v>
+        <v>357</v>
+      </c>
+      <c r="D54" s="44">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E54" s="42">
-        <v>7.0000000000000001E-3</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="F54" s="42">
-        <v>1.4E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="G54" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H54" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22878,22 +22853,22 @@
         <v>362</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D55" s="44">
-        <v>2.5000000000000001E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E55" s="42">
-        <v>1.7000000000000001E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F55" s="42">
-        <v>3.5000000000000003E-2</v>
+        <v>0.107</v>
       </c>
       <c r="G55" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H55" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22905,22 +22880,22 @@
         <v>362</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="D56" s="44">
-        <v>8.1000000000000003E-2</v>
+        <v>359</v>
+      </c>
+      <c r="D56" s="42">
+        <v>0.28899999999999998</v>
       </c>
       <c r="E56" s="42">
-        <v>5.5E-2</v>
+        <v>0.128</v>
       </c>
       <c r="F56" s="42">
-        <v>0.107</v>
+        <v>0.499</v>
       </c>
       <c r="G56" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H56" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22932,22 +22907,22 @@
         <v>362</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D57" s="42">
-        <v>0.28899999999999998</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="E57" s="42">
-        <v>0.128</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="F57" s="42">
-        <v>0.499</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="G57" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H57" s="17" t="b">
         <f t="shared" si="1"/>
@@ -22958,52 +22933,25 @@
       <c r="A58" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>360</v>
+      <c r="B58" t="s">
+        <v>289</v>
+      </c>
+      <c r="C58" t="s">
+        <v>361</v>
       </c>
       <c r="D58" s="42">
-        <v>0.58199999999999996</v>
+        <v>7.8E-2</v>
       </c>
       <c r="E58" s="42">
-        <v>0.40600000000000003</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="F58" s="42">
-        <v>0.74299999999999999</v>
+        <v>0.111</v>
       </c>
       <c r="G58" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H58" s="17" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="B59" t="s">
-        <v>289</v>
-      </c>
-      <c r="C59" t="s">
-        <v>361</v>
-      </c>
-      <c r="D59" s="42">
-        <v>7.8E-2</v>
-      </c>
-      <c r="E59" s="42">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="F59" s="42">
-        <v>0.111</v>
-      </c>
-      <c r="G59" t="s">
-        <v>400</v>
-      </c>
-      <c r="H59" s="17" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Make forcepopsize, initcd4weight, and treatbycd4before parameters
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BC0446-2919-4C04-B71D-68C0D8881CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEEBEB0-A94A-457C-AD67-822EA0902B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="489">
   <si>
     <t>Susceptible</t>
   </si>
@@ -1484,6 +1484,27 @@
   </si>
   <si>
     <t>Percent of people who know their status who are retained in care</t>
+  </si>
+  <si>
+    <t>(1900, 2100)</t>
+  </si>
+  <si>
+    <t>initcd4weight</t>
+  </si>
+  <si>
+    <t>Weighting for initialization where low values represent early stage epidemics</t>
+  </si>
+  <si>
+    <t>forcepopsize</t>
+  </si>
+  <si>
+    <t>Force all population sizes to match initial value with exponential growth curve</t>
+  </si>
+  <si>
+    <t>treatbycd4before</t>
+  </si>
+  <si>
+    <t>Treatment prioritized by CD4 count before this date</t>
   </si>
 </sst>
 </file>
@@ -17697,8 +17718,8 @@
   <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L28" sqref="L28"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20256,15 +20277,73 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D109" s="6"/>
+      <c r="A109" s="38" t="s">
+        <v>487</v>
+      </c>
+      <c r="B109" s="38" t="s">
+        <v>488</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="D109" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E109" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F109" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G109" s="38">
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D110" s="6"/>
+      <c r="A110" s="38" t="s">
+        <v>483</v>
+      </c>
+      <c r="B110" s="38" t="s">
+        <v>484</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D110" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E110" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F110" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G110" s="38">
+        <v>0</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="6"/>
+      <c r="A111" s="38" t="s">
+        <v>485</v>
+      </c>
+      <c r="B111" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="C111" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D111" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E111" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="F111" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G111" s="38">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C112" s="6"/>
@@ -20294,7 +20373,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD37"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add metaparameters for relhivbirth and transdeathtx
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEEBEB0-A94A-457C-AD67-822EA0902B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3980C3D5-257F-498D-980E-7E8707289919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="493">
   <si>
     <t>Susceptible</t>
   </si>
@@ -1505,6 +1505,18 @@
   </si>
   <si>
     <t>Treatment prioritized by CD4 count before this date</t>
+  </si>
+  <si>
+    <t>Time dependent additional reduction in relative death rate on ART (unitless)</t>
+  </si>
+  <si>
+    <t>transdeathtx</t>
+  </si>
+  <si>
+    <t>relhivbirth</t>
+  </si>
+  <si>
+    <t>Relative likelihood that females with HIV give birth</t>
   </si>
 </sst>
 </file>
@@ -17718,8 +17730,8 @@
   <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B115" sqref="B115"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20346,20 +20358,100 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C112" s="6"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="6"/>
-    </row>
-    <row r="113" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="A112" s="38" t="s">
+        <v>490</v>
+      </c>
+      <c r="B112" s="38" t="s">
+        <v>489</v>
+      </c>
+      <c r="C112" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D112" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E112" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F112" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G112" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="38" t="s">
+        <v>491</v>
+      </c>
+      <c r="B113" s="38" t="s">
+        <v>492</v>
+      </c>
+      <c r="C113" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D113" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E113" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="F113" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G113" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="38"/>
+      <c r="B114" s="38"/>
+      <c r="C114" s="38"/>
+      <c r="D114" s="38"/>
+      <c r="E114" s="38"/>
+      <c r="F114" s="38"/>
+      <c r="G114" s="38"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Merge 2.10.8 back into 2.10.7 as they make sense to happen at the same time
Also change treatbycd4before into a yearpar

transdeathtx to have a (0, maxmeta) range and default to 1 as a relative risk.
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3980C3D5-257F-498D-980E-7E8707289919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3EEDD2-A47F-4198-A2D4-FCB2780CA275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="492">
   <si>
     <t>Susceptible</t>
   </si>
@@ -1486,9 +1486,6 @@
     <t>Percent of people who know their status who are retained in care</t>
   </si>
   <si>
-    <t>(1900, 2100)</t>
-  </si>
-  <si>
     <t>initcd4weight</t>
   </si>
   <si>
@@ -1507,9 +1504,6 @@
     <t>Treatment prioritized by CD4 count before this date</t>
   </si>
   <si>
-    <t>Time dependent additional reduction in relative death rate on ART (unitless)</t>
-  </si>
-  <si>
     <t>transdeathtx</t>
   </si>
   <si>
@@ -1517,6 +1511,9 @@
   </si>
   <si>
     <t>Relative likelihood that females with HIV give birth</t>
+  </si>
+  <si>
+    <t>Relative death rate on ART (unitless, time based adjustment to constant treatment effect)</t>
   </si>
 </sst>
 </file>
@@ -17730,8 +17727,8 @@
   <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C114" sqref="C114"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N89" sqref="N89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20290,19 +20287,19 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="B109" s="38" t="s">
         <v>487</v>
       </c>
-      <c r="B109" s="38" t="s">
-        <v>488</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>482</v>
+      <c r="C109" s="38" t="s">
+        <v>170</v>
       </c>
       <c r="D109" s="38" t="s">
         <v>110</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F109" s="38" t="s">
         <v>92</v>
@@ -20313,10 +20310,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="38" t="s">
+        <v>482</v>
+      </c>
+      <c r="B110" s="38" t="s">
         <v>483</v>
-      </c>
-      <c r="B110" s="38" t="s">
-        <v>484</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>91</v>
@@ -20336,10 +20333,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="38" t="s">
+        <v>484</v>
+      </c>
+      <c r="B111" s="38" t="s">
         <v>485</v>
-      </c>
-      <c r="B111" s="38" t="s">
-        <v>486</v>
       </c>
       <c r="C111" s="38" t="s">
         <v>84</v>
@@ -20359,10 +20356,10 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="38" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B112" s="38" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C112" s="38" t="s">
         <v>91</v>
@@ -20382,10 +20379,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="38" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B113" s="38" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C113" s="38" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
Change returntocare to be a rate instead of duration
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3EEDD2-A47F-4198-A2D4-FCB2780CA275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6663D8-2F92-463F-826B-BC06DFF13CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="493">
   <si>
     <t>Susceptible</t>
   </si>
@@ -1432,9 +1432,6 @@
     <t>returntocare</t>
   </si>
   <si>
-    <t>Average time taken to be returned to care after loss to follow-up (years)</t>
-  </si>
-  <si>
     <t>Proportion of exposure events covered by ARV-based post-exposure prophylaxis</t>
   </si>
   <si>
@@ -1498,12 +1495,6 @@
     <t>Force all population sizes to match initial value with exponential growth curve</t>
   </si>
   <si>
-    <t>treatbycd4before</t>
-  </si>
-  <si>
-    <t>Treatment prioritized by CD4 count before this date</t>
-  </si>
-  <si>
     <t>transdeathtx</t>
   </si>
   <si>
@@ -1514,6 +1505,18 @@
   </si>
   <si>
     <t>Relative death rate on ART (unitless, time based adjustment to constant treatment effect)</t>
+  </si>
+  <si>
+    <t>allcd4eligibletx </t>
+  </si>
+  <si>
+    <t>No CD4 eligibility criteria for treatment from this year</t>
+  </si>
+  <si>
+    <t>Return to care rate (per year)</t>
+  </si>
+  <si>
+    <t>Percentage of people lost to follow-up who are returned to care per year (%/year)</t>
   </si>
 </sst>
 </file>
@@ -17726,9 +17729,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N89" sqref="N89"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17868,10 +17871,10 @@
     </row>
     <row r="6" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
+        <v>473</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>474</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>475</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>96</v>
@@ -18093,7 +18096,7 @@
         <v>457</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C15" s="38" t="s">
         <v>84</v>
@@ -18119,7 +18122,7 @@
         <v>131</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>84</v>
@@ -18289,10 +18292,10 @@
         <v>463</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>464</v>
+        <v>491</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>85</v>
@@ -18507,7 +18510,7 @@
         <v>169</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>170</v>
@@ -18530,7 +18533,7 @@
         <v>173</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>170</v>
@@ -18553,7 +18556,7 @@
         <v>174</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>170</v>
@@ -18576,7 +18579,7 @@
         <v>175</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>170</v>
@@ -18599,7 +18602,7 @@
         <v>176</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>170</v>
@@ -18622,7 +18625,7 @@
         <v>126</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>88</v>
@@ -18645,7 +18648,7 @@
         <v>124</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>84</v>
@@ -20287,10 +20290,10 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="38" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B109" s="38" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="C109" s="38" t="s">
         <v>170</v>
@@ -20310,10 +20313,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="38" t="s">
+        <v>481</v>
+      </c>
+      <c r="B110" s="38" t="s">
         <v>482</v>
-      </c>
-      <c r="B110" s="38" t="s">
-        <v>483</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>91</v>
@@ -20333,10 +20336,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="38" t="s">
+        <v>483</v>
+      </c>
+      <c r="B111" s="38" t="s">
         <v>484</v>
-      </c>
-      <c r="B111" s="38" t="s">
-        <v>485</v>
       </c>
       <c r="C111" s="38" t="s">
         <v>84</v>
@@ -20356,10 +20359,10 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="38" t="s">
+        <v>485</v>
+      </c>
+      <c r="B112" s="38" t="s">
         <v>488</v>
-      </c>
-      <c r="B112" s="38" t="s">
-        <v>491</v>
       </c>
       <c r="C112" s="38" t="s">
         <v>91</v>
@@ -20379,10 +20382,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="38" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B113" s="38" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C113" s="38" t="s">
         <v>91</v>
@@ -20460,9 +20463,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20543,10 +20546,10 @@
         <v>307</v>
       </c>
       <c r="C4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E4" t="s">
         <v>399</v>
@@ -20686,7 +20689,7 @@
         <v>131</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E11" t="s">
         <v>399</v>
@@ -20706,7 +20709,7 @@
         <v>457</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E12" t="s">
         <v>399</v>
@@ -20926,7 +20929,7 @@
         <v>296</v>
       </c>
       <c r="D23" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E23" t="s">
         <v>399</v>
@@ -20946,7 +20949,7 @@
         <v>297</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E24" t="s">
         <v>399</v>
@@ -20966,7 +20969,7 @@
         <v>298</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E25" t="s">
         <v>399</v>
@@ -20986,7 +20989,7 @@
         <v>299</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E26" t="s">
         <v>399</v>
@@ -21006,7 +21009,7 @@
         <v>300</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E27" t="s">
         <v>399</v>
@@ -21106,10 +21109,10 @@
         <v>463</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>464</v>
+        <v>492</v>
       </c>
       <c r="E32" t="s">
-        <v>401</v>
+        <v>444</v>
       </c>
       <c r="F32" t="s">
         <v>404</v>
@@ -21326,7 +21329,7 @@
         <v>126</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E43" t="s">
         <v>399</v>

</xml_diff>

<commit_message>
rename metapars to improve clarity
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6663D8-2F92-463F-826B-BC06DFF13CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B010A315-B223-4805-A6F4-38A925978A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -1477,9 +1477,6 @@
     <t>Percent of people who know their status who are on ART</t>
   </si>
   <si>
-    <t>Percent of pregnant women with HIV on PMTCT</t>
-  </si>
-  <si>
     <t>Percent of people who know their status who are retained in care</t>
   </si>
   <si>
@@ -1495,18 +1492,12 @@
     <t>Force all population sizes to match initial value with exponential growth curve</t>
   </si>
   <si>
-    <t>transdeathtx</t>
-  </si>
-  <si>
     <t>relhivbirth</t>
   </si>
   <si>
     <t>Relative likelihood that females with HIV give birth</t>
   </si>
   <si>
-    <t>Relative death rate on ART (unitless, time based adjustment to constant treatment effect)</t>
-  </si>
-  <si>
     <t>allcd4eligibletx </t>
   </si>
   <si>
@@ -1517,6 +1508,15 @@
   </si>
   <si>
     <t>Percentage of people lost to follow-up who are returned to care per year (%/year)</t>
+  </si>
+  <si>
+    <t>Coverage of pregnant women who receive ARV for PMTCT</t>
+  </si>
+  <si>
+    <t>rrcomorbiditydeathtx</t>
+  </si>
+  <si>
+    <t>Relative risk of death rate on ART (unitless, time-based adjustment for treatment of comorbidities)</t>
   </si>
 </sst>
 </file>
@@ -15144,7 +15144,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17729,9 +17729,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q39" sqref="Q39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18292,7 +18292,7 @@
         <v>463</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C23" s="38" t="s">
         <v>96</v>
@@ -20290,10 +20290,10 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="38" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B109" s="38" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C109" s="38" t="s">
         <v>170</v>
@@ -20313,10 +20313,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="38" t="s">
+        <v>480</v>
+      </c>
+      <c r="B110" s="38" t="s">
         <v>481</v>
-      </c>
-      <c r="B110" s="38" t="s">
-        <v>482</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>91</v>
@@ -20336,10 +20336,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="38" t="s">
+        <v>482</v>
+      </c>
+      <c r="B111" s="38" t="s">
         <v>483</v>
-      </c>
-      <c r="B111" s="38" t="s">
-        <v>484</v>
       </c>
       <c r="C111" s="38" t="s">
         <v>84</v>
@@ -20359,10 +20359,10 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="38" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="B112" s="38" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="C112" s="38" t="s">
         <v>91</v>
@@ -20382,10 +20382,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="38" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B113" s="38" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C113" s="38" t="s">
         <v>91</v>
@@ -20463,9 +20463,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M30" sqref="M30"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20949,7 +20949,7 @@
         <v>297</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E24" t="s">
         <v>399</v>
@@ -20989,7 +20989,7 @@
         <v>299</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>479</v>
+        <v>490</v>
       </c>
       <c r="E26" t="s">
         <v>399</v>
@@ -21109,7 +21109,7 @@
         <v>463</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E32" t="s">
         <v>444</v>

</xml_diff>

<commit_message>
Remove a ' ' from a parameter name
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B010A315-B223-4805-A6F4-38A925978A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEC059E-8486-4226-A768-B53CA25A304F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1498,9 +1498,6 @@
     <t>Relative likelihood that females with HIV give birth</t>
   </si>
   <si>
-    <t>allcd4eligibletx </t>
-  </si>
-  <si>
     <t>No CD4 eligibility criteria for treatment from this year</t>
   </si>
   <si>
@@ -1517,6 +1514,9 @@
   </si>
   <si>
     <t>Relative risk of death rate on ART (unitless, time-based adjustment for treatment of comorbidities)</t>
+  </si>
+  <si>
+    <t>allcd4eligibletx</t>
   </si>
 </sst>
 </file>
@@ -17731,7 +17731,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C122" sqref="C122"/>
+      <selection pane="bottomLeft" activeCell="N137" sqref="N137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18292,7 +18292,7 @@
         <v>463</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C23" s="38" t="s">
         <v>96</v>
@@ -20290,10 +20290,10 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="38" t="s">
+        <v>492</v>
+      </c>
+      <c r="B109" s="38" t="s">
         <v>486</v>
-      </c>
-      <c r="B109" s="38" t="s">
-        <v>487</v>
       </c>
       <c r="C109" s="38" t="s">
         <v>170</v>
@@ -20359,10 +20359,10 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="38" t="s">
+        <v>490</v>
+      </c>
+      <c r="B112" s="38" t="s">
         <v>491</v>
-      </c>
-      <c r="B112" s="38" t="s">
-        <v>492</v>
       </c>
       <c r="C112" s="38" t="s">
         <v>91</v>
@@ -20989,7 +20989,7 @@
         <v>299</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E26" t="s">
         <v>399</v>
@@ -21109,7 +21109,7 @@
         <v>463</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E32" t="s">
         <v>444</v>

</xml_diff>

<commit_message>
Fix manual fit settings for projects
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEC059E-8486-4226-A768-B53CA25A304F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE279E9B-ED8C-4DA0-ACE8-5C67CC85F47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -17730,8 +17730,8 @@
   <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N137" sqref="N137"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z88" sqref="Z88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20305,7 +20305,7 @@
         <v>171</v>
       </c>
       <c r="F109" s="38" t="s">
-        <v>92</v>
+        <v>172</v>
       </c>
       <c r="G109" s="38">
         <v>0</v>
@@ -20328,7 +20328,7 @@
         <v>178</v>
       </c>
       <c r="F110" s="38" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="G110" s="38">
         <v>0</v>
@@ -20351,7 +20351,7 @@
         <v>178</v>
       </c>
       <c r="F111" s="38" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="G111" s="38">
         <v>0</v>
@@ -20374,7 +20374,7 @@
         <v>105</v>
       </c>
       <c r="F112" s="38" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G112" s="38">
         <v>0</v>
@@ -20397,7 +20397,7 @@
         <v>178</v>
       </c>
       <c r="F113" s="38" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="G113" s="38">
         <v>0</v>

</xml_diff>

<commit_message>
Add basic immigration to the model and update spreadsheets
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE279E9B-ED8C-4DA0-ACE8-5C67CC85F47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE079279-4F1F-4A7B-9AFE-9056854A3FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="502">
   <si>
     <t>Susceptible</t>
   </si>
@@ -1517,6 +1517,33 @@
   </si>
   <si>
     <t>allcd4eligibletx</t>
+  </si>
+  <si>
+    <t>Migration</t>
+  </si>
+  <si>
+    <t>propemigrate</t>
+  </si>
+  <si>
+    <t>numimmigrate</t>
+  </si>
+  <si>
+    <t>immihivprev</t>
+  </si>
+  <si>
+    <t>immipropdiag</t>
+  </si>
+  <si>
+    <t>Number of people who immigrate into population per year</t>
+  </si>
+  <si>
+    <t>HIV prevalence of immigrants into population per year</t>
+  </si>
+  <si>
+    <t>Proportion of people living with HIV who immigrate who are diagnosed prior to arrival</t>
+  </si>
+  <si>
+    <t>Percentage of people who emigrate per year</t>
   </si>
 </sst>
 </file>
@@ -15144,7 +15171,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17730,8 +17757,8 @@
   <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z88" sqref="Z88"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20404,28 +20431,96 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="38"/>
-      <c r="B114" s="38"/>
-      <c r="C114" s="38"/>
-      <c r="D114" s="38"/>
-      <c r="E114" s="38"/>
-      <c r="F114" s="38"/>
-      <c r="G114" s="38"/>
+      <c r="A114" t="s">
+        <v>494</v>
+      </c>
+      <c r="B114" s="38" t="s">
+        <v>501</v>
+      </c>
+      <c r="C114" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D114" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E114" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F114" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G114" s="38">
+        <v>1</v>
+      </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="6"/>
+      <c r="A115" t="s">
+        <v>495</v>
+      </c>
+      <c r="B115" s="38" t="s">
+        <v>498</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D115" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E115" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F115" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G115" s="38">
+        <v>1</v>
+      </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="6"/>
+      <c r="A116" t="s">
+        <v>496</v>
+      </c>
+      <c r="B116" s="38" t="s">
+        <v>499</v>
+      </c>
+      <c r="C116" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D116" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E116" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F116" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G116" s="38">
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C117" s="6"/>
-      <c r="D117" s="6"/>
-      <c r="E117" s="6"/>
+      <c r="A117" t="s">
+        <v>497</v>
+      </c>
+      <c r="B117" s="38" t="s">
+        <v>500</v>
+      </c>
+      <c r="C117" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D117" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E117" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F117" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G117" s="38">
+        <v>1</v>
+      </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C118" s="6"/>
@@ -20461,11 +20556,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21538,6 +21633,86 @@
         <v>404</v>
       </c>
     </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>493</v>
+      </c>
+      <c r="B54" t="s">
+        <v>307</v>
+      </c>
+      <c r="C54" t="s">
+        <v>494</v>
+      </c>
+      <c r="D54" s="38" t="s">
+        <v>501</v>
+      </c>
+      <c r="E54" t="s">
+        <v>399</v>
+      </c>
+      <c r="F54" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>493</v>
+      </c>
+      <c r="B55" t="s">
+        <v>307</v>
+      </c>
+      <c r="C55" t="s">
+        <v>495</v>
+      </c>
+      <c r="D55" s="38" t="s">
+        <v>498</v>
+      </c>
+      <c r="E55" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="F55" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>493</v>
+      </c>
+      <c r="B56" t="s">
+        <v>307</v>
+      </c>
+      <c r="C56" t="s">
+        <v>496</v>
+      </c>
+      <c r="D56" s="38" t="s">
+        <v>499</v>
+      </c>
+      <c r="E56" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="F56" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>493</v>
+      </c>
+      <c r="B57" t="s">
+        <v>307</v>
+      </c>
+      <c r="C57" t="s">
+        <v>497</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>500</v>
+      </c>
+      <c r="E57" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="F57" t="s">
+        <v>404</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -21549,7 +21724,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update 'numcirc' to default to "general" not "percentage" format in databooks (and to load correctly)
</commit_message>
<xml_diff>
--- a/optima/model-inputs.xlsx
+++ b/optima/model-inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\optima\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE42946-C6C5-42D5-A591-6D99CF7FD4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8405AB57-2F09-41EA-BDAF-C562A963DA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -17753,9 +17753,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G128" sqref="G128"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20536,9 +20536,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54:D57"/>
+      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21405,7 +21405,7 @@
         <v>466</v>
       </c>
       <c r="E43" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="F43" t="s">
         <v>441</v>

</xml_diff>